<commit_message>
Code updated 23-01-30 11:30:32
</commit_message>
<xml_diff>
--- a/Season_Attack/83.xlsx
+++ b/Season_Attack/83.xlsx
@@ -82,8 +82,8 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G163"/>
+  <dimension ref="A1:I164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,6 +426,16 @@
           <t>01-28_0</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>01-29_A</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>01-29_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -452,9 +462,15 @@
       <c r="F2" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>4416</t>
+      <c r="G2" t="n">
+        <v>4416</v>
+      </c>
+      <c r="H2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2515</t>
         </is>
       </c>
     </row>
@@ -483,9 +499,15 @@
       <c r="F3" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>6054</t>
+      <c r="G3" t="n">
+        <v>6054</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2796</t>
         </is>
       </c>
     </row>
@@ -514,9 +536,15 @@
       <c r="F4" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>6411</t>
+      <c r="G4" t="n">
+        <v>6411</v>
+      </c>
+      <c r="H4" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>2939</t>
         </is>
       </c>
     </row>
@@ -545,9 +573,15 @@
       <c r="F5" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>6434</t>
+      <c r="G5" t="n">
+        <v>6434</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2848</t>
         </is>
       </c>
     </row>
@@ -576,9 +610,15 @@
       <c r="F6" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>6299</t>
+      <c r="G6" t="n">
+        <v>6299</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>2791</t>
         </is>
       </c>
     </row>
@@ -604,12 +644,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F7" s="3" t="n">
+      <c r="F7" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>6498</t>
+      <c r="G7" t="n">
+        <v>6498</v>
+      </c>
+      <c r="H7" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>2985</t>
         </is>
       </c>
     </row>
@@ -638,9 +684,15 @@
       <c r="F8" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>5750</t>
+      <c r="G8" t="n">
+        <v>5750</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>2772</t>
         </is>
       </c>
     </row>
@@ -666,12 +718,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F9" s="3" t="n">
+      <c r="F9" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>6188</t>
+      <c r="G9" t="n">
+        <v>6188</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>2815</t>
         </is>
       </c>
     </row>
@@ -697,12 +755,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F10" s="3" t="n">
+      <c r="F10" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>5621</t>
+      <c r="G10" t="n">
+        <v>5621</v>
+      </c>
+      <c r="H10" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>2912</t>
         </is>
       </c>
     </row>
@@ -728,12 +792,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F11" s="3" t="n">
+      <c r="F11" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>7216</t>
+      <c r="G11" t="n">
+        <v>7216</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>2868</t>
         </is>
       </c>
     </row>
@@ -762,9 +832,15 @@
       <c r="F12" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>6389</t>
+      <c r="G12" t="n">
+        <v>6389</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>2812</t>
         </is>
       </c>
     </row>
@@ -790,12 +866,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="F13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>2603</t>
         </is>
       </c>
     </row>
@@ -821,12 +903,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F14" s="3" t="n">
+      <c r="F14" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>7227</t>
+      <c r="G14" t="n">
+        <v>7227</v>
+      </c>
+      <c r="H14" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>3106</t>
         </is>
       </c>
     </row>
@@ -855,9 +943,15 @@
       <c r="F15" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>6048</t>
+      <c r="G15" t="n">
+        <v>6048</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>2811</t>
         </is>
       </c>
     </row>
@@ -883,12 +977,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F16" s="3" t="n">
+      <c r="F16" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>6625</t>
+      <c r="G16" t="n">
+        <v>6625</v>
+      </c>
+      <c r="H16" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>3018</t>
         </is>
       </c>
     </row>
@@ -917,9 +1017,15 @@
       <c r="F17" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>4056</t>
+      <c r="G17" t="n">
+        <v>4056</v>
+      </c>
+      <c r="H17" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>2877</t>
         </is>
       </c>
     </row>
@@ -948,9 +1054,15 @@
       <c r="F18" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>5543</t>
+      <c r="G18" t="n">
+        <v>5543</v>
+      </c>
+      <c r="H18" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>2686</t>
         </is>
       </c>
     </row>
@@ -979,9 +1091,15 @@
       <c r="F19" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>6279</t>
+      <c r="G19" t="n">
+        <v>6279</v>
+      </c>
+      <c r="H19" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>2801</t>
         </is>
       </c>
     </row>
@@ -1007,12 +1125,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F20" s="3" t="n">
+      <c r="F20" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>7329</t>
+      <c r="G20" t="n">
+        <v>7329</v>
+      </c>
+      <c r="H20" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>3034</t>
         </is>
       </c>
     </row>
@@ -1041,9 +1165,15 @@
       <c r="F21" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>6002</t>
+      <c r="G21" t="n">
+        <v>6002</v>
+      </c>
+      <c r="H21" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>2758</t>
         </is>
       </c>
     </row>
@@ -1069,12 +1199,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F22" s="3" t="n">
+      <c r="F22" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>6114</t>
+      <c r="G22" t="n">
+        <v>6114</v>
+      </c>
+      <c r="H22" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>2739</t>
         </is>
       </c>
     </row>
@@ -1103,9 +1239,15 @@
       <c r="F23" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>5670</t>
+      <c r="G23" t="n">
+        <v>5670</v>
+      </c>
+      <c r="H23" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>2677</t>
         </is>
       </c>
     </row>
@@ -1131,12 +1273,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F24" s="3" t="n">
+      <c r="F24" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>6588</t>
+      <c r="G24" t="n">
+        <v>6588</v>
+      </c>
+      <c r="H24" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>2998</t>
         </is>
       </c>
     </row>
@@ -1162,10 +1310,16 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F25" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G25" t="inlineStr">
+      <c r="F25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1193,12 +1347,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F26" s="3" t="n">
+      <c r="F26" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>5947</t>
+      <c r="G26" t="n">
+        <v>5947</v>
+      </c>
+      <c r="H26" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>3092</t>
         </is>
       </c>
     </row>
@@ -1224,12 +1384,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F27" s="3" t="n">
+      <c r="F27" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>6784</t>
+      <c r="G27" t="n">
+        <v>6784</v>
+      </c>
+      <c r="H27" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>2800</t>
         </is>
       </c>
     </row>
@@ -1258,9 +1424,15 @@
       <c r="F28" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>6433</t>
+      <c r="G28" t="n">
+        <v>6433</v>
+      </c>
+      <c r="H28" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>2886</t>
         </is>
       </c>
     </row>
@@ -1270,7 +1442,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>"煙神在此 爾等跪拜 ᶻᵍˣ"</t>
+          <t>"Smok3y Is Back"</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1286,12 +1458,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F29" s="3" t="n">
+      <c r="F29" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>7374</t>
+      <c r="G29" t="n">
+        <v>7374</v>
+      </c>
+      <c r="H29" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>3148</t>
         </is>
       </c>
     </row>
@@ -1320,9 +1498,15 @@
       <c r="F30" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>6317</t>
+      <c r="G30" t="n">
+        <v>6317</v>
+      </c>
+      <c r="H30" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>2886</t>
         </is>
       </c>
     </row>
@@ -1348,12 +1532,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F31" s="3" t="n">
+      <c r="F31" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>6466</t>
+      <c r="G31" t="n">
+        <v>6466</v>
+      </c>
+      <c r="H31" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>2954</t>
         </is>
       </c>
     </row>
@@ -1382,9 +1572,15 @@
       <c r="F32" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>6679</t>
+      <c r="G32" t="n">
+        <v>6679</v>
+      </c>
+      <c r="H32" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>2983</t>
         </is>
       </c>
     </row>
@@ -1413,9 +1609,15 @@
       <c r="F33" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>6658</t>
+      <c r="G33" t="n">
+        <v>6658</v>
+      </c>
+      <c r="H33" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>2796</t>
         </is>
       </c>
     </row>
@@ -1441,12 +1643,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F34" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="F34" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -1472,12 +1680,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F35" s="3" t="n">
+      <c r="F35" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>6798</t>
+      <c r="G35" t="n">
+        <v>6798</v>
+      </c>
+      <c r="H35" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>2996</t>
         </is>
       </c>
     </row>
@@ -1506,9 +1720,15 @@
       <c r="F36" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>6063</t>
+      <c r="G36" t="n">
+        <v>6063</v>
+      </c>
+      <c r="H36" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>2899</t>
         </is>
       </c>
     </row>
@@ -1537,9 +1757,15 @@
       <c r="F37" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>5301</t>
+      <c r="G37" t="n">
+        <v>5301</v>
+      </c>
+      <c r="H37" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>2888</t>
         </is>
       </c>
     </row>
@@ -1565,12 +1791,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F38" s="3" t="n">
+      <c r="F38" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>6215</t>
+      <c r="G38" t="n">
+        <v>6215</v>
+      </c>
+      <c r="H38" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>2927</t>
         </is>
       </c>
     </row>
@@ -1599,9 +1831,15 @@
       <c r="F39" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>5910</t>
+      <c r="G39" t="n">
+        <v>5910</v>
+      </c>
+      <c r="H39" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>2871</t>
         </is>
       </c>
     </row>
@@ -1627,12 +1865,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F40" s="3" t="n">
+      <c r="F40" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>7316</t>
+      <c r="G40" t="n">
+        <v>7316</v>
+      </c>
+      <c r="H40" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>2973</t>
         </is>
       </c>
     </row>
@@ -1661,9 +1905,15 @@
       <c r="F41" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>6103</t>
+      <c r="G41" t="n">
+        <v>6103</v>
+      </c>
+      <c r="H41" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>2818</t>
         </is>
       </c>
     </row>
@@ -1689,12 +1939,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F42" s="3" t="n">
+      <c r="F42" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>7170</t>
+      <c r="G42" t="n">
+        <v>7170</v>
+      </c>
+      <c r="H42" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>2940</t>
         </is>
       </c>
     </row>
@@ -1720,12 +1976,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F43" s="3" t="n">
+      <c r="F43" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>6366</t>
+      <c r="G43" t="n">
+        <v>6366</v>
+      </c>
+      <c r="H43" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>2992</t>
         </is>
       </c>
     </row>
@@ -1751,12 +2013,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F44" s="3" t="n">
+      <c r="F44" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>6177</t>
+      <c r="G44" t="n">
+        <v>6177</v>
+      </c>
+      <c r="H44" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>2997</t>
         </is>
       </c>
     </row>
@@ -1785,9 +2053,15 @@
       <c r="F45" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>5664</t>
+      <c r="G45" t="n">
+        <v>5664</v>
+      </c>
+      <c r="H45" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>2899</t>
         </is>
       </c>
     </row>
@@ -1813,12 +2087,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F46" s="3" t="n">
+      <c r="F46" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>6343</t>
+      <c r="G46" t="n">
+        <v>6343</v>
+      </c>
+      <c r="H46" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>2873</t>
         </is>
       </c>
     </row>
@@ -1844,12 +2124,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F47" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="F47" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0</v>
+      </c>
+      <c r="H47" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>2585</t>
         </is>
       </c>
     </row>
@@ -1875,12 +2161,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F48" s="3" t="n">
+      <c r="F48" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>6514</t>
+      <c r="G48" t="n">
+        <v>6514</v>
+      </c>
+      <c r="H48" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>2877</t>
         </is>
       </c>
     </row>
@@ -1909,9 +2201,15 @@
       <c r="F49" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>5015</t>
+      <c r="G49" t="n">
+        <v>5015</v>
+      </c>
+      <c r="H49" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>2681</t>
         </is>
       </c>
     </row>
@@ -1921,7 +2219,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>㊥JOSE</t>
+          <t>"落日幻影 哈哈哈"</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1937,12 +2235,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F50" s="3" t="n">
+      <c r="F50" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>7116</t>
+      <c r="G50" t="n">
+        <v>7116</v>
+      </c>
+      <c r="H50" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>2880</t>
         </is>
       </c>
     </row>
@@ -1968,12 +2272,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F51" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="F51" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H51" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>2489</t>
         </is>
       </c>
     </row>
@@ -1999,12 +2309,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F52" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>3564</t>
+      <c r="F52" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G52" t="n">
+        <v>3564</v>
+      </c>
+      <c r="H52" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2030,12 +2346,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F53" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>3067</t>
+      <c r="F53" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G53" t="n">
+        <v>3067</v>
+      </c>
+      <c r="H53" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2064,9 +2386,15 @@
       <c r="F54" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>5983</t>
+      <c r="G54" t="n">
+        <v>5983</v>
+      </c>
+      <c r="H54" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>2920</t>
         </is>
       </c>
     </row>
@@ -2092,12 +2420,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F55" s="3" t="n">
+      <c r="F55" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>4614</t>
+      <c r="G55" t="n">
+        <v>4614</v>
+      </c>
+      <c r="H55" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>2819</t>
         </is>
       </c>
     </row>
@@ -2126,9 +2460,15 @@
       <c r="F56" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>4699</t>
+      <c r="G56" t="n">
+        <v>4699</v>
+      </c>
+      <c r="H56" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>2686</t>
         </is>
       </c>
     </row>
@@ -2157,9 +2497,15 @@
       <c r="F57" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>5823</t>
+      <c r="G57" t="n">
+        <v>5823</v>
+      </c>
+      <c r="H57" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>2810</t>
         </is>
       </c>
     </row>
@@ -2185,12 +2531,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F58" s="3" t="n">
+      <c r="F58" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>4843</t>
+      <c r="G58" t="n">
+        <v>4843</v>
+      </c>
+      <c r="H58" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>2788</t>
         </is>
       </c>
     </row>
@@ -2219,9 +2571,15 @@
       <c r="F59" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>5336</t>
+      <c r="G59" t="n">
+        <v>5336</v>
+      </c>
+      <c r="H59" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>2772</t>
         </is>
       </c>
     </row>
@@ -2247,10 +2605,16 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F60" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G60" t="inlineStr">
+      <c r="F60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G60" t="n">
+        <v>0</v>
+      </c>
+      <c r="H60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I60" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2278,12 +2642,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F61" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>5381</t>
+      <c r="F61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" t="n">
+        <v>5381</v>
+      </c>
+      <c r="H61" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>2820</t>
         </is>
       </c>
     </row>
@@ -2309,12 +2679,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F62" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>3781</t>
+      <c r="F62" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G62" t="n">
+        <v>3781</v>
+      </c>
+      <c r="H62" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>2510</t>
         </is>
       </c>
     </row>
@@ -2340,12 +2716,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F63" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>3304</t>
+      <c r="F63" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G63" t="n">
+        <v>3304</v>
+      </c>
+      <c r="H63" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>2439</t>
         </is>
       </c>
     </row>
@@ -2374,9 +2756,15 @@
       <c r="F64" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>5409</t>
+      <c r="G64" t="n">
+        <v>5409</v>
+      </c>
+      <c r="H64" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>2786</t>
         </is>
       </c>
     </row>
@@ -2402,12 +2790,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F65" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>2930</t>
+      <c r="F65" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G65" t="n">
+        <v>2930</v>
+      </c>
+      <c r="H65" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2436,9 +2830,15 @@
       <c r="F66" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>6284</t>
+      <c r="G66" t="n">
+        <v>6284</v>
+      </c>
+      <c r="H66" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>2836</t>
         </is>
       </c>
     </row>
@@ -2467,9 +2867,15 @@
       <c r="F67" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>4744</t>
+      <c r="G67" t="n">
+        <v>4744</v>
+      </c>
+      <c r="H67" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>2786</t>
         </is>
       </c>
     </row>
@@ -2498,9 +2904,15 @@
       <c r="F68" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>4676</t>
+      <c r="G68" t="n">
+        <v>4676</v>
+      </c>
+      <c r="H68" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>2519</t>
         </is>
       </c>
     </row>
@@ -2529,9 +2941,15 @@
       <c r="F69" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>4824</t>
+      <c r="G69" t="n">
+        <v>4824</v>
+      </c>
+      <c r="H69" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>2739</t>
         </is>
       </c>
     </row>
@@ -2560,9 +2978,15 @@
       <c r="F70" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>4425</t>
+      <c r="G70" t="n">
+        <v>4425</v>
+      </c>
+      <c r="H70" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>2658</t>
         </is>
       </c>
     </row>
@@ -2591,9 +3015,15 @@
       <c r="F71" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>4630</t>
+      <c r="G71" t="n">
+        <v>4630</v>
+      </c>
+      <c r="H71" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>2680</t>
         </is>
       </c>
     </row>
@@ -2622,9 +3052,15 @@
       <c r="F72" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>4589</t>
+      <c r="G72" t="n">
+        <v>4589</v>
+      </c>
+      <c r="H72" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>2552</t>
         </is>
       </c>
     </row>
@@ -2653,9 +3089,15 @@
       <c r="F73" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>4173</t>
+      <c r="G73" t="n">
+        <v>4173</v>
+      </c>
+      <c r="H73" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>2659</t>
         </is>
       </c>
     </row>
@@ -2684,9 +3126,15 @@
       <c r="F74" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>5373</t>
+      <c r="G74" t="n">
+        <v>5373</v>
+      </c>
+      <c r="H74" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>2759</t>
         </is>
       </c>
     </row>
@@ -2715,9 +3163,15 @@
       <c r="F75" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>5715</t>
+      <c r="G75" t="n">
+        <v>5715</v>
+      </c>
+      <c r="H75" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>2828</t>
         </is>
       </c>
     </row>
@@ -2743,10 +3197,16 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F76" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G76" t="inlineStr">
+      <c r="F76" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G76" t="n">
+        <v>0</v>
+      </c>
+      <c r="H76" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I76" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2777,9 +3237,15 @@
       <c r="F77" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>5508</t>
+      <c r="G77" t="n">
+        <v>5508</v>
+      </c>
+      <c r="H77" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>2930</t>
         </is>
       </c>
     </row>
@@ -2805,10 +3271,16 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F78" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G78" t="inlineStr">
+      <c r="F78" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G78" t="n">
+        <v>0</v>
+      </c>
+      <c r="H78" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2839,9 +3311,15 @@
       <c r="F79" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>5063</t>
+      <c r="G79" t="n">
+        <v>5063</v>
+      </c>
+      <c r="H79" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>2774</t>
         </is>
       </c>
     </row>
@@ -2867,12 +3345,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F80" s="3" t="n">
+      <c r="F80" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>5279</t>
+      <c r="G80" t="n">
+        <v>5279</v>
+      </c>
+      <c r="H80" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>2886</t>
         </is>
       </c>
     </row>
@@ -2898,12 +3382,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F81" s="3" t="n">
+      <c r="F81" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>5198</t>
+      <c r="G81" t="n">
+        <v>5198</v>
+      </c>
+      <c r="H81" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>2900</t>
         </is>
       </c>
     </row>
@@ -2932,9 +3422,15 @@
       <c r="F82" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>4807</t>
+      <c r="G82" t="n">
+        <v>4807</v>
+      </c>
+      <c r="H82" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>2802</t>
         </is>
       </c>
     </row>
@@ -2960,14 +3456,14 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F83" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>4528</t>
-        </is>
-      </c>
+      <c r="F83" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G83" t="n">
+        <v>4528</v>
+      </c>
+      <c r="H83" s="2" t="inlineStr"/>
+      <c r="I83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -2991,12 +3487,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F84" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>3931</t>
+      <c r="F84" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G84" t="n">
+        <v>3931</v>
+      </c>
+      <c r="H84" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>2572</t>
         </is>
       </c>
     </row>
@@ -3025,9 +3527,15 @@
       <c r="F85" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>3968</t>
+      <c r="G85" t="n">
+        <v>3968</v>
+      </c>
+      <c r="H85" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>2494</t>
         </is>
       </c>
     </row>
@@ -3056,9 +3564,15 @@
       <c r="F86" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>5085</t>
+      <c r="G86" t="n">
+        <v>5085</v>
+      </c>
+      <c r="H86" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>2970</t>
         </is>
       </c>
     </row>
@@ -3087,9 +3601,15 @@
       <c r="F87" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G87" t="inlineStr">
-        <is>
-          <t>3160</t>
+      <c r="G87" t="n">
+        <v>3160</v>
+      </c>
+      <c r="H87" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>2525</t>
         </is>
       </c>
     </row>
@@ -3118,9 +3638,15 @@
       <c r="F88" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G88" t="inlineStr">
-        <is>
-          <t>3631</t>
+      <c r="G88" t="n">
+        <v>3631</v>
+      </c>
+      <c r="H88" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>2589</t>
         </is>
       </c>
     </row>
@@ -3144,6 +3670,8 @@
       <c r="E89" t="inlineStr"/>
       <c r="F89" s="2" t="inlineStr"/>
       <c r="G89" t="inlineStr"/>
+      <c r="H89" s="2" t="inlineStr"/>
+      <c r="I89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -3170,9 +3698,15 @@
       <c r="F90" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>2878</t>
+      <c r="G90" t="n">
+        <v>2878</v>
+      </c>
+      <c r="H90" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>2454</t>
         </is>
       </c>
     </row>
@@ -3198,12 +3732,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F91" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>2102</t>
+      <c r="F91" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G91" t="n">
+        <v>2102</v>
+      </c>
+      <c r="H91" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3232,9 +3772,15 @@
       <c r="F92" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>3037</t>
+      <c r="G92" t="n">
+        <v>3037</v>
+      </c>
+      <c r="H92" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>2513</t>
         </is>
       </c>
     </row>
@@ -3263,9 +3809,15 @@
       <c r="F93" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>2969</t>
+      <c r="G93" t="n">
+        <v>2969</v>
+      </c>
+      <c r="H93" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>2470</t>
         </is>
       </c>
     </row>
@@ -3291,12 +3843,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F94" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G94" t="inlineStr">
-        <is>
-          <t>3193</t>
+      <c r="F94" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G94" t="n">
+        <v>3193</v>
+      </c>
+      <c r="H94" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3322,12 +3880,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F95" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>2386</t>
+      <c r="F95" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G95" t="n">
+        <v>2386</v>
+      </c>
+      <c r="H95" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>1984</t>
         </is>
       </c>
     </row>
@@ -3353,12 +3917,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F96" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>2417</t>
+      <c r="F96" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G96" t="n">
+        <v>2417</v>
+      </c>
+      <c r="H96" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>1993</t>
         </is>
       </c>
     </row>
@@ -3387,9 +3957,15 @@
       <c r="F97" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>4278</t>
+      <c r="G97" t="n">
+        <v>4278</v>
+      </c>
+      <c r="H97" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>2480</t>
         </is>
       </c>
     </row>
@@ -3418,9 +3994,15 @@
       <c r="F98" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>2094</t>
+      <c r="G98" t="n">
+        <v>2094</v>
+      </c>
+      <c r="H98" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>2278</t>
         </is>
       </c>
     </row>
@@ -3449,9 +4031,15 @@
       <c r="F99" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G99" t="inlineStr">
-        <is>
-          <t>4103</t>
+      <c r="G99" t="n">
+        <v>4103</v>
+      </c>
+      <c r="H99" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>2638</t>
         </is>
       </c>
     </row>
@@ -3480,9 +4068,15 @@
       <c r="F100" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="G100" t="inlineStr">
-        <is>
-          <t>2587</t>
+      <c r="G100" t="n">
+        <v>2587</v>
+      </c>
+      <c r="H100" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>2470</t>
         </is>
       </c>
     </row>
@@ -3511,9 +4105,15 @@
       <c r="F101" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="G101" t="inlineStr">
-        <is>
-          <t>4671</t>
+      <c r="G101" t="n">
+        <v>4671</v>
+      </c>
+      <c r="H101" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>2776</t>
         </is>
       </c>
     </row>
@@ -3542,9 +4142,15 @@
       <c r="F102" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G102" t="inlineStr">
-        <is>
-          <t>4238</t>
+      <c r="G102" t="n">
+        <v>4238</v>
+      </c>
+      <c r="H102" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>2645</t>
         </is>
       </c>
     </row>
@@ -3573,9 +4179,15 @@
       <c r="F103" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="G103" t="inlineStr">
-        <is>
-          <t>4418</t>
+      <c r="G103" t="n">
+        <v>4418</v>
+      </c>
+      <c r="H103" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>2623</t>
         </is>
       </c>
     </row>
@@ -3604,9 +4216,15 @@
       <c r="F104" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="G104" t="inlineStr">
-        <is>
-          <t>4645</t>
+      <c r="G104" t="n">
+        <v>4645</v>
+      </c>
+      <c r="H104" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>2830</t>
         </is>
       </c>
     </row>
@@ -3635,9 +4253,15 @@
       <c r="F105" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="G105" t="inlineStr">
-        <is>
-          <t>4487</t>
+      <c r="G105" t="n">
+        <v>4487</v>
+      </c>
+      <c r="H105" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>2703</t>
         </is>
       </c>
     </row>
@@ -3666,9 +4290,15 @@
       <c r="F106" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G106" t="inlineStr">
-        <is>
-          <t>2754</t>
+      <c r="G106" t="n">
+        <v>2754</v>
+      </c>
+      <c r="H106" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>2501</t>
         </is>
       </c>
     </row>
@@ -3694,12 +4324,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F107" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G107" t="inlineStr">
-        <is>
-          <t>2839</t>
+      <c r="F107" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G107" t="n">
+        <v>2839</v>
+      </c>
+      <c r="H107" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3728,9 +4364,15 @@
       <c r="F108" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="G108" t="inlineStr">
-        <is>
-          <t>6067</t>
+      <c r="G108" t="n">
+        <v>6067</v>
+      </c>
+      <c r="H108" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -3759,9 +4401,15 @@
       <c r="F109" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G109" t="inlineStr">
-        <is>
-          <t>4147</t>
+      <c r="G109" t="n">
+        <v>4147</v>
+      </c>
+      <c r="H109" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>2736</t>
         </is>
       </c>
     </row>
@@ -3790,9 +4438,15 @@
       <c r="F110" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G110" t="inlineStr">
-        <is>
-          <t>4010</t>
+      <c r="G110" t="n">
+        <v>4010</v>
+      </c>
+      <c r="H110" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>2668</t>
         </is>
       </c>
     </row>
@@ -3818,12 +4472,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F111" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G111" t="inlineStr">
-        <is>
-          <t>2824</t>
+      <c r="F111" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G111" t="n">
+        <v>2824</v>
+      </c>
+      <c r="H111" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3849,12 +4509,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F112" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G112" t="inlineStr">
-        <is>
-          <t>3632</t>
+      <c r="F112" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G112" t="n">
+        <v>3632</v>
+      </c>
+      <c r="H112" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>2478</t>
         </is>
       </c>
     </row>
@@ -3880,12 +4546,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F113" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G113" t="inlineStr">
-        <is>
-          <t>3749</t>
+      <c r="F113" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G113" t="n">
+        <v>3749</v>
+      </c>
+      <c r="H113" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>2551</t>
         </is>
       </c>
     </row>
@@ -3911,12 +4583,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F114" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G114" t="inlineStr">
-        <is>
-          <t>3877</t>
+      <c r="F114" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G114" t="n">
+        <v>3877</v>
+      </c>
+      <c r="H114" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3945,9 +4623,15 @@
       <c r="F115" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G115" t="inlineStr">
-        <is>
-          <t>4616</t>
+      <c r="G115" t="n">
+        <v>4616</v>
+      </c>
+      <c r="H115" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>2738</t>
         </is>
       </c>
     </row>
@@ -3976,9 +4660,15 @@
       <c r="F116" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="G116" t="inlineStr">
-        <is>
-          <t>2662</t>
+      <c r="G116" t="n">
+        <v>2662</v>
+      </c>
+      <c r="H116" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>2510</t>
         </is>
       </c>
     </row>
@@ -4007,9 +4697,15 @@
       <c r="F117" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="G117" t="inlineStr">
-        <is>
-          <t>3202</t>
+      <c r="G117" t="n">
+        <v>3202</v>
+      </c>
+      <c r="H117" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>2509</t>
         </is>
       </c>
     </row>
@@ -4038,9 +4734,15 @@
       <c r="F118" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G118" t="inlineStr">
-        <is>
-          <t>3884</t>
+      <c r="G118" t="n">
+        <v>3884</v>
+      </c>
+      <c r="H118" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>2763</t>
         </is>
       </c>
     </row>
@@ -4066,12 +4768,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F119" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G119" t="inlineStr">
-        <is>
-          <t>3190</t>
+      <c r="F119" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G119" t="n">
+        <v>3190</v>
+      </c>
+      <c r="H119" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4097,12 +4805,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F120" s="3" t="n">
+      <c r="F120" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="G120" t="inlineStr">
-        <is>
-          <t>4123</t>
+      <c r="G120" t="n">
+        <v>4123</v>
+      </c>
+      <c r="H120" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>2760</t>
         </is>
       </c>
     </row>
@@ -4131,9 +4845,15 @@
       <c r="F121" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G121" t="inlineStr">
-        <is>
-          <t>3533</t>
+      <c r="G121" t="n">
+        <v>3533</v>
+      </c>
+      <c r="H121" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>2484</t>
         </is>
       </c>
     </row>
@@ -4162,9 +4882,15 @@
       <c r="F122" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="G122" t="inlineStr">
-        <is>
-          <t>4037</t>
+      <c r="G122" t="n">
+        <v>4037</v>
+      </c>
+      <c r="H122" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>2542</t>
         </is>
       </c>
     </row>
@@ -4193,9 +4919,15 @@
       <c r="F123" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="G123" t="inlineStr">
-        <is>
-          <t>3148</t>
+      <c r="G123" t="n">
+        <v>3148</v>
+      </c>
+      <c r="H123" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>2539</t>
         </is>
       </c>
     </row>
@@ -4224,9 +4956,15 @@
       <c r="F124" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="G124" t="inlineStr">
-        <is>
-          <t>3404</t>
+      <c r="G124" t="n">
+        <v>3404</v>
+      </c>
+      <c r="H124" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>2568</t>
         </is>
       </c>
     </row>
@@ -4255,9 +4993,15 @@
       <c r="F125" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G125" t="inlineStr">
-        <is>
-          <t>3470</t>
+      <c r="G125" t="n">
+        <v>3470</v>
+      </c>
+      <c r="H125" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I125" t="inlineStr">
+        <is>
+          <t>2521</t>
         </is>
       </c>
     </row>
@@ -4286,9 +5030,15 @@
       <c r="F126" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G126" t="inlineStr">
-        <is>
-          <t>3951</t>
+      <c r="G126" t="n">
+        <v>3951</v>
+      </c>
+      <c r="H126" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>2692</t>
         </is>
       </c>
     </row>
@@ -4314,12 +5064,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F127" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G127" t="inlineStr">
-        <is>
-          <t>3354</t>
+      <c r="F127" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G127" t="n">
+        <v>3354</v>
+      </c>
+      <c r="H127" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I127" t="inlineStr">
+        <is>
+          <t>2547</t>
         </is>
       </c>
     </row>
@@ -4345,12 +5101,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F128" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G128" t="inlineStr">
-        <is>
-          <t>2095</t>
+      <c r="F128" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G128" t="n">
+        <v>2095</v>
+      </c>
+      <c r="H128" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I128" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4376,12 +5138,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F129" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G129" t="inlineStr">
-        <is>
-          <t>2463</t>
+      <c r="F129" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G129" t="n">
+        <v>2463</v>
+      </c>
+      <c r="H129" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I129" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4410,9 +5178,15 @@
       <c r="F130" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="G130" t="inlineStr">
-        <is>
-          <t>3035</t>
+      <c r="G130" t="n">
+        <v>3035</v>
+      </c>
+      <c r="H130" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I130" t="inlineStr">
+        <is>
+          <t>2504</t>
         </is>
       </c>
     </row>
@@ -4438,12 +5212,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F131" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G131" t="inlineStr">
-        <is>
-          <t>2744</t>
+      <c r="F131" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G131" t="n">
+        <v>2744</v>
+      </c>
+      <c r="H131" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I131" t="inlineStr">
+        <is>
+          <t>2424</t>
         </is>
       </c>
     </row>
@@ -4472,9 +5252,15 @@
       <c r="F132" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="G132" t="inlineStr">
-        <is>
-          <t>1062</t>
+      <c r="G132" t="n">
+        <v>1062</v>
+      </c>
+      <c r="H132" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I132" t="inlineStr">
+        <is>
+          <t>1020</t>
         </is>
       </c>
     </row>
@@ -4503,9 +5289,15 @@
       <c r="F133" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="G133" t="inlineStr">
-        <is>
-          <t>2417</t>
+      <c r="G133" t="n">
+        <v>2417</v>
+      </c>
+      <c r="H133" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I133" t="inlineStr">
+        <is>
+          <t>2013</t>
         </is>
       </c>
     </row>
@@ -4534,9 +5326,15 @@
       <c r="F134" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="G134" t="inlineStr">
-        <is>
-          <t>3982</t>
+      <c r="G134" t="n">
+        <v>3982</v>
+      </c>
+      <c r="H134" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="I134" t="inlineStr">
+        <is>
+          <t>2584</t>
         </is>
       </c>
     </row>
@@ -4562,10 +5360,16 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F135" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G135" t="inlineStr">
+      <c r="F135" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G135" t="n">
+        <v>0</v>
+      </c>
+      <c r="H135" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I135" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4593,12 +5397,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F136" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G136" t="inlineStr">
-        <is>
-          <t>996</t>
+      <c r="F136" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G136" t="n">
+        <v>996</v>
+      </c>
+      <c r="H136" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I136" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4624,12 +5434,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F137" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G137" t="inlineStr">
-        <is>
-          <t>2051</t>
+      <c r="F137" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G137" t="n">
+        <v>2051</v>
+      </c>
+      <c r="H137" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I137" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4652,15 +5468,21 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F138" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="G138" t="inlineStr">
-        <is>
-          <t>3162</t>
+      <c r="G138" t="n">
+        <v>3162</v>
+      </c>
+      <c r="H138" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I138" t="inlineStr">
+        <is>
+          <t>2591</t>
         </is>
       </c>
     </row>
@@ -4686,12 +5508,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F139" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G139" t="inlineStr">
-        <is>
-          <t>3128</t>
+      <c r="F139" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G139" t="n">
+        <v>3128</v>
+      </c>
+      <c r="H139" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I139" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4720,9 +5548,15 @@
       <c r="F140" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="G140" t="inlineStr">
-        <is>
-          <t>2902</t>
+      <c r="G140" t="n">
+        <v>2902</v>
+      </c>
+      <c r="H140" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I140" t="inlineStr">
+        <is>
+          <t>2454</t>
         </is>
       </c>
     </row>
@@ -4748,12 +5582,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F141" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G141" t="inlineStr">
-        <is>
-          <t>2373</t>
+      <c r="F141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G141" t="n">
+        <v>2373</v>
+      </c>
+      <c r="H141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I141" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4779,12 +5619,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F142" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G142" t="inlineStr">
-        <is>
-          <t>2482</t>
+      <c r="F142" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G142" t="n">
+        <v>2482</v>
+      </c>
+      <c r="H142" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I142" t="inlineStr">
+        <is>
+          <t>2317</t>
         </is>
       </c>
     </row>
@@ -4810,12 +5656,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F143" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G143" t="inlineStr">
-        <is>
-          <t>1883</t>
+      <c r="F143" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G143" t="n">
+        <v>1883</v>
+      </c>
+      <c r="H143" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I143" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4841,12 +5693,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F144" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G144" t="inlineStr">
-        <is>
-          <t>2892</t>
+      <c r="F144" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G144" t="n">
+        <v>2892</v>
+      </c>
+      <c r="H144" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="I144" t="inlineStr">
+        <is>
+          <t>2499</t>
         </is>
       </c>
     </row>
@@ -4872,10 +5730,16 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F145" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G145" t="inlineStr">
+      <c r="F145" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G145" t="n">
+        <v>0</v>
+      </c>
+      <c r="H145" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I145" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4903,12 +5767,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F146" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G146" t="inlineStr">
-        <is>
-          <t>2164</t>
+      <c r="F146" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G146" t="n">
+        <v>2164</v>
+      </c>
+      <c r="H146" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I146" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4934,12 +5804,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F147" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G147" t="inlineStr">
-        <is>
-          <t>2030</t>
+      <c r="F147" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G147" t="n">
+        <v>2030</v>
+      </c>
+      <c r="H147" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I147" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4965,10 +5841,16 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F148" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G148" t="inlineStr">
+      <c r="F148" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G148" t="n">
+        <v>0</v>
+      </c>
+      <c r="H148" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4996,10 +5878,16 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F149" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G149" t="inlineStr">
+      <c r="F149" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G149" t="n">
+        <v>0</v>
+      </c>
+      <c r="H149" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I149" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5027,12 +5915,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F150" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G150" t="inlineStr">
-        <is>
-          <t>2445</t>
+      <c r="F150" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G150" t="n">
+        <v>2445</v>
+      </c>
+      <c r="H150" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I150" t="inlineStr">
+        <is>
+          <t>1997</t>
         </is>
       </c>
     </row>
@@ -5058,12 +5952,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F151" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G151" t="inlineStr">
-        <is>
-          <t>1587</t>
+      <c r="F151" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G151" t="n">
+        <v>1587</v>
+      </c>
+      <c r="H151" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I151" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -5092,9 +5992,15 @@
       <c r="F152" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G152" t="inlineStr">
-        <is>
-          <t>1733</t>
+      <c r="G152" t="n">
+        <v>1733</v>
+      </c>
+      <c r="H152" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I152" t="inlineStr">
+        <is>
+          <t>1500</t>
         </is>
       </c>
     </row>
@@ -5123,7 +6029,13 @@
       <c r="F153" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="G153" t="inlineStr">
+      <c r="G153" t="n">
+        <v>1637</v>
+      </c>
+      <c r="H153" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="I153" t="inlineStr">
         <is>
           <t>1637</t>
         </is>
@@ -5151,12 +6063,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F154" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G154" t="inlineStr">
-        <is>
-          <t>1304</t>
+      <c r="F154" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G154" t="n">
+        <v>1304</v>
+      </c>
+      <c r="H154" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I154" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -5185,9 +6103,15 @@
       <c r="F155" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="G155" t="inlineStr">
-        <is>
-          <t>5823</t>
+      <c r="G155" t="n">
+        <v>5823</v>
+      </c>
+      <c r="H155" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="I155" t="inlineStr">
+        <is>
+          <t>2629</t>
         </is>
       </c>
     </row>
@@ -5213,10 +6137,16 @@
           <t>Chinese</t>
         </is>
       </c>
-      <c r="F156" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G156" t="inlineStr">
+      <c r="F156" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G156" t="n">
+        <v>0</v>
+      </c>
+      <c r="H156" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I156" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5244,10 +6174,16 @@
           <t>Chinese</t>
         </is>
       </c>
-      <c r="F157" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G157" t="inlineStr">
+      <c r="F157" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G157" t="n">
+        <v>0</v>
+      </c>
+      <c r="H157" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I157" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5278,11 +6214,11 @@
       <c r="F158" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="G158" t="inlineStr">
-        <is>
-          <t>6282</t>
-        </is>
-      </c>
+      <c r="G158" t="n">
+        <v>6282</v>
+      </c>
+      <c r="H158" s="2" t="inlineStr"/>
+      <c r="I158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" t="n">
@@ -5306,10 +6242,16 @@
           <t>Chinese</t>
         </is>
       </c>
-      <c r="F159" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G159" t="inlineStr">
+      <c r="F159" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G159" t="n">
+        <v>0</v>
+      </c>
+      <c r="H159" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I159" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5337,12 +6279,18 @@
           <t>Chinese</t>
         </is>
       </c>
-      <c r="F160" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G160" t="inlineStr">
-        <is>
-          <t>3430</t>
+      <c r="F160" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G160" t="n">
+        <v>3430</v>
+      </c>
+      <c r="H160" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I160" t="inlineStr">
+        <is>
+          <t>2525</t>
         </is>
       </c>
     </row>
@@ -5368,10 +6316,16 @@
           <t>Chinese</t>
         </is>
       </c>
-      <c r="F161" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G161" t="inlineStr">
+      <c r="F161" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G161" t="n">
+        <v>0</v>
+      </c>
+      <c r="H161" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I161" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5399,12 +6353,18 @@
           <t>Chinese</t>
         </is>
       </c>
-      <c r="F162" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G162" t="inlineStr">
-        <is>
-          <t>3206</t>
+      <c r="F162" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G162" t="n">
+        <v>3206</v>
+      </c>
+      <c r="H162" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I162" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -5430,12 +6390,47 @@
           <t>Chinese</t>
         </is>
       </c>
-      <c r="F163" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G163" t="inlineStr">
-        <is>
-          <t>2636</t>
+      <c r="F163" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G163" t="n">
+        <v>2636</v>
+      </c>
+      <c r="H163" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I163" t="inlineStr">
+        <is>
+          <t>2503</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>58605234</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>八嘎呀路</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr"/>
+      <c r="D164" t="inlineStr"/>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F164" s="2" t="inlineStr"/>
+      <c r="G164" t="inlineStr"/>
+      <c r="H164" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="I164" t="inlineStr">
+        <is>
+          <t>2008</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-01-31 11:30:32
</commit_message>
<xml_diff>
--- a/Season_Attack/83.xlsx
+++ b/Season_Attack/83.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I164"/>
+  <dimension ref="A1:K164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,6 +436,16 @@
           <t>01-29_0</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>01-30_A</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>01-30_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -468,9 +478,15 @@
       <c r="H2" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>2515</t>
+      <c r="I2" t="n">
+        <v>2515</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>2779</t>
         </is>
       </c>
     </row>
@@ -505,9 +521,15 @@
       <c r="H3" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>2796</t>
+      <c r="I3" t="n">
+        <v>2796</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>3081</t>
         </is>
       </c>
     </row>
@@ -542,9 +564,15 @@
       <c r="H4" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>2939</t>
+      <c r="I4" t="n">
+        <v>2939</v>
+      </c>
+      <c r="J4" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>3341</t>
         </is>
       </c>
     </row>
@@ -579,9 +607,15 @@
       <c r="H5" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>2848</t>
+      <c r="I5" t="n">
+        <v>2848</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>3168</t>
         </is>
       </c>
     </row>
@@ -616,9 +650,15 @@
       <c r="H6" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>2791</t>
+      <c r="I6" t="n">
+        <v>2791</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>3058</t>
         </is>
       </c>
     </row>
@@ -653,9 +693,15 @@
       <c r="H7" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>2985</t>
+      <c r="I7" t="n">
+        <v>2985</v>
+      </c>
+      <c r="J7" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>3329</t>
         </is>
       </c>
     </row>
@@ -690,9 +736,15 @@
       <c r="H8" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>2772</t>
+      <c r="I8" t="n">
+        <v>2772</v>
+      </c>
+      <c r="J8" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>3042</t>
         </is>
       </c>
     </row>
@@ -727,9 +779,15 @@
       <c r="H9" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>2815</t>
+      <c r="I9" t="n">
+        <v>2815</v>
+      </c>
+      <c r="J9" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>3014</t>
         </is>
       </c>
     </row>
@@ -764,9 +822,15 @@
       <c r="H10" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>2912</t>
+      <c r="I10" t="n">
+        <v>2912</v>
+      </c>
+      <c r="J10" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>3131</t>
         </is>
       </c>
     </row>
@@ -801,9 +865,15 @@
       <c r="H11" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>2868</t>
+      <c r="I11" t="n">
+        <v>2868</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>3273</t>
         </is>
       </c>
     </row>
@@ -838,9 +908,15 @@
       <c r="H12" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>2812</t>
+      <c r="I12" t="n">
+        <v>2812</v>
+      </c>
+      <c r="J12" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>3047</t>
         </is>
       </c>
     </row>
@@ -875,7 +951,13 @@
       <c r="H13" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="I13" t="n">
+        <v>2603</v>
+      </c>
+      <c r="J13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="inlineStr">
         <is>
           <t>2603</t>
         </is>
@@ -912,9 +994,15 @@
       <c r="H14" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>3106</t>
+      <c r="I14" t="n">
+        <v>3106</v>
+      </c>
+      <c r="J14" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>3541</t>
         </is>
       </c>
     </row>
@@ -949,9 +1037,15 @@
       <c r="H15" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>2811</t>
+      <c r="I15" t="n">
+        <v>2811</v>
+      </c>
+      <c r="J15" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>3135</t>
         </is>
       </c>
     </row>
@@ -986,9 +1080,15 @@
       <c r="H16" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>3018</t>
+      <c r="I16" t="n">
+        <v>3018</v>
+      </c>
+      <c r="J16" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>3332</t>
         </is>
       </c>
     </row>
@@ -1023,9 +1123,15 @@
       <c r="H17" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>2877</t>
+      <c r="I17" t="n">
+        <v>2877</v>
+      </c>
+      <c r="J17" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>3016</t>
         </is>
       </c>
     </row>
@@ -1060,9 +1166,15 @@
       <c r="H18" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>2686</t>
+      <c r="I18" t="n">
+        <v>2686</v>
+      </c>
+      <c r="J18" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>3011</t>
         </is>
       </c>
     </row>
@@ -1097,9 +1209,15 @@
       <c r="H19" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>2801</t>
+      <c r="I19" t="n">
+        <v>2801</v>
+      </c>
+      <c r="J19" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>3090</t>
         </is>
       </c>
     </row>
@@ -1134,9 +1252,15 @@
       <c r="H20" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>3034</t>
+      <c r="I20" t="n">
+        <v>3034</v>
+      </c>
+      <c r="J20" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>3451</t>
         </is>
       </c>
     </row>
@@ -1171,9 +1295,15 @@
       <c r="H21" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>2758</t>
+      <c r="I21" t="n">
+        <v>2758</v>
+      </c>
+      <c r="J21" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>2780</t>
         </is>
       </c>
     </row>
@@ -1208,9 +1338,15 @@
       <c r="H22" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>2739</t>
+      <c r="I22" t="n">
+        <v>2739</v>
+      </c>
+      <c r="J22" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>3184</t>
         </is>
       </c>
     </row>
@@ -1245,9 +1381,15 @@
       <c r="H23" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>2677</t>
+      <c r="I23" t="n">
+        <v>2677</v>
+      </c>
+      <c r="J23" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>2664</t>
         </is>
       </c>
     </row>
@@ -1282,9 +1424,15 @@
       <c r="H24" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>2998</t>
+      <c r="I24" t="n">
+        <v>2998</v>
+      </c>
+      <c r="J24" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>3292</t>
         </is>
       </c>
     </row>
@@ -1319,7 +1467,13 @@
       <c r="H25" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I25" t="inlineStr">
+      <c r="I25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1356,9 +1510,15 @@
       <c r="H26" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>3092</t>
+      <c r="I26" t="n">
+        <v>3092</v>
+      </c>
+      <c r="J26" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>3472</t>
         </is>
       </c>
     </row>
@@ -1393,9 +1553,15 @@
       <c r="H27" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>2800</t>
+      <c r="I27" t="n">
+        <v>2800</v>
+      </c>
+      <c r="J27" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>3143</t>
         </is>
       </c>
     </row>
@@ -1430,9 +1596,15 @@
       <c r="H28" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>2886</t>
+      <c r="I28" t="n">
+        <v>2886</v>
+      </c>
+      <c r="J28" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>2989</t>
         </is>
       </c>
     </row>
@@ -1467,9 +1639,15 @@
       <c r="H29" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>3148</t>
+      <c r="I29" t="n">
+        <v>3148</v>
+      </c>
+      <c r="J29" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>3547</t>
         </is>
       </c>
     </row>
@@ -1504,9 +1682,15 @@
       <c r="H30" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>2886</t>
+      <c r="I30" t="n">
+        <v>2886</v>
+      </c>
+      <c r="J30" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>3253</t>
         </is>
       </c>
     </row>
@@ -1541,9 +1725,15 @@
       <c r="H31" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>2954</t>
+      <c r="I31" t="n">
+        <v>2954</v>
+      </c>
+      <c r="J31" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>3302</t>
         </is>
       </c>
     </row>
@@ -1578,9 +1768,15 @@
       <c r="H32" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>2983</t>
+      <c r="I32" t="n">
+        <v>2983</v>
+      </c>
+      <c r="J32" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>3456</t>
         </is>
       </c>
     </row>
@@ -1615,9 +1811,15 @@
       <c r="H33" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>2796</t>
+      <c r="I33" t="n">
+        <v>2796</v>
+      </c>
+      <c r="J33" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>3148</t>
         </is>
       </c>
     </row>
@@ -1652,7 +1854,13 @@
       <c r="H34" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I34" t="inlineStr">
+      <c r="I34" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J34" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1689,9 +1897,15 @@
       <c r="H35" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>2996</t>
+      <c r="I35" t="n">
+        <v>2996</v>
+      </c>
+      <c r="J35" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>3416</t>
         </is>
       </c>
     </row>
@@ -1726,9 +1940,15 @@
       <c r="H36" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>2899</t>
+      <c r="I36" t="n">
+        <v>2899</v>
+      </c>
+      <c r="J36" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>3206</t>
         </is>
       </c>
     </row>
@@ -1763,9 +1983,15 @@
       <c r="H37" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>2888</t>
+      <c r="I37" t="n">
+        <v>2888</v>
+      </c>
+      <c r="J37" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>3209</t>
         </is>
       </c>
     </row>
@@ -1800,9 +2026,15 @@
       <c r="H38" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>2927</t>
+      <c r="I38" t="n">
+        <v>2927</v>
+      </c>
+      <c r="J38" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>3333</t>
         </is>
       </c>
     </row>
@@ -1837,9 +2069,15 @@
       <c r="H39" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>2871</t>
+      <c r="I39" t="n">
+        <v>2871</v>
+      </c>
+      <c r="J39" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>3123</t>
         </is>
       </c>
     </row>
@@ -1874,9 +2112,15 @@
       <c r="H40" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>2973</t>
+      <c r="I40" t="n">
+        <v>2973</v>
+      </c>
+      <c r="J40" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>3349</t>
         </is>
       </c>
     </row>
@@ -1911,9 +2155,15 @@
       <c r="H41" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I41" t="inlineStr">
-        <is>
-          <t>2818</t>
+      <c r="I41" t="n">
+        <v>2818</v>
+      </c>
+      <c r="J41" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>3135</t>
         </is>
       </c>
     </row>
@@ -1948,9 +2198,15 @@
       <c r="H42" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>2940</t>
+      <c r="I42" t="n">
+        <v>2940</v>
+      </c>
+      <c r="J42" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>3389</t>
         </is>
       </c>
     </row>
@@ -1985,9 +2241,15 @@
       <c r="H43" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>2992</t>
+      <c r="I43" t="n">
+        <v>2992</v>
+      </c>
+      <c r="J43" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>3334</t>
         </is>
       </c>
     </row>
@@ -2022,9 +2284,15 @@
       <c r="H44" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>2997</t>
+      <c r="I44" t="n">
+        <v>2997</v>
+      </c>
+      <c r="J44" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>3422</t>
         </is>
       </c>
     </row>
@@ -2059,9 +2327,15 @@
       <c r="H45" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I45" t="inlineStr">
-        <is>
-          <t>2899</t>
+      <c r="I45" t="n">
+        <v>2899</v>
+      </c>
+      <c r="J45" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>3148</t>
         </is>
       </c>
     </row>
@@ -2096,9 +2370,15 @@
       <c r="H46" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I46" t="inlineStr">
-        <is>
-          <t>2873</t>
+      <c r="I46" t="n">
+        <v>2873</v>
+      </c>
+      <c r="J46" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>3146</t>
         </is>
       </c>
     </row>
@@ -2133,9 +2413,15 @@
       <c r="H47" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="I47" t="inlineStr">
-        <is>
-          <t>2585</t>
+      <c r="I47" t="n">
+        <v>2585</v>
+      </c>
+      <c r="J47" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>2601</t>
         </is>
       </c>
     </row>
@@ -2170,9 +2456,15 @@
       <c r="H48" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>2877</t>
+      <c r="I48" t="n">
+        <v>2877</v>
+      </c>
+      <c r="J48" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>3206</t>
         </is>
       </c>
     </row>
@@ -2207,9 +2499,15 @@
       <c r="H49" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I49" t="inlineStr">
-        <is>
-          <t>2681</t>
+      <c r="I49" t="n">
+        <v>2681</v>
+      </c>
+      <c r="J49" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>3001</t>
         </is>
       </c>
     </row>
@@ -2244,9 +2542,15 @@
       <c r="H50" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="I50" t="inlineStr">
-        <is>
-          <t>2880</t>
+      <c r="I50" t="n">
+        <v>2880</v>
+      </c>
+      <c r="J50" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>3245</t>
         </is>
       </c>
     </row>
@@ -2281,9 +2585,15 @@
       <c r="H51" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I51" t="inlineStr">
-        <is>
-          <t>2489</t>
+      <c r="I51" t="n">
+        <v>2489</v>
+      </c>
+      <c r="J51" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>2701</t>
         </is>
       </c>
     </row>
@@ -2318,9 +2628,15 @@
       <c r="H52" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I52" t="n">
+        <v>0</v>
+      </c>
+      <c r="J52" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>2515</t>
         </is>
       </c>
     </row>
@@ -2355,9 +2671,15 @@
       <c r="H53" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I53" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I53" t="n">
+        <v>0</v>
+      </c>
+      <c r="J53" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>2512</t>
         </is>
       </c>
     </row>
@@ -2392,9 +2714,15 @@
       <c r="H54" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I54" t="inlineStr">
-        <is>
-          <t>2920</t>
+      <c r="I54" t="n">
+        <v>2920</v>
+      </c>
+      <c r="J54" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>3377</t>
         </is>
       </c>
     </row>
@@ -2429,9 +2757,15 @@
       <c r="H55" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I55" t="inlineStr">
-        <is>
-          <t>2819</t>
+      <c r="I55" t="n">
+        <v>2819</v>
+      </c>
+      <c r="J55" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>2915</t>
         </is>
       </c>
     </row>
@@ -2466,9 +2800,15 @@
       <c r="H56" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="I56" t="inlineStr">
-        <is>
-          <t>2686</t>
+      <c r="I56" t="n">
+        <v>2686</v>
+      </c>
+      <c r="J56" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>2900</t>
         </is>
       </c>
     </row>
@@ -2503,9 +2843,15 @@
       <c r="H57" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I57" t="inlineStr">
-        <is>
-          <t>2810</t>
+      <c r="I57" t="n">
+        <v>2810</v>
+      </c>
+      <c r="J57" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>3111</t>
         </is>
       </c>
     </row>
@@ -2540,9 +2886,15 @@
       <c r="H58" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I58" t="inlineStr">
-        <is>
-          <t>2788</t>
+      <c r="I58" t="n">
+        <v>2788</v>
+      </c>
+      <c r="J58" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>2886</t>
         </is>
       </c>
     </row>
@@ -2577,9 +2929,15 @@
       <c r="H59" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I59" t="inlineStr">
-        <is>
-          <t>2772</t>
+      <c r="I59" t="n">
+        <v>2772</v>
+      </c>
+      <c r="J59" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>3037</t>
         </is>
       </c>
     </row>
@@ -2614,7 +2972,13 @@
       <c r="H60" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I60" t="inlineStr">
+      <c r="I60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K60" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2651,9 +3015,15 @@
       <c r="H61" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I61" t="inlineStr">
-        <is>
-          <t>2820</t>
+      <c r="I61" t="n">
+        <v>2820</v>
+      </c>
+      <c r="J61" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>3155</t>
         </is>
       </c>
     </row>
@@ -2688,7 +3058,13 @@
       <c r="H62" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I62" t="inlineStr">
+      <c r="I62" t="n">
+        <v>2510</v>
+      </c>
+      <c r="J62" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K62" t="inlineStr">
         <is>
           <t>2510</t>
         </is>
@@ -2725,9 +3101,15 @@
       <c r="H63" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I63" t="inlineStr">
-        <is>
-          <t>2439</t>
+      <c r="I63" t="n">
+        <v>2439</v>
+      </c>
+      <c r="J63" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>2403</t>
         </is>
       </c>
     </row>
@@ -2762,9 +3144,15 @@
       <c r="H64" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="I64" t="inlineStr">
-        <is>
-          <t>2786</t>
+      <c r="I64" t="n">
+        <v>2786</v>
+      </c>
+      <c r="J64" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>3094</t>
         </is>
       </c>
     </row>
@@ -2799,7 +3187,13 @@
       <c r="H65" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I65" t="inlineStr">
+      <c r="I65" t="n">
+        <v>0</v>
+      </c>
+      <c r="J65" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K65" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2836,9 +3230,15 @@
       <c r="H66" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I66" t="inlineStr">
-        <is>
-          <t>2836</t>
+      <c r="I66" t="n">
+        <v>2836</v>
+      </c>
+      <c r="J66" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>3061</t>
         </is>
       </c>
     </row>
@@ -2873,9 +3273,15 @@
       <c r="H67" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="I67" t="inlineStr">
-        <is>
-          <t>2786</t>
+      <c r="I67" t="n">
+        <v>2786</v>
+      </c>
+      <c r="J67" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>2956</t>
         </is>
       </c>
     </row>
@@ -2910,9 +3316,15 @@
       <c r="H68" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I68" t="inlineStr">
-        <is>
-          <t>2519</t>
+      <c r="I68" t="n">
+        <v>2519</v>
+      </c>
+      <c r="J68" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>2516</t>
         </is>
       </c>
     </row>
@@ -2947,9 +3359,15 @@
       <c r="H69" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="I69" t="inlineStr">
-        <is>
-          <t>2739</t>
+      <c r="I69" t="n">
+        <v>2739</v>
+      </c>
+      <c r="J69" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>2957</t>
         </is>
       </c>
     </row>
@@ -2984,9 +3402,15 @@
       <c r="H70" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="I70" t="inlineStr">
-        <is>
-          <t>2658</t>
+      <c r="I70" t="n">
+        <v>2658</v>
+      </c>
+      <c r="J70" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>2838</t>
         </is>
       </c>
     </row>
@@ -3021,9 +3445,15 @@
       <c r="H71" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I71" t="inlineStr">
-        <is>
-          <t>2680</t>
+      <c r="I71" t="n">
+        <v>2680</v>
+      </c>
+      <c r="J71" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>2928</t>
         </is>
       </c>
     </row>
@@ -3058,9 +3488,15 @@
       <c r="H72" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I72" t="inlineStr">
-        <is>
-          <t>2552</t>
+      <c r="I72" t="n">
+        <v>2552</v>
+      </c>
+      <c r="J72" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>2573</t>
         </is>
       </c>
     </row>
@@ -3095,9 +3531,15 @@
       <c r="H73" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="I73" t="inlineStr">
-        <is>
-          <t>2659</t>
+      <c r="I73" t="n">
+        <v>2659</v>
+      </c>
+      <c r="J73" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>2869</t>
         </is>
       </c>
     </row>
@@ -3120,7 +3562,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F74" s="5" t="n">
@@ -3132,9 +3574,15 @@
       <c r="H74" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="I74" t="inlineStr">
-        <is>
-          <t>2759</t>
+      <c r="I74" t="n">
+        <v>2759</v>
+      </c>
+      <c r="J74" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>3027</t>
         </is>
       </c>
     </row>
@@ -3169,9 +3617,15 @@
       <c r="H75" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I75" t="inlineStr">
-        <is>
-          <t>2828</t>
+      <c r="I75" t="n">
+        <v>2828</v>
+      </c>
+      <c r="J75" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>3085</t>
         </is>
       </c>
     </row>
@@ -3206,7 +3660,13 @@
       <c r="H76" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I76" t="inlineStr">
+      <c r="I76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J76" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K76" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3243,9 +3703,15 @@
       <c r="H77" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I77" t="inlineStr">
-        <is>
-          <t>2930</t>
+      <c r="I77" t="n">
+        <v>2930</v>
+      </c>
+      <c r="J77" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>3210</t>
         </is>
       </c>
     </row>
@@ -3280,9 +3746,15 @@
       <c r="H78" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I78" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I78" t="n">
+        <v>0</v>
+      </c>
+      <c r="J78" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -3317,9 +3789,15 @@
       <c r="H79" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="I79" t="inlineStr">
-        <is>
-          <t>2774</t>
+      <c r="I79" t="n">
+        <v>2774</v>
+      </c>
+      <c r="J79" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>2994</t>
         </is>
       </c>
     </row>
@@ -3354,9 +3832,15 @@
       <c r="H80" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I80" t="inlineStr">
-        <is>
-          <t>2886</t>
+      <c r="I80" t="n">
+        <v>2886</v>
+      </c>
+      <c r="J80" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>3067</t>
         </is>
       </c>
     </row>
@@ -3391,9 +3875,15 @@
       <c r="H81" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="I81" t="inlineStr">
-        <is>
-          <t>2900</t>
+      <c r="I81" t="n">
+        <v>2900</v>
+      </c>
+      <c r="J81" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>3018</t>
         </is>
       </c>
     </row>
@@ -3428,9 +3918,15 @@
       <c r="H82" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="I82" t="inlineStr">
-        <is>
-          <t>2802</t>
+      <c r="I82" t="n">
+        <v>2802</v>
+      </c>
+      <c r="J82" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>3035</t>
         </is>
       </c>
     </row>
@@ -3464,6 +3960,8 @@
       </c>
       <c r="H83" s="2" t="inlineStr"/>
       <c r="I83" t="inlineStr"/>
+      <c r="J83" s="2" t="inlineStr"/>
+      <c r="K83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -3496,9 +3994,15 @@
       <c r="H84" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I84" t="inlineStr">
-        <is>
-          <t>2572</t>
+      <c r="I84" t="n">
+        <v>2572</v>
+      </c>
+      <c r="J84" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>2715</t>
         </is>
       </c>
     </row>
@@ -3533,9 +4037,15 @@
       <c r="H85" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I85" t="inlineStr">
-        <is>
-          <t>2494</t>
+      <c r="I85" t="n">
+        <v>2494</v>
+      </c>
+      <c r="J85" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>2504</t>
         </is>
       </c>
     </row>
@@ -3570,9 +4080,15 @@
       <c r="H86" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I86" t="inlineStr">
-        <is>
-          <t>2970</t>
+      <c r="I86" t="n">
+        <v>2970</v>
+      </c>
+      <c r="J86" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>3141</t>
         </is>
       </c>
     </row>
@@ -3607,9 +4123,15 @@
       <c r="H87" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I87" t="inlineStr">
-        <is>
-          <t>2525</t>
+      <c r="I87" t="n">
+        <v>2525</v>
+      </c>
+      <c r="J87" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>2558</t>
         </is>
       </c>
     </row>
@@ -3644,9 +4166,15 @@
       <c r="H88" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="I88" t="inlineStr">
-        <is>
-          <t>2589</t>
+      <c r="I88" t="n">
+        <v>2589</v>
+      </c>
+      <c r="J88" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>2521</t>
         </is>
       </c>
     </row>
@@ -3672,6 +4200,8 @@
       <c r="G89" t="inlineStr"/>
       <c r="H89" s="2" t="inlineStr"/>
       <c r="I89" t="inlineStr"/>
+      <c r="J89" s="2" t="inlineStr"/>
+      <c r="K89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -3704,9 +4234,15 @@
       <c r="H90" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I90" t="inlineStr">
-        <is>
-          <t>2454</t>
+      <c r="I90" t="n">
+        <v>2454</v>
+      </c>
+      <c r="J90" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>2456</t>
         </is>
       </c>
     </row>
@@ -3741,7 +4277,13 @@
       <c r="H91" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I91" t="inlineStr">
+      <c r="I91" t="n">
+        <v>0</v>
+      </c>
+      <c r="J91" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3778,9 +4320,15 @@
       <c r="H92" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I92" t="inlineStr">
-        <is>
-          <t>2513</t>
+      <c r="I92" t="n">
+        <v>2513</v>
+      </c>
+      <c r="J92" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>2601</t>
         </is>
       </c>
     </row>
@@ -3815,9 +4363,15 @@
       <c r="H93" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I93" t="inlineStr">
-        <is>
-          <t>2470</t>
+      <c r="I93" t="n">
+        <v>2470</v>
+      </c>
+      <c r="J93" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>2610</t>
         </is>
       </c>
     </row>
@@ -3852,7 +4406,13 @@
       <c r="H94" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I94" t="inlineStr">
+      <c r="I94" t="n">
+        <v>0</v>
+      </c>
+      <c r="J94" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3889,9 +4449,15 @@
       <c r="H95" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I95" t="inlineStr">
-        <is>
-          <t>1984</t>
+      <c r="I95" t="n">
+        <v>1984</v>
+      </c>
+      <c r="J95" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>2038</t>
         </is>
       </c>
     </row>
@@ -3926,9 +4492,15 @@
       <c r="H96" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I96" t="inlineStr">
-        <is>
-          <t>1993</t>
+      <c r="I96" t="n">
+        <v>1993</v>
+      </c>
+      <c r="J96" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>2012</t>
         </is>
       </c>
     </row>
@@ -3963,9 +4535,15 @@
       <c r="H97" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I97" t="inlineStr">
-        <is>
-          <t>2480</t>
+      <c r="I97" t="n">
+        <v>2480</v>
+      </c>
+      <c r="J97" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>2467</t>
         </is>
       </c>
     </row>
@@ -4000,9 +4578,15 @@
       <c r="H98" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I98" t="inlineStr">
-        <is>
-          <t>2278</t>
+      <c r="I98" t="n">
+        <v>2278</v>
+      </c>
+      <c r="J98" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>2267</t>
         </is>
       </c>
     </row>
@@ -4037,9 +4621,15 @@
       <c r="H99" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I99" t="inlineStr">
-        <is>
-          <t>2638</t>
+      <c r="I99" t="n">
+        <v>2638</v>
+      </c>
+      <c r="J99" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>2746</t>
         </is>
       </c>
     </row>
@@ -4074,9 +4664,15 @@
       <c r="H100" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I100" t="inlineStr">
-        <is>
-          <t>2470</t>
+      <c r="I100" t="n">
+        <v>2470</v>
+      </c>
+      <c r="J100" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>2424</t>
         </is>
       </c>
     </row>
@@ -4111,9 +4707,15 @@
       <c r="H101" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I101" t="inlineStr">
-        <is>
-          <t>2776</t>
+      <c r="I101" t="n">
+        <v>2776</v>
+      </c>
+      <c r="J101" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>3038</t>
         </is>
       </c>
     </row>
@@ -4148,9 +4750,15 @@
       <c r="H102" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I102" t="inlineStr">
-        <is>
-          <t>2645</t>
+      <c r="I102" t="n">
+        <v>2645</v>
+      </c>
+      <c r="J102" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>2851</t>
         </is>
       </c>
     </row>
@@ -4185,9 +4793,15 @@
       <c r="H103" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="I103" t="inlineStr">
-        <is>
-          <t>2623</t>
+      <c r="I103" t="n">
+        <v>2623</v>
+      </c>
+      <c r="J103" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>2813</t>
         </is>
       </c>
     </row>
@@ -4222,9 +4836,15 @@
       <c r="H104" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I104" t="inlineStr">
-        <is>
-          <t>2830</t>
+      <c r="I104" t="n">
+        <v>2830</v>
+      </c>
+      <c r="J104" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="K104" t="inlineStr">
+        <is>
+          <t>3045</t>
         </is>
       </c>
     </row>
@@ -4259,9 +4879,15 @@
       <c r="H105" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="I105" t="inlineStr">
-        <is>
-          <t>2703</t>
+      <c r="I105" t="n">
+        <v>2703</v>
+      </c>
+      <c r="J105" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="K105" t="inlineStr">
+        <is>
+          <t>2802</t>
         </is>
       </c>
     </row>
@@ -4296,9 +4922,15 @@
       <c r="H106" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I106" t="inlineStr">
-        <is>
-          <t>2501</t>
+      <c r="I106" t="n">
+        <v>2501</v>
+      </c>
+      <c r="J106" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>2464</t>
         </is>
       </c>
     </row>
@@ -4333,7 +4965,13 @@
       <c r="H107" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I107" t="inlineStr">
+      <c r="I107" t="n">
+        <v>0</v>
+      </c>
+      <c r="J107" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K107" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4370,9 +5008,15 @@
       <c r="H108" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I108" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="I108" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J108" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K108" t="inlineStr">
+        <is>
+          <t>2496</t>
         </is>
       </c>
     </row>
@@ -4407,9 +5051,15 @@
       <c r="H109" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I109" t="inlineStr">
-        <is>
-          <t>2736</t>
+      <c r="I109" t="n">
+        <v>2736</v>
+      </c>
+      <c r="J109" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>2774</t>
         </is>
       </c>
     </row>
@@ -4444,9 +5094,15 @@
       <c r="H110" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I110" t="inlineStr">
-        <is>
-          <t>2668</t>
+      <c r="I110" t="n">
+        <v>2668</v>
+      </c>
+      <c r="J110" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="K110" t="inlineStr">
+        <is>
+          <t>2711</t>
         </is>
       </c>
     </row>
@@ -4481,9 +5137,15 @@
       <c r="H111" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I111" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I111" t="n">
+        <v>0</v>
+      </c>
+      <c r="J111" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K111" t="inlineStr">
+        <is>
+          <t>2499</t>
         </is>
       </c>
     </row>
@@ -4518,9 +5180,15 @@
       <c r="H112" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I112" t="inlineStr">
-        <is>
-          <t>2478</t>
+      <c r="I112" t="n">
+        <v>2478</v>
+      </c>
+      <c r="J112" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K112" t="inlineStr">
+        <is>
+          <t>2479</t>
         </is>
       </c>
     </row>
@@ -4555,9 +5223,15 @@
       <c r="H113" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I113" t="inlineStr">
-        <is>
-          <t>2551</t>
+      <c r="I113" t="n">
+        <v>2551</v>
+      </c>
+      <c r="J113" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>2710</t>
         </is>
       </c>
     </row>
@@ -4592,9 +5266,15 @@
       <c r="H114" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I114" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I114" t="n">
+        <v>0</v>
+      </c>
+      <c r="J114" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K114" t="inlineStr">
+        <is>
+          <t>2557</t>
         </is>
       </c>
     </row>
@@ -4629,9 +5309,15 @@
       <c r="H115" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I115" t="inlineStr">
-        <is>
-          <t>2738</t>
+      <c r="I115" t="n">
+        <v>2738</v>
+      </c>
+      <c r="J115" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>2892</t>
         </is>
       </c>
     </row>
@@ -4666,9 +5352,15 @@
       <c r="H116" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="I116" t="inlineStr">
-        <is>
-          <t>2510</t>
+      <c r="I116" t="n">
+        <v>2510</v>
+      </c>
+      <c r="J116" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>2490</t>
         </is>
       </c>
     </row>
@@ -4703,9 +5395,15 @@
       <c r="H117" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="I117" t="inlineStr">
-        <is>
-          <t>2509</t>
+      <c r="I117" t="n">
+        <v>2509</v>
+      </c>
+      <c r="J117" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>2522</t>
         </is>
       </c>
     </row>
@@ -4740,9 +5438,15 @@
       <c r="H118" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="I118" t="inlineStr">
-        <is>
-          <t>2763</t>
+      <c r="I118" t="n">
+        <v>2763</v>
+      </c>
+      <c r="J118" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="K118" t="inlineStr">
+        <is>
+          <t>2839</t>
         </is>
       </c>
     </row>
@@ -4777,7 +5481,13 @@
       <c r="H119" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I119" t="inlineStr">
+      <c r="I119" t="n">
+        <v>0</v>
+      </c>
+      <c r="J119" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K119" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4814,9 +5524,15 @@
       <c r="H120" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="I120" t="inlineStr">
-        <is>
-          <t>2760</t>
+      <c r="I120" t="n">
+        <v>2760</v>
+      </c>
+      <c r="J120" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="K120" t="inlineStr">
+        <is>
+          <t>2813</t>
         </is>
       </c>
     </row>
@@ -4851,9 +5567,15 @@
       <c r="H121" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I121" t="inlineStr">
-        <is>
-          <t>2484</t>
+      <c r="I121" t="n">
+        <v>2484</v>
+      </c>
+      <c r="J121" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K121" t="inlineStr">
+        <is>
+          <t>2611</t>
         </is>
       </c>
     </row>
@@ -4888,9 +5610,15 @@
       <c r="H122" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I122" t="inlineStr">
-        <is>
-          <t>2542</t>
+      <c r="I122" t="n">
+        <v>2542</v>
+      </c>
+      <c r="J122" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K122" t="inlineStr">
+        <is>
+          <t>2540</t>
         </is>
       </c>
     </row>
@@ -4925,9 +5653,15 @@
       <c r="H123" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I123" t="inlineStr">
-        <is>
-          <t>2539</t>
+      <c r="I123" t="n">
+        <v>2539</v>
+      </c>
+      <c r="J123" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K123" t="inlineStr">
+        <is>
+          <t>2642</t>
         </is>
       </c>
     </row>
@@ -4962,9 +5696,15 @@
       <c r="H124" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I124" t="inlineStr">
-        <is>
-          <t>2568</t>
+      <c r="I124" t="n">
+        <v>2568</v>
+      </c>
+      <c r="J124" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K124" t="inlineStr">
+        <is>
+          <t>2671</t>
         </is>
       </c>
     </row>
@@ -4999,9 +5739,15 @@
       <c r="H125" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I125" t="inlineStr">
-        <is>
-          <t>2521</t>
+      <c r="I125" t="n">
+        <v>2521</v>
+      </c>
+      <c r="J125" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K125" t="inlineStr">
+        <is>
+          <t>2592</t>
         </is>
       </c>
     </row>
@@ -5036,9 +5782,15 @@
       <c r="H126" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I126" t="inlineStr">
-        <is>
-          <t>2692</t>
+      <c r="I126" t="n">
+        <v>2692</v>
+      </c>
+      <c r="J126" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K126" t="inlineStr">
+        <is>
+          <t>2781</t>
         </is>
       </c>
     </row>
@@ -5073,9 +5825,15 @@
       <c r="H127" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I127" t="inlineStr">
-        <is>
-          <t>2547</t>
+      <c r="I127" t="n">
+        <v>2547</v>
+      </c>
+      <c r="J127" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K127" t="inlineStr">
+        <is>
+          <t>2489</t>
         </is>
       </c>
     </row>
@@ -5110,7 +5868,13 @@
       <c r="H128" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I128" t="inlineStr">
+      <c r="I128" t="n">
+        <v>0</v>
+      </c>
+      <c r="J128" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5147,7 +5911,13 @@
       <c r="H129" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I129" t="inlineStr">
+      <c r="I129" t="n">
+        <v>0</v>
+      </c>
+      <c r="J129" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5184,9 +5954,15 @@
       <c r="H130" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I130" t="inlineStr">
-        <is>
-          <t>2504</t>
+      <c r="I130" t="n">
+        <v>2504</v>
+      </c>
+      <c r="J130" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K130" t="inlineStr">
+        <is>
+          <t>2558</t>
         </is>
       </c>
     </row>
@@ -5221,9 +5997,15 @@
       <c r="H131" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I131" t="inlineStr">
-        <is>
-          <t>2424</t>
+      <c r="I131" t="n">
+        <v>2424</v>
+      </c>
+      <c r="J131" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K131" t="inlineStr">
+        <is>
+          <t>2380</t>
         </is>
       </c>
     </row>
@@ -5258,9 +6040,15 @@
       <c r="H132" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="I132" t="inlineStr">
-        <is>
-          <t>1020</t>
+      <c r="I132" t="n">
+        <v>1020</v>
+      </c>
+      <c r="J132" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K132" t="inlineStr">
+        <is>
+          <t>1040</t>
         </is>
       </c>
     </row>
@@ -5295,9 +6083,15 @@
       <c r="H133" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="I133" t="inlineStr">
-        <is>
-          <t>2013</t>
+      <c r="I133" t="n">
+        <v>2013</v>
+      </c>
+      <c r="J133" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="K133" t="inlineStr">
+        <is>
+          <t>2067</t>
         </is>
       </c>
     </row>
@@ -5332,9 +6126,15 @@
       <c r="H134" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="I134" t="inlineStr">
-        <is>
-          <t>2584</t>
+      <c r="I134" t="n">
+        <v>2584</v>
+      </c>
+      <c r="J134" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="K134" t="inlineStr">
+        <is>
+          <t>2762</t>
         </is>
       </c>
     </row>
@@ -5369,7 +6169,13 @@
       <c r="H135" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I135" t="inlineStr">
+      <c r="I135" t="n">
+        <v>0</v>
+      </c>
+      <c r="J135" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K135" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5406,7 +6212,13 @@
       <c r="H136" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I136" t="inlineStr">
+      <c r="I136" t="n">
+        <v>0</v>
+      </c>
+      <c r="J136" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K136" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5443,7 +6255,13 @@
       <c r="H137" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I137" t="inlineStr">
+      <c r="I137" t="n">
+        <v>0</v>
+      </c>
+      <c r="J137" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5480,9 +6298,15 @@
       <c r="H138" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="I138" t="inlineStr">
-        <is>
-          <t>2591</t>
+      <c r="I138" t="n">
+        <v>2591</v>
+      </c>
+      <c r="J138" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K138" t="inlineStr">
+        <is>
+          <t>2761</t>
         </is>
       </c>
     </row>
@@ -5517,7 +6341,13 @@
       <c r="H139" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I139" t="inlineStr">
+      <c r="I139" t="n">
+        <v>0</v>
+      </c>
+      <c r="J139" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K139" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5554,9 +6384,15 @@
       <c r="H140" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I140" t="inlineStr">
-        <is>
-          <t>2454</t>
+      <c r="I140" t="n">
+        <v>2454</v>
+      </c>
+      <c r="J140" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="K140" t="inlineStr">
+        <is>
+          <t>2564</t>
         </is>
       </c>
     </row>
@@ -5591,7 +6427,13 @@
       <c r="H141" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I141" t="inlineStr">
+      <c r="I141" t="n">
+        <v>0</v>
+      </c>
+      <c r="J141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K141" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5628,9 +6470,15 @@
       <c r="H142" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="I142" t="inlineStr">
-        <is>
-          <t>2317</t>
+      <c r="I142" t="n">
+        <v>2317</v>
+      </c>
+      <c r="J142" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="K142" t="inlineStr">
+        <is>
+          <t>2508</t>
         </is>
       </c>
     </row>
@@ -5665,7 +6513,13 @@
       <c r="H143" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I143" t="inlineStr">
+      <c r="I143" t="n">
+        <v>0</v>
+      </c>
+      <c r="J143" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K143" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5702,9 +6556,15 @@
       <c r="H144" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="I144" t="inlineStr">
-        <is>
-          <t>2499</t>
+      <c r="I144" t="n">
+        <v>2499</v>
+      </c>
+      <c r="J144" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K144" t="inlineStr">
+        <is>
+          <t>2453</t>
         </is>
       </c>
     </row>
@@ -5739,7 +6599,13 @@
       <c r="H145" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I145" t="inlineStr">
+      <c r="I145" t="n">
+        <v>0</v>
+      </c>
+      <c r="J145" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K145" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5776,7 +6642,13 @@
       <c r="H146" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I146" t="inlineStr">
+      <c r="I146" t="n">
+        <v>0</v>
+      </c>
+      <c r="J146" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5813,7 +6685,13 @@
       <c r="H147" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I147" t="inlineStr">
+      <c r="I147" t="n">
+        <v>0</v>
+      </c>
+      <c r="J147" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K147" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5850,7 +6728,13 @@
       <c r="H148" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I148" t="inlineStr">
+      <c r="I148" t="n">
+        <v>0</v>
+      </c>
+      <c r="J148" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5887,7 +6771,13 @@
       <c r="H149" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I149" t="inlineStr">
+      <c r="I149" t="n">
+        <v>0</v>
+      </c>
+      <c r="J149" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K149" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5924,9 +6814,15 @@
       <c r="H150" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="I150" t="inlineStr">
-        <is>
-          <t>1997</t>
+      <c r="I150" t="n">
+        <v>1997</v>
+      </c>
+      <c r="J150" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="K150" t="inlineStr">
+        <is>
+          <t>2224</t>
         </is>
       </c>
     </row>
@@ -5961,9 +6857,15 @@
       <c r="H151" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I151" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I151" t="n">
+        <v>0</v>
+      </c>
+      <c r="J151" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K151" t="inlineStr">
+        <is>
+          <t>1500</t>
         </is>
       </c>
     </row>
@@ -5998,9 +6900,15 @@
       <c r="H152" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I152" t="inlineStr">
-        <is>
-          <t>1500</t>
+      <c r="I152" t="n">
+        <v>1500</v>
+      </c>
+      <c r="J152" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="K152" t="inlineStr">
+        <is>
+          <t>1581</t>
         </is>
       </c>
     </row>
@@ -6035,9 +6943,15 @@
       <c r="H153" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="I153" t="inlineStr">
-        <is>
-          <t>1637</t>
+      <c r="I153" t="n">
+        <v>1637</v>
+      </c>
+      <c r="J153" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="K153" t="inlineStr">
+        <is>
+          <t>1689</t>
         </is>
       </c>
     </row>
@@ -6072,7 +6986,13 @@
       <c r="H154" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I154" t="inlineStr">
+      <c r="I154" t="n">
+        <v>0</v>
+      </c>
+      <c r="J154" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6109,9 +7029,15 @@
       <c r="H155" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="I155" t="inlineStr">
-        <is>
-          <t>2629</t>
+      <c r="I155" t="n">
+        <v>2629</v>
+      </c>
+      <c r="J155" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="K155" t="inlineStr">
+        <is>
+          <t>2807</t>
         </is>
       </c>
     </row>
@@ -6146,7 +7072,13 @@
       <c r="H156" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I156" t="inlineStr">
+      <c r="I156" t="n">
+        <v>0</v>
+      </c>
+      <c r="J156" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K156" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6183,7 +7115,13 @@
       <c r="H157" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I157" t="inlineStr">
+      <c r="I157" t="n">
+        <v>0</v>
+      </c>
+      <c r="J157" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K157" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6219,6 +7157,14 @@
       </c>
       <c r="H158" s="2" t="inlineStr"/>
       <c r="I158" t="inlineStr"/>
+      <c r="J158" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K158" t="inlineStr">
+        <is>
+          <t>3283</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="n">
@@ -6251,7 +7197,13 @@
       <c r="H159" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I159" t="inlineStr">
+      <c r="I159" t="n">
+        <v>0</v>
+      </c>
+      <c r="J159" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K159" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6288,9 +7240,15 @@
       <c r="H160" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I160" t="inlineStr">
-        <is>
-          <t>2525</t>
+      <c r="I160" t="n">
+        <v>2525</v>
+      </c>
+      <c r="J160" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K160" t="inlineStr">
+        <is>
+          <t>2550</t>
         </is>
       </c>
     </row>
@@ -6325,7 +7283,13 @@
       <c r="H161" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I161" t="inlineStr">
+      <c r="I161" t="n">
+        <v>0</v>
+      </c>
+      <c r="J161" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K161" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6362,7 +7326,13 @@
       <c r="H162" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I162" t="inlineStr">
+      <c r="I162" t="n">
+        <v>0</v>
+      </c>
+      <c r="J162" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K162" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6399,17 +7369,21 @@
       <c r="H163" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="I163" t="inlineStr">
-        <is>
-          <t>2503</t>
+      <c r="I163" t="n">
+        <v>2503</v>
+      </c>
+      <c r="J163" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K163" t="inlineStr">
+        <is>
+          <t>2470</t>
         </is>
       </c>
     </row>
     <row r="164">
-      <c r="A164" t="inlineStr">
-        <is>
-          <t>58605234</t>
-        </is>
+      <c r="A164" t="n">
+        <v>58605234</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
@@ -6428,9 +7402,15 @@
       <c r="H164" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="I164" t="inlineStr">
-        <is>
-          <t>2008</t>
+      <c r="I164" t="n">
+        <v>2008</v>
+      </c>
+      <c r="J164" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K164" t="inlineStr">
+        <is>
+          <t>1994</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-02-01 11:30:32
</commit_message>
<xml_diff>
--- a/Season_Attack/83.xlsx
+++ b/Season_Attack/83.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K164"/>
+  <dimension ref="A1:M166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,6 +446,16 @@
           <t>01-30_0</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>01-31_A</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>01-31_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -484,9 +494,15 @@
       <c r="J2" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>2779</t>
+      <c r="K2" t="n">
+        <v>2779</v>
+      </c>
+      <c r="L2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>2763</t>
         </is>
       </c>
     </row>
@@ -527,9 +543,15 @@
       <c r="J3" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>3081</t>
+      <c r="K3" t="n">
+        <v>3081</v>
+      </c>
+      <c r="L3" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>3358</t>
         </is>
       </c>
     </row>
@@ -570,9 +592,15 @@
       <c r="J4" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>3341</t>
+      <c r="K4" t="n">
+        <v>3341</v>
+      </c>
+      <c r="L4" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>3651</t>
         </is>
       </c>
     </row>
@@ -613,9 +641,15 @@
       <c r="J5" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>3168</t>
+      <c r="K5" t="n">
+        <v>3168</v>
+      </c>
+      <c r="L5" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>3477</t>
         </is>
       </c>
     </row>
@@ -656,9 +690,15 @@
       <c r="J6" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>3058</t>
+      <c r="K6" t="n">
+        <v>3058</v>
+      </c>
+      <c r="L6" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>3358</t>
         </is>
       </c>
     </row>
@@ -699,9 +739,15 @@
       <c r="J7" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>3329</t>
+      <c r="K7" t="n">
+        <v>3329</v>
+      </c>
+      <c r="L7" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>3660</t>
         </is>
       </c>
     </row>
@@ -742,9 +788,15 @@
       <c r="J8" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>3042</t>
+      <c r="K8" t="n">
+        <v>3042</v>
+      </c>
+      <c r="L8" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>3368</t>
         </is>
       </c>
     </row>
@@ -785,9 +837,15 @@
       <c r="J9" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>3014</t>
+      <c r="K9" t="n">
+        <v>3014</v>
+      </c>
+      <c r="L9" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>3299</t>
         </is>
       </c>
     </row>
@@ -828,9 +886,15 @@
       <c r="J10" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>3131</t>
+      <c r="K10" t="n">
+        <v>3131</v>
+      </c>
+      <c r="L10" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>3469</t>
         </is>
       </c>
     </row>
@@ -871,9 +935,15 @@
       <c r="J11" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>3273</t>
+      <c r="K11" t="n">
+        <v>3273</v>
+      </c>
+      <c r="L11" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>3458</t>
         </is>
       </c>
     </row>
@@ -914,9 +984,15 @@
       <c r="J12" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>3047</t>
+      <c r="K12" t="n">
+        <v>3047</v>
+      </c>
+      <c r="L12" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>3305</t>
         </is>
       </c>
     </row>
@@ -957,7 +1033,13 @@
       <c r="J13" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K13" t="inlineStr">
+      <c r="K13" t="n">
+        <v>2603</v>
+      </c>
+      <c r="L13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="inlineStr">
         <is>
           <t>2603</t>
         </is>
@@ -1000,9 +1082,15 @@
       <c r="J14" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>3541</t>
+      <c r="K14" t="n">
+        <v>3541</v>
+      </c>
+      <c r="L14" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>3896</t>
         </is>
       </c>
     </row>
@@ -1043,9 +1131,15 @@
       <c r="J15" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>3135</t>
+      <c r="K15" t="n">
+        <v>3135</v>
+      </c>
+      <c r="L15" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>3415</t>
         </is>
       </c>
     </row>
@@ -1086,9 +1180,15 @@
       <c r="J16" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>3332</t>
+      <c r="K16" t="n">
+        <v>3332</v>
+      </c>
+      <c r="L16" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>3688</t>
         </is>
       </c>
     </row>
@@ -1129,9 +1229,15 @@
       <c r="J17" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>3016</t>
+      <c r="K17" t="n">
+        <v>3016</v>
+      </c>
+      <c r="L17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>3044</t>
         </is>
       </c>
     </row>
@@ -1172,9 +1278,15 @@
       <c r="J18" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>3011</t>
+      <c r="K18" t="n">
+        <v>3011</v>
+      </c>
+      <c r="L18" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>3316</t>
         </is>
       </c>
     </row>
@@ -1215,9 +1327,15 @@
       <c r="J19" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>3090</t>
+      <c r="K19" t="n">
+        <v>3090</v>
+      </c>
+      <c r="L19" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>3372</t>
         </is>
       </c>
     </row>
@@ -1258,9 +1376,15 @@
       <c r="J20" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>3451</t>
+      <c r="K20" t="n">
+        <v>3451</v>
+      </c>
+      <c r="L20" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>3890</t>
         </is>
       </c>
     </row>
@@ -1301,7 +1425,13 @@
       <c r="J21" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="K21" t="inlineStr">
+      <c r="K21" t="n">
+        <v>2780</v>
+      </c>
+      <c r="L21" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" t="inlineStr">
         <is>
           <t>2780</t>
         </is>
@@ -1344,9 +1474,15 @@
       <c r="J22" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>3184</t>
+      <c r="K22" t="n">
+        <v>3184</v>
+      </c>
+      <c r="L22" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>3465</t>
         </is>
       </c>
     </row>
@@ -1387,9 +1523,15 @@
       <c r="J23" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>2664</t>
+      <c r="K23" t="n">
+        <v>2664</v>
+      </c>
+      <c r="L23" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>2588</t>
         </is>
       </c>
     </row>
@@ -1430,9 +1572,15 @@
       <c r="J24" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>3292</t>
+      <c r="K24" t="n">
+        <v>3292</v>
+      </c>
+      <c r="L24" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>3625</t>
         </is>
       </c>
     </row>
@@ -1473,7 +1621,13 @@
       <c r="J25" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K25" t="inlineStr">
+      <c r="K25" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1516,9 +1670,15 @@
       <c r="J26" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>3472</t>
+      <c r="K26" t="n">
+        <v>3472</v>
+      </c>
+      <c r="L26" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>3771</t>
         </is>
       </c>
     </row>
@@ -1559,9 +1719,15 @@
       <c r="J27" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="K27" t="inlineStr">
-        <is>
-          <t>3143</t>
+      <c r="K27" t="n">
+        <v>3143</v>
+      </c>
+      <c r="L27" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>3685</t>
         </is>
       </c>
     </row>
@@ -1602,9 +1768,15 @@
       <c r="J28" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>2989</t>
+      <c r="K28" t="n">
+        <v>2989</v>
+      </c>
+      <c r="L28" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>3114</t>
         </is>
       </c>
     </row>
@@ -1645,9 +1817,15 @@
       <c r="J29" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>3547</t>
+      <c r="K29" t="n">
+        <v>3547</v>
+      </c>
+      <c r="L29" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>3864</t>
         </is>
       </c>
     </row>
@@ -1688,9 +1866,15 @@
       <c r="J30" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="K30" t="inlineStr">
-        <is>
-          <t>3253</t>
+      <c r="K30" t="n">
+        <v>3253</v>
+      </c>
+      <c r="L30" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>3550</t>
         </is>
       </c>
     </row>
@@ -1731,9 +1915,15 @@
       <c r="J31" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="K31" t="inlineStr">
-        <is>
-          <t>3302</t>
+      <c r="K31" t="n">
+        <v>3302</v>
+      </c>
+      <c r="L31" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>3448</t>
         </is>
       </c>
     </row>
@@ -1774,9 +1964,15 @@
       <c r="J32" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t>3456</t>
+      <c r="K32" t="n">
+        <v>3456</v>
+      </c>
+      <c r="L32" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>3783</t>
         </is>
       </c>
     </row>
@@ -1817,9 +2013,15 @@
       <c r="J33" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="K33" t="inlineStr">
-        <is>
-          <t>3148</t>
+      <c r="K33" t="n">
+        <v>3148</v>
+      </c>
+      <c r="L33" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>3564</t>
         </is>
       </c>
     </row>
@@ -1860,9 +2062,15 @@
       <c r="J34" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="K34" t="n">
+        <v>2500</v>
+      </c>
+      <c r="L34" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>3066</t>
         </is>
       </c>
     </row>
@@ -1903,9 +2111,15 @@
       <c r="J35" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="K35" t="inlineStr">
-        <is>
-          <t>3416</t>
+      <c r="K35" t="n">
+        <v>3416</v>
+      </c>
+      <c r="L35" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>3780</t>
         </is>
       </c>
     </row>
@@ -1946,9 +2160,15 @@
       <c r="J36" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>3206</t>
+      <c r="K36" t="n">
+        <v>3206</v>
+      </c>
+      <c r="L36" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>3494</t>
         </is>
       </c>
     </row>
@@ -1989,9 +2209,15 @@
       <c r="J37" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="K37" t="inlineStr">
-        <is>
-          <t>3209</t>
+      <c r="K37" t="n">
+        <v>3209</v>
+      </c>
+      <c r="L37" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>3437</t>
         </is>
       </c>
     </row>
@@ -2032,9 +2258,15 @@
       <c r="J38" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="K38" t="inlineStr">
-        <is>
-          <t>3333</t>
+      <c r="K38" t="n">
+        <v>3333</v>
+      </c>
+      <c r="L38" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>3663</t>
         </is>
       </c>
     </row>
@@ -2075,9 +2307,15 @@
       <c r="J39" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>3123</t>
+      <c r="K39" t="n">
+        <v>3123</v>
+      </c>
+      <c r="L39" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>3503</t>
         </is>
       </c>
     </row>
@@ -2118,9 +2356,15 @@
       <c r="J40" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="K40" t="inlineStr">
-        <is>
-          <t>3349</t>
+      <c r="K40" t="n">
+        <v>3349</v>
+      </c>
+      <c r="L40" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>3703</t>
         </is>
       </c>
     </row>
@@ -2161,9 +2405,15 @@
       <c r="J41" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K41" t="inlineStr">
-        <is>
-          <t>3135</t>
+      <c r="K41" t="n">
+        <v>3135</v>
+      </c>
+      <c r="L41" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>3480</t>
         </is>
       </c>
     </row>
@@ -2204,9 +2454,15 @@
       <c r="J42" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>3389</t>
+      <c r="K42" t="n">
+        <v>3389</v>
+      </c>
+      <c r="L42" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>3718</t>
         </is>
       </c>
     </row>
@@ -2247,9 +2503,15 @@
       <c r="J43" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="K43" t="inlineStr">
-        <is>
-          <t>3334</t>
+      <c r="K43" t="n">
+        <v>3334</v>
+      </c>
+      <c r="L43" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>3623</t>
         </is>
       </c>
     </row>
@@ -2290,9 +2552,15 @@
       <c r="J44" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="K44" t="inlineStr">
-        <is>
-          <t>3422</t>
+      <c r="K44" t="n">
+        <v>3422</v>
+      </c>
+      <c r="L44" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>3576</t>
         </is>
       </c>
     </row>
@@ -2333,9 +2601,15 @@
       <c r="J45" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="K45" t="inlineStr">
-        <is>
-          <t>3148</t>
+      <c r="K45" t="n">
+        <v>3148</v>
+      </c>
+      <c r="L45" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>3363</t>
         </is>
       </c>
     </row>
@@ -2376,9 +2650,15 @@
       <c r="J46" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>3146</t>
+      <c r="K46" t="n">
+        <v>3146</v>
+      </c>
+      <c r="L46" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>3339</t>
         </is>
       </c>
     </row>
@@ -2419,9 +2699,15 @@
       <c r="J47" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K47" t="inlineStr">
-        <is>
-          <t>2601</t>
+      <c r="K47" t="n">
+        <v>2601</v>
+      </c>
+      <c r="L47" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>3010</t>
         </is>
       </c>
     </row>
@@ -2462,9 +2748,15 @@
       <c r="J48" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>3206</t>
+      <c r="K48" t="n">
+        <v>3206</v>
+      </c>
+      <c r="L48" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>3486</t>
         </is>
       </c>
     </row>
@@ -2505,9 +2797,15 @@
       <c r="J49" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>3001</t>
+      <c r="K49" t="n">
+        <v>3001</v>
+      </c>
+      <c r="L49" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>3248</t>
         </is>
       </c>
     </row>
@@ -2548,9 +2846,15 @@
       <c r="J50" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="K50" t="inlineStr">
-        <is>
-          <t>3245</t>
+      <c r="K50" t="n">
+        <v>3245</v>
+      </c>
+      <c r="L50" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>3719</t>
         </is>
       </c>
     </row>
@@ -2591,9 +2895,15 @@
       <c r="J51" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K51" t="inlineStr">
-        <is>
-          <t>2701</t>
+      <c r="K51" t="n">
+        <v>2701</v>
+      </c>
+      <c r="L51" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>2720</t>
         </is>
       </c>
     </row>
@@ -2634,9 +2944,15 @@
       <c r="J52" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>2515</t>
+      <c r="K52" t="n">
+        <v>2515</v>
+      </c>
+      <c r="L52" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>2603</t>
         </is>
       </c>
     </row>
@@ -2677,9 +2993,15 @@
       <c r="J53" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="K53" t="inlineStr">
-        <is>
-          <t>2512</t>
+      <c r="K53" t="n">
+        <v>2512</v>
+      </c>
+      <c r="L53" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>2675</t>
         </is>
       </c>
     </row>
@@ -2720,9 +3042,15 @@
       <c r="J54" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="K54" t="inlineStr">
-        <is>
-          <t>3377</t>
+      <c r="K54" t="n">
+        <v>3377</v>
+      </c>
+      <c r="L54" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>3665</t>
         </is>
       </c>
     </row>
@@ -2763,9 +3091,15 @@
       <c r="J55" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="K55" t="inlineStr">
-        <is>
-          <t>2915</t>
+      <c r="K55" t="n">
+        <v>2915</v>
+      </c>
+      <c r="L55" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>3031</t>
         </is>
       </c>
     </row>
@@ -2806,9 +3140,15 @@
       <c r="J56" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K56" t="inlineStr">
-        <is>
-          <t>2900</t>
+      <c r="K56" t="n">
+        <v>2900</v>
+      </c>
+      <c r="L56" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>3159</t>
         </is>
       </c>
     </row>
@@ -2849,9 +3189,15 @@
       <c r="J57" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K57" t="inlineStr">
-        <is>
-          <t>3111</t>
+      <c r="K57" t="n">
+        <v>3111</v>
+      </c>
+      <c r="L57" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>3352</t>
         </is>
       </c>
     </row>
@@ -2892,9 +3238,15 @@
       <c r="J58" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="K58" t="inlineStr">
-        <is>
-          <t>2886</t>
+      <c r="K58" t="n">
+        <v>2886</v>
+      </c>
+      <c r="L58" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>3043</t>
         </is>
       </c>
     </row>
@@ -2935,9 +3287,15 @@
       <c r="J59" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="K59" t="inlineStr">
-        <is>
-          <t>3037</t>
+      <c r="K59" t="n">
+        <v>3037</v>
+      </c>
+      <c r="L59" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>3308</t>
         </is>
       </c>
     </row>
@@ -2978,7 +3336,13 @@
       <c r="J60" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K60" t="inlineStr">
+      <c r="K60" t="n">
+        <v>0</v>
+      </c>
+      <c r="L60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M60" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3021,9 +3385,15 @@
       <c r="J61" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="K61" t="inlineStr">
-        <is>
-          <t>3155</t>
+      <c r="K61" t="n">
+        <v>3155</v>
+      </c>
+      <c r="L61" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>3483</t>
         </is>
       </c>
     </row>
@@ -3064,7 +3434,13 @@
       <c r="J62" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K62" t="inlineStr">
+      <c r="K62" t="n">
+        <v>2510</v>
+      </c>
+      <c r="L62" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M62" t="inlineStr">
         <is>
           <t>2510</t>
         </is>
@@ -3107,9 +3483,15 @@
       <c r="J63" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K63" t="inlineStr">
-        <is>
-          <t>2403</t>
+      <c r="K63" t="n">
+        <v>2403</v>
+      </c>
+      <c r="L63" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>2395</t>
         </is>
       </c>
     </row>
@@ -3150,9 +3532,15 @@
       <c r="J64" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="K64" t="inlineStr">
-        <is>
-          <t>3094</t>
+      <c r="K64" t="n">
+        <v>3094</v>
+      </c>
+      <c r="L64" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>3399</t>
         </is>
       </c>
     </row>
@@ -3193,7 +3581,13 @@
       <c r="J65" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K65" t="inlineStr">
+      <c r="K65" t="n">
+        <v>0</v>
+      </c>
+      <c r="L65" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M65" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3236,9 +3630,15 @@
       <c r="J66" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="K66" t="inlineStr">
-        <is>
-          <t>3061</t>
+      <c r="K66" t="n">
+        <v>3061</v>
+      </c>
+      <c r="L66" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>3466</t>
         </is>
       </c>
     </row>
@@ -3279,9 +3679,15 @@
       <c r="J67" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="K67" t="inlineStr">
-        <is>
-          <t>2956</t>
+      <c r="K67" t="n">
+        <v>2956</v>
+      </c>
+      <c r="L67" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>3201</t>
         </is>
       </c>
     </row>
@@ -3322,9 +3728,15 @@
       <c r="J68" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K68" t="inlineStr">
-        <is>
-          <t>2516</t>
+      <c r="K68" t="n">
+        <v>2516</v>
+      </c>
+      <c r="L68" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M68" t="inlineStr">
+        <is>
+          <t>2512</t>
         </is>
       </c>
     </row>
@@ -3365,9 +3777,15 @@
       <c r="J69" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="K69" t="inlineStr">
-        <is>
-          <t>2957</t>
+      <c r="K69" t="n">
+        <v>2957</v>
+      </c>
+      <c r="L69" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="M69" t="inlineStr">
+        <is>
+          <t>3131</t>
         </is>
       </c>
     </row>
@@ -3408,9 +3826,15 @@
       <c r="J70" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="K70" t="inlineStr">
-        <is>
-          <t>2838</t>
+      <c r="K70" t="n">
+        <v>2838</v>
+      </c>
+      <c r="L70" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="M70" t="inlineStr">
+        <is>
+          <t>2899</t>
         </is>
       </c>
     </row>
@@ -3451,9 +3875,15 @@
       <c r="J71" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="K71" t="inlineStr">
-        <is>
-          <t>2928</t>
+      <c r="K71" t="n">
+        <v>2928</v>
+      </c>
+      <c r="L71" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M71" t="inlineStr">
+        <is>
+          <t>3048</t>
         </is>
       </c>
     </row>
@@ -3494,9 +3924,15 @@
       <c r="J72" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K72" t="inlineStr">
-        <is>
-          <t>2573</t>
+      <c r="K72" t="n">
+        <v>2573</v>
+      </c>
+      <c r="L72" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>2641</t>
         </is>
       </c>
     </row>
@@ -3537,9 +3973,15 @@
       <c r="J73" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="K73" t="inlineStr">
-        <is>
-          <t>2869</t>
+      <c r="K73" t="n">
+        <v>2869</v>
+      </c>
+      <c r="L73" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="M73" t="inlineStr">
+        <is>
+          <t>2993</t>
         </is>
       </c>
     </row>
@@ -3562,7 +4004,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F74" s="5" t="n">
@@ -3580,9 +4022,15 @@
       <c r="J74" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="K74" t="inlineStr">
-        <is>
-          <t>3027</t>
+      <c r="K74" t="n">
+        <v>3027</v>
+      </c>
+      <c r="L74" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>3320</t>
         </is>
       </c>
     </row>
@@ -3623,9 +4071,15 @@
       <c r="J75" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K75" t="inlineStr">
-        <is>
-          <t>3085</t>
+      <c r="K75" t="n">
+        <v>3085</v>
+      </c>
+      <c r="L75" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="M75" t="inlineStr">
+        <is>
+          <t>3293</t>
         </is>
       </c>
     </row>
@@ -3666,7 +4120,13 @@
       <c r="J76" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K76" t="inlineStr">
+      <c r="K76" t="n">
+        <v>0</v>
+      </c>
+      <c r="L76" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M76" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3709,9 +4169,15 @@
       <c r="J77" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="K77" t="inlineStr">
-        <is>
-          <t>3210</t>
+      <c r="K77" t="n">
+        <v>3210</v>
+      </c>
+      <c r="L77" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>3463</t>
         </is>
       </c>
     </row>
@@ -3752,7 +4218,13 @@
       <c r="J78" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K78" t="inlineStr">
+      <c r="K78" t="n">
+        <v>2500</v>
+      </c>
+      <c r="L78" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M78" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -3795,9 +4267,15 @@
       <c r="J79" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="K79" t="inlineStr">
-        <is>
-          <t>2994</t>
+      <c r="K79" t="n">
+        <v>2994</v>
+      </c>
+      <c r="L79" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="M79" t="inlineStr">
+        <is>
+          <t>3320</t>
         </is>
       </c>
     </row>
@@ -3838,9 +4316,15 @@
       <c r="J80" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="K80" t="inlineStr">
-        <is>
-          <t>3067</t>
+      <c r="K80" t="n">
+        <v>3067</v>
+      </c>
+      <c r="L80" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="M80" t="inlineStr">
+        <is>
+          <t>3356</t>
         </is>
       </c>
     </row>
@@ -3881,9 +4365,15 @@
       <c r="J81" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="K81" t="inlineStr">
-        <is>
-          <t>3018</t>
+      <c r="K81" t="n">
+        <v>3018</v>
+      </c>
+      <c r="L81" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="M81" t="inlineStr">
+        <is>
+          <t>3236</t>
         </is>
       </c>
     </row>
@@ -3924,9 +4414,15 @@
       <c r="J82" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="K82" t="inlineStr">
-        <is>
-          <t>3035</t>
+      <c r="K82" t="n">
+        <v>3035</v>
+      </c>
+      <c r="L82" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="M82" t="inlineStr">
+        <is>
+          <t>3152</t>
         </is>
       </c>
     </row>
@@ -3962,6 +4458,8 @@
       <c r="I83" t="inlineStr"/>
       <c r="J83" s="2" t="inlineStr"/>
       <c r="K83" t="inlineStr"/>
+      <c r="L83" s="2" t="inlineStr"/>
+      <c r="M83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -4000,9 +4498,15 @@
       <c r="J84" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K84" t="inlineStr">
-        <is>
-          <t>2715</t>
+      <c r="K84" t="n">
+        <v>2715</v>
+      </c>
+      <c r="L84" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M84" t="inlineStr">
+        <is>
+          <t>2741</t>
         </is>
       </c>
     </row>
@@ -4043,9 +4547,15 @@
       <c r="J85" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K85" t="inlineStr">
-        <is>
-          <t>2504</t>
+      <c r="K85" t="n">
+        <v>2504</v>
+      </c>
+      <c r="L85" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M85" t="inlineStr">
+        <is>
+          <t>2499</t>
         </is>
       </c>
     </row>
@@ -4086,9 +4596,15 @@
       <c r="J86" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="K86" t="inlineStr">
-        <is>
-          <t>3141</t>
+      <c r="K86" t="n">
+        <v>3141</v>
+      </c>
+      <c r="L86" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M86" t="inlineStr">
+        <is>
+          <t>3368</t>
         </is>
       </c>
     </row>
@@ -4129,9 +4645,15 @@
       <c r="J87" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K87" t="inlineStr">
-        <is>
-          <t>2558</t>
+      <c r="K87" t="n">
+        <v>2558</v>
+      </c>
+      <c r="L87" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M87" t="inlineStr">
+        <is>
+          <t>2670</t>
         </is>
       </c>
     </row>
@@ -4172,9 +4694,15 @@
       <c r="J88" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K88" t="inlineStr">
-        <is>
-          <t>2521</t>
+      <c r="K88" t="n">
+        <v>2521</v>
+      </c>
+      <c r="L88" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="M88" t="inlineStr">
+        <is>
+          <t>2663</t>
         </is>
       </c>
     </row>
@@ -4202,6 +4730,8 @@
       <c r="I89" t="inlineStr"/>
       <c r="J89" s="2" t="inlineStr"/>
       <c r="K89" t="inlineStr"/>
+      <c r="L89" s="2" t="inlineStr"/>
+      <c r="M89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -4240,9 +4770,15 @@
       <c r="J90" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="K90" t="inlineStr">
-        <is>
-          <t>2456</t>
+      <c r="K90" t="n">
+        <v>2456</v>
+      </c>
+      <c r="L90" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="M90" t="inlineStr">
+        <is>
+          <t>2450</t>
         </is>
       </c>
     </row>
@@ -4283,7 +4819,13 @@
       <c r="J91" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K91" t="inlineStr">
+      <c r="K91" t="n">
+        <v>0</v>
+      </c>
+      <c r="L91" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4326,9 +4868,15 @@
       <c r="J92" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K92" t="inlineStr">
-        <is>
-          <t>2601</t>
+      <c r="K92" t="n">
+        <v>2601</v>
+      </c>
+      <c r="L92" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M92" t="inlineStr">
+        <is>
+          <t>2660</t>
         </is>
       </c>
     </row>
@@ -4369,9 +4917,15 @@
       <c r="J93" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="K93" t="inlineStr">
-        <is>
-          <t>2610</t>
+      <c r="K93" t="n">
+        <v>2610</v>
+      </c>
+      <c r="L93" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="M93" t="inlineStr">
+        <is>
+          <t>2714</t>
         </is>
       </c>
     </row>
@@ -4412,7 +4966,13 @@
       <c r="J94" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K94" t="inlineStr">
+      <c r="K94" t="n">
+        <v>0</v>
+      </c>
+      <c r="L94" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4455,9 +5015,15 @@
       <c r="J95" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="K95" t="inlineStr">
-        <is>
-          <t>2038</t>
+      <c r="K95" t="n">
+        <v>2038</v>
+      </c>
+      <c r="L95" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="M95" t="inlineStr">
+        <is>
+          <t>2088</t>
         </is>
       </c>
     </row>
@@ -4498,9 +5064,15 @@
       <c r="J96" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K96" t="inlineStr">
-        <is>
-          <t>2012</t>
+      <c r="K96" t="n">
+        <v>2012</v>
+      </c>
+      <c r="L96" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M96" t="inlineStr">
+        <is>
+          <t>2004</t>
         </is>
       </c>
     </row>
@@ -4541,9 +5113,15 @@
       <c r="J97" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K97" t="inlineStr">
-        <is>
-          <t>2467</t>
+      <c r="K97" t="n">
+        <v>2467</v>
+      </c>
+      <c r="L97" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M97" t="inlineStr">
+        <is>
+          <t>2465</t>
         </is>
       </c>
     </row>
@@ -4584,9 +5162,15 @@
       <c r="J98" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K98" t="inlineStr">
-        <is>
-          <t>2267</t>
+      <c r="K98" t="n">
+        <v>2267</v>
+      </c>
+      <c r="L98" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="M98" t="inlineStr">
+        <is>
+          <t>2376</t>
         </is>
       </c>
     </row>
@@ -4627,9 +5211,15 @@
       <c r="J99" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K99" t="inlineStr">
-        <is>
-          <t>2746</t>
+      <c r="K99" t="n">
+        <v>2746</v>
+      </c>
+      <c r="L99" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="M99" t="inlineStr">
+        <is>
+          <t>2843</t>
         </is>
       </c>
     </row>
@@ -4670,9 +5260,15 @@
       <c r="J100" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K100" t="inlineStr">
-        <is>
-          <t>2424</t>
+      <c r="K100" t="n">
+        <v>2424</v>
+      </c>
+      <c r="L100" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="M100" t="inlineStr">
+        <is>
+          <t>2492</t>
         </is>
       </c>
     </row>
@@ -4713,9 +5309,15 @@
       <c r="J101" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="K101" t="inlineStr">
-        <is>
-          <t>3038</t>
+      <c r="K101" t="n">
+        <v>3038</v>
+      </c>
+      <c r="L101" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="M101" t="inlineStr">
+        <is>
+          <t>3240</t>
         </is>
       </c>
     </row>
@@ -4756,9 +5358,15 @@
       <c r="J102" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K102" t="inlineStr">
-        <is>
-          <t>2851</t>
+      <c r="K102" t="n">
+        <v>2851</v>
+      </c>
+      <c r="L102" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M102" t="inlineStr">
+        <is>
+          <t>2980</t>
         </is>
       </c>
     </row>
@@ -4799,9 +5407,15 @@
       <c r="J103" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="K103" t="inlineStr">
-        <is>
-          <t>2813</t>
+      <c r="K103" t="n">
+        <v>2813</v>
+      </c>
+      <c r="L103" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="M103" t="inlineStr">
+        <is>
+          <t>2845</t>
         </is>
       </c>
     </row>
@@ -4842,9 +5456,15 @@
       <c r="J104" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="K104" t="inlineStr">
-        <is>
-          <t>3045</t>
+      <c r="K104" t="n">
+        <v>3045</v>
+      </c>
+      <c r="L104" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="M104" t="inlineStr">
+        <is>
+          <t>3240</t>
         </is>
       </c>
     </row>
@@ -4885,7 +5505,13 @@
       <c r="J105" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="K105" t="inlineStr">
+      <c r="K105" t="n">
+        <v>2802</v>
+      </c>
+      <c r="L105" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M105" t="inlineStr">
         <is>
           <t>2802</t>
         </is>
@@ -4928,9 +5554,15 @@
       <c r="J106" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K106" t="inlineStr">
-        <is>
-          <t>2464</t>
+      <c r="K106" t="n">
+        <v>2464</v>
+      </c>
+      <c r="L106" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M106" t="inlineStr">
+        <is>
+          <t>2488</t>
         </is>
       </c>
     </row>
@@ -4971,9 +5603,15 @@
       <c r="J107" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K107" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K107" t="n">
+        <v>0</v>
+      </c>
+      <c r="L107" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M107" t="inlineStr">
+        <is>
+          <t>2480</t>
         </is>
       </c>
     </row>
@@ -5014,9 +5652,15 @@
       <c r="J108" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K108" t="inlineStr">
-        <is>
-          <t>2496</t>
+      <c r="K108" t="n">
+        <v>2496</v>
+      </c>
+      <c r="L108" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M108" t="inlineStr">
+        <is>
+          <t>2493</t>
         </is>
       </c>
     </row>
@@ -5057,9 +5701,15 @@
       <c r="J109" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K109" t="inlineStr">
-        <is>
-          <t>2774</t>
+      <c r="K109" t="n">
+        <v>2774</v>
+      </c>
+      <c r="L109" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M109" t="inlineStr">
+        <is>
+          <t>2859</t>
         </is>
       </c>
     </row>
@@ -5100,9 +5750,15 @@
       <c r="J110" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="K110" t="inlineStr">
-        <is>
-          <t>2711</t>
+      <c r="K110" t="n">
+        <v>2711</v>
+      </c>
+      <c r="L110" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="M110" t="inlineStr">
+        <is>
+          <t>2921</t>
         </is>
       </c>
     </row>
@@ -5143,9 +5799,15 @@
       <c r="J111" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K111" t="inlineStr">
-        <is>
-          <t>2499</t>
+      <c r="K111" t="n">
+        <v>2499</v>
+      </c>
+      <c r="L111" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="M111" t="inlineStr">
+        <is>
+          <t>2545</t>
         </is>
       </c>
     </row>
@@ -5186,9 +5848,15 @@
       <c r="J112" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K112" t="inlineStr">
-        <is>
-          <t>2479</t>
+      <c r="K112" t="n">
+        <v>2479</v>
+      </c>
+      <c r="L112" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M112" t="inlineStr">
+        <is>
+          <t>2474</t>
         </is>
       </c>
     </row>
@@ -5229,9 +5897,15 @@
       <c r="J113" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="K113" t="inlineStr">
-        <is>
-          <t>2710</t>
+      <c r="K113" t="n">
+        <v>2710</v>
+      </c>
+      <c r="L113" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="M113" t="inlineStr">
+        <is>
+          <t>2815</t>
         </is>
       </c>
     </row>
@@ -5272,9 +5946,15 @@
       <c r="J114" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K114" t="inlineStr">
-        <is>
-          <t>2557</t>
+      <c r="K114" t="n">
+        <v>2557</v>
+      </c>
+      <c r="L114" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M114" t="inlineStr">
+        <is>
+          <t>2645</t>
         </is>
       </c>
     </row>
@@ -5315,9 +5995,15 @@
       <c r="J115" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="K115" t="inlineStr">
-        <is>
-          <t>2892</t>
+      <c r="K115" t="n">
+        <v>2892</v>
+      </c>
+      <c r="L115" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="M115" t="inlineStr">
+        <is>
+          <t>3040</t>
         </is>
       </c>
     </row>
@@ -5358,9 +6044,15 @@
       <c r="J116" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="K116" t="inlineStr">
-        <is>
-          <t>2490</t>
+      <c r="K116" t="n">
+        <v>2490</v>
+      </c>
+      <c r="L116" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="M116" t="inlineStr">
+        <is>
+          <t>2496</t>
         </is>
       </c>
     </row>
@@ -5401,9 +6093,15 @@
       <c r="J117" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="K117" t="inlineStr">
-        <is>
-          <t>2522</t>
+      <c r="K117" t="n">
+        <v>2522</v>
+      </c>
+      <c r="L117" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="M117" t="inlineStr">
+        <is>
+          <t>2611</t>
         </is>
       </c>
     </row>
@@ -5444,9 +6142,15 @@
       <c r="J118" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="K118" t="inlineStr">
-        <is>
-          <t>2839</t>
+      <c r="K118" t="n">
+        <v>2839</v>
+      </c>
+      <c r="L118" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="M118" t="inlineStr">
+        <is>
+          <t>3008</t>
         </is>
       </c>
     </row>
@@ -5487,7 +6191,13 @@
       <c r="J119" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K119" t="inlineStr">
+      <c r="K119" t="n">
+        <v>0</v>
+      </c>
+      <c r="L119" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M119" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5530,9 +6240,15 @@
       <c r="J120" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="K120" t="inlineStr">
-        <is>
-          <t>2813</t>
+      <c r="K120" t="n">
+        <v>2813</v>
+      </c>
+      <c r="L120" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="M120" t="inlineStr">
+        <is>
+          <t>2978</t>
         </is>
       </c>
     </row>
@@ -5573,9 +6289,15 @@
       <c r="J121" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K121" t="inlineStr">
-        <is>
-          <t>2611</t>
+      <c r="K121" t="n">
+        <v>2611</v>
+      </c>
+      <c r="L121" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M121" t="inlineStr">
+        <is>
+          <t>2683</t>
         </is>
       </c>
     </row>
@@ -5616,9 +6338,15 @@
       <c r="J122" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K122" t="inlineStr">
-        <is>
-          <t>2540</t>
+      <c r="K122" t="n">
+        <v>2540</v>
+      </c>
+      <c r="L122" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M122" t="inlineStr">
+        <is>
+          <t>2641</t>
         </is>
       </c>
     </row>
@@ -5659,9 +6387,15 @@
       <c r="J123" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="K123" t="inlineStr">
-        <is>
-          <t>2642</t>
+      <c r="K123" t="n">
+        <v>2642</v>
+      </c>
+      <c r="L123" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M123" t="inlineStr">
+        <is>
+          <t>2536</t>
         </is>
       </c>
     </row>
@@ -5702,9 +6436,15 @@
       <c r="J124" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K124" t="inlineStr">
-        <is>
-          <t>2671</t>
+      <c r="K124" t="n">
+        <v>2671</v>
+      </c>
+      <c r="L124" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M124" t="inlineStr">
+        <is>
+          <t>2727</t>
         </is>
       </c>
     </row>
@@ -5745,9 +6485,15 @@
       <c r="J125" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K125" t="inlineStr">
-        <is>
-          <t>2592</t>
+      <c r="K125" t="n">
+        <v>2592</v>
+      </c>
+      <c r="L125" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M125" t="inlineStr">
+        <is>
+          <t>2774</t>
         </is>
       </c>
     </row>
@@ -5788,9 +6534,15 @@
       <c r="J126" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K126" t="inlineStr">
-        <is>
-          <t>2781</t>
+      <c r="K126" t="n">
+        <v>2781</v>
+      </c>
+      <c r="L126" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M126" t="inlineStr">
+        <is>
+          <t>2910</t>
         </is>
       </c>
     </row>
@@ -5831,9 +6583,15 @@
       <c r="J127" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K127" t="inlineStr">
-        <is>
-          <t>2489</t>
+      <c r="K127" t="n">
+        <v>2489</v>
+      </c>
+      <c r="L127" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M127" t="inlineStr">
+        <is>
+          <t>2671</t>
         </is>
       </c>
     </row>
@@ -5874,7 +6632,13 @@
       <c r="J128" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K128" t="inlineStr">
+      <c r="K128" t="n">
+        <v>0</v>
+      </c>
+      <c r="L128" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5917,7 +6681,13 @@
       <c r="J129" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K129" t="inlineStr">
+      <c r="K129" t="n">
+        <v>0</v>
+      </c>
+      <c r="L129" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5960,9 +6730,15 @@
       <c r="J130" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K130" t="inlineStr">
-        <is>
-          <t>2558</t>
+      <c r="K130" t="n">
+        <v>2558</v>
+      </c>
+      <c r="L130" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M130" t="inlineStr">
+        <is>
+          <t>2647</t>
         </is>
       </c>
     </row>
@@ -6003,9 +6779,15 @@
       <c r="J131" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K131" t="inlineStr">
-        <is>
-          <t>2380</t>
+      <c r="K131" t="n">
+        <v>2380</v>
+      </c>
+      <c r="L131" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M131" t="inlineStr">
+        <is>
+          <t>2365</t>
         </is>
       </c>
     </row>
@@ -6046,9 +6828,15 @@
       <c r="J132" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="K132" t="inlineStr">
-        <is>
-          <t>1040</t>
+      <c r="K132" t="n">
+        <v>1040</v>
+      </c>
+      <c r="L132" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M132" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -6089,7 +6877,13 @@
       <c r="J133" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="K133" t="inlineStr">
+      <c r="K133" t="n">
+        <v>2067</v>
+      </c>
+      <c r="L133" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M133" t="inlineStr">
         <is>
           <t>2067</t>
         </is>
@@ -6132,9 +6926,15 @@
       <c r="J134" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="K134" t="inlineStr">
-        <is>
-          <t>2762</t>
+      <c r="K134" t="n">
+        <v>2762</v>
+      </c>
+      <c r="L134" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="M134" t="inlineStr">
+        <is>
+          <t>2860</t>
         </is>
       </c>
     </row>
@@ -6175,7 +6975,13 @@
       <c r="J135" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K135" t="inlineStr">
+      <c r="K135" t="n">
+        <v>0</v>
+      </c>
+      <c r="L135" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M135" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6218,7 +7024,13 @@
       <c r="J136" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K136" t="inlineStr">
+      <c r="K136" t="n">
+        <v>0</v>
+      </c>
+      <c r="L136" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M136" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6261,7 +7073,13 @@
       <c r="J137" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K137" t="inlineStr">
+      <c r="K137" t="n">
+        <v>0</v>
+      </c>
+      <c r="L137" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6304,9 +7122,15 @@
       <c r="J138" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="K138" t="inlineStr">
-        <is>
-          <t>2761</t>
+      <c r="K138" t="n">
+        <v>2761</v>
+      </c>
+      <c r="L138" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="M138" t="inlineStr">
+        <is>
+          <t>2722</t>
         </is>
       </c>
     </row>
@@ -6347,7 +7171,13 @@
       <c r="J139" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K139" t="inlineStr">
+      <c r="K139" t="n">
+        <v>0</v>
+      </c>
+      <c r="L139" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M139" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6390,9 +7220,15 @@
       <c r="J140" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="K140" t="inlineStr">
-        <is>
-          <t>2564</t>
+      <c r="K140" t="n">
+        <v>2564</v>
+      </c>
+      <c r="L140" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="M140" t="inlineStr">
+        <is>
+          <t>2587</t>
         </is>
       </c>
     </row>
@@ -6433,7 +7269,13 @@
       <c r="J141" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K141" t="inlineStr">
+      <c r="K141" t="n">
+        <v>0</v>
+      </c>
+      <c r="L141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M141" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6476,9 +7318,15 @@
       <c r="J142" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K142" t="inlineStr">
-        <is>
-          <t>2508</t>
+      <c r="K142" t="n">
+        <v>2508</v>
+      </c>
+      <c r="L142" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M142" t="inlineStr">
+        <is>
+          <t>2580</t>
         </is>
       </c>
     </row>
@@ -6519,11 +7367,11 @@
       <c r="J143" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K143" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="K143" t="n">
+        <v>0</v>
+      </c>
+      <c r="L143" s="2" t="inlineStr"/>
+      <c r="M143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -6562,9 +7410,15 @@
       <c r="J144" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K144" t="inlineStr">
-        <is>
-          <t>2453</t>
+      <c r="K144" t="n">
+        <v>2453</v>
+      </c>
+      <c r="L144" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="M144" t="inlineStr">
+        <is>
+          <t>2472</t>
         </is>
       </c>
     </row>
@@ -6605,7 +7459,13 @@
       <c r="J145" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K145" t="inlineStr">
+      <c r="K145" t="n">
+        <v>0</v>
+      </c>
+      <c r="L145" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M145" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6648,7 +7508,13 @@
       <c r="J146" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K146" t="inlineStr">
+      <c r="K146" t="n">
+        <v>0</v>
+      </c>
+      <c r="L146" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6691,7 +7557,13 @@
       <c r="J147" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K147" t="inlineStr">
+      <c r="K147" t="n">
+        <v>0</v>
+      </c>
+      <c r="L147" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M147" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6734,7 +7606,13 @@
       <c r="J148" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K148" t="inlineStr">
+      <c r="K148" t="n">
+        <v>0</v>
+      </c>
+      <c r="L148" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6777,7 +7655,13 @@
       <c r="J149" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K149" t="inlineStr">
+      <c r="K149" t="n">
+        <v>0</v>
+      </c>
+      <c r="L149" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M149" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6820,9 +7704,15 @@
       <c r="J150" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="K150" t="inlineStr">
-        <is>
-          <t>2224</t>
+      <c r="K150" t="n">
+        <v>2224</v>
+      </c>
+      <c r="L150" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="M150" t="inlineStr">
+        <is>
+          <t>2342</t>
         </is>
       </c>
     </row>
@@ -6863,7 +7753,13 @@
       <c r="J151" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K151" t="inlineStr">
+      <c r="K151" t="n">
+        <v>1500</v>
+      </c>
+      <c r="L151" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M151" t="inlineStr">
         <is>
           <t>1500</t>
         </is>
@@ -6906,9 +7802,15 @@
       <c r="J152" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="K152" t="inlineStr">
-        <is>
-          <t>1581</t>
+      <c r="K152" t="n">
+        <v>1581</v>
+      </c>
+      <c r="L152" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="M152" t="inlineStr">
+        <is>
+          <t>1609</t>
         </is>
       </c>
     </row>
@@ -6949,9 +7851,15 @@
       <c r="J153" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="K153" t="inlineStr">
-        <is>
-          <t>1689</t>
+      <c r="K153" t="n">
+        <v>1689</v>
+      </c>
+      <c r="L153" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="M153" t="inlineStr">
+        <is>
+          <t>1729</t>
         </is>
       </c>
     </row>
@@ -6992,7 +7900,13 @@
       <c r="J154" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K154" t="inlineStr">
+      <c r="K154" t="n">
+        <v>0</v>
+      </c>
+      <c r="L154" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7035,9 +7949,15 @@
       <c r="J155" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="K155" t="inlineStr">
-        <is>
-          <t>2807</t>
+      <c r="K155" t="n">
+        <v>2807</v>
+      </c>
+      <c r="L155" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="M155" t="inlineStr">
+        <is>
+          <t>2925</t>
         </is>
       </c>
     </row>
@@ -7078,7 +7998,13 @@
       <c r="J156" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K156" t="inlineStr">
+      <c r="K156" t="n">
+        <v>0</v>
+      </c>
+      <c r="L156" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M156" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7121,7 +8047,13 @@
       <c r="J157" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K157" t="inlineStr">
+      <c r="K157" t="n">
+        <v>0</v>
+      </c>
+      <c r="L157" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M157" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7160,9 +8092,15 @@
       <c r="J158" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="K158" t="inlineStr">
-        <is>
-          <t>3283</t>
+      <c r="K158" t="n">
+        <v>3283</v>
+      </c>
+      <c r="L158" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="M158" t="inlineStr">
+        <is>
+          <t>3591</t>
         </is>
       </c>
     </row>
@@ -7203,7 +8141,13 @@
       <c r="J159" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K159" t="inlineStr">
+      <c r="K159" t="n">
+        <v>0</v>
+      </c>
+      <c r="L159" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M159" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7246,9 +8190,15 @@
       <c r="J160" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K160" t="inlineStr">
-        <is>
-          <t>2550</t>
+      <c r="K160" t="n">
+        <v>2550</v>
+      </c>
+      <c r="L160" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="M160" t="inlineStr">
+        <is>
+          <t>2582</t>
         </is>
       </c>
     </row>
@@ -7289,7 +8239,13 @@
       <c r="J161" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K161" t="inlineStr">
+      <c r="K161" t="n">
+        <v>0</v>
+      </c>
+      <c r="L161" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M161" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7332,7 +8288,13 @@
       <c r="J162" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K162" t="inlineStr">
+      <c r="K162" t="n">
+        <v>0</v>
+      </c>
+      <c r="L162" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M162" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7375,9 +8337,15 @@
       <c r="J163" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K163" t="inlineStr">
-        <is>
-          <t>2470</t>
+      <c r="K163" t="n">
+        <v>2470</v>
+      </c>
+      <c r="L163" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="M163" t="inlineStr">
+        <is>
+          <t>2461</t>
         </is>
       </c>
     </row>
@@ -7408,9 +8376,81 @@
       <c r="J164" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="K164" t="inlineStr">
-        <is>
-          <t>1994</t>
+      <c r="K164" t="n">
+        <v>1994</v>
+      </c>
+      <c r="L164" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="M164" t="inlineStr">
+        <is>
+          <t>2058</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>58739336</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>Player-58739336</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr"/>
+      <c r="D165" t="inlineStr"/>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F165" s="2" t="inlineStr"/>
+      <c r="G165" t="inlineStr"/>
+      <c r="H165" s="2" t="inlineStr"/>
+      <c r="I165" t="inlineStr"/>
+      <c r="J165" s="2" t="inlineStr"/>
+      <c r="K165" t="inlineStr"/>
+      <c r="L165" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="M165" t="inlineStr">
+        <is>
+          <t>1753</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>58739866</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>Player-58739866</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr"/>
+      <c r="D166" t="inlineStr"/>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F166" s="2" t="inlineStr"/>
+      <c r="G166" t="inlineStr"/>
+      <c r="H166" s="2" t="inlineStr"/>
+      <c r="I166" t="inlineStr"/>
+      <c r="J166" s="2" t="inlineStr"/>
+      <c r="K166" t="inlineStr"/>
+      <c r="L166" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="M166" t="inlineStr">
+        <is>
+          <t>1418</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-02-02 11:30:39
</commit_message>
<xml_diff>
--- a/Season_Attack/83.xlsx
+++ b/Season_Attack/83.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M166"/>
+  <dimension ref="A1:O166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,6 +456,16 @@
           <t>01-31_0</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>02-01_A</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>02-01_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -500,9 +510,15 @@
       <c r="L2" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>2763</t>
+      <c r="M2" t="n">
+        <v>2763</v>
+      </c>
+      <c r="N2" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>3126</t>
         </is>
       </c>
     </row>
@@ -549,9 +565,15 @@
       <c r="L3" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>3358</t>
+      <c r="M3" t="n">
+        <v>3358</v>
+      </c>
+      <c r="N3" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>3601</t>
         </is>
       </c>
     </row>
@@ -598,9 +620,15 @@
       <c r="L4" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>3651</t>
+      <c r="M4" t="n">
+        <v>3651</v>
+      </c>
+      <c r="N4" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>3888</t>
         </is>
       </c>
     </row>
@@ -647,9 +675,15 @@
       <c r="L5" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>3477</t>
+      <c r="M5" t="n">
+        <v>3477</v>
+      </c>
+      <c r="N5" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>3762</t>
         </is>
       </c>
     </row>
@@ -696,9 +730,15 @@
       <c r="L6" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>3358</t>
+      <c r="M6" t="n">
+        <v>3358</v>
+      </c>
+      <c r="N6" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>3697</t>
         </is>
       </c>
     </row>
@@ -745,9 +785,15 @@
       <c r="L7" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>3660</t>
+      <c r="M7" t="n">
+        <v>3660</v>
+      </c>
+      <c r="N7" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>4029</t>
         </is>
       </c>
     </row>
@@ -794,9 +840,15 @@
       <c r="L8" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>3368</t>
+      <c r="M8" t="n">
+        <v>3368</v>
+      </c>
+      <c r="N8" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>3628</t>
         </is>
       </c>
     </row>
@@ -843,9 +895,15 @@
       <c r="L9" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>3299</t>
+      <c r="M9" t="n">
+        <v>3299</v>
+      </c>
+      <c r="N9" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>3534</t>
         </is>
       </c>
     </row>
@@ -892,9 +950,15 @@
       <c r="L10" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>3469</t>
+      <c r="M10" t="n">
+        <v>3469</v>
+      </c>
+      <c r="N10" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>3588</t>
         </is>
       </c>
     </row>
@@ -941,9 +1005,15 @@
       <c r="L11" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>3458</t>
+      <c r="M11" t="n">
+        <v>3458</v>
+      </c>
+      <c r="N11" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>3674</t>
         </is>
       </c>
     </row>
@@ -990,9 +1060,15 @@
       <c r="L12" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>3305</t>
+      <c r="M12" t="n">
+        <v>3305</v>
+      </c>
+      <c r="N12" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>3521</t>
         </is>
       </c>
     </row>
@@ -1039,7 +1115,13 @@
       <c r="L13" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M13" t="inlineStr">
+      <c r="M13" t="n">
+        <v>2603</v>
+      </c>
+      <c r="N13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" t="inlineStr">
         <is>
           <t>2603</t>
         </is>
@@ -1088,9 +1170,15 @@
       <c r="L14" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>3896</t>
+      <c r="M14" t="n">
+        <v>3896</v>
+      </c>
+      <c r="N14" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>4267</t>
         </is>
       </c>
     </row>
@@ -1137,9 +1225,15 @@
       <c r="L15" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>3415</t>
+      <c r="M15" t="n">
+        <v>3415</v>
+      </c>
+      <c r="N15" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>3678</t>
         </is>
       </c>
     </row>
@@ -1186,9 +1280,15 @@
       <c r="L16" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>3688</t>
+      <c r="M16" t="n">
+        <v>3688</v>
+      </c>
+      <c r="N16" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>4067</t>
         </is>
       </c>
     </row>
@@ -1235,9 +1335,15 @@
       <c r="L17" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>3044</t>
+      <c r="M17" t="n">
+        <v>3044</v>
+      </c>
+      <c r="N17" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>3233</t>
         </is>
       </c>
     </row>
@@ -1284,9 +1390,15 @@
       <c r="L18" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>3316</t>
+      <c r="M18" t="n">
+        <v>3316</v>
+      </c>
+      <c r="N18" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>3527</t>
         </is>
       </c>
     </row>
@@ -1333,9 +1445,15 @@
       <c r="L19" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>3372</t>
+      <c r="M19" t="n">
+        <v>3372</v>
+      </c>
+      <c r="N19" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>3664</t>
         </is>
       </c>
     </row>
@@ -1382,9 +1500,15 @@
       <c r="L20" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>3890</t>
+      <c r="M20" t="n">
+        <v>3890</v>
+      </c>
+      <c r="N20" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>4259</t>
         </is>
       </c>
     </row>
@@ -1431,7 +1555,13 @@
       <c r="L21" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M21" t="inlineStr">
+      <c r="M21" t="n">
+        <v>2780</v>
+      </c>
+      <c r="N21" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O21" t="inlineStr">
         <is>
           <t>2780</t>
         </is>
@@ -1480,9 +1610,15 @@
       <c r="L22" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="M22" t="inlineStr">
-        <is>
-          <t>3465</t>
+      <c r="M22" t="n">
+        <v>3465</v>
+      </c>
+      <c r="N22" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>3703</t>
         </is>
       </c>
     </row>
@@ -1529,9 +1665,15 @@
       <c r="L23" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="M23" t="inlineStr">
-        <is>
-          <t>2588</t>
+      <c r="M23" t="n">
+        <v>2588</v>
+      </c>
+      <c r="N23" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>2884</t>
         </is>
       </c>
     </row>
@@ -1578,9 +1720,15 @@
       <c r="L24" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M24" t="inlineStr">
-        <is>
-          <t>3625</t>
+      <c r="M24" t="n">
+        <v>3625</v>
+      </c>
+      <c r="N24" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>3839</t>
         </is>
       </c>
     </row>
@@ -1627,7 +1775,13 @@
       <c r="L25" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M25" t="inlineStr">
+      <c r="M25" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1676,9 +1830,15 @@
       <c r="L26" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="M26" t="inlineStr">
-        <is>
-          <t>3771</t>
+      <c r="M26" t="n">
+        <v>3771</v>
+      </c>
+      <c r="N26" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>4114</t>
         </is>
       </c>
     </row>
@@ -1725,9 +1885,15 @@
       <c r="L27" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="M27" t="inlineStr">
-        <is>
-          <t>3685</t>
+      <c r="M27" t="n">
+        <v>3685</v>
+      </c>
+      <c r="N27" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>4095</t>
         </is>
       </c>
     </row>
@@ -1774,9 +1940,15 @@
       <c r="L28" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="M28" t="inlineStr">
-        <is>
-          <t>3114</t>
+      <c r="M28" t="n">
+        <v>3114</v>
+      </c>
+      <c r="N28" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>3355</t>
         </is>
       </c>
     </row>
@@ -1823,9 +1995,15 @@
       <c r="L29" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="M29" t="inlineStr">
-        <is>
-          <t>3864</t>
+      <c r="M29" t="n">
+        <v>3864</v>
+      </c>
+      <c r="N29" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>4161</t>
         </is>
       </c>
     </row>
@@ -1872,9 +2050,15 @@
       <c r="L30" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M30" t="inlineStr">
-        <is>
-          <t>3550</t>
+      <c r="M30" t="n">
+        <v>3550</v>
+      </c>
+      <c r="N30" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>3911</t>
         </is>
       </c>
     </row>
@@ -1921,9 +2105,15 @@
       <c r="L31" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M31" t="inlineStr">
-        <is>
-          <t>3448</t>
+      <c r="M31" t="n">
+        <v>3448</v>
+      </c>
+      <c r="N31" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>3674</t>
         </is>
       </c>
     </row>
@@ -1970,9 +2160,15 @@
       <c r="L32" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="M32" t="inlineStr">
-        <is>
-          <t>3783</t>
+      <c r="M32" t="n">
+        <v>3783</v>
+      </c>
+      <c r="N32" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>4070</t>
         </is>
       </c>
     </row>
@@ -2019,9 +2215,15 @@
       <c r="L33" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="M33" t="inlineStr">
-        <is>
-          <t>3564</t>
+      <c r="M33" t="n">
+        <v>3564</v>
+      </c>
+      <c r="N33" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>3769</t>
         </is>
       </c>
     </row>
@@ -2068,9 +2270,15 @@
       <c r="L34" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="M34" t="inlineStr">
-        <is>
-          <t>3066</t>
+      <c r="M34" t="n">
+        <v>3066</v>
+      </c>
+      <c r="N34" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>3638</t>
         </is>
       </c>
     </row>
@@ -2117,9 +2325,15 @@
       <c r="L35" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="M35" t="inlineStr">
-        <is>
-          <t>3780</t>
+      <c r="M35" t="n">
+        <v>3780</v>
+      </c>
+      <c r="N35" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>4043</t>
         </is>
       </c>
     </row>
@@ -2166,9 +2380,15 @@
       <c r="L36" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="M36" t="inlineStr">
-        <is>
-          <t>3494</t>
+      <c r="M36" t="n">
+        <v>3494</v>
+      </c>
+      <c r="N36" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>3838</t>
         </is>
       </c>
     </row>
@@ -2215,9 +2435,15 @@
       <c r="L37" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M37" t="inlineStr">
-        <is>
-          <t>3437</t>
+      <c r="M37" t="n">
+        <v>3437</v>
+      </c>
+      <c r="N37" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>3651</t>
         </is>
       </c>
     </row>
@@ -2264,9 +2490,15 @@
       <c r="L38" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M38" t="inlineStr">
-        <is>
-          <t>3663</t>
+      <c r="M38" t="n">
+        <v>3663</v>
+      </c>
+      <c r="N38" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>3888</t>
         </is>
       </c>
     </row>
@@ -2313,9 +2545,15 @@
       <c r="L39" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="M39" t="inlineStr">
-        <is>
-          <t>3503</t>
+      <c r="M39" t="n">
+        <v>3503</v>
+      </c>
+      <c r="N39" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>3706</t>
         </is>
       </c>
     </row>
@@ -2362,9 +2600,15 @@
       <c r="L40" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M40" t="inlineStr">
-        <is>
-          <t>3703</t>
+      <c r="M40" t="n">
+        <v>3703</v>
+      </c>
+      <c r="N40" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>4234</t>
         </is>
       </c>
     </row>
@@ -2411,9 +2655,15 @@
       <c r="L41" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M41" t="inlineStr">
-        <is>
-          <t>3480</t>
+      <c r="M41" t="n">
+        <v>3480</v>
+      </c>
+      <c r="N41" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>3744</t>
         </is>
       </c>
     </row>
@@ -2460,9 +2710,15 @@
       <c r="L42" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M42" t="inlineStr">
-        <is>
-          <t>3718</t>
+      <c r="M42" t="n">
+        <v>3718</v>
+      </c>
+      <c r="N42" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>4090</t>
         </is>
       </c>
     </row>
@@ -2509,9 +2765,15 @@
       <c r="L43" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M43" t="inlineStr">
-        <is>
-          <t>3623</t>
+      <c r="M43" t="n">
+        <v>3623</v>
+      </c>
+      <c r="N43" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>3822</t>
         </is>
       </c>
     </row>
@@ -2534,7 +2796,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F44" s="4" t="n">
@@ -2558,9 +2820,15 @@
       <c r="L44" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="M44" t="inlineStr">
-        <is>
-          <t>3576</t>
+      <c r="M44" t="n">
+        <v>3576</v>
+      </c>
+      <c r="N44" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>3738</t>
         </is>
       </c>
     </row>
@@ -2607,9 +2875,15 @@
       <c r="L45" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M45" t="inlineStr">
-        <is>
-          <t>3363</t>
+      <c r="M45" t="n">
+        <v>3363</v>
+      </c>
+      <c r="N45" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>3508</t>
         </is>
       </c>
     </row>
@@ -2656,9 +2930,15 @@
       <c r="L46" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="M46" t="inlineStr">
-        <is>
-          <t>3339</t>
+      <c r="M46" t="n">
+        <v>3339</v>
+      </c>
+      <c r="N46" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>3495</t>
         </is>
       </c>
     </row>
@@ -2705,7 +2985,13 @@
       <c r="L47" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="M47" t="inlineStr">
+      <c r="M47" t="n">
+        <v>3010</v>
+      </c>
+      <c r="N47" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O47" t="inlineStr">
         <is>
           <t>3010</t>
         </is>
@@ -2754,9 +3040,15 @@
       <c r="L48" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="M48" t="inlineStr">
-        <is>
-          <t>3486</t>
+      <c r="M48" t="n">
+        <v>3486</v>
+      </c>
+      <c r="N48" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>3746</t>
         </is>
       </c>
     </row>
@@ -2803,9 +3095,15 @@
       <c r="L49" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="M49" t="inlineStr">
-        <is>
-          <t>3248</t>
+      <c r="M49" t="n">
+        <v>3248</v>
+      </c>
+      <c r="N49" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>3391</t>
         </is>
       </c>
     </row>
@@ -2852,9 +3150,15 @@
       <c r="L50" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="M50" t="inlineStr">
-        <is>
-          <t>3719</t>
+      <c r="M50" t="n">
+        <v>3719</v>
+      </c>
+      <c r="N50" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>3919</t>
         </is>
       </c>
     </row>
@@ -2901,9 +3205,15 @@
       <c r="L51" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M51" t="inlineStr">
-        <is>
-          <t>2720</t>
+      <c r="M51" t="n">
+        <v>2720</v>
+      </c>
+      <c r="N51" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>2706</t>
         </is>
       </c>
     </row>
@@ -2950,9 +3260,15 @@
       <c r="L52" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M52" t="inlineStr">
-        <is>
-          <t>2603</t>
+      <c r="M52" t="n">
+        <v>2603</v>
+      </c>
+      <c r="N52" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>2667</t>
         </is>
       </c>
     </row>
@@ -2999,9 +3315,15 @@
       <c r="L53" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="M53" t="inlineStr">
-        <is>
-          <t>2675</t>
+      <c r="M53" t="n">
+        <v>2675</v>
+      </c>
+      <c r="N53" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>2672</t>
         </is>
       </c>
     </row>
@@ -3048,9 +3370,15 @@
       <c r="L54" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="M54" t="inlineStr">
-        <is>
-          <t>3665</t>
+      <c r="M54" t="n">
+        <v>3665</v>
+      </c>
+      <c r="N54" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>3876</t>
         </is>
       </c>
     </row>
@@ -3097,9 +3425,15 @@
       <c r="L55" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="M55" t="inlineStr">
-        <is>
-          <t>3031</t>
+      <c r="M55" t="n">
+        <v>3031</v>
+      </c>
+      <c r="N55" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>3181</t>
         </is>
       </c>
     </row>
@@ -3146,9 +3480,15 @@
       <c r="L56" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="M56" t="inlineStr">
-        <is>
-          <t>3159</t>
+      <c r="M56" t="n">
+        <v>3159</v>
+      </c>
+      <c r="N56" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>3310</t>
         </is>
       </c>
     </row>
@@ -3195,9 +3535,15 @@
       <c r="L57" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M57" t="inlineStr">
-        <is>
-          <t>3352</t>
+      <c r="M57" t="n">
+        <v>3352</v>
+      </c>
+      <c r="N57" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>3657</t>
         </is>
       </c>
     </row>
@@ -3244,9 +3590,15 @@
       <c r="L58" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M58" t="inlineStr">
-        <is>
-          <t>3043</t>
+      <c r="M58" t="n">
+        <v>3043</v>
+      </c>
+      <c r="N58" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>3236</t>
         </is>
       </c>
     </row>
@@ -3293,9 +3645,15 @@
       <c r="L59" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="M59" t="inlineStr">
-        <is>
-          <t>3308</t>
+      <c r="M59" t="n">
+        <v>3308</v>
+      </c>
+      <c r="N59" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O59" t="inlineStr">
+        <is>
+          <t>3325</t>
         </is>
       </c>
     </row>
@@ -3342,7 +3700,13 @@
       <c r="L60" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M60" t="inlineStr">
+      <c r="M60" t="n">
+        <v>0</v>
+      </c>
+      <c r="N60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O60" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3391,9 +3755,15 @@
       <c r="L61" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="M61" t="inlineStr">
-        <is>
-          <t>3483</t>
+      <c r="M61" t="n">
+        <v>3483</v>
+      </c>
+      <c r="N61" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>3823</t>
         </is>
       </c>
     </row>
@@ -3440,9 +3810,15 @@
       <c r="L62" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M62" t="inlineStr">
-        <is>
-          <t>2510</t>
+      <c r="M62" t="n">
+        <v>2510</v>
+      </c>
+      <c r="N62" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O62" t="inlineStr">
+        <is>
+          <t>2527</t>
         </is>
       </c>
     </row>
@@ -3489,9 +3865,15 @@
       <c r="L63" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M63" t="inlineStr">
-        <is>
-          <t>2395</t>
+      <c r="M63" t="n">
+        <v>2395</v>
+      </c>
+      <c r="N63" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>2707</t>
         </is>
       </c>
     </row>
@@ -3538,9 +3920,15 @@
       <c r="L64" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="M64" t="inlineStr">
-        <is>
-          <t>3399</t>
+      <c r="M64" t="n">
+        <v>3399</v>
+      </c>
+      <c r="N64" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="O64" t="inlineStr">
+        <is>
+          <t>3658</t>
         </is>
       </c>
     </row>
@@ -3587,11 +3975,11 @@
       <c r="L65" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M65" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="M65" t="n">
+        <v>0</v>
+      </c>
+      <c r="N65" s="2" t="inlineStr"/>
+      <c r="O65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -3636,9 +4024,15 @@
       <c r="L66" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="M66" t="inlineStr">
-        <is>
-          <t>3466</t>
+      <c r="M66" t="n">
+        <v>3466</v>
+      </c>
+      <c r="N66" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>3747</t>
         </is>
       </c>
     </row>
@@ -3685,9 +4079,15 @@
       <c r="L67" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M67" t="inlineStr">
-        <is>
-          <t>3201</t>
+      <c r="M67" t="n">
+        <v>3201</v>
+      </c>
+      <c r="N67" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>3342</t>
         </is>
       </c>
     </row>
@@ -3734,9 +4134,15 @@
       <c r="L68" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M68" t="inlineStr">
-        <is>
-          <t>2512</t>
+      <c r="M68" t="n">
+        <v>2512</v>
+      </c>
+      <c r="N68" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O68" t="inlineStr">
+        <is>
+          <t>2528</t>
         </is>
       </c>
     </row>
@@ -3783,9 +4189,15 @@
       <c r="L69" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="M69" t="inlineStr">
-        <is>
-          <t>3131</t>
+      <c r="M69" t="n">
+        <v>3131</v>
+      </c>
+      <c r="N69" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>3323</t>
         </is>
       </c>
     </row>
@@ -3832,9 +4244,15 @@
       <c r="L70" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="M70" t="inlineStr">
-        <is>
-          <t>2899</t>
+      <c r="M70" t="n">
+        <v>2899</v>
+      </c>
+      <c r="N70" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="O70" t="inlineStr">
+        <is>
+          <t>3098</t>
         </is>
       </c>
     </row>
@@ -3881,9 +4299,15 @@
       <c r="L71" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M71" t="inlineStr">
-        <is>
-          <t>3048</t>
+      <c r="M71" t="n">
+        <v>3048</v>
+      </c>
+      <c r="N71" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>3279</t>
         </is>
       </c>
     </row>
@@ -3930,9 +4354,15 @@
       <c r="L72" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M72" t="inlineStr">
-        <is>
-          <t>2641</t>
+      <c r="M72" t="n">
+        <v>2641</v>
+      </c>
+      <c r="N72" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O72" t="inlineStr">
+        <is>
+          <t>2638</t>
         </is>
       </c>
     </row>
@@ -3979,9 +4409,15 @@
       <c r="L73" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="M73" t="inlineStr">
-        <is>
-          <t>2993</t>
+      <c r="M73" t="n">
+        <v>2993</v>
+      </c>
+      <c r="N73" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>3133</t>
         </is>
       </c>
     </row>
@@ -4028,9 +4464,15 @@
       <c r="L74" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="M74" t="inlineStr">
-        <is>
-          <t>3320</t>
+      <c r="M74" t="n">
+        <v>3320</v>
+      </c>
+      <c r="N74" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>3515</t>
         </is>
       </c>
     </row>
@@ -4077,9 +4519,15 @@
       <c r="L75" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="M75" t="inlineStr">
-        <is>
-          <t>3293</t>
+      <c r="M75" t="n">
+        <v>3293</v>
+      </c>
+      <c r="N75" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>3556</t>
         </is>
       </c>
     </row>
@@ -4126,11 +4574,11 @@
       <c r="L76" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M76" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="M76" t="n">
+        <v>0</v>
+      </c>
+      <c r="N76" s="2" t="inlineStr"/>
+      <c r="O76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -4175,9 +4623,15 @@
       <c r="L77" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="M77" t="inlineStr">
-        <is>
-          <t>3463</t>
+      <c r="M77" t="n">
+        <v>3463</v>
+      </c>
+      <c r="N77" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>3645</t>
         </is>
       </c>
     </row>
@@ -4224,7 +4678,13 @@
       <c r="L78" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M78" t="inlineStr">
+      <c r="M78" t="n">
+        <v>2500</v>
+      </c>
+      <c r="N78" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O78" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -4273,9 +4733,15 @@
       <c r="L79" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="M79" t="inlineStr">
-        <is>
-          <t>3320</t>
+      <c r="M79" t="n">
+        <v>3320</v>
+      </c>
+      <c r="N79" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>3417</t>
         </is>
       </c>
     </row>
@@ -4322,9 +4788,15 @@
       <c r="L80" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="M80" t="inlineStr">
-        <is>
-          <t>3356</t>
+      <c r="M80" t="n">
+        <v>3356</v>
+      </c>
+      <c r="N80" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>3628</t>
         </is>
       </c>
     </row>
@@ -4371,9 +4843,15 @@
       <c r="L81" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="M81" t="inlineStr">
-        <is>
-          <t>3236</t>
+      <c r="M81" t="n">
+        <v>3236</v>
+      </c>
+      <c r="N81" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>3518</t>
         </is>
       </c>
     </row>
@@ -4420,9 +4898,15 @@
       <c r="L82" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="M82" t="inlineStr">
-        <is>
-          <t>3152</t>
+      <c r="M82" t="n">
+        <v>3152</v>
+      </c>
+      <c r="N82" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>3351</t>
         </is>
       </c>
     </row>
@@ -4460,6 +4944,8 @@
       <c r="K83" t="inlineStr"/>
       <c r="L83" s="2" t="inlineStr"/>
       <c r="M83" t="inlineStr"/>
+      <c r="N83" s="2" t="inlineStr"/>
+      <c r="O83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -4504,9 +4990,15 @@
       <c r="L84" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M84" t="inlineStr">
-        <is>
-          <t>2741</t>
+      <c r="M84" t="n">
+        <v>2741</v>
+      </c>
+      <c r="N84" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>2757</t>
         </is>
       </c>
     </row>
@@ -4553,9 +5045,15 @@
       <c r="L85" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M85" t="inlineStr">
-        <is>
-          <t>2499</t>
+      <c r="M85" t="n">
+        <v>2499</v>
+      </c>
+      <c r="N85" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>2764</t>
         </is>
       </c>
     </row>
@@ -4602,9 +5100,15 @@
       <c r="L86" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M86" t="inlineStr">
-        <is>
-          <t>3368</t>
+      <c r="M86" t="n">
+        <v>3368</v>
+      </c>
+      <c r="N86" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="O86" t="inlineStr">
+        <is>
+          <t>3686</t>
         </is>
       </c>
     </row>
@@ -4651,9 +5155,15 @@
       <c r="L87" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M87" t="inlineStr">
-        <is>
-          <t>2670</t>
+      <c r="M87" t="n">
+        <v>2670</v>
+      </c>
+      <c r="N87" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O87" t="inlineStr">
+        <is>
+          <t>2705</t>
         </is>
       </c>
     </row>
@@ -4700,9 +5210,15 @@
       <c r="L88" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="M88" t="inlineStr">
-        <is>
-          <t>2663</t>
+      <c r="M88" t="n">
+        <v>2663</v>
+      </c>
+      <c r="N88" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O88" t="inlineStr">
+        <is>
+          <t>2868</t>
         </is>
       </c>
     </row>
@@ -4732,6 +5248,8 @@
       <c r="K89" t="inlineStr"/>
       <c r="L89" s="2" t="inlineStr"/>
       <c r="M89" t="inlineStr"/>
+      <c r="N89" s="2" t="inlineStr"/>
+      <c r="O89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -4776,9 +5294,15 @@
       <c r="L90" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="M90" t="inlineStr">
-        <is>
-          <t>2450</t>
+      <c r="M90" t="n">
+        <v>2450</v>
+      </c>
+      <c r="N90" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>2497</t>
         </is>
       </c>
     </row>
@@ -4825,11 +5349,11 @@
       <c r="L91" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M91" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="M91" t="n">
+        <v>0</v>
+      </c>
+      <c r="N91" s="2" t="inlineStr"/>
+      <c r="O91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -4874,9 +5398,15 @@
       <c r="L92" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M92" t="inlineStr">
-        <is>
-          <t>2660</t>
+      <c r="M92" t="n">
+        <v>2660</v>
+      </c>
+      <c r="N92" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O92" t="inlineStr">
+        <is>
+          <t>2619</t>
         </is>
       </c>
     </row>
@@ -4923,9 +5453,15 @@
       <c r="L93" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="M93" t="inlineStr">
-        <is>
-          <t>2714</t>
+      <c r="M93" t="n">
+        <v>2714</v>
+      </c>
+      <c r="N93" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="O93" t="inlineStr">
+        <is>
+          <t>2671</t>
         </is>
       </c>
     </row>
@@ -4972,7 +5508,13 @@
       <c r="L94" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M94" t="inlineStr">
+      <c r="M94" t="n">
+        <v>0</v>
+      </c>
+      <c r="N94" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5021,9 +5563,15 @@
       <c r="L95" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="M95" t="inlineStr">
-        <is>
-          <t>2088</t>
+      <c r="M95" t="n">
+        <v>2088</v>
+      </c>
+      <c r="N95" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="O95" t="inlineStr">
+        <is>
+          <t>2462</t>
         </is>
       </c>
     </row>
@@ -5070,9 +5618,15 @@
       <c r="L96" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M96" t="inlineStr">
-        <is>
-          <t>2004</t>
+      <c r="M96" t="n">
+        <v>2004</v>
+      </c>
+      <c r="N96" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O96" t="inlineStr">
+        <is>
+          <t>2011</t>
         </is>
       </c>
     </row>
@@ -5119,9 +5673,15 @@
       <c r="L97" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M97" t="inlineStr">
-        <is>
-          <t>2465</t>
+      <c r="M97" t="n">
+        <v>2465</v>
+      </c>
+      <c r="N97" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="O97" t="inlineStr">
+        <is>
+          <t>2556</t>
         </is>
       </c>
     </row>
@@ -5168,9 +5728,15 @@
       <c r="L98" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="M98" t="inlineStr">
-        <is>
-          <t>2376</t>
+      <c r="M98" t="n">
+        <v>2376</v>
+      </c>
+      <c r="N98" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O98" t="inlineStr">
+        <is>
+          <t>2341</t>
         </is>
       </c>
     </row>
@@ -5217,9 +5783,15 @@
       <c r="L99" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="M99" t="inlineStr">
-        <is>
-          <t>2843</t>
+      <c r="M99" t="n">
+        <v>2843</v>
+      </c>
+      <c r="N99" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="O99" t="inlineStr">
+        <is>
+          <t>2899</t>
         </is>
       </c>
     </row>
@@ -5266,9 +5838,15 @@
       <c r="L100" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="M100" t="inlineStr">
-        <is>
-          <t>2492</t>
+      <c r="M100" t="n">
+        <v>2492</v>
+      </c>
+      <c r="N100" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O100" t="inlineStr">
+        <is>
+          <t>2441</t>
         </is>
       </c>
     </row>
@@ -5315,9 +5893,15 @@
       <c r="L101" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="M101" t="inlineStr">
-        <is>
-          <t>3240</t>
+      <c r="M101" t="n">
+        <v>3240</v>
+      </c>
+      <c r="N101" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="O101" t="inlineStr">
+        <is>
+          <t>3433</t>
         </is>
       </c>
     </row>
@@ -5364,9 +5948,15 @@
       <c r="L102" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M102" t="inlineStr">
-        <is>
-          <t>2980</t>
+      <c r="M102" t="n">
+        <v>2980</v>
+      </c>
+      <c r="N102" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O102" t="inlineStr">
+        <is>
+          <t>3085</t>
         </is>
       </c>
     </row>
@@ -5413,9 +6003,15 @@
       <c r="L103" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="M103" t="inlineStr">
-        <is>
-          <t>2845</t>
+      <c r="M103" t="n">
+        <v>2845</v>
+      </c>
+      <c r="N103" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O103" t="inlineStr">
+        <is>
+          <t>2831</t>
         </is>
       </c>
     </row>
@@ -5462,9 +6058,15 @@
       <c r="L104" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="M104" t="inlineStr">
-        <is>
-          <t>3240</t>
+      <c r="M104" t="n">
+        <v>3240</v>
+      </c>
+      <c r="N104" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="O104" t="inlineStr">
+        <is>
+          <t>3406</t>
         </is>
       </c>
     </row>
@@ -5511,9 +6113,15 @@
       <c r="L105" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M105" t="inlineStr">
-        <is>
-          <t>2802</t>
+      <c r="M105" t="n">
+        <v>2802</v>
+      </c>
+      <c r="N105" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="O105" t="inlineStr">
+        <is>
+          <t>3101</t>
         </is>
       </c>
     </row>
@@ -5560,9 +6168,15 @@
       <c r="L106" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M106" t="inlineStr">
-        <is>
-          <t>2488</t>
+      <c r="M106" t="n">
+        <v>2488</v>
+      </c>
+      <c r="N106" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O106" t="inlineStr">
+        <is>
+          <t>2470</t>
         </is>
       </c>
     </row>
@@ -5609,9 +6223,15 @@
       <c r="L107" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M107" t="inlineStr">
-        <is>
-          <t>2480</t>
+      <c r="M107" t="n">
+        <v>2480</v>
+      </c>
+      <c r="N107" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O107" t="inlineStr">
+        <is>
+          <t>2491</t>
         </is>
       </c>
     </row>
@@ -5658,9 +6278,15 @@
       <c r="L108" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M108" t="inlineStr">
-        <is>
-          <t>2493</t>
+      <c r="M108" t="n">
+        <v>2493</v>
+      </c>
+      <c r="N108" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O108" t="inlineStr">
+        <is>
+          <t>2519</t>
         </is>
       </c>
     </row>
@@ -5707,9 +6333,15 @@
       <c r="L109" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M109" t="inlineStr">
-        <is>
-          <t>2859</t>
+      <c r="M109" t="n">
+        <v>2859</v>
+      </c>
+      <c r="N109" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="O109" t="inlineStr">
+        <is>
+          <t>2973</t>
         </is>
       </c>
     </row>
@@ -5756,9 +6388,15 @@
       <c r="L110" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="M110" t="inlineStr">
-        <is>
-          <t>2921</t>
+      <c r="M110" t="n">
+        <v>2921</v>
+      </c>
+      <c r="N110" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="O110" t="inlineStr">
+        <is>
+          <t>3021</t>
         </is>
       </c>
     </row>
@@ -5805,9 +6443,15 @@
       <c r="L111" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="M111" t="inlineStr">
-        <is>
-          <t>2545</t>
+      <c r="M111" t="n">
+        <v>2545</v>
+      </c>
+      <c r="N111" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="O111" t="inlineStr">
+        <is>
+          <t>2583</t>
         </is>
       </c>
     </row>
@@ -5854,9 +6498,15 @@
       <c r="L112" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M112" t="inlineStr">
-        <is>
-          <t>2474</t>
+      <c r="M112" t="n">
+        <v>2474</v>
+      </c>
+      <c r="N112" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O112" t="inlineStr">
+        <is>
+          <t>2486</t>
         </is>
       </c>
     </row>
@@ -5903,9 +6553,15 @@
       <c r="L113" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="M113" t="inlineStr">
-        <is>
-          <t>2815</t>
+      <c r="M113" t="n">
+        <v>2815</v>
+      </c>
+      <c r="N113" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="O113" t="inlineStr">
+        <is>
+          <t>2879</t>
         </is>
       </c>
     </row>
@@ -5952,9 +6608,15 @@
       <c r="L114" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M114" t="inlineStr">
-        <is>
-          <t>2645</t>
+      <c r="M114" t="n">
+        <v>2645</v>
+      </c>
+      <c r="N114" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O114" t="inlineStr">
+        <is>
+          <t>2797</t>
         </is>
       </c>
     </row>
@@ -6001,9 +6663,15 @@
       <c r="L115" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="M115" t="inlineStr">
-        <is>
-          <t>3040</t>
+      <c r="M115" t="n">
+        <v>3040</v>
+      </c>
+      <c r="N115" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="O115" t="inlineStr">
+        <is>
+          <t>3195</t>
         </is>
       </c>
     </row>
@@ -6050,9 +6718,15 @@
       <c r="L116" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="M116" t="inlineStr">
-        <is>
-          <t>2496</t>
+      <c r="M116" t="n">
+        <v>2496</v>
+      </c>
+      <c r="N116" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="O116" t="inlineStr">
+        <is>
+          <t>2545</t>
         </is>
       </c>
     </row>
@@ -6099,9 +6773,15 @@
       <c r="L117" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="M117" t="inlineStr">
-        <is>
-          <t>2611</t>
+      <c r="M117" t="n">
+        <v>2611</v>
+      </c>
+      <c r="N117" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="O117" t="inlineStr">
+        <is>
+          <t>2680</t>
         </is>
       </c>
     </row>
@@ -6148,9 +6828,15 @@
       <c r="L118" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="M118" t="inlineStr">
-        <is>
-          <t>3008</t>
+      <c r="M118" t="n">
+        <v>3008</v>
+      </c>
+      <c r="N118" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="O118" t="inlineStr">
+        <is>
+          <t>3078</t>
         </is>
       </c>
     </row>
@@ -6197,7 +6883,13 @@
       <c r="L119" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M119" t="inlineStr">
+      <c r="M119" t="n">
+        <v>0</v>
+      </c>
+      <c r="N119" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O119" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6246,9 +6938,15 @@
       <c r="L120" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="M120" t="inlineStr">
-        <is>
-          <t>2978</t>
+      <c r="M120" t="n">
+        <v>2978</v>
+      </c>
+      <c r="N120" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="O120" t="inlineStr">
+        <is>
+          <t>3069</t>
         </is>
       </c>
     </row>
@@ -6295,9 +6993,15 @@
       <c r="L121" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M121" t="inlineStr">
-        <is>
-          <t>2683</t>
+      <c r="M121" t="n">
+        <v>2683</v>
+      </c>
+      <c r="N121" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="O121" t="inlineStr">
+        <is>
+          <t>2719</t>
         </is>
       </c>
     </row>
@@ -6344,9 +7048,15 @@
       <c r="L122" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M122" t="inlineStr">
-        <is>
-          <t>2641</t>
+      <c r="M122" t="n">
+        <v>2641</v>
+      </c>
+      <c r="N122" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O122" t="inlineStr">
+        <is>
+          <t>2743</t>
         </is>
       </c>
     </row>
@@ -6393,7 +7103,13 @@
       <c r="L123" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M123" t="inlineStr">
+      <c r="M123" t="n">
+        <v>2536</v>
+      </c>
+      <c r="N123" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O123" t="inlineStr">
         <is>
           <t>2536</t>
         </is>
@@ -6442,9 +7158,15 @@
       <c r="L124" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M124" t="inlineStr">
-        <is>
-          <t>2727</t>
+      <c r="M124" t="n">
+        <v>2727</v>
+      </c>
+      <c r="N124" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="O124" t="inlineStr">
+        <is>
+          <t>2810</t>
         </is>
       </c>
     </row>
@@ -6491,9 +7213,15 @@
       <c r="L125" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M125" t="inlineStr">
-        <is>
-          <t>2774</t>
+      <c r="M125" t="n">
+        <v>2774</v>
+      </c>
+      <c r="N125" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O125" t="inlineStr">
+        <is>
+          <t>2846</t>
         </is>
       </c>
     </row>
@@ -6540,9 +7268,15 @@
       <c r="L126" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M126" t="inlineStr">
-        <is>
-          <t>2910</t>
+      <c r="M126" t="n">
+        <v>2910</v>
+      </c>
+      <c r="N126" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O126" t="inlineStr">
+        <is>
+          <t>3036</t>
         </is>
       </c>
     </row>
@@ -6589,9 +7323,15 @@
       <c r="L127" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M127" t="inlineStr">
-        <is>
-          <t>2671</t>
+      <c r="M127" t="n">
+        <v>2671</v>
+      </c>
+      <c r="N127" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O127" t="inlineStr">
+        <is>
+          <t>2832</t>
         </is>
       </c>
     </row>
@@ -6638,7 +7378,13 @@
       <c r="L128" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M128" t="inlineStr">
+      <c r="M128" t="n">
+        <v>0</v>
+      </c>
+      <c r="N128" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6687,7 +7433,13 @@
       <c r="L129" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M129" t="inlineStr">
+      <c r="M129" t="n">
+        <v>0</v>
+      </c>
+      <c r="N129" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6736,9 +7488,15 @@
       <c r="L130" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M130" t="inlineStr">
-        <is>
-          <t>2647</t>
+      <c r="M130" t="n">
+        <v>2647</v>
+      </c>
+      <c r="N130" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O130" t="inlineStr">
+        <is>
+          <t>2639</t>
         </is>
       </c>
     </row>
@@ -6785,9 +7543,15 @@
       <c r="L131" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M131" t="inlineStr">
-        <is>
-          <t>2365</t>
+      <c r="M131" t="n">
+        <v>2365</v>
+      </c>
+      <c r="N131" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O131" t="inlineStr">
+        <is>
+          <t>2650</t>
         </is>
       </c>
     </row>
@@ -6834,9 +7598,15 @@
       <c r="L132" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M132" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M132" t="n">
+        <v>0</v>
+      </c>
+      <c r="N132" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O132" t="inlineStr">
+        <is>
+          <t>1061</t>
         </is>
       </c>
     </row>
@@ -6883,9 +7653,15 @@
       <c r="L133" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M133" t="inlineStr">
-        <is>
-          <t>2067</t>
+      <c r="M133" t="n">
+        <v>2067</v>
+      </c>
+      <c r="N133" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O133" t="inlineStr">
+        <is>
+          <t>2061</t>
         </is>
       </c>
     </row>
@@ -6932,9 +7708,15 @@
       <c r="L134" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="M134" t="inlineStr">
-        <is>
-          <t>2860</t>
+      <c r="M134" t="n">
+        <v>2860</v>
+      </c>
+      <c r="N134" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="O134" t="inlineStr">
+        <is>
+          <t>2971</t>
         </is>
       </c>
     </row>
@@ -6981,7 +7763,13 @@
       <c r="L135" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M135" t="inlineStr">
+      <c r="M135" t="n">
+        <v>0</v>
+      </c>
+      <c r="N135" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O135" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7030,7 +7818,13 @@
       <c r="L136" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M136" t="inlineStr">
+      <c r="M136" t="n">
+        <v>0</v>
+      </c>
+      <c r="N136" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O136" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7079,7 +7873,13 @@
       <c r="L137" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M137" t="inlineStr">
+      <c r="M137" t="n">
+        <v>0</v>
+      </c>
+      <c r="N137" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7128,9 +7928,15 @@
       <c r="L138" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="M138" t="inlineStr">
-        <is>
-          <t>2722</t>
+      <c r="M138" t="n">
+        <v>2722</v>
+      </c>
+      <c r="N138" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="O138" t="inlineStr">
+        <is>
+          <t>2873</t>
         </is>
       </c>
     </row>
@@ -7177,7 +7983,13 @@
       <c r="L139" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M139" t="inlineStr">
+      <c r="M139" t="n">
+        <v>0</v>
+      </c>
+      <c r="N139" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O139" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7226,9 +8038,15 @@
       <c r="L140" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="M140" t="inlineStr">
-        <is>
-          <t>2587</t>
+      <c r="M140" t="n">
+        <v>2587</v>
+      </c>
+      <c r="N140" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="O140" t="inlineStr">
+        <is>
+          <t>2659</t>
         </is>
       </c>
     </row>
@@ -7275,7 +8093,13 @@
       <c r="L141" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M141" t="inlineStr">
+      <c r="M141" t="n">
+        <v>0</v>
+      </c>
+      <c r="N141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O141" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7324,9 +8148,15 @@
       <c r="L142" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="M142" t="inlineStr">
-        <is>
-          <t>2580</t>
+      <c r="M142" t="n">
+        <v>2580</v>
+      </c>
+      <c r="N142" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="O142" t="inlineStr">
+        <is>
+          <t>2659</t>
         </is>
       </c>
     </row>
@@ -7372,6 +8202,8 @@
       </c>
       <c r="L143" s="2" t="inlineStr"/>
       <c r="M143" t="inlineStr"/>
+      <c r="N143" s="2" t="inlineStr"/>
+      <c r="O143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -7416,9 +8248,15 @@
       <c r="L144" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="M144" t="inlineStr">
-        <is>
-          <t>2472</t>
+      <c r="M144" t="n">
+        <v>2472</v>
+      </c>
+      <c r="N144" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="O144" t="inlineStr">
+        <is>
+          <t>2497</t>
         </is>
       </c>
     </row>
@@ -7465,7 +8303,13 @@
       <c r="L145" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M145" t="inlineStr">
+      <c r="M145" t="n">
+        <v>0</v>
+      </c>
+      <c r="N145" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O145" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7514,7 +8358,13 @@
       <c r="L146" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M146" t="inlineStr">
+      <c r="M146" t="n">
+        <v>0</v>
+      </c>
+      <c r="N146" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7563,7 +8413,13 @@
       <c r="L147" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M147" t="inlineStr">
+      <c r="M147" t="n">
+        <v>0</v>
+      </c>
+      <c r="N147" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O147" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7612,7 +8468,13 @@
       <c r="L148" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M148" t="inlineStr">
+      <c r="M148" t="n">
+        <v>0</v>
+      </c>
+      <c r="N148" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7661,7 +8523,13 @@
       <c r="L149" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M149" t="inlineStr">
+      <c r="M149" t="n">
+        <v>0</v>
+      </c>
+      <c r="N149" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O149" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7710,9 +8578,15 @@
       <c r="L150" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="M150" t="inlineStr">
-        <is>
-          <t>2342</t>
+      <c r="M150" t="n">
+        <v>2342</v>
+      </c>
+      <c r="N150" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="O150" t="inlineStr">
+        <is>
+          <t>2320</t>
         </is>
       </c>
     </row>
@@ -7759,9 +8633,15 @@
       <c r="L151" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M151" t="inlineStr">
-        <is>
-          <t>1500</t>
+      <c r="M151" t="n">
+        <v>1500</v>
+      </c>
+      <c r="N151" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O151" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -7808,9 +8688,15 @@
       <c r="L152" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="M152" t="inlineStr">
-        <is>
-          <t>1609</t>
+      <c r="M152" t="n">
+        <v>1609</v>
+      </c>
+      <c r="N152" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O152" t="inlineStr">
+        <is>
+          <t>1602</t>
         </is>
       </c>
     </row>
@@ -7857,9 +8743,15 @@
       <c r="L153" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="M153" t="inlineStr">
-        <is>
-          <t>1729</t>
+      <c r="M153" t="n">
+        <v>1729</v>
+      </c>
+      <c r="N153" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="O153" t="inlineStr">
+        <is>
+          <t>1778</t>
         </is>
       </c>
     </row>
@@ -7906,7 +8798,13 @@
       <c r="L154" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M154" t="inlineStr">
+      <c r="M154" t="n">
+        <v>0</v>
+      </c>
+      <c r="N154" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7955,9 +8853,15 @@
       <c r="L155" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="M155" t="inlineStr">
-        <is>
-          <t>2925</t>
+      <c r="M155" t="n">
+        <v>2925</v>
+      </c>
+      <c r="N155" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="O155" t="inlineStr">
+        <is>
+          <t>3585</t>
         </is>
       </c>
     </row>
@@ -8004,7 +8908,13 @@
       <c r="L156" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M156" t="inlineStr">
+      <c r="M156" t="n">
+        <v>0</v>
+      </c>
+      <c r="N156" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O156" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8053,7 +8963,13 @@
       <c r="L157" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M157" t="inlineStr">
+      <c r="M157" t="n">
+        <v>0</v>
+      </c>
+      <c r="N157" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O157" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8098,9 +9014,15 @@
       <c r="L158" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="M158" t="inlineStr">
-        <is>
-          <t>3591</t>
+      <c r="M158" t="n">
+        <v>3591</v>
+      </c>
+      <c r="N158" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="O158" t="inlineStr">
+        <is>
+          <t>3822</t>
         </is>
       </c>
     </row>
@@ -8147,7 +9069,13 @@
       <c r="L159" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M159" t="inlineStr">
+      <c r="M159" t="n">
+        <v>0</v>
+      </c>
+      <c r="N159" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O159" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8196,9 +9124,15 @@
       <c r="L160" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="M160" t="inlineStr">
-        <is>
-          <t>2582</t>
+      <c r="M160" t="n">
+        <v>2582</v>
+      </c>
+      <c r="N160" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="O160" t="inlineStr">
+        <is>
+          <t>2739</t>
         </is>
       </c>
     </row>
@@ -8245,7 +9179,13 @@
       <c r="L161" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M161" t="inlineStr">
+      <c r="M161" t="n">
+        <v>0</v>
+      </c>
+      <c r="N161" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O161" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8294,9 +9234,15 @@
       <c r="L162" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M162" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M162" t="n">
+        <v>0</v>
+      </c>
+      <c r="N162" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O162" t="inlineStr">
+        <is>
+          <t>2511</t>
         </is>
       </c>
     </row>
@@ -8343,9 +9289,15 @@
       <c r="L163" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="M163" t="inlineStr">
-        <is>
-          <t>2461</t>
+      <c r="M163" t="n">
+        <v>2461</v>
+      </c>
+      <c r="N163" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O163" t="inlineStr">
+        <is>
+          <t>2437</t>
         </is>
       </c>
     </row>
@@ -8382,17 +9334,21 @@
       <c r="L164" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="M164" t="inlineStr">
-        <is>
-          <t>2058</t>
+      <c r="M164" t="n">
+        <v>2058</v>
+      </c>
+      <c r="N164" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O164" t="inlineStr">
+        <is>
+          <t>2052</t>
         </is>
       </c>
     </row>
     <row r="165">
-      <c r="A165" t="inlineStr">
-        <is>
-          <t>58739336</t>
-        </is>
+      <c r="A165" t="n">
+        <v>58739336</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>
@@ -8415,17 +9371,21 @@
       <c r="L165" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="M165" t="inlineStr">
-        <is>
-          <t>1753</t>
+      <c r="M165" t="n">
+        <v>1753</v>
+      </c>
+      <c r="N165" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="O165" t="inlineStr">
+        <is>
+          <t>2000</t>
         </is>
       </c>
     </row>
     <row r="166">
-      <c r="A166" t="inlineStr">
-        <is>
-          <t>58739866</t>
-        </is>
+      <c r="A166" t="n">
+        <v>58739866</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>
@@ -8448,9 +9408,15 @@
       <c r="L166" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="M166" t="inlineStr">
-        <is>
-          <t>1418</t>
+      <c r="M166" t="n">
+        <v>1418</v>
+      </c>
+      <c r="N166" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O166" t="inlineStr">
+        <is>
+          <t>1512</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-02-03 11:30:34
</commit_message>
<xml_diff>
--- a/Season_Attack/83.xlsx
+++ b/Season_Attack/83.xlsx
@@ -83,8 +83,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O166"/>
+  <dimension ref="A1:Q166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,6 +466,16 @@
           <t>02-01_0</t>
         </is>
       </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>02-02_A</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>02-02_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -516,9 +526,15 @@
       <c r="N2" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>3126</t>
+      <c r="O2" t="n">
+        <v>3126</v>
+      </c>
+      <c r="P2" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>3416</t>
         </is>
       </c>
     </row>
@@ -571,9 +587,15 @@
       <c r="N3" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>3601</t>
+      <c r="O3" t="n">
+        <v>3601</v>
+      </c>
+      <c r="P3" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>3970</t>
         </is>
       </c>
     </row>
@@ -605,30 +627,36 @@
       <c r="G4" t="n">
         <v>6411</v>
       </c>
-      <c r="H4" s="4" t="n">
+      <c r="H4" s="5" t="n">
         <v>35</v>
       </c>
       <c r="I4" t="n">
         <v>2939</v>
       </c>
-      <c r="J4" s="4" t="n">
+      <c r="J4" s="5" t="n">
         <v>35</v>
       </c>
       <c r="K4" t="n">
         <v>3341</v>
       </c>
-      <c r="L4" s="4" t="n">
+      <c r="L4" s="5" t="n">
         <v>36</v>
       </c>
       <c r="M4" t="n">
         <v>3651</v>
       </c>
-      <c r="N4" s="4" t="n">
+      <c r="N4" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>3888</t>
+      <c r="O4" t="n">
+        <v>3888</v>
+      </c>
+      <c r="P4" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>4145</t>
         </is>
       </c>
     </row>
@@ -681,9 +709,15 @@
       <c r="N5" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>3762</t>
+      <c r="O5" t="n">
+        <v>3762</v>
+      </c>
+      <c r="P5" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>4075</t>
         </is>
       </c>
     </row>
@@ -736,9 +770,15 @@
       <c r="N6" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>3697</t>
+      <c r="O6" t="n">
+        <v>3697</v>
+      </c>
+      <c r="P6" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>4001</t>
         </is>
       </c>
     </row>
@@ -764,36 +804,42 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F7" s="4" t="n">
+      <c r="F7" s="5" t="n">
         <v>35</v>
       </c>
       <c r="G7" t="n">
         <v>6498</v>
       </c>
-      <c r="H7" s="4" t="n">
+      <c r="H7" s="5" t="n">
         <v>35</v>
       </c>
       <c r="I7" t="n">
         <v>2985</v>
       </c>
-      <c r="J7" s="4" t="n">
+      <c r="J7" s="5" t="n">
         <v>35</v>
       </c>
       <c r="K7" t="n">
         <v>3329</v>
       </c>
-      <c r="L7" s="4" t="n">
+      <c r="L7" s="5" t="n">
         <v>35</v>
       </c>
       <c r="M7" t="n">
         <v>3660</v>
       </c>
-      <c r="N7" s="4" t="n">
+      <c r="N7" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>4029</t>
+      <c r="O7" t="n">
+        <v>4029</v>
+      </c>
+      <c r="P7" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>4299</t>
         </is>
       </c>
     </row>
@@ -846,9 +892,15 @@
       <c r="N8" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>3628</t>
+      <c r="O8" t="n">
+        <v>3628</v>
+      </c>
+      <c r="P8" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>3910</t>
         </is>
       </c>
     </row>
@@ -874,7 +926,7 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F9" s="4" t="n">
+      <c r="F9" s="5" t="n">
         <v>33</v>
       </c>
       <c r="G9" t="n">
@@ -898,12 +950,18 @@
       <c r="M9" t="n">
         <v>3299</v>
       </c>
-      <c r="N9" s="4" t="n">
+      <c r="N9" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>3534</t>
+      <c r="O9" t="n">
+        <v>3534</v>
+      </c>
+      <c r="P9" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>3705</t>
         </is>
       </c>
     </row>
@@ -929,36 +987,42 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F10" s="4" t="n">
+      <c r="F10" s="5" t="n">
         <v>40</v>
       </c>
       <c r="G10" t="n">
         <v>5621</v>
       </c>
-      <c r="H10" s="4" t="n">
+      <c r="H10" s="5" t="n">
         <v>40</v>
       </c>
       <c r="I10" t="n">
         <v>2912</v>
       </c>
-      <c r="J10" s="4" t="n">
+      <c r="J10" s="5" t="n">
         <v>40</v>
       </c>
       <c r="K10" t="n">
         <v>3131</v>
       </c>
-      <c r="L10" s="4" t="n">
+      <c r="L10" s="5" t="n">
         <v>40</v>
       </c>
       <c r="M10" t="n">
         <v>3469</v>
       </c>
-      <c r="N10" s="4" t="n">
+      <c r="N10" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>3588</t>
+      <c r="O10" t="n">
+        <v>3588</v>
+      </c>
+      <c r="P10" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>3799</t>
         </is>
       </c>
     </row>
@@ -984,7 +1048,7 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F11" s="4" t="n">
+      <c r="F11" s="5" t="n">
         <v>40</v>
       </c>
       <c r="G11" t="n">
@@ -1011,9 +1075,15 @@
       <c r="N11" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>3674</t>
+      <c r="O11" t="n">
+        <v>3674</v>
+      </c>
+      <c r="P11" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>3940</t>
         </is>
       </c>
     </row>
@@ -1066,9 +1136,15 @@
       <c r="N12" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>3521</t>
+      <c r="O12" t="n">
+        <v>3521</v>
+      </c>
+      <c r="P12" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>3744</t>
         </is>
       </c>
     </row>
@@ -1100,7 +1176,7 @@
       <c r="G13" t="n">
         <v>0</v>
       </c>
-      <c r="H13" s="5" t="n">
+      <c r="H13" s="4" t="n">
         <v>5</v>
       </c>
       <c r="I13" t="n">
@@ -1121,9 +1197,15 @@
       <c r="N13" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>2603</t>
+      <c r="O13" t="n">
+        <v>2603</v>
+      </c>
+      <c r="P13" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>2657</t>
         </is>
       </c>
     </row>
@@ -1149,36 +1231,42 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F14" s="4" t="n">
+      <c r="F14" s="5" t="n">
         <v>31</v>
       </c>
       <c r="G14" t="n">
         <v>7227</v>
       </c>
-      <c r="H14" s="4" t="n">
+      <c r="H14" s="5" t="n">
         <v>36</v>
       </c>
       <c r="I14" t="n">
         <v>3106</v>
       </c>
-      <c r="J14" s="4" t="n">
+      <c r="J14" s="5" t="n">
         <v>37</v>
       </c>
       <c r="K14" t="n">
         <v>3541</v>
       </c>
-      <c r="L14" s="4" t="n">
+      <c r="L14" s="5" t="n">
         <v>37</v>
       </c>
       <c r="M14" t="n">
         <v>3896</v>
       </c>
-      <c r="N14" s="4" t="n">
+      <c r="N14" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>4267</t>
+      <c r="O14" t="n">
+        <v>4267</v>
+      </c>
+      <c r="P14" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>4700</t>
         </is>
       </c>
     </row>
@@ -1231,9 +1319,15 @@
       <c r="N15" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>3678</t>
+      <c r="O15" t="n">
+        <v>3678</v>
+      </c>
+      <c r="P15" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>3941</t>
         </is>
       </c>
     </row>
@@ -1259,7 +1353,7 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F16" s="4" t="n">
+      <c r="F16" s="5" t="n">
         <v>33</v>
       </c>
       <c r="G16" t="n">
@@ -1271,7 +1365,7 @@
       <c r="I16" t="n">
         <v>3018</v>
       </c>
-      <c r="J16" s="4" t="n">
+      <c r="J16" s="5" t="n">
         <v>31</v>
       </c>
       <c r="K16" t="n">
@@ -1286,9 +1380,15 @@
       <c r="N16" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>4067</t>
+      <c r="O16" t="n">
+        <v>4067</v>
+      </c>
+      <c r="P16" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>4444</t>
         </is>
       </c>
     </row>
@@ -1320,13 +1420,13 @@
       <c r="G17" t="n">
         <v>4056</v>
       </c>
-      <c r="H17" s="4" t="n">
+      <c r="H17" s="5" t="n">
         <v>33</v>
       </c>
       <c r="I17" t="n">
         <v>2877</v>
       </c>
-      <c r="J17" s="5" t="n">
+      <c r="J17" s="4" t="n">
         <v>9</v>
       </c>
       <c r="K17" t="n">
@@ -1338,12 +1438,18 @@
       <c r="M17" t="n">
         <v>3044</v>
       </c>
-      <c r="N17" s="5" t="n">
+      <c r="N17" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="O17" t="inlineStr">
-        <is>
-          <t>3233</t>
+      <c r="O17" t="n">
+        <v>3233</v>
+      </c>
+      <c r="P17" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>3598</t>
         </is>
       </c>
     </row>
@@ -1375,7 +1481,7 @@
       <c r="G18" t="n">
         <v>5543</v>
       </c>
-      <c r="H18" s="5" t="n">
+      <c r="H18" s="4" t="n">
         <v>13</v>
       </c>
       <c r="I18" t="n">
@@ -1396,9 +1502,15 @@
       <c r="N18" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>3527</t>
+      <c r="O18" t="n">
+        <v>3527</v>
+      </c>
+      <c r="P18" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>3755</t>
         </is>
       </c>
     </row>
@@ -1424,7 +1536,7 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F19" s="5" t="n">
+      <c r="F19" s="4" t="n">
         <v>18</v>
       </c>
       <c r="G19" t="n">
@@ -1451,9 +1563,15 @@
       <c r="N19" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="O19" t="inlineStr">
-        <is>
-          <t>3664</t>
+      <c r="O19" t="n">
+        <v>3664</v>
+      </c>
+      <c r="P19" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>3971</t>
         </is>
       </c>
     </row>
@@ -1479,7 +1597,7 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F20" s="4" t="n">
+      <c r="F20" s="5" t="n">
         <v>40</v>
       </c>
       <c r="G20" t="n">
@@ -1491,7 +1609,7 @@
       <c r="I20" t="n">
         <v>3034</v>
       </c>
-      <c r="J20" s="4" t="n">
+      <c r="J20" s="5" t="n">
         <v>33</v>
       </c>
       <c r="K20" t="n">
@@ -1503,12 +1621,18 @@
       <c r="M20" t="n">
         <v>3890</v>
       </c>
-      <c r="N20" s="4" t="n">
+      <c r="N20" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="O20" t="inlineStr">
-        <is>
-          <t>4259</t>
+      <c r="O20" t="n">
+        <v>4259</v>
+      </c>
+      <c r="P20" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>4579</t>
         </is>
       </c>
     </row>
@@ -1546,7 +1670,7 @@
       <c r="I21" t="n">
         <v>2758</v>
       </c>
-      <c r="J21" s="5" t="n">
+      <c r="J21" s="4" t="n">
         <v>1</v>
       </c>
       <c r="K21" t="n">
@@ -1561,9 +1685,15 @@
       <c r="N21" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O21" t="inlineStr">
-        <is>
-          <t>2780</t>
+      <c r="O21" t="n">
+        <v>2780</v>
+      </c>
+      <c r="P21" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>3100</t>
         </is>
       </c>
     </row>
@@ -1589,36 +1719,42 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F22" s="4" t="n">
+      <c r="F22" s="5" t="n">
         <v>36</v>
       </c>
       <c r="G22" t="n">
         <v>6114</v>
       </c>
-      <c r="H22" s="4" t="n">
+      <c r="H22" s="5" t="n">
         <v>34</v>
       </c>
       <c r="I22" t="n">
         <v>2739</v>
       </c>
-      <c r="J22" s="4" t="n">
+      <c r="J22" s="5" t="n">
         <v>40</v>
       </c>
       <c r="K22" t="n">
         <v>3184</v>
       </c>
-      <c r="L22" s="4" t="n">
+      <c r="L22" s="5" t="n">
         <v>39</v>
       </c>
       <c r="M22" t="n">
         <v>3465</v>
       </c>
-      <c r="N22" s="4" t="n">
+      <c r="N22" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="O22" t="inlineStr">
-        <is>
-          <t>3703</t>
+      <c r="O22" t="n">
+        <v>3703</v>
+      </c>
+      <c r="P22" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>4032</t>
         </is>
       </c>
     </row>
@@ -1650,30 +1786,36 @@
       <c r="G23" t="n">
         <v>5670</v>
       </c>
-      <c r="H23" s="4" t="n">
+      <c r="H23" s="5" t="n">
         <v>33</v>
       </c>
       <c r="I23" t="n">
         <v>2677</v>
       </c>
-      <c r="J23" s="4" t="n">
+      <c r="J23" s="5" t="n">
         <v>33</v>
       </c>
       <c r="K23" t="n">
         <v>2664</v>
       </c>
-      <c r="L23" s="5" t="n">
+      <c r="L23" s="4" t="n">
         <v>5</v>
       </c>
       <c r="M23" t="n">
         <v>2588</v>
       </c>
-      <c r="N23" s="4" t="n">
+      <c r="N23" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>2884</t>
+      <c r="O23" t="n">
+        <v>2884</v>
+      </c>
+      <c r="P23" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>2998</t>
         </is>
       </c>
     </row>
@@ -1699,36 +1841,42 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F24" s="4" t="n">
+      <c r="F24" s="5" t="n">
         <v>33</v>
       </c>
       <c r="G24" t="n">
         <v>6588</v>
       </c>
-      <c r="H24" s="4" t="n">
+      <c r="H24" s="5" t="n">
         <v>33</v>
       </c>
       <c r="I24" t="n">
         <v>2998</v>
       </c>
-      <c r="J24" s="4" t="n">
+      <c r="J24" s="5" t="n">
         <v>33</v>
       </c>
       <c r="K24" t="n">
         <v>3292</v>
       </c>
-      <c r="L24" s="4" t="n">
+      <c r="L24" s="5" t="n">
         <v>33</v>
       </c>
       <c r="M24" t="n">
         <v>3625</v>
       </c>
-      <c r="N24" s="4" t="n">
+      <c r="N24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="O24" t="inlineStr">
-        <is>
-          <t>3839</t>
+      <c r="O24" t="n">
+        <v>3839</v>
+      </c>
+      <c r="P24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>4157</t>
         </is>
       </c>
     </row>
@@ -1781,7 +1929,13 @@
       <c r="N25" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O25" t="inlineStr">
+      <c r="O25" t="n">
+        <v>0</v>
+      </c>
+      <c r="P25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1809,36 +1963,42 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F26" s="4" t="n">
+      <c r="F26" s="5" t="n">
         <v>40</v>
       </c>
       <c r="G26" t="n">
         <v>5947</v>
       </c>
-      <c r="H26" s="4" t="n">
+      <c r="H26" s="5" t="n">
         <v>40</v>
       </c>
       <c r="I26" t="n">
         <v>3092</v>
       </c>
-      <c r="J26" s="4" t="n">
+      <c r="J26" s="5" t="n">
         <v>40</v>
       </c>
       <c r="K26" t="n">
         <v>3472</v>
       </c>
-      <c r="L26" s="4" t="n">
+      <c r="L26" s="5" t="n">
         <v>40</v>
       </c>
       <c r="M26" t="n">
         <v>3771</v>
       </c>
-      <c r="N26" s="4" t="n">
+      <c r="N26" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="O26" t="inlineStr">
-        <is>
-          <t>4114</t>
+      <c r="O26" t="n">
+        <v>4114</v>
+      </c>
+      <c r="P26" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>4396</t>
         </is>
       </c>
     </row>
@@ -1864,7 +2024,7 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F27" s="4" t="n">
+      <c r="F27" s="5" t="n">
         <v>39</v>
       </c>
       <c r="G27" t="n">
@@ -1876,24 +2036,30 @@
       <c r="I27" t="n">
         <v>2800</v>
       </c>
-      <c r="J27" s="4" t="n">
+      <c r="J27" s="5" t="n">
         <v>33</v>
       </c>
       <c r="K27" t="n">
         <v>3143</v>
       </c>
-      <c r="L27" s="4" t="n">
+      <c r="L27" s="5" t="n">
         <v>34</v>
       </c>
       <c r="M27" t="n">
         <v>3685</v>
       </c>
-      <c r="N27" s="4" t="n">
+      <c r="N27" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="O27" t="inlineStr">
-        <is>
-          <t>4095</t>
+      <c r="O27" t="n">
+        <v>4095</v>
+      </c>
+      <c r="P27" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>4352</t>
         </is>
       </c>
     </row>
@@ -1946,9 +2112,15 @@
       <c r="N28" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="O28" t="inlineStr">
-        <is>
-          <t>3355</t>
+      <c r="O28" t="n">
+        <v>3355</v>
+      </c>
+      <c r="P28" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>3411</t>
         </is>
       </c>
     </row>
@@ -1974,36 +2146,42 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F29" s="4" t="n">
+      <c r="F29" s="5" t="n">
         <v>40</v>
       </c>
       <c r="G29" t="n">
         <v>7374</v>
       </c>
-      <c r="H29" s="4" t="n">
+      <c r="H29" s="5" t="n">
         <v>40</v>
       </c>
       <c r="I29" t="n">
         <v>3148</v>
       </c>
-      <c r="J29" s="4" t="n">
+      <c r="J29" s="5" t="n">
         <v>40</v>
       </c>
       <c r="K29" t="n">
         <v>3547</v>
       </c>
-      <c r="L29" s="4" t="n">
+      <c r="L29" s="5" t="n">
         <v>31</v>
       </c>
       <c r="M29" t="n">
         <v>3864</v>
       </c>
-      <c r="N29" s="4" t="n">
+      <c r="N29" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="O29" t="inlineStr">
-        <is>
-          <t>4161</t>
+      <c r="O29" t="n">
+        <v>4161</v>
+      </c>
+      <c r="P29" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>4458</t>
         </is>
       </c>
     </row>
@@ -2047,18 +2225,24 @@
       <c r="K30" t="n">
         <v>3253</v>
       </c>
-      <c r="L30" s="4" t="n">
+      <c r="L30" s="5" t="n">
         <v>33</v>
       </c>
       <c r="M30" t="n">
         <v>3550</v>
       </c>
-      <c r="N30" s="4" t="n">
+      <c r="N30" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="O30" t="inlineStr">
-        <is>
-          <t>3911</t>
+      <c r="O30" t="n">
+        <v>3911</v>
+      </c>
+      <c r="P30" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>4224</t>
         </is>
       </c>
     </row>
@@ -2084,36 +2268,42 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F31" s="4" t="n">
+      <c r="F31" s="5" t="n">
         <v>39</v>
       </c>
       <c r="G31" t="n">
         <v>6466</v>
       </c>
-      <c r="H31" s="4" t="n">
+      <c r="H31" s="5" t="n">
         <v>33</v>
       </c>
       <c r="I31" t="n">
         <v>2954</v>
       </c>
-      <c r="J31" s="4" t="n">
+      <c r="J31" s="5" t="n">
         <v>33</v>
       </c>
       <c r="K31" t="n">
         <v>3302</v>
       </c>
-      <c r="L31" s="4" t="n">
+      <c r="L31" s="5" t="n">
         <v>33</v>
       </c>
       <c r="M31" t="n">
         <v>3448</v>
       </c>
-      <c r="N31" s="4" t="n">
+      <c r="N31" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="O31" t="inlineStr">
-        <is>
-          <t>3674</t>
+      <c r="O31" t="n">
+        <v>3674</v>
+      </c>
+      <c r="P31" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>3806</t>
         </is>
       </c>
     </row>
@@ -2139,25 +2329,25 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F32" s="5" t="n">
+      <c r="F32" s="4" t="n">
         <v>14</v>
       </c>
       <c r="G32" t="n">
         <v>6679</v>
       </c>
-      <c r="H32" s="4" t="n">
+      <c r="H32" s="5" t="n">
         <v>33</v>
       </c>
       <c r="I32" t="n">
         <v>2983</v>
       </c>
-      <c r="J32" s="4" t="n">
+      <c r="J32" s="5" t="n">
         <v>35</v>
       </c>
       <c r="K32" t="n">
         <v>3456</v>
       </c>
-      <c r="L32" s="4" t="n">
+      <c r="L32" s="5" t="n">
         <v>35</v>
       </c>
       <c r="M32" t="n">
@@ -2166,9 +2356,15 @@
       <c r="N32" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="O32" t="inlineStr">
-        <is>
-          <t>4070</t>
+      <c r="O32" t="n">
+        <v>4070</v>
+      </c>
+      <c r="P32" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>4479</t>
         </is>
       </c>
     </row>
@@ -2200,30 +2396,36 @@
       <c r="G33" t="n">
         <v>6658</v>
       </c>
-      <c r="H33" s="4" t="n">
+      <c r="H33" s="5" t="n">
         <v>33</v>
       </c>
       <c r="I33" t="n">
         <v>2796</v>
       </c>
-      <c r="J33" s="4" t="n">
+      <c r="J33" s="5" t="n">
         <v>31</v>
       </c>
       <c r="K33" t="n">
         <v>3148</v>
       </c>
-      <c r="L33" s="4" t="n">
+      <c r="L33" s="5" t="n">
         <v>39</v>
       </c>
       <c r="M33" t="n">
         <v>3564</v>
       </c>
-      <c r="N33" s="4" t="n">
+      <c r="N33" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="O33" t="inlineStr">
-        <is>
-          <t>3769</t>
+      <c r="O33" t="n">
+        <v>3769</v>
+      </c>
+      <c r="P33" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>4340</t>
         </is>
       </c>
     </row>
@@ -2267,18 +2469,24 @@
       <c r="K34" t="n">
         <v>2500</v>
       </c>
-      <c r="L34" s="4" t="n">
+      <c r="L34" s="5" t="n">
         <v>40</v>
       </c>
       <c r="M34" t="n">
         <v>3066</v>
       </c>
-      <c r="N34" s="4" t="n">
+      <c r="N34" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="O34" t="inlineStr">
-        <is>
-          <t>3638</t>
+      <c r="O34" t="n">
+        <v>3638</v>
+      </c>
+      <c r="P34" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>4041</t>
         </is>
       </c>
     </row>
@@ -2304,7 +2512,7 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F35" s="4" t="n">
+      <c r="F35" s="5" t="n">
         <v>32</v>
       </c>
       <c r="G35" t="n">
@@ -2316,24 +2524,30 @@
       <c r="I35" t="n">
         <v>2996</v>
       </c>
-      <c r="J35" s="4" t="n">
+      <c r="J35" s="5" t="n">
         <v>32</v>
       </c>
       <c r="K35" t="n">
         <v>3416</v>
       </c>
-      <c r="L35" s="4" t="n">
+      <c r="L35" s="5" t="n">
         <v>34</v>
       </c>
       <c r="M35" t="n">
         <v>3780</v>
       </c>
-      <c r="N35" s="4" t="n">
+      <c r="N35" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="O35" t="inlineStr">
-        <is>
-          <t>4043</t>
+      <c r="O35" t="n">
+        <v>4043</v>
+      </c>
+      <c r="P35" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>4344</t>
         </is>
       </c>
     </row>
@@ -2371,13 +2585,13 @@
       <c r="I36" t="n">
         <v>2899</v>
       </c>
-      <c r="J36" s="4" t="n">
+      <c r="J36" s="5" t="n">
         <v>33</v>
       </c>
       <c r="K36" t="n">
         <v>3206</v>
       </c>
-      <c r="L36" s="4" t="n">
+      <c r="L36" s="5" t="n">
         <v>36</v>
       </c>
       <c r="M36" t="n">
@@ -2386,9 +2600,15 @@
       <c r="N36" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="O36" t="inlineStr">
-        <is>
-          <t>3838</t>
+      <c r="O36" t="n">
+        <v>3838</v>
+      </c>
+      <c r="P36" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>4117</t>
         </is>
       </c>
     </row>
@@ -2414,36 +2634,42 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F37" s="5" t="n">
+      <c r="F37" s="4" t="n">
         <v>7</v>
       </c>
       <c r="G37" t="n">
         <v>5301</v>
       </c>
-      <c r="H37" s="4" t="n">
+      <c r="H37" s="5" t="n">
         <v>33</v>
       </c>
       <c r="I37" t="n">
         <v>2888</v>
       </c>
-      <c r="J37" s="4" t="n">
+      <c r="J37" s="5" t="n">
         <v>33</v>
       </c>
       <c r="K37" t="n">
         <v>3209</v>
       </c>
-      <c r="L37" s="4" t="n">
+      <c r="L37" s="5" t="n">
         <v>33</v>
       </c>
       <c r="M37" t="n">
         <v>3437</v>
       </c>
-      <c r="N37" s="4" t="n">
+      <c r="N37" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="O37" t="inlineStr">
-        <is>
-          <t>3651</t>
+      <c r="O37" t="n">
+        <v>3651</v>
+      </c>
+      <c r="P37" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>3837</t>
         </is>
       </c>
     </row>
@@ -2469,13 +2695,13 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F38" s="4" t="n">
+      <c r="F38" s="5" t="n">
         <v>32</v>
       </c>
       <c r="G38" t="n">
         <v>6215</v>
       </c>
-      <c r="H38" s="4" t="n">
+      <c r="H38" s="5" t="n">
         <v>34</v>
       </c>
       <c r="I38" t="n">
@@ -2487,18 +2713,24 @@
       <c r="K38" t="n">
         <v>3333</v>
       </c>
-      <c r="L38" s="4" t="n">
+      <c r="L38" s="5" t="n">
         <v>33</v>
       </c>
       <c r="M38" t="n">
         <v>3663</v>
       </c>
-      <c r="N38" s="4" t="n">
+      <c r="N38" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="O38" t="inlineStr">
-        <is>
-          <t>3888</t>
+      <c r="O38" t="n">
+        <v>3888</v>
+      </c>
+      <c r="P38" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>4178</t>
         </is>
       </c>
     </row>
@@ -2530,30 +2762,36 @@
       <c r="G39" t="n">
         <v>5910</v>
       </c>
-      <c r="H39" s="4" t="n">
+      <c r="H39" s="5" t="n">
         <v>35</v>
       </c>
       <c r="I39" t="n">
         <v>2871</v>
       </c>
-      <c r="J39" s="4" t="n">
+      <c r="J39" s="5" t="n">
         <v>35</v>
       </c>
       <c r="K39" t="n">
         <v>3123</v>
       </c>
-      <c r="L39" s="4" t="n">
+      <c r="L39" s="5" t="n">
         <v>35</v>
       </c>
       <c r="M39" t="n">
         <v>3503</v>
       </c>
-      <c r="N39" s="4" t="n">
+      <c r="N39" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="O39" t="inlineStr">
-        <is>
-          <t>3706</t>
+      <c r="O39" t="n">
+        <v>3706</v>
+      </c>
+      <c r="P39" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>3949</t>
         </is>
       </c>
     </row>
@@ -2579,7 +2817,7 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F40" s="4" t="n">
+      <c r="F40" s="5" t="n">
         <v>37</v>
       </c>
       <c r="G40" t="n">
@@ -2597,18 +2835,24 @@
       <c r="K40" t="n">
         <v>3349</v>
       </c>
-      <c r="L40" s="4" t="n">
+      <c r="L40" s="5" t="n">
         <v>33</v>
       </c>
       <c r="M40" t="n">
         <v>3703</v>
       </c>
-      <c r="N40" s="4" t="n">
+      <c r="N40" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="O40" t="inlineStr">
-        <is>
-          <t>4234</t>
+      <c r="O40" t="n">
+        <v>4234</v>
+      </c>
+      <c r="P40" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>4525</t>
         </is>
       </c>
     </row>
@@ -2661,9 +2905,15 @@
       <c r="N41" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O41" t="inlineStr">
-        <is>
-          <t>3744</t>
+      <c r="O41" t="n">
+        <v>3744</v>
+      </c>
+      <c r="P41" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>4076</t>
         </is>
       </c>
     </row>
@@ -2689,36 +2939,42 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F42" s="4" t="n">
+      <c r="F42" s="5" t="n">
         <v>35</v>
       </c>
       <c r="G42" t="n">
         <v>7170</v>
       </c>
-      <c r="H42" s="4" t="n">
+      <c r="H42" s="5" t="n">
         <v>34</v>
       </c>
       <c r="I42" t="n">
         <v>2940</v>
       </c>
-      <c r="J42" s="4" t="n">
+      <c r="J42" s="5" t="n">
         <v>34</v>
       </c>
       <c r="K42" t="n">
         <v>3389</v>
       </c>
-      <c r="L42" s="4" t="n">
+      <c r="L42" s="5" t="n">
         <v>33</v>
       </c>
       <c r="M42" t="n">
         <v>3718</v>
       </c>
-      <c r="N42" s="4" t="n">
+      <c r="N42" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="O42" t="inlineStr">
-        <is>
-          <t>4090</t>
+      <c r="O42" t="n">
+        <v>4090</v>
+      </c>
+      <c r="P42" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>4498</t>
         </is>
       </c>
     </row>
@@ -2744,36 +3000,42 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F43" s="4" t="n">
+      <c r="F43" s="5" t="n">
         <v>38</v>
       </c>
       <c r="G43" t="n">
         <v>6366</v>
       </c>
-      <c r="H43" s="4" t="n">
+      <c r="H43" s="5" t="n">
         <v>33</v>
       </c>
       <c r="I43" t="n">
         <v>2992</v>
       </c>
-      <c r="J43" s="4" t="n">
+      <c r="J43" s="5" t="n">
         <v>33</v>
       </c>
       <c r="K43" t="n">
         <v>3334</v>
       </c>
-      <c r="L43" s="4" t="n">
+      <c r="L43" s="5" t="n">
         <v>33</v>
       </c>
       <c r="M43" t="n">
         <v>3623</v>
       </c>
-      <c r="N43" s="4" t="n">
+      <c r="N43" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="O43" t="inlineStr">
-        <is>
-          <t>3822</t>
+      <c r="O43" t="n">
+        <v>3822</v>
+      </c>
+      <c r="P43" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>4083</t>
         </is>
       </c>
     </row>
@@ -2799,36 +3061,42 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F44" s="4" t="n">
+      <c r="F44" s="5" t="n">
         <v>40</v>
       </c>
       <c r="G44" t="n">
         <v>6177</v>
       </c>
-      <c r="H44" s="4" t="n">
+      <c r="H44" s="5" t="n">
         <v>40</v>
       </c>
       <c r="I44" t="n">
         <v>2997</v>
       </c>
-      <c r="J44" s="4" t="n">
+      <c r="J44" s="5" t="n">
         <v>40</v>
       </c>
       <c r="K44" t="n">
         <v>3422</v>
       </c>
-      <c r="L44" s="4" t="n">
+      <c r="L44" s="5" t="n">
         <v>40</v>
       </c>
       <c r="M44" t="n">
         <v>3576</v>
       </c>
-      <c r="N44" s="4" t="n">
+      <c r="N44" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="O44" t="inlineStr">
-        <is>
-          <t>3738</t>
+      <c r="O44" t="n">
+        <v>3738</v>
+      </c>
+      <c r="P44" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>4148</t>
         </is>
       </c>
     </row>
@@ -2854,36 +3122,42 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F45" s="5" t="n">
+      <c r="F45" s="4" t="n">
         <v>1</v>
       </c>
       <c r="G45" t="n">
         <v>5664</v>
       </c>
-      <c r="H45" s="4" t="n">
+      <c r="H45" s="5" t="n">
         <v>33</v>
       </c>
       <c r="I45" t="n">
         <v>2899</v>
       </c>
-      <c r="J45" s="4" t="n">
+      <c r="J45" s="5" t="n">
         <v>33</v>
       </c>
       <c r="K45" t="n">
         <v>3148</v>
       </c>
-      <c r="L45" s="4" t="n">
+      <c r="L45" s="5" t="n">
         <v>33</v>
       </c>
       <c r="M45" t="n">
         <v>3363</v>
       </c>
-      <c r="N45" s="4" t="n">
+      <c r="N45" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="O45" t="inlineStr">
-        <is>
-          <t>3508</t>
+      <c r="O45" t="n">
+        <v>3508</v>
+      </c>
+      <c r="P45" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>3766</t>
         </is>
       </c>
     </row>
@@ -2909,7 +3183,7 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F46" s="4" t="n">
+      <c r="F46" s="5" t="n">
         <v>33</v>
       </c>
       <c r="G46" t="n">
@@ -2936,9 +3210,15 @@
       <c r="N46" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="O46" t="inlineStr">
-        <is>
-          <t>3495</t>
+      <c r="O46" t="n">
+        <v>3495</v>
+      </c>
+      <c r="P46" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q46" t="inlineStr">
+        <is>
+          <t>3724</t>
         </is>
       </c>
     </row>
@@ -2970,7 +3250,7 @@
       <c r="G47" t="n">
         <v>0</v>
       </c>
-      <c r="H47" s="5" t="n">
+      <c r="H47" s="4" t="n">
         <v>5</v>
       </c>
       <c r="I47" t="n">
@@ -2991,9 +3271,15 @@
       <c r="N47" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O47" t="inlineStr">
-        <is>
-          <t>3010</t>
+      <c r="O47" t="n">
+        <v>3010</v>
+      </c>
+      <c r="P47" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q47" t="inlineStr">
+        <is>
+          <t>3037</t>
         </is>
       </c>
     </row>
@@ -3019,36 +3305,42 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F48" s="4" t="n">
+      <c r="F48" s="5" t="n">
         <v>40</v>
       </c>
       <c r="G48" t="n">
         <v>6514</v>
       </c>
-      <c r="H48" s="4" t="n">
+      <c r="H48" s="5" t="n">
         <v>35</v>
       </c>
       <c r="I48" t="n">
         <v>2877</v>
       </c>
-      <c r="J48" s="4" t="n">
+      <c r="J48" s="5" t="n">
         <v>36</v>
       </c>
       <c r="K48" t="n">
         <v>3206</v>
       </c>
-      <c r="L48" s="4" t="n">
+      <c r="L48" s="5" t="n">
         <v>35</v>
       </c>
       <c r="M48" t="n">
         <v>3486</v>
       </c>
-      <c r="N48" s="4" t="n">
+      <c r="N48" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="O48" t="inlineStr">
-        <is>
-          <t>3746</t>
+      <c r="O48" t="n">
+        <v>3746</v>
+      </c>
+      <c r="P48" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>4069</t>
         </is>
       </c>
     </row>
@@ -3074,7 +3366,7 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F49" s="5" t="n">
+      <c r="F49" s="4" t="n">
         <v>13</v>
       </c>
       <c r="G49" t="n">
@@ -3092,18 +3384,24 @@
       <c r="K49" t="n">
         <v>3001</v>
       </c>
-      <c r="L49" s="4" t="n">
+      <c r="L49" s="5" t="n">
         <v>34</v>
       </c>
       <c r="M49" t="n">
         <v>3248</v>
       </c>
-      <c r="N49" s="4" t="n">
+      <c r="N49" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="O49" t="inlineStr">
-        <is>
-          <t>3391</t>
+      <c r="O49" t="n">
+        <v>3391</v>
+      </c>
+      <c r="P49" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q49" t="inlineStr">
+        <is>
+          <t>3469</t>
         </is>
       </c>
     </row>
@@ -3129,36 +3427,42 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F50" s="4" t="n">
+      <c r="F50" s="5" t="n">
         <v>40</v>
       </c>
       <c r="G50" t="n">
         <v>7116</v>
       </c>
-      <c r="H50" s="4" t="n">
+      <c r="H50" s="5" t="n">
         <v>31</v>
       </c>
       <c r="I50" t="n">
         <v>2880</v>
       </c>
-      <c r="J50" s="4" t="n">
+      <c r="J50" s="5" t="n">
         <v>33</v>
       </c>
       <c r="K50" t="n">
         <v>3245</v>
       </c>
-      <c r="L50" s="4" t="n">
+      <c r="L50" s="5" t="n">
         <v>40</v>
       </c>
       <c r="M50" t="n">
         <v>3719</v>
       </c>
-      <c r="N50" s="4" t="n">
+      <c r="N50" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="O50" t="inlineStr">
-        <is>
-          <t>3919</t>
+      <c r="O50" t="n">
+        <v>3919</v>
+      </c>
+      <c r="P50" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>4294</t>
         </is>
       </c>
     </row>
@@ -3211,9 +3515,15 @@
       <c r="N51" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O51" t="inlineStr">
-        <is>
-          <t>2706</t>
+      <c r="O51" t="n">
+        <v>2706</v>
+      </c>
+      <c r="P51" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q51" t="inlineStr">
+        <is>
+          <t>2716</t>
         </is>
       </c>
     </row>
@@ -3266,9 +3576,15 @@
       <c r="N52" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O52" t="inlineStr">
-        <is>
-          <t>2667</t>
+      <c r="O52" t="n">
+        <v>2667</v>
+      </c>
+      <c r="P52" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q52" t="inlineStr">
+        <is>
+          <t>2690</t>
         </is>
       </c>
     </row>
@@ -3306,13 +3622,13 @@
       <c r="I53" t="n">
         <v>0</v>
       </c>
-      <c r="J53" s="5" t="n">
+      <c r="J53" s="4" t="n">
         <v>1</v>
       </c>
       <c r="K53" t="n">
         <v>2512</v>
       </c>
-      <c r="L53" s="5" t="n">
+      <c r="L53" s="4" t="n">
         <v>9</v>
       </c>
       <c r="M53" t="n">
@@ -3321,9 +3637,15 @@
       <c r="N53" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O53" t="inlineStr">
-        <is>
-          <t>2672</t>
+      <c r="O53" t="n">
+        <v>2672</v>
+      </c>
+      <c r="P53" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q53" t="inlineStr">
+        <is>
+          <t>2762</t>
         </is>
       </c>
     </row>
@@ -3376,9 +3698,15 @@
       <c r="N54" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="O54" t="inlineStr">
-        <is>
-          <t>3876</t>
+      <c r="O54" t="n">
+        <v>3876</v>
+      </c>
+      <c r="P54" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="Q54" t="inlineStr">
+        <is>
+          <t>4108</t>
         </is>
       </c>
     </row>
@@ -3404,36 +3732,42 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F55" s="4" t="n">
+      <c r="F55" s="5" t="n">
         <v>40</v>
       </c>
       <c r="G55" t="n">
         <v>4614</v>
       </c>
-      <c r="H55" s="4" t="n">
+      <c r="H55" s="5" t="n">
         <v>40</v>
       </c>
       <c r="I55" t="n">
         <v>2819</v>
       </c>
-      <c r="J55" s="4" t="n">
+      <c r="J55" s="5" t="n">
         <v>40</v>
       </c>
       <c r="K55" t="n">
         <v>2915</v>
       </c>
-      <c r="L55" s="4" t="n">
+      <c r="L55" s="5" t="n">
         <v>40</v>
       </c>
       <c r="M55" t="n">
         <v>3031</v>
       </c>
-      <c r="N55" s="4" t="n">
+      <c r="N55" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="O55" t="inlineStr">
-        <is>
-          <t>3181</t>
+      <c r="O55" t="n">
+        <v>3181</v>
+      </c>
+      <c r="P55" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q55" t="inlineStr">
+        <is>
+          <t>3299</t>
         </is>
       </c>
     </row>
@@ -3486,9 +3820,15 @@
       <c r="N56" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O56" t="inlineStr">
-        <is>
-          <t>3310</t>
+      <c r="O56" t="n">
+        <v>3310</v>
+      </c>
+      <c r="P56" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q56" t="inlineStr">
+        <is>
+          <t>3521</t>
         </is>
       </c>
     </row>
@@ -3541,9 +3881,15 @@
       <c r="N57" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O57" t="inlineStr">
-        <is>
-          <t>3657</t>
+      <c r="O57" t="n">
+        <v>3657</v>
+      </c>
+      <c r="P57" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="Q57" t="inlineStr">
+        <is>
+          <t>3908</t>
         </is>
       </c>
     </row>
@@ -3569,36 +3915,42 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F58" s="4" t="n">
+      <c r="F58" s="5" t="n">
         <v>35</v>
       </c>
       <c r="G58" t="n">
         <v>4843</v>
       </c>
-      <c r="H58" s="4" t="n">
+      <c r="H58" s="5" t="n">
         <v>33</v>
       </c>
       <c r="I58" t="n">
         <v>2788</v>
       </c>
-      <c r="J58" s="4" t="n">
+      <c r="J58" s="5" t="n">
         <v>34</v>
       </c>
       <c r="K58" t="n">
         <v>2886</v>
       </c>
-      <c r="L58" s="4" t="n">
+      <c r="L58" s="5" t="n">
         <v>33</v>
       </c>
       <c r="M58" t="n">
         <v>3043</v>
       </c>
-      <c r="N58" s="4" t="n">
+      <c r="N58" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="O58" t="inlineStr">
-        <is>
-          <t>3236</t>
+      <c r="O58" t="n">
+        <v>3236</v>
+      </c>
+      <c r="P58" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q58" t="inlineStr">
+        <is>
+          <t>3447</t>
         </is>
       </c>
     </row>
@@ -3624,7 +3976,7 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F59" s="5" t="n">
+      <c r="F59" s="4" t="n">
         <v>8</v>
       </c>
       <c r="G59" t="n">
@@ -3651,9 +4003,15 @@
       <c r="N59" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O59" t="inlineStr">
-        <is>
-          <t>3325</t>
+      <c r="O59" t="n">
+        <v>3325</v>
+      </c>
+      <c r="P59" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q59" t="inlineStr">
+        <is>
+          <t>3725</t>
         </is>
       </c>
     </row>
@@ -3706,7 +4064,13 @@
       <c r="N60" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O60" t="inlineStr">
+      <c r="O60" t="n">
+        <v>0</v>
+      </c>
+      <c r="P60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q60" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3761,9 +4125,15 @@
       <c r="N61" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="O61" t="inlineStr">
-        <is>
-          <t>3823</t>
+      <c r="O61" t="n">
+        <v>3823</v>
+      </c>
+      <c r="P61" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q61" t="inlineStr">
+        <is>
+          <t>4003</t>
         </is>
       </c>
     </row>
@@ -3816,9 +4186,15 @@
       <c r="N62" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O62" t="inlineStr">
-        <is>
-          <t>2527</t>
+      <c r="O62" t="n">
+        <v>2527</v>
+      </c>
+      <c r="P62" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q62" t="inlineStr">
+        <is>
+          <t>2609</t>
         </is>
       </c>
     </row>
@@ -3871,9 +4247,15 @@
       <c r="N63" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O63" t="inlineStr">
-        <is>
-          <t>2707</t>
+      <c r="O63" t="n">
+        <v>2707</v>
+      </c>
+      <c r="P63" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q63" t="inlineStr">
+        <is>
+          <t>2917</t>
         </is>
       </c>
     </row>
@@ -3926,9 +4308,15 @@
       <c r="N64" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="O64" t="inlineStr">
-        <is>
-          <t>3658</t>
+      <c r="O64" t="n">
+        <v>3658</v>
+      </c>
+      <c r="P64" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="Q64" t="inlineStr">
+        <is>
+          <t>3826</t>
         </is>
       </c>
     </row>
@@ -3980,6 +4368,8 @@
       </c>
       <c r="N65" s="2" t="inlineStr"/>
       <c r="O65" t="inlineStr"/>
+      <c r="P65" s="2" t="inlineStr"/>
+      <c r="Q65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -4030,9 +4420,15 @@
       <c r="N66" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="O66" t="inlineStr">
-        <is>
-          <t>3747</t>
+      <c r="O66" t="n">
+        <v>3747</v>
+      </c>
+      <c r="P66" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q66" t="inlineStr">
+        <is>
+          <t>3950</t>
         </is>
       </c>
     </row>
@@ -4064,30 +4460,36 @@
       <c r="G67" t="n">
         <v>4744</v>
       </c>
-      <c r="H67" s="4" t="n">
+      <c r="H67" s="5" t="n">
         <v>36</v>
       </c>
       <c r="I67" t="n">
         <v>2786</v>
       </c>
-      <c r="J67" s="4" t="n">
+      <c r="J67" s="5" t="n">
         <v>33</v>
       </c>
       <c r="K67" t="n">
         <v>2956</v>
       </c>
-      <c r="L67" s="4" t="n">
+      <c r="L67" s="5" t="n">
         <v>33</v>
       </c>
       <c r="M67" t="n">
         <v>3201</v>
       </c>
-      <c r="N67" s="4" t="n">
+      <c r="N67" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="O67" t="inlineStr">
-        <is>
-          <t>3342</t>
+      <c r="O67" t="n">
+        <v>3342</v>
+      </c>
+      <c r="P67" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q67" t="inlineStr">
+        <is>
+          <t>3480</t>
         </is>
       </c>
     </row>
@@ -4140,9 +4542,15 @@
       <c r="N68" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O68" t="inlineStr">
-        <is>
-          <t>2528</t>
+      <c r="O68" t="n">
+        <v>2528</v>
+      </c>
+      <c r="P68" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q68" t="inlineStr">
+        <is>
+          <t>2547</t>
         </is>
       </c>
     </row>
@@ -4195,9 +4603,15 @@
       <c r="N69" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="O69" t="inlineStr">
-        <is>
-          <t>3323</t>
+      <c r="O69" t="n">
+        <v>3323</v>
+      </c>
+      <c r="P69" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q69" t="inlineStr">
+        <is>
+          <t>3550</t>
         </is>
       </c>
     </row>
@@ -4223,13 +4637,13 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F70" s="5" t="n">
+      <c r="F70" s="4" t="n">
         <v>14</v>
       </c>
       <c r="G70" t="n">
         <v>4425</v>
       </c>
-      <c r="H70" s="5" t="n">
+      <c r="H70" s="4" t="n">
         <v>17</v>
       </c>
       <c r="I70" t="n">
@@ -4241,7 +4655,7 @@
       <c r="K70" t="n">
         <v>2838</v>
       </c>
-      <c r="L70" s="5" t="n">
+      <c r="L70" s="4" t="n">
         <v>5</v>
       </c>
       <c r="M70" t="n">
@@ -4250,9 +4664,15 @@
       <c r="N70" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="O70" t="inlineStr">
-        <is>
-          <t>3098</t>
+      <c r="O70" t="n">
+        <v>3098</v>
+      </c>
+      <c r="P70" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q70" t="inlineStr">
+        <is>
+          <t>3169</t>
         </is>
       </c>
     </row>
@@ -4290,7 +4710,7 @@
       <c r="I71" t="n">
         <v>2680</v>
       </c>
-      <c r="J71" s="5" t="n">
+      <c r="J71" s="4" t="n">
         <v>19</v>
       </c>
       <c r="K71" t="n">
@@ -4305,9 +4725,15 @@
       <c r="N71" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O71" t="inlineStr">
-        <is>
-          <t>3279</t>
+      <c r="O71" t="n">
+        <v>3279</v>
+      </c>
+      <c r="P71" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q71" t="inlineStr">
+        <is>
+          <t>3387</t>
         </is>
       </c>
     </row>
@@ -4360,9 +4786,15 @@
       <c r="N72" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O72" t="inlineStr">
-        <is>
-          <t>2638</t>
+      <c r="O72" t="n">
+        <v>2638</v>
+      </c>
+      <c r="P72" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q72" t="inlineStr">
+        <is>
+          <t>2628</t>
         </is>
       </c>
     </row>
@@ -4415,9 +4847,15 @@
       <c r="N73" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="O73" t="inlineStr">
-        <is>
-          <t>3133</t>
+      <c r="O73" t="n">
+        <v>3133</v>
+      </c>
+      <c r="P73" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="Q73" t="inlineStr">
+        <is>
+          <t>3246</t>
         </is>
       </c>
     </row>
@@ -4443,7 +4881,7 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F74" s="5" t="n">
+      <c r="F74" s="4" t="n">
         <v>15</v>
       </c>
       <c r="G74" t="n">
@@ -4470,9 +4908,15 @@
       <c r="N74" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="O74" t="inlineStr">
-        <is>
-          <t>3515</t>
+      <c r="O74" t="n">
+        <v>3515</v>
+      </c>
+      <c r="P74" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q74" t="inlineStr">
+        <is>
+          <t>3695</t>
         </is>
       </c>
     </row>
@@ -4525,9 +4969,15 @@
       <c r="N75" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O75" t="inlineStr">
-        <is>
-          <t>3556</t>
+      <c r="O75" t="n">
+        <v>3556</v>
+      </c>
+      <c r="P75" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q75" t="inlineStr">
+        <is>
+          <t>3818</t>
         </is>
       </c>
     </row>
@@ -4579,6 +5029,8 @@
       </c>
       <c r="N76" s="2" t="inlineStr"/>
       <c r="O76" t="inlineStr"/>
+      <c r="P76" s="2" t="inlineStr"/>
+      <c r="Q76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -4629,9 +5081,15 @@
       <c r="N77" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="O77" t="inlineStr">
-        <is>
-          <t>3645</t>
+      <c r="O77" t="n">
+        <v>3645</v>
+      </c>
+      <c r="P77" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q77" t="inlineStr">
+        <is>
+          <t>3889</t>
         </is>
       </c>
     </row>
@@ -4684,7 +5142,13 @@
       <c r="N78" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O78" t="inlineStr">
+      <c r="O78" t="n">
+        <v>2500</v>
+      </c>
+      <c r="P78" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q78" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -4739,9 +5203,15 @@
       <c r="N79" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="O79" t="inlineStr">
-        <is>
-          <t>3417</t>
+      <c r="O79" t="n">
+        <v>3417</v>
+      </c>
+      <c r="P79" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="Q79" t="inlineStr">
+        <is>
+          <t>3653</t>
         </is>
       </c>
     </row>
@@ -4767,7 +5237,7 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F80" s="4" t="n">
+      <c r="F80" s="5" t="n">
         <v>33</v>
       </c>
       <c r="G80" t="n">
@@ -4779,24 +5249,30 @@
       <c r="I80" t="n">
         <v>2886</v>
       </c>
-      <c r="J80" s="4" t="n">
+      <c r="J80" s="5" t="n">
         <v>32</v>
       </c>
       <c r="K80" t="n">
         <v>3067</v>
       </c>
-      <c r="L80" s="4" t="n">
+      <c r="L80" s="5" t="n">
         <v>31</v>
       </c>
       <c r="M80" t="n">
         <v>3356</v>
       </c>
-      <c r="N80" s="4" t="n">
+      <c r="N80" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="O80" t="inlineStr">
-        <is>
-          <t>3628</t>
+      <c r="O80" t="n">
+        <v>3628</v>
+      </c>
+      <c r="P80" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q80" t="inlineStr">
+        <is>
+          <t>3827</t>
         </is>
       </c>
     </row>
@@ -4822,36 +5298,42 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F81" s="4" t="n">
+      <c r="F81" s="5" t="n">
         <v>35</v>
       </c>
       <c r="G81" t="n">
         <v>5198</v>
       </c>
-      <c r="H81" s="4" t="n">
+      <c r="H81" s="5" t="n">
         <v>35</v>
       </c>
       <c r="I81" t="n">
         <v>2900</v>
       </c>
-      <c r="J81" s="4" t="n">
+      <c r="J81" s="5" t="n">
         <v>34</v>
       </c>
       <c r="K81" t="n">
         <v>3018</v>
       </c>
-      <c r="L81" s="4" t="n">
+      <c r="L81" s="5" t="n">
         <v>34</v>
       </c>
       <c r="M81" t="n">
         <v>3236</v>
       </c>
-      <c r="N81" s="4" t="n">
+      <c r="N81" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="O81" t="inlineStr">
-        <is>
-          <t>3518</t>
+      <c r="O81" t="n">
+        <v>3518</v>
+      </c>
+      <c r="P81" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="Q81" t="inlineStr">
+        <is>
+          <t>3676</t>
         </is>
       </c>
     </row>
@@ -4904,9 +5386,15 @@
       <c r="N82" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="O82" t="inlineStr">
-        <is>
-          <t>3351</t>
+      <c r="O82" t="n">
+        <v>3351</v>
+      </c>
+      <c r="P82" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q82" t="inlineStr">
+        <is>
+          <t>3486</t>
         </is>
       </c>
     </row>
@@ -4946,6 +5434,8 @@
       <c r="M83" t="inlineStr"/>
       <c r="N83" s="2" t="inlineStr"/>
       <c r="O83" t="inlineStr"/>
+      <c r="P83" s="2" t="inlineStr"/>
+      <c r="Q83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -4996,9 +5486,15 @@
       <c r="N84" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O84" t="inlineStr">
-        <is>
-          <t>2757</t>
+      <c r="O84" t="n">
+        <v>2757</v>
+      </c>
+      <c r="P84" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q84" t="inlineStr">
+        <is>
+          <t>2845</t>
         </is>
       </c>
     </row>
@@ -5024,7 +5520,7 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F85" s="5" t="n">
+      <c r="F85" s="4" t="n">
         <v>2</v>
       </c>
       <c r="G85" t="n">
@@ -5048,12 +5544,18 @@
       <c r="M85" t="n">
         <v>2499</v>
       </c>
-      <c r="N85" s="5" t="n">
+      <c r="N85" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="O85" t="inlineStr">
-        <is>
-          <t>2764</t>
+      <c r="O85" t="n">
+        <v>2764</v>
+      </c>
+      <c r="P85" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q85" t="inlineStr">
+        <is>
+          <t>2751</t>
         </is>
       </c>
     </row>
@@ -5085,30 +5587,36 @@
       <c r="G86" t="n">
         <v>5085</v>
       </c>
-      <c r="H86" s="4" t="n">
+      <c r="H86" s="5" t="n">
         <v>33</v>
       </c>
       <c r="I86" t="n">
         <v>2970</v>
       </c>
-      <c r="J86" s="4" t="n">
+      <c r="J86" s="5" t="n">
         <v>33</v>
       </c>
       <c r="K86" t="n">
         <v>3141</v>
       </c>
-      <c r="L86" s="4" t="n">
+      <c r="L86" s="5" t="n">
         <v>33</v>
       </c>
       <c r="M86" t="n">
         <v>3368</v>
       </c>
-      <c r="N86" s="4" t="n">
+      <c r="N86" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="O86" t="inlineStr">
-        <is>
-          <t>3686</t>
+      <c r="O86" t="n">
+        <v>3686</v>
+      </c>
+      <c r="P86" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q86" t="inlineStr">
+        <is>
+          <t>3861</t>
         </is>
       </c>
     </row>
@@ -5161,9 +5669,15 @@
       <c r="N87" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O87" t="inlineStr">
-        <is>
-          <t>2705</t>
+      <c r="O87" t="n">
+        <v>2705</v>
+      </c>
+      <c r="P87" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q87" t="inlineStr">
+        <is>
+          <t>2735</t>
         </is>
       </c>
     </row>
@@ -5195,7 +5709,7 @@
       <c r="G88" t="n">
         <v>3631</v>
       </c>
-      <c r="H88" s="5" t="n">
+      <c r="H88" s="4" t="n">
         <v>12</v>
       </c>
       <c r="I88" t="n">
@@ -5207,7 +5721,7 @@
       <c r="K88" t="n">
         <v>2521</v>
       </c>
-      <c r="L88" s="5" t="n">
+      <c r="L88" s="4" t="n">
         <v>11</v>
       </c>
       <c r="M88" t="n">
@@ -5216,9 +5730,15 @@
       <c r="N88" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O88" t="inlineStr">
-        <is>
-          <t>2868</t>
+      <c r="O88" t="n">
+        <v>2868</v>
+      </c>
+      <c r="P88" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q88" t="inlineStr">
+        <is>
+          <t>2914</t>
         </is>
       </c>
     </row>
@@ -5250,6 +5770,8 @@
       <c r="M89" t="inlineStr"/>
       <c r="N89" s="2" t="inlineStr"/>
       <c r="O89" t="inlineStr"/>
+      <c r="P89" s="2" t="inlineStr"/>
+      <c r="Q89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -5285,24 +5807,30 @@
       <c r="I90" t="n">
         <v>2454</v>
       </c>
-      <c r="J90" s="5" t="n">
+      <c r="J90" s="4" t="n">
         <v>5</v>
       </c>
       <c r="K90" t="n">
         <v>2456</v>
       </c>
-      <c r="L90" s="5" t="n">
+      <c r="L90" s="4" t="n">
         <v>1</v>
       </c>
       <c r="M90" t="n">
         <v>2450</v>
       </c>
-      <c r="N90" s="5" t="n">
+      <c r="N90" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="O90" t="inlineStr">
-        <is>
-          <t>2497</t>
+      <c r="O90" t="n">
+        <v>2497</v>
+      </c>
+      <c r="P90" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q90" t="inlineStr">
+        <is>
+          <t>2595</t>
         </is>
       </c>
     </row>
@@ -5354,6 +5882,8 @@
       </c>
       <c r="N91" s="2" t="inlineStr"/>
       <c r="O91" t="inlineStr"/>
+      <c r="P91" s="2" t="inlineStr"/>
+      <c r="Q91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -5404,9 +5934,15 @@
       <c r="N92" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O92" t="inlineStr">
-        <is>
-          <t>2619</t>
+      <c r="O92" t="n">
+        <v>2619</v>
+      </c>
+      <c r="P92" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q92" t="inlineStr">
+        <is>
+          <t>2733</t>
         </is>
       </c>
     </row>
@@ -5450,18 +5986,24 @@
       <c r="K93" t="n">
         <v>2610</v>
       </c>
-      <c r="L93" s="5" t="n">
+      <c r="L93" s="4" t="n">
         <v>14</v>
       </c>
       <c r="M93" t="n">
         <v>2714</v>
       </c>
-      <c r="N93" s="5" t="n">
+      <c r="N93" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="O93" t="inlineStr">
-        <is>
-          <t>2671</t>
+      <c r="O93" t="n">
+        <v>2671</v>
+      </c>
+      <c r="P93" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q93" t="inlineStr">
+        <is>
+          <t>2647</t>
         </is>
       </c>
     </row>
@@ -5514,7 +6056,13 @@
       <c r="N94" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O94" t="inlineStr">
+      <c r="O94" t="n">
+        <v>0</v>
+      </c>
+      <c r="P94" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5554,13 +6102,13 @@
       <c r="I95" t="n">
         <v>1984</v>
       </c>
-      <c r="J95" s="5" t="n">
+      <c r="J95" s="4" t="n">
         <v>5</v>
       </c>
       <c r="K95" t="n">
         <v>2038</v>
       </c>
-      <c r="L95" s="5" t="n">
+      <c r="L95" s="4" t="n">
         <v>6</v>
       </c>
       <c r="M95" t="n">
@@ -5569,9 +6117,15 @@
       <c r="N95" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="O95" t="inlineStr">
-        <is>
-          <t>2462</t>
+      <c r="O95" t="n">
+        <v>2462</v>
+      </c>
+      <c r="P95" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q95" t="inlineStr">
+        <is>
+          <t>2423</t>
         </is>
       </c>
     </row>
@@ -5624,9 +6178,15 @@
       <c r="N96" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O96" t="inlineStr">
-        <is>
-          <t>2011</t>
+      <c r="O96" t="n">
+        <v>2011</v>
+      </c>
+      <c r="P96" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q96" t="inlineStr">
+        <is>
+          <t>2070</t>
         </is>
       </c>
     </row>
@@ -5676,12 +6236,18 @@
       <c r="M97" t="n">
         <v>2465</v>
       </c>
-      <c r="N97" s="5" t="n">
+      <c r="N97" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="O97" t="inlineStr">
-        <is>
-          <t>2556</t>
+      <c r="O97" t="n">
+        <v>2556</v>
+      </c>
+      <c r="P97" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q97" t="inlineStr">
+        <is>
+          <t>2555</t>
         </is>
       </c>
     </row>
@@ -5725,7 +6291,7 @@
       <c r="K98" t="n">
         <v>2267</v>
       </c>
-      <c r="L98" s="5" t="n">
+      <c r="L98" s="4" t="n">
         <v>11</v>
       </c>
       <c r="M98" t="n">
@@ -5734,9 +6300,15 @@
       <c r="N98" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O98" t="inlineStr">
-        <is>
-          <t>2341</t>
+      <c r="O98" t="n">
+        <v>2341</v>
+      </c>
+      <c r="P98" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q98" t="inlineStr">
+        <is>
+          <t>2313</t>
         </is>
       </c>
     </row>
@@ -5780,18 +6352,24 @@
       <c r="K99" t="n">
         <v>2746</v>
       </c>
-      <c r="L99" s="5" t="n">
+      <c r="L99" s="4" t="n">
         <v>19</v>
       </c>
       <c r="M99" t="n">
         <v>2843</v>
       </c>
-      <c r="N99" s="5" t="n">
+      <c r="N99" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="O99" t="inlineStr">
-        <is>
-          <t>2899</t>
+      <c r="O99" t="n">
+        <v>2899</v>
+      </c>
+      <c r="P99" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q99" t="inlineStr">
+        <is>
+          <t>2969</t>
         </is>
       </c>
     </row>
@@ -5817,7 +6395,7 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F100" s="5" t="n">
+      <c r="F100" s="4" t="n">
         <v>1</v>
       </c>
       <c r="G100" t="n">
@@ -5835,7 +6413,7 @@
       <c r="K100" t="n">
         <v>2424</v>
       </c>
-      <c r="L100" s="5" t="n">
+      <c r="L100" s="4" t="n">
         <v>10</v>
       </c>
       <c r="M100" t="n">
@@ -5844,9 +6422,15 @@
       <c r="N100" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O100" t="inlineStr">
-        <is>
-          <t>2441</t>
+      <c r="O100" t="n">
+        <v>2441</v>
+      </c>
+      <c r="P100" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q100" t="inlineStr">
+        <is>
+          <t>2418</t>
         </is>
       </c>
     </row>
@@ -5872,7 +6456,7 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F101" s="5" t="n">
+      <c r="F101" s="4" t="n">
         <v>15</v>
       </c>
       <c r="G101" t="n">
@@ -5899,9 +6483,15 @@
       <c r="N101" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="O101" t="inlineStr">
-        <is>
-          <t>3433</t>
+      <c r="O101" t="n">
+        <v>3433</v>
+      </c>
+      <c r="P101" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="Q101" t="inlineStr">
+        <is>
+          <t>3513</t>
         </is>
       </c>
     </row>
@@ -5954,9 +6544,15 @@
       <c r="N102" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O102" t="inlineStr">
-        <is>
-          <t>3085</t>
+      <c r="O102" t="n">
+        <v>3085</v>
+      </c>
+      <c r="P102" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q102" t="inlineStr">
+        <is>
+          <t>3212</t>
         </is>
       </c>
     </row>
@@ -6000,7 +6596,7 @@
       <c r="K103" t="n">
         <v>2813</v>
       </c>
-      <c r="L103" s="5" t="n">
+      <c r="L103" s="4" t="n">
         <v>16</v>
       </c>
       <c r="M103" t="n">
@@ -6009,9 +6605,15 @@
       <c r="N103" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O103" t="inlineStr">
-        <is>
-          <t>2831</t>
+      <c r="O103" t="n">
+        <v>2831</v>
+      </c>
+      <c r="P103" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q103" t="inlineStr">
+        <is>
+          <t>2870</t>
         </is>
       </c>
     </row>
@@ -6037,7 +6639,7 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F104" s="5" t="n">
+      <c r="F104" s="4" t="n">
         <v>8</v>
       </c>
       <c r="G104" t="n">
@@ -6049,24 +6651,30 @@
       <c r="I104" t="n">
         <v>2830</v>
       </c>
-      <c r="J104" s="4" t="n">
+      <c r="J104" s="5" t="n">
         <v>32</v>
       </c>
       <c r="K104" t="n">
         <v>3045</v>
       </c>
-      <c r="L104" s="4" t="n">
+      <c r="L104" s="5" t="n">
         <v>31</v>
       </c>
       <c r="M104" t="n">
         <v>3240</v>
       </c>
-      <c r="N104" s="4" t="n">
+      <c r="N104" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="O104" t="inlineStr">
-        <is>
-          <t>3406</t>
+      <c r="O104" t="n">
+        <v>3406</v>
+      </c>
+      <c r="P104" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q104" t="inlineStr">
+        <is>
+          <t>3542</t>
         </is>
       </c>
     </row>
@@ -6104,7 +6712,7 @@
       <c r="I105" t="n">
         <v>2703</v>
       </c>
-      <c r="J105" s="5" t="n">
+      <c r="J105" s="4" t="n">
         <v>9</v>
       </c>
       <c r="K105" t="n">
@@ -6116,12 +6724,18 @@
       <c r="M105" t="n">
         <v>2802</v>
       </c>
-      <c r="N105" s="5" t="n">
+      <c r="N105" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="O105" t="inlineStr">
-        <is>
-          <t>3101</t>
+      <c r="O105" t="n">
+        <v>3101</v>
+      </c>
+      <c r="P105" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="Q105" t="inlineStr">
+        <is>
+          <t>3198</t>
         </is>
       </c>
     </row>
@@ -6174,9 +6788,15 @@
       <c r="N106" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O106" t="inlineStr">
-        <is>
-          <t>2470</t>
+      <c r="O106" t="n">
+        <v>2470</v>
+      </c>
+      <c r="P106" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q106" t="inlineStr">
+        <is>
+          <t>2454</t>
         </is>
       </c>
     </row>
@@ -6229,9 +6849,15 @@
       <c r="N107" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O107" t="inlineStr">
-        <is>
-          <t>2491</t>
+      <c r="O107" t="n">
+        <v>2491</v>
+      </c>
+      <c r="P107" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q107" t="inlineStr">
+        <is>
+          <t>2537</t>
         </is>
       </c>
     </row>
@@ -6284,9 +6910,15 @@
       <c r="N108" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O108" t="inlineStr">
-        <is>
-          <t>2519</t>
+      <c r="O108" t="n">
+        <v>2519</v>
+      </c>
+      <c r="P108" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q108" t="inlineStr">
+        <is>
+          <t>2563</t>
         </is>
       </c>
     </row>
@@ -6336,12 +6968,18 @@
       <c r="M109" t="n">
         <v>2859</v>
       </c>
-      <c r="N109" s="5" t="n">
+      <c r="N109" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="O109" t="inlineStr">
-        <is>
-          <t>2973</t>
+      <c r="O109" t="n">
+        <v>2973</v>
+      </c>
+      <c r="P109" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q109" t="inlineStr">
+        <is>
+          <t>3080</t>
         </is>
       </c>
     </row>
@@ -6394,9 +7032,15 @@
       <c r="N110" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="O110" t="inlineStr">
-        <is>
-          <t>3021</t>
+      <c r="O110" t="n">
+        <v>3021</v>
+      </c>
+      <c r="P110" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q110" t="inlineStr">
+        <is>
+          <t>3164</t>
         </is>
       </c>
     </row>
@@ -6440,18 +7084,24 @@
       <c r="K111" t="n">
         <v>2499</v>
       </c>
-      <c r="L111" s="5" t="n">
+      <c r="L111" s="4" t="n">
         <v>5</v>
       </c>
       <c r="M111" t="n">
         <v>2545</v>
       </c>
-      <c r="N111" s="5" t="n">
+      <c r="N111" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="O111" t="inlineStr">
-        <is>
-          <t>2583</t>
+      <c r="O111" t="n">
+        <v>2583</v>
+      </c>
+      <c r="P111" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q111" t="inlineStr">
+        <is>
+          <t>2566</t>
         </is>
       </c>
     </row>
@@ -6504,9 +7154,15 @@
       <c r="N112" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O112" t="inlineStr">
-        <is>
-          <t>2486</t>
+      <c r="O112" t="n">
+        <v>2486</v>
+      </c>
+      <c r="P112" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q112" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -6544,24 +7200,30 @@
       <c r="I113" t="n">
         <v>2551</v>
       </c>
-      <c r="J113" s="5" t="n">
+      <c r="J113" s="4" t="n">
         <v>10</v>
       </c>
       <c r="K113" t="n">
         <v>2710</v>
       </c>
-      <c r="L113" s="5" t="n">
+      <c r="L113" s="4" t="n">
         <v>1</v>
       </c>
       <c r="M113" t="n">
         <v>2815</v>
       </c>
-      <c r="N113" s="5" t="n">
+      <c r="N113" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="O113" t="inlineStr">
-        <is>
-          <t>2879</t>
+      <c r="O113" t="n">
+        <v>2879</v>
+      </c>
+      <c r="P113" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q113" t="inlineStr">
+        <is>
+          <t>3029</t>
         </is>
       </c>
     </row>
@@ -6614,9 +7276,15 @@
       <c r="N114" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O114" t="inlineStr">
-        <is>
-          <t>2797</t>
+      <c r="O114" t="n">
+        <v>2797</v>
+      </c>
+      <c r="P114" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q114" t="inlineStr">
+        <is>
+          <t>2977</t>
         </is>
       </c>
     </row>
@@ -6654,24 +7322,30 @@
       <c r="I115" t="n">
         <v>2738</v>
       </c>
-      <c r="J115" s="5" t="n">
+      <c r="J115" s="4" t="n">
         <v>16</v>
       </c>
       <c r="K115" t="n">
         <v>2892</v>
       </c>
-      <c r="L115" s="5" t="n">
+      <c r="L115" s="4" t="n">
         <v>11</v>
       </c>
       <c r="M115" t="n">
         <v>3040</v>
       </c>
-      <c r="N115" s="5" t="n">
+      <c r="N115" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="O115" t="inlineStr">
-        <is>
-          <t>3195</t>
+      <c r="O115" t="n">
+        <v>3195</v>
+      </c>
+      <c r="P115" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q115" t="inlineStr">
+        <is>
+          <t>3527</t>
         </is>
       </c>
     </row>
@@ -6697,36 +7371,42 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F116" s="5" t="n">
+      <c r="F116" s="4" t="n">
         <v>5</v>
       </c>
       <c r="G116" t="n">
         <v>2662</v>
       </c>
-      <c r="H116" s="5" t="n">
+      <c r="H116" s="4" t="n">
         <v>3</v>
       </c>
       <c r="I116" t="n">
         <v>2510</v>
       </c>
-      <c r="J116" s="5" t="n">
+      <c r="J116" s="4" t="n">
         <v>2</v>
       </c>
       <c r="K116" t="n">
         <v>2490</v>
       </c>
-      <c r="L116" s="5" t="n">
+      <c r="L116" s="4" t="n">
         <v>6</v>
       </c>
       <c r="M116" t="n">
         <v>2496</v>
       </c>
-      <c r="N116" s="5" t="n">
+      <c r="N116" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="O116" t="inlineStr">
-        <is>
-          <t>2545</t>
+      <c r="O116" t="n">
+        <v>2545</v>
+      </c>
+      <c r="P116" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q116" t="inlineStr">
+        <is>
+          <t>2573</t>
         </is>
       </c>
     </row>
@@ -6752,36 +7432,42 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F117" s="5" t="n">
+      <c r="F117" s="4" t="n">
         <v>5</v>
       </c>
       <c r="G117" t="n">
         <v>3202</v>
       </c>
-      <c r="H117" s="5" t="n">
+      <c r="H117" s="4" t="n">
         <v>5</v>
       </c>
       <c r="I117" t="n">
         <v>2509</v>
       </c>
-      <c r="J117" s="5" t="n">
+      <c r="J117" s="4" t="n">
         <v>5</v>
       </c>
       <c r="K117" t="n">
         <v>2522</v>
       </c>
-      <c r="L117" s="5" t="n">
+      <c r="L117" s="4" t="n">
         <v>6</v>
       </c>
       <c r="M117" t="n">
         <v>2611</v>
       </c>
-      <c r="N117" s="5" t="n">
+      <c r="N117" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="O117" t="inlineStr">
-        <is>
-          <t>2680</t>
+      <c r="O117" t="n">
+        <v>2680</v>
+      </c>
+      <c r="P117" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q117" t="inlineStr">
+        <is>
+          <t>2778</t>
         </is>
       </c>
     </row>
@@ -6834,9 +7520,15 @@
       <c r="N118" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="O118" t="inlineStr">
-        <is>
-          <t>3078</t>
+      <c r="O118" t="n">
+        <v>3078</v>
+      </c>
+      <c r="P118" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="Q118" t="inlineStr">
+        <is>
+          <t>3119</t>
         </is>
       </c>
     </row>
@@ -6889,7 +7581,13 @@
       <c r="N119" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O119" t="inlineStr">
+      <c r="O119" t="n">
+        <v>0</v>
+      </c>
+      <c r="P119" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q119" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6917,19 +7615,19 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F120" s="4" t="n">
+      <c r="F120" s="5" t="n">
         <v>34</v>
       </c>
       <c r="G120" t="n">
         <v>4123</v>
       </c>
-      <c r="H120" s="4" t="n">
+      <c r="H120" s="5" t="n">
         <v>31</v>
       </c>
       <c r="I120" t="n">
         <v>2760</v>
       </c>
-      <c r="J120" s="4" t="n">
+      <c r="J120" s="5" t="n">
         <v>31</v>
       </c>
       <c r="K120" t="n">
@@ -6944,9 +7642,15 @@
       <c r="N120" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="O120" t="inlineStr">
-        <is>
-          <t>3069</t>
+      <c r="O120" t="n">
+        <v>3069</v>
+      </c>
+      <c r="P120" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q120" t="inlineStr">
+        <is>
+          <t>3206</t>
         </is>
       </c>
     </row>
@@ -6996,12 +7700,18 @@
       <c r="M121" t="n">
         <v>2683</v>
       </c>
-      <c r="N121" s="5" t="n">
+      <c r="N121" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="O121" t="inlineStr">
-        <is>
-          <t>2719</t>
+      <c r="O121" t="n">
+        <v>2719</v>
+      </c>
+      <c r="P121" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q121" t="inlineStr">
+        <is>
+          <t>2656</t>
         </is>
       </c>
     </row>
@@ -7027,7 +7737,7 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F122" s="5" t="n">
+      <c r="F122" s="4" t="n">
         <v>5</v>
       </c>
       <c r="G122" t="n">
@@ -7054,9 +7764,15 @@
       <c r="N122" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O122" t="inlineStr">
-        <is>
-          <t>2743</t>
+      <c r="O122" t="n">
+        <v>2743</v>
+      </c>
+      <c r="P122" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q122" t="inlineStr">
+        <is>
+          <t>2781</t>
         </is>
       </c>
     </row>
@@ -7109,9 +7825,15 @@
       <c r="N123" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O123" t="inlineStr">
-        <is>
-          <t>2536</t>
+      <c r="O123" t="n">
+        <v>2536</v>
+      </c>
+      <c r="P123" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q123" t="inlineStr">
+        <is>
+          <t>2495</t>
         </is>
       </c>
     </row>
@@ -7137,7 +7859,7 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F124" s="5" t="n">
+      <c r="F124" s="4" t="n">
         <v>16</v>
       </c>
       <c r="G124" t="n">
@@ -7161,12 +7883,18 @@
       <c r="M124" t="n">
         <v>2727</v>
       </c>
-      <c r="N124" s="5" t="n">
+      <c r="N124" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="O124" t="inlineStr">
-        <is>
-          <t>2810</t>
+      <c r="O124" t="n">
+        <v>2810</v>
+      </c>
+      <c r="P124" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="Q124" t="inlineStr">
+        <is>
+          <t>2875</t>
         </is>
       </c>
     </row>
@@ -7219,9 +7947,15 @@
       <c r="N125" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O125" t="inlineStr">
-        <is>
-          <t>2846</t>
+      <c r="O125" t="n">
+        <v>2846</v>
+      </c>
+      <c r="P125" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q125" t="inlineStr">
+        <is>
+          <t>2898</t>
         </is>
       </c>
     </row>
@@ -7274,9 +8008,15 @@
       <c r="N126" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O126" t="inlineStr">
-        <is>
-          <t>3036</t>
+      <c r="O126" t="n">
+        <v>3036</v>
+      </c>
+      <c r="P126" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q126" t="inlineStr">
+        <is>
+          <t>3119</t>
         </is>
       </c>
     </row>
@@ -7329,9 +8069,15 @@
       <c r="N127" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O127" t="inlineStr">
-        <is>
-          <t>2832</t>
+      <c r="O127" t="n">
+        <v>2832</v>
+      </c>
+      <c r="P127" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q127" t="inlineStr">
+        <is>
+          <t>2882</t>
         </is>
       </c>
     </row>
@@ -7384,7 +8130,13 @@
       <c r="N128" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O128" t="inlineStr">
+      <c r="O128" t="n">
+        <v>0</v>
+      </c>
+      <c r="P128" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7439,7 +8191,13 @@
       <c r="N129" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O129" t="inlineStr">
+      <c r="O129" t="n">
+        <v>0</v>
+      </c>
+      <c r="P129" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7494,9 +8252,15 @@
       <c r="N130" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O130" t="inlineStr">
-        <is>
-          <t>2639</t>
+      <c r="O130" t="n">
+        <v>2639</v>
+      </c>
+      <c r="P130" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q130" t="inlineStr">
+        <is>
+          <t>2716</t>
         </is>
       </c>
     </row>
@@ -7549,9 +8313,15 @@
       <c r="N131" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O131" t="inlineStr">
-        <is>
-          <t>2650</t>
+      <c r="O131" t="n">
+        <v>2650</v>
+      </c>
+      <c r="P131" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q131" t="inlineStr">
+        <is>
+          <t>2637</t>
         </is>
       </c>
     </row>
@@ -7577,19 +8347,19 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F132" s="5" t="n">
+      <c r="F132" s="4" t="n">
         <v>2</v>
       </c>
       <c r="G132" t="n">
         <v>1062</v>
       </c>
-      <c r="H132" s="5" t="n">
+      <c r="H132" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I132" t="n">
         <v>1020</v>
       </c>
-      <c r="J132" s="5" t="n">
+      <c r="J132" s="4" t="n">
         <v>1</v>
       </c>
       <c r="K132" t="n">
@@ -7601,12 +8371,18 @@
       <c r="M132" t="n">
         <v>0</v>
       </c>
-      <c r="N132" s="5" t="n">
+      <c r="N132" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="O132" t="inlineStr">
-        <is>
-          <t>1061</t>
+      <c r="O132" t="n">
+        <v>1061</v>
+      </c>
+      <c r="P132" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q132" t="inlineStr">
+        <is>
+          <t>1199</t>
         </is>
       </c>
     </row>
@@ -7638,13 +8414,13 @@
       <c r="G133" t="n">
         <v>2417</v>
       </c>
-      <c r="H133" s="5" t="n">
+      <c r="H133" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I133" t="n">
         <v>2013</v>
       </c>
-      <c r="J133" s="5" t="n">
+      <c r="J133" s="4" t="n">
         <v>4</v>
       </c>
       <c r="K133" t="n">
@@ -7659,9 +8435,15 @@
       <c r="N133" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O133" t="inlineStr">
-        <is>
-          <t>2061</t>
+      <c r="O133" t="n">
+        <v>2061</v>
+      </c>
+      <c r="P133" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q133" t="inlineStr">
+        <is>
+          <t>2095</t>
         </is>
       </c>
     </row>
@@ -7714,9 +8496,15 @@
       <c r="N134" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="O134" t="inlineStr">
-        <is>
-          <t>2971</t>
+      <c r="O134" t="n">
+        <v>2971</v>
+      </c>
+      <c r="P134" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q134" t="inlineStr">
+        <is>
+          <t>3129</t>
         </is>
       </c>
     </row>
@@ -7769,7 +8557,13 @@
       <c r="N135" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O135" t="inlineStr">
+      <c r="O135" t="n">
+        <v>0</v>
+      </c>
+      <c r="P135" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q135" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7824,7 +8618,13 @@
       <c r="N136" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O136" t="inlineStr">
+      <c r="O136" t="n">
+        <v>0</v>
+      </c>
+      <c r="P136" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q136" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7879,7 +8679,13 @@
       <c r="N137" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O137" t="inlineStr">
+      <c r="O137" t="n">
+        <v>0</v>
+      </c>
+      <c r="P137" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7934,9 +8740,15 @@
       <c r="N138" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="O138" t="inlineStr">
-        <is>
-          <t>2873</t>
+      <c r="O138" t="n">
+        <v>2873</v>
+      </c>
+      <c r="P138" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q138" t="inlineStr">
+        <is>
+          <t>2959</t>
         </is>
       </c>
     </row>
@@ -7989,7 +8801,13 @@
       <c r="N139" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O139" t="inlineStr">
+      <c r="O139" t="n">
+        <v>0</v>
+      </c>
+      <c r="P139" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q139" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8017,7 +8835,7 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F140" s="5" t="n">
+      <c r="F140" s="4" t="n">
         <v>5</v>
       </c>
       <c r="G140" t="n">
@@ -8029,24 +8847,30 @@
       <c r="I140" t="n">
         <v>2454</v>
       </c>
-      <c r="J140" s="5" t="n">
+      <c r="J140" s="4" t="n">
         <v>11</v>
       </c>
       <c r="K140" t="n">
         <v>2564</v>
       </c>
-      <c r="L140" s="5" t="n">
+      <c r="L140" s="4" t="n">
         <v>6</v>
       </c>
       <c r="M140" t="n">
         <v>2587</v>
       </c>
-      <c r="N140" s="5" t="n">
+      <c r="N140" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="O140" t="inlineStr">
-        <is>
-          <t>2659</t>
+      <c r="O140" t="n">
+        <v>2659</v>
+      </c>
+      <c r="P140" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q140" t="inlineStr">
+        <is>
+          <t>2623</t>
         </is>
       </c>
     </row>
@@ -8099,7 +8923,13 @@
       <c r="N141" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O141" t="inlineStr">
+      <c r="O141" t="n">
+        <v>0</v>
+      </c>
+      <c r="P141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q141" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8154,9 +8984,15 @@
       <c r="N142" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="O142" t="inlineStr">
-        <is>
-          <t>2659</t>
+      <c r="O142" t="n">
+        <v>2659</v>
+      </c>
+      <c r="P142" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q142" t="inlineStr">
+        <is>
+          <t>2734</t>
         </is>
       </c>
     </row>
@@ -8204,6 +9040,8 @@
       <c r="M143" t="inlineStr"/>
       <c r="N143" s="2" t="inlineStr"/>
       <c r="O143" t="inlineStr"/>
+      <c r="P143" s="2" t="inlineStr"/>
+      <c r="Q143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -8233,7 +9071,7 @@
       <c r="G144" t="n">
         <v>2892</v>
       </c>
-      <c r="H144" s="5" t="n">
+      <c r="H144" s="4" t="n">
         <v>12</v>
       </c>
       <c r="I144" t="n">
@@ -8245,18 +9083,24 @@
       <c r="K144" t="n">
         <v>2453</v>
       </c>
-      <c r="L144" s="5" t="n">
+      <c r="L144" s="4" t="n">
         <v>7</v>
       </c>
       <c r="M144" t="n">
         <v>2472</v>
       </c>
-      <c r="N144" s="5" t="n">
+      <c r="N144" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="O144" t="inlineStr">
-        <is>
-          <t>2497</t>
+      <c r="O144" t="n">
+        <v>2497</v>
+      </c>
+      <c r="P144" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q144" t="inlineStr">
+        <is>
+          <t>2491</t>
         </is>
       </c>
     </row>
@@ -8309,7 +9153,13 @@
       <c r="N145" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O145" t="inlineStr">
+      <c r="O145" t="n">
+        <v>0</v>
+      </c>
+      <c r="P145" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q145" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8364,7 +9214,13 @@
       <c r="N146" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O146" t="inlineStr">
+      <c r="O146" t="n">
+        <v>0</v>
+      </c>
+      <c r="P146" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8419,7 +9275,13 @@
       <c r="N147" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O147" t="inlineStr">
+      <c r="O147" t="n">
+        <v>0</v>
+      </c>
+      <c r="P147" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q147" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8474,7 +9336,13 @@
       <c r="N148" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O148" t="inlineStr">
+      <c r="O148" t="n">
+        <v>0</v>
+      </c>
+      <c r="P148" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8529,7 +9397,13 @@
       <c r="N149" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O149" t="inlineStr">
+      <c r="O149" t="n">
+        <v>0</v>
+      </c>
+      <c r="P149" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q149" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8563,30 +9437,36 @@
       <c r="G150" t="n">
         <v>2445</v>
       </c>
-      <c r="H150" s="5" t="n">
+      <c r="H150" s="4" t="n">
         <v>2</v>
       </c>
       <c r="I150" t="n">
         <v>1997</v>
       </c>
-      <c r="J150" s="5" t="n">
+      <c r="J150" s="4" t="n">
         <v>9</v>
       </c>
       <c r="K150" t="n">
         <v>2224</v>
       </c>
-      <c r="L150" s="5" t="n">
+      <c r="L150" s="4" t="n">
         <v>19</v>
       </c>
       <c r="M150" t="n">
         <v>2342</v>
       </c>
-      <c r="N150" s="5" t="n">
+      <c r="N150" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="O150" t="inlineStr">
-        <is>
-          <t>2320</t>
+      <c r="O150" t="n">
+        <v>2320</v>
+      </c>
+      <c r="P150" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q150" t="inlineStr">
+        <is>
+          <t>2339</t>
         </is>
       </c>
     </row>
@@ -8639,7 +9519,13 @@
       <c r="N151" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O151" t="inlineStr">
+      <c r="O151" t="n">
+        <v>0</v>
+      </c>
+      <c r="P151" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q151" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8667,7 +9553,7 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F152" s="5" t="n">
+      <c r="F152" s="4" t="n">
         <v>3</v>
       </c>
       <c r="G152" t="n">
@@ -8679,13 +9565,13 @@
       <c r="I152" t="n">
         <v>1500</v>
       </c>
-      <c r="J152" s="5" t="n">
+      <c r="J152" s="4" t="n">
         <v>5</v>
       </c>
       <c r="K152" t="n">
         <v>1581</v>
       </c>
-      <c r="L152" s="5" t="n">
+      <c r="L152" s="4" t="n">
         <v>3</v>
       </c>
       <c r="M152" t="n">
@@ -8694,9 +9580,15 @@
       <c r="N152" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O152" t="inlineStr">
-        <is>
-          <t>1602</t>
+      <c r="O152" t="n">
+        <v>1602</v>
+      </c>
+      <c r="P152" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q152" t="inlineStr">
+        <is>
+          <t>1611</t>
         </is>
       </c>
     </row>
@@ -8722,36 +9614,42 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F153" s="5" t="n">
+      <c r="F153" s="4" t="n">
         <v>14</v>
       </c>
       <c r="G153" t="n">
         <v>1637</v>
       </c>
-      <c r="H153" s="5" t="n">
+      <c r="H153" s="4" t="n">
         <v>8</v>
       </c>
       <c r="I153" t="n">
         <v>1637</v>
       </c>
-      <c r="J153" s="5" t="n">
+      <c r="J153" s="4" t="n">
         <v>4</v>
       </c>
       <c r="K153" t="n">
         <v>1689</v>
       </c>
-      <c r="L153" s="5" t="n">
+      <c r="L153" s="4" t="n">
         <v>4</v>
       </c>
       <c r="M153" t="n">
         <v>1729</v>
       </c>
-      <c r="N153" s="5" t="n">
+      <c r="N153" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="O153" t="inlineStr">
-        <is>
-          <t>1778</t>
+      <c r="O153" t="n">
+        <v>1778</v>
+      </c>
+      <c r="P153" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q153" t="inlineStr">
+        <is>
+          <t>1832</t>
         </is>
       </c>
     </row>
@@ -8804,7 +9702,13 @@
       <c r="N154" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O154" t="inlineStr">
+      <c r="O154" t="n">
+        <v>0</v>
+      </c>
+      <c r="P154" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8838,30 +9742,36 @@
       <c r="G155" t="n">
         <v>5823</v>
       </c>
-      <c r="H155" s="5" t="n">
+      <c r="H155" s="4" t="n">
         <v>7</v>
       </c>
       <c r="I155" t="n">
         <v>2629</v>
       </c>
-      <c r="J155" s="5" t="n">
+      <c r="J155" s="4" t="n">
         <v>10</v>
       </c>
       <c r="K155" t="n">
         <v>2807</v>
       </c>
-      <c r="L155" s="5" t="n">
+      <c r="L155" s="4" t="n">
         <v>9</v>
       </c>
       <c r="M155" t="n">
         <v>2925</v>
       </c>
-      <c r="N155" s="4" t="n">
+      <c r="N155" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="O155" t="inlineStr">
-        <is>
-          <t>3585</t>
+      <c r="O155" t="n">
+        <v>3585</v>
+      </c>
+      <c r="P155" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="Q155" t="inlineStr">
+        <is>
+          <t>3738</t>
         </is>
       </c>
     </row>
@@ -8914,7 +9824,13 @@
       <c r="N156" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O156" t="inlineStr">
+      <c r="O156" t="n">
+        <v>0</v>
+      </c>
+      <c r="P156" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q156" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8969,7 +9885,13 @@
       <c r="N157" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O157" t="inlineStr">
+      <c r="O157" t="n">
+        <v>0</v>
+      </c>
+      <c r="P157" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q157" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8994,7 +9916,7 @@
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>Chinese</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F158" s="2" t="n">
@@ -9005,24 +9927,30 @@
       </c>
       <c r="H158" s="2" t="inlineStr"/>
       <c r="I158" t="inlineStr"/>
-      <c r="J158" s="4" t="n">
+      <c r="J158" s="5" t="n">
         <v>33</v>
       </c>
       <c r="K158" t="n">
         <v>3283</v>
       </c>
-      <c r="L158" s="4" t="n">
+      <c r="L158" s="5" t="n">
         <v>32</v>
       </c>
       <c r="M158" t="n">
         <v>3591</v>
       </c>
-      <c r="N158" s="4" t="n">
+      <c r="N158" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="O158" t="inlineStr">
-        <is>
-          <t>3822</t>
+      <c r="O158" t="n">
+        <v>3822</v>
+      </c>
+      <c r="P158" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q158" t="inlineStr">
+        <is>
+          <t>4130</t>
         </is>
       </c>
     </row>
@@ -9075,7 +10003,13 @@
       <c r="N159" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O159" t="inlineStr">
+      <c r="O159" t="n">
+        <v>0</v>
+      </c>
+      <c r="P159" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q159" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9121,18 +10055,24 @@
       <c r="K160" t="n">
         <v>2550</v>
       </c>
-      <c r="L160" s="5" t="n">
+      <c r="L160" s="4" t="n">
         <v>6</v>
       </c>
       <c r="M160" t="n">
         <v>2582</v>
       </c>
-      <c r="N160" s="5" t="n">
+      <c r="N160" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="O160" t="inlineStr">
-        <is>
-          <t>2739</t>
+      <c r="O160" t="n">
+        <v>2739</v>
+      </c>
+      <c r="P160" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q160" t="inlineStr">
+        <is>
+          <t>2744</t>
         </is>
       </c>
     </row>
@@ -9185,7 +10125,13 @@
       <c r="N161" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O161" t="inlineStr">
+      <c r="O161" t="n">
+        <v>0</v>
+      </c>
+      <c r="P161" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q161" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9240,9 +10186,15 @@
       <c r="N162" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O162" t="inlineStr">
-        <is>
-          <t>2511</t>
+      <c r="O162" t="n">
+        <v>2511</v>
+      </c>
+      <c r="P162" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q162" t="inlineStr">
+        <is>
+          <t>2632</t>
         </is>
       </c>
     </row>
@@ -9286,7 +10238,7 @@
       <c r="K163" t="n">
         <v>2470</v>
       </c>
-      <c r="L163" s="5" t="n">
+      <c r="L163" s="4" t="n">
         <v>1</v>
       </c>
       <c r="M163" t="n">
@@ -9295,11 +10247,11 @@
       <c r="N163" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O163" t="inlineStr">
-        <is>
-          <t>2437</t>
-        </is>
-      </c>
+      <c r="O163" t="n">
+        <v>2437</v>
+      </c>
+      <c r="P163" s="2" t="inlineStr"/>
+      <c r="Q163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" t="n">
@@ -9319,7 +10271,7 @@
       </c>
       <c r="F164" s="2" t="inlineStr"/>
       <c r="G164" t="inlineStr"/>
-      <c r="H164" s="5" t="n">
+      <c r="H164" s="4" t="n">
         <v>10</v>
       </c>
       <c r="I164" t="n">
@@ -9331,7 +10283,7 @@
       <c r="K164" t="n">
         <v>1994</v>
       </c>
-      <c r="L164" s="5" t="n">
+      <c r="L164" s="4" t="n">
         <v>8</v>
       </c>
       <c r="M164" t="n">
@@ -9340,9 +10292,15 @@
       <c r="N164" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O164" t="inlineStr">
-        <is>
-          <t>2052</t>
+      <c r="O164" t="n">
+        <v>2052</v>
+      </c>
+      <c r="P164" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q164" t="inlineStr">
+        <is>
+          <t>2133</t>
         </is>
       </c>
     </row>
@@ -9377,9 +10335,15 @@
       <c r="N165" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="O165" t="inlineStr">
-        <is>
-          <t>2000</t>
+      <c r="O165" t="n">
+        <v>2000</v>
+      </c>
+      <c r="P165" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q165" t="inlineStr">
+        <is>
+          <t>2162</t>
         </is>
       </c>
     </row>
@@ -9414,9 +10378,15 @@
       <c r="N166" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O166" t="inlineStr">
-        <is>
-          <t>1512</t>
+      <c r="O166" t="n">
+        <v>1512</v>
+      </c>
+      <c r="P166" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q166" t="inlineStr">
+        <is>
+          <t>1490</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-02-05 11:30:33
</commit_message>
<xml_diff>
--- a/Season_Attack/83.xlsx
+++ b/Season_Attack/83.xlsx
@@ -83,8 +83,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G167"/>
+  <dimension ref="A1:I168"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,6 +426,16 @@
           <t>02-03_0</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>02-04_A</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>02-04_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -452,9 +462,15 @@
       <c r="F2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>3406</t>
+      <c r="G2" t="n">
+        <v>3406</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>3456</t>
         </is>
       </c>
     </row>
@@ -483,9 +499,15 @@
       <c r="F3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>4415</t>
+      <c r="G3" t="n">
+        <v>4415</v>
+      </c>
+      <c r="H3" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>4667</t>
         </is>
       </c>
     </row>
@@ -514,9 +536,15 @@
       <c r="F4" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>4354</t>
+      <c r="G4" t="n">
+        <v>4354</v>
+      </c>
+      <c r="H4" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>4553</t>
         </is>
       </c>
     </row>
@@ -539,15 +567,21 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>4342</t>
+      <c r="G5" t="n">
+        <v>4342</v>
+      </c>
+      <c r="H5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>4652</t>
         </is>
       </c>
     </row>
@@ -576,9 +610,15 @@
       <c r="F6" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>4325</t>
+      <c r="G6" t="n">
+        <v>4325</v>
+      </c>
+      <c r="H6" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>4624</t>
         </is>
       </c>
     </row>
@@ -601,15 +641,21 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F7" s="4" t="n">
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F7" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>4608</t>
+      <c r="G7" t="n">
+        <v>4608</v>
+      </c>
+      <c r="H7" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>5062</t>
         </is>
       </c>
     </row>
@@ -632,15 +678,21 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>4123</t>
+      <c r="G8" t="n">
+        <v>4123</v>
+      </c>
+      <c r="H8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>4401</t>
         </is>
       </c>
     </row>
@@ -666,14 +718,14 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F9" s="4" t="n">
+      <c r="F9" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>3805</t>
-        </is>
-      </c>
+      <c r="G9" t="n">
+        <v>3805</v>
+      </c>
+      <c r="H9" s="3" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -697,12 +749,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F10" s="4" t="n">
+      <c r="F10" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>4157</t>
+      <c r="G10" t="n">
+        <v>4157</v>
+      </c>
+      <c r="H10" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>4290</t>
         </is>
       </c>
     </row>
@@ -731,9 +789,15 @@
       <c r="F11" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>4181</t>
+      <c r="G11" t="n">
+        <v>4181</v>
+      </c>
+      <c r="H11" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>4447</t>
         </is>
       </c>
     </row>
@@ -756,15 +820,21 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F12" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>3917</t>
+      <c r="G12" t="n">
+        <v>3917</v>
+      </c>
+      <c r="H12" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>4103</t>
         </is>
       </c>
     </row>
@@ -790,10 +860,16 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F13" s="5" t="n">
+      <c r="F13" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="G13" t="n">
+        <v>2686</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="inlineStr">
         <is>
           <t>2686</t>
         </is>
@@ -818,15 +894,21 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F14" s="4" t="n">
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F14" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>5000</t>
+      <c r="G14" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H14" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>5299</t>
         </is>
       </c>
     </row>
@@ -849,15 +931,21 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F15" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>4188</t>
+      <c r="G15" t="n">
+        <v>4188</v>
+      </c>
+      <c r="H15" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>4457</t>
         </is>
       </c>
     </row>
@@ -883,12 +971,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F16" s="4" t="n">
+      <c r="F16" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>4551</t>
+      <c r="G16" t="n">
+        <v>4551</v>
+      </c>
+      <c r="H16" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>4635</t>
         </is>
       </c>
     </row>
@@ -914,12 +1008,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F17" s="4" t="n">
+      <c r="F17" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>3776</t>
+      <c r="G17" t="n">
+        <v>3776</v>
+      </c>
+      <c r="H17" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>3930</t>
         </is>
       </c>
     </row>
@@ -948,9 +1048,15 @@
       <c r="F18" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>3989</t>
+      <c r="G18" t="n">
+        <v>3989</v>
+      </c>
+      <c r="H18" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>4053</t>
         </is>
       </c>
     </row>
@@ -979,9 +1085,15 @@
       <c r="F19" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>4275</t>
+      <c r="G19" t="n">
+        <v>4275</v>
+      </c>
+      <c r="H19" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>4549</t>
         </is>
       </c>
     </row>
@@ -1004,15 +1116,21 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F20" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>4861</t>
+      <c r="G20" t="n">
+        <v>4861</v>
+      </c>
+      <c r="H20" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>5249</t>
         </is>
       </c>
     </row>
@@ -1041,9 +1159,15 @@
       <c r="F21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>3100</t>
+      <c r="G21" t="n">
+        <v>3100</v>
+      </c>
+      <c r="H21" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>3411</t>
         </is>
       </c>
     </row>
@@ -1069,12 +1193,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F22" s="4" t="n">
+      <c r="F22" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>4292</t>
+      <c r="G22" t="n">
+        <v>4292</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>4580</t>
         </is>
       </c>
     </row>
@@ -1103,9 +1233,15 @@
       <c r="F23" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>3316</t>
+      <c r="G23" t="n">
+        <v>3316</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>3826</t>
         </is>
       </c>
     </row>
@@ -1131,12 +1267,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F24" s="4" t="n">
+      <c r="F24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>4601</t>
+      <c r="G24" t="n">
+        <v>4601</v>
+      </c>
+      <c r="H24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>4701</t>
         </is>
       </c>
     </row>
@@ -1165,7 +1307,13 @@
       <c r="F25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G25" t="inlineStr">
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1190,15 +1338,21 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F26" s="4" t="n">
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F26" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>4590</t>
+      <c r="G26" t="n">
+        <v>4590</v>
+      </c>
+      <c r="H26" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>4815</t>
         </is>
       </c>
     </row>
@@ -1224,12 +1378,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F27" s="4" t="n">
+      <c r="F27" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>4493</t>
+      <c r="G27" t="n">
+        <v>4493</v>
+      </c>
+      <c r="H27" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>4948</t>
         </is>
       </c>
     </row>
@@ -1258,9 +1418,15 @@
       <c r="F28" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>3584</t>
+      <c r="G28" t="n">
+        <v>3584</v>
+      </c>
+      <c r="H28" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>3803</t>
         </is>
       </c>
     </row>
@@ -1286,12 +1452,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F29" s="4" t="n">
+      <c r="F29" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>4828</t>
+      <c r="G29" t="n">
+        <v>4828</v>
+      </c>
+      <c r="H29" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>5198</t>
         </is>
       </c>
     </row>
@@ -1314,15 +1486,21 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F30" s="4" t="n">
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F30" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>4569</t>
+      <c r="G30" t="n">
+        <v>4569</v>
+      </c>
+      <c r="H30" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>4872</t>
         </is>
       </c>
     </row>
@@ -1345,15 +1523,21 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F31" s="4" t="n">
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F31" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>4007</t>
+      <c r="G31" t="n">
+        <v>4007</v>
+      </c>
+      <c r="H31" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>4245</t>
         </is>
       </c>
     </row>
@@ -1382,9 +1566,15 @@
       <c r="F32" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>4578</t>
+      <c r="G32" t="n">
+        <v>4578</v>
+      </c>
+      <c r="H32" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>5072</t>
         </is>
       </c>
     </row>
@@ -1410,12 +1600,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F33" s="4" t="n">
+      <c r="F33" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>4611</t>
+      <c r="G33" t="n">
+        <v>4611</v>
+      </c>
+      <c r="H33" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>4908</t>
         </is>
       </c>
     </row>
@@ -1441,12 +1637,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F34" s="4" t="n">
+      <c r="F34" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>4415</t>
+      <c r="G34" t="n">
+        <v>4415</v>
+      </c>
+      <c r="H34" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>4727</t>
         </is>
       </c>
     </row>
@@ -1469,15 +1671,21 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F35" s="4" t="n">
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F35" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>4686</t>
+      <c r="G35" t="n">
+        <v>4686</v>
+      </c>
+      <c r="H35" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>4897</t>
         </is>
       </c>
     </row>
@@ -1503,12 +1711,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F36" s="4" t="n">
+      <c r="F36" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>4395</t>
+      <c r="G36" t="n">
+        <v>4395</v>
+      </c>
+      <c r="H36" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>4635</t>
         </is>
       </c>
     </row>
@@ -1534,12 +1748,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F37" s="4" t="n">
+      <c r="F37" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>4013</t>
+      <c r="G37" t="n">
+        <v>4013</v>
+      </c>
+      <c r="H37" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>4321</t>
         </is>
       </c>
     </row>
@@ -1562,15 +1782,21 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F38" s="4" t="n">
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F38" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>4343</t>
+      <c r="G38" t="n">
+        <v>4343</v>
+      </c>
+      <c r="H38" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>4613</t>
         </is>
       </c>
     </row>
@@ -1596,12 +1822,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F39" s="4" t="n">
+      <c r="F39" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>4189</t>
+      <c r="G39" t="n">
+        <v>4189</v>
+      </c>
+      <c r="H39" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>4260</t>
         </is>
       </c>
     </row>
@@ -1627,12 +1859,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F40" s="4" t="n">
+      <c r="F40" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>4857</t>
+      <c r="G40" t="n">
+        <v>4857</v>
+      </c>
+      <c r="H40" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>5223</t>
         </is>
       </c>
     </row>
@@ -1658,12 +1896,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F41" s="5" t="n">
+      <c r="F41" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>4336</t>
+      <c r="G41" t="n">
+        <v>4336</v>
+      </c>
+      <c r="H41" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>4545</t>
         </is>
       </c>
     </row>
@@ -1689,12 +1933,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F42" s="4" t="n">
+      <c r="F42" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>4787</t>
+      <c r="G42" t="n">
+        <v>4787</v>
+      </c>
+      <c r="H42" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>5071</t>
         </is>
       </c>
     </row>
@@ -1717,15 +1967,21 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F43" s="4" t="n">
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F43" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>4282</t>
+      <c r="G43" t="n">
+        <v>4282</v>
+      </c>
+      <c r="H43" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>4608</t>
         </is>
       </c>
     </row>
@@ -1751,12 +2007,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F44" s="4" t="n">
+      <c r="F44" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>4371</t>
+      <c r="G44" t="n">
+        <v>4371</v>
+      </c>
+      <c r="H44" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>4707</t>
         </is>
       </c>
     </row>
@@ -1782,12 +2044,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F45" s="4" t="n">
+      <c r="F45" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>3933</t>
+      <c r="G45" t="n">
+        <v>3933</v>
+      </c>
+      <c r="H45" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>4249</t>
         </is>
       </c>
     </row>
@@ -1816,9 +2084,15 @@
       <c r="F46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>3980</t>
+      <c r="G46" t="n">
+        <v>3980</v>
+      </c>
+      <c r="H46" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>4142</t>
         </is>
       </c>
     </row>
@@ -1847,7 +2121,13 @@
       <c r="F47" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G47" t="inlineStr">
+      <c r="G47" t="n">
+        <v>3037</v>
+      </c>
+      <c r="H47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I47" t="inlineStr">
         <is>
           <t>3037</t>
         </is>
@@ -1872,15 +2152,21 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>总馆</t>
-        </is>
-      </c>
-      <c r="F48" s="4" t="n">
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F48" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>4350</t>
+      <c r="G48" t="n">
+        <v>4350</v>
+      </c>
+      <c r="H48" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>4682</t>
         </is>
       </c>
     </row>
@@ -1906,12 +2192,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F49" s="4" t="n">
+      <c r="F49" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>3683</t>
+      <c r="G49" t="n">
+        <v>3683</v>
+      </c>
+      <c r="H49" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>3888</t>
         </is>
       </c>
     </row>
@@ -1937,12 +2229,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F50" s="4" t="n">
+      <c r="F50" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>4701</t>
+      <c r="G50" t="n">
+        <v>4701</v>
+      </c>
+      <c r="H50" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>4991</t>
         </is>
       </c>
     </row>
@@ -1971,9 +2269,15 @@
       <c r="F51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>2729</t>
+      <c r="G51" t="n">
+        <v>2729</v>
+      </c>
+      <c r="H51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>2782</t>
         </is>
       </c>
     </row>
@@ -2002,9 +2306,15 @@
       <c r="F52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>2688</t>
+      <c r="G52" t="n">
+        <v>2688</v>
+      </c>
+      <c r="H52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>2711</t>
         </is>
       </c>
     </row>
@@ -2030,10 +2340,16 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F53" s="5" t="n">
+      <c r="F53" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="G53" t="inlineStr">
+      <c r="G53" t="n">
+        <v>2902</v>
+      </c>
+      <c r="H53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I53" t="inlineStr">
         <is>
           <t>2902</t>
         </is>
@@ -2061,12 +2377,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F54" s="4" t="n">
+      <c r="F54" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>4368</t>
+      <c r="G54" t="n">
+        <v>4368</v>
+      </c>
+      <c r="H54" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>4627</t>
         </is>
       </c>
     </row>
@@ -2092,12 +2414,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F55" s="4" t="n">
+      <c r="F55" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>3514</t>
+      <c r="G55" t="n">
+        <v>3514</v>
+      </c>
+      <c r="H55" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>3677</t>
         </is>
       </c>
     </row>
@@ -2126,9 +2454,15 @@
       <c r="F56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>3689</t>
+      <c r="G56" t="n">
+        <v>3689</v>
+      </c>
+      <c r="H56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>3818</t>
         </is>
       </c>
     </row>
@@ -2157,9 +2491,15 @@
       <c r="F57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>4100</t>
+      <c r="G57" t="n">
+        <v>4100</v>
+      </c>
+      <c r="H57" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>4300</t>
         </is>
       </c>
     </row>
@@ -2185,12 +2525,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F58" s="4" t="n">
+      <c r="F58" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>3561</t>
+      <c r="G58" t="n">
+        <v>3561</v>
+      </c>
+      <c r="H58" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>3822</t>
         </is>
       </c>
     </row>
@@ -2219,9 +2565,15 @@
       <c r="F59" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>4003</t>
+      <c r="G59" t="n">
+        <v>4003</v>
+      </c>
+      <c r="H59" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>4296</t>
         </is>
       </c>
     </row>
@@ -2250,7 +2602,13 @@
       <c r="F60" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G60" t="inlineStr">
+      <c r="G60" t="n">
+        <v>0</v>
+      </c>
+      <c r="H60" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I60" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2281,9 +2639,15 @@
       <c r="F61" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>4226</t>
+      <c r="G61" t="n">
+        <v>4226</v>
+      </c>
+      <c r="H61" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>4474</t>
         </is>
       </c>
     </row>
@@ -2312,7 +2676,13 @@
       <c r="F62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G62" t="inlineStr">
+      <c r="G62" t="n">
+        <v>2609</v>
+      </c>
+      <c r="H62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I62" t="inlineStr">
         <is>
           <t>2609</t>
         </is>
@@ -2343,9 +2713,15 @@
       <c r="F63" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>3036</t>
+      <c r="G63" t="n">
+        <v>3036</v>
+      </c>
+      <c r="H63" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>3120</t>
         </is>
       </c>
     </row>
@@ -2374,9 +2750,15 @@
       <c r="F64" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>4035</t>
+      <c r="G64" t="n">
+        <v>4035</v>
+      </c>
+      <c r="H64" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>4145</t>
         </is>
       </c>
     </row>
@@ -2400,6 +2782,8 @@
       <c r="E65" t="inlineStr"/>
       <c r="F65" s="3" t="inlineStr"/>
       <c r="G65" t="inlineStr"/>
+      <c r="H65" s="3" t="inlineStr"/>
+      <c r="I65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -2426,9 +2810,15 @@
       <c r="F66" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>4271</t>
+      <c r="G66" t="n">
+        <v>4271</v>
+      </c>
+      <c r="H66" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>4446</t>
         </is>
       </c>
     </row>
@@ -2454,12 +2844,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F67" s="4" t="n">
+      <c r="F67" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>3666</t>
+      <c r="G67" t="n">
+        <v>3666</v>
+      </c>
+      <c r="H67" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>3891</t>
         </is>
       </c>
     </row>
@@ -2488,9 +2884,15 @@
       <c r="F68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>2547</t>
+      <c r="G68" t="n">
+        <v>2547</v>
+      </c>
+      <c r="H68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>2555</t>
         </is>
       </c>
     </row>
@@ -2519,9 +2921,15 @@
       <c r="F69" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>3704</t>
+      <c r="G69" t="n">
+        <v>3704</v>
+      </c>
+      <c r="H69" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>3740</t>
         </is>
       </c>
     </row>
@@ -2550,9 +2958,15 @@
       <c r="F70" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>3406</t>
+      <c r="G70" t="n">
+        <v>3406</v>
+      </c>
+      <c r="H70" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>3533</t>
         </is>
       </c>
     </row>
@@ -2581,9 +2995,15 @@
       <c r="F71" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>3614</t>
+      <c r="G71" t="n">
+        <v>3614</v>
+      </c>
+      <c r="H71" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>3688</t>
         </is>
       </c>
     </row>
@@ -2612,9 +3032,15 @@
       <c r="F72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>2664</t>
+      <c r="G72" t="n">
+        <v>2664</v>
+      </c>
+      <c r="H72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>2719</t>
         </is>
       </c>
     </row>
@@ -2643,9 +3069,15 @@
       <c r="F73" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>3363</t>
+      <c r="G73" t="n">
+        <v>3363</v>
+      </c>
+      <c r="H73" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>3522</t>
         </is>
       </c>
     </row>
@@ -2674,9 +3106,15 @@
       <c r="F74" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>3918</t>
+      <c r="G74" t="n">
+        <v>3918</v>
+      </c>
+      <c r="H74" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>4177</t>
         </is>
       </c>
     </row>
@@ -2702,12 +3140,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F75" s="5" t="n">
+      <c r="F75" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>4051</t>
+      <c r="G75" t="n">
+        <v>4051</v>
+      </c>
+      <c r="H75" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>4363</t>
         </is>
       </c>
     </row>
@@ -2731,6 +3175,8 @@
       <c r="E76" t="inlineStr"/>
       <c r="F76" s="3" t="inlineStr"/>
       <c r="G76" t="inlineStr"/>
+      <c r="H76" s="3" t="inlineStr"/>
+      <c r="I76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -2757,9 +3203,15 @@
       <c r="F77" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>4244</t>
+      <c r="G77" t="n">
+        <v>4244</v>
+      </c>
+      <c r="H77" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>4442</t>
         </is>
       </c>
     </row>
@@ -2788,7 +3240,13 @@
       <c r="F78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G78" t="inlineStr">
+      <c r="G78" t="n">
+        <v>2500</v>
+      </c>
+      <c r="H78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I78" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -2819,9 +3277,15 @@
       <c r="F79" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>3859</t>
+      <c r="G79" t="n">
+        <v>3859</v>
+      </c>
+      <c r="H79" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>4011</t>
         </is>
       </c>
     </row>
@@ -2847,12 +3311,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F80" s="4" t="n">
+      <c r="F80" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>3945</t>
+      <c r="G80" t="n">
+        <v>3945</v>
+      </c>
+      <c r="H80" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>4180</t>
         </is>
       </c>
     </row>
@@ -2878,12 +3348,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F81" s="4" t="n">
+      <c r="F81" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>4053</t>
+      <c r="G81" t="n">
+        <v>4053</v>
+      </c>
+      <c r="H81" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>4122</t>
         </is>
       </c>
     </row>
@@ -2912,9 +3388,15 @@
       <c r="F82" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>3638</t>
+      <c r="G82" t="n">
+        <v>3638</v>
+      </c>
+      <c r="H82" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>3815</t>
         </is>
       </c>
     </row>
@@ -2938,6 +3420,8 @@
       <c r="E83" t="inlineStr"/>
       <c r="F83" s="3" t="inlineStr"/>
       <c r="G83" t="inlineStr"/>
+      <c r="H83" s="3" t="inlineStr"/>
+      <c r="I83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -2961,12 +3445,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F84" s="5" t="n">
+      <c r="F84" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>2954</t>
+      <c r="G84" t="n">
+        <v>2954</v>
+      </c>
+      <c r="H84" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>3001</t>
         </is>
       </c>
     </row>
@@ -2995,9 +3485,15 @@
       <c r="F85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>2824</t>
+      <c r="G85" t="n">
+        <v>2824</v>
+      </c>
+      <c r="H85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>2819</t>
         </is>
       </c>
     </row>
@@ -3023,12 +3519,18 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F86" s="4" t="n">
+      <c r="F86" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>3929</t>
+      <c r="G86" t="n">
+        <v>3929</v>
+      </c>
+      <c r="H86" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>3982</t>
         </is>
       </c>
     </row>
@@ -3057,9 +3559,15 @@
       <c r="F87" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G87" t="inlineStr">
-        <is>
-          <t>2801</t>
+      <c r="G87" t="n">
+        <v>2801</v>
+      </c>
+      <c r="H87" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>2867</t>
         </is>
       </c>
     </row>
@@ -3088,9 +3596,15 @@
       <c r="F88" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G88" t="inlineStr">
-        <is>
-          <t>2975</t>
+      <c r="G88" t="n">
+        <v>2975</v>
+      </c>
+      <c r="H88" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>3155</t>
         </is>
       </c>
     </row>
@@ -3114,6 +3628,8 @@
       <c r="E89" t="inlineStr"/>
       <c r="F89" s="3" t="inlineStr"/>
       <c r="G89" t="inlineStr"/>
+      <c r="H89" s="3" t="inlineStr"/>
+      <c r="I89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -3140,9 +3656,15 @@
       <c r="F90" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>2724</t>
+      <c r="G90" t="n">
+        <v>2724</v>
+      </c>
+      <c r="H90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>2619</t>
         </is>
       </c>
     </row>
@@ -3166,6 +3688,8 @@
       <c r="E91" t="inlineStr"/>
       <c r="F91" s="3" t="inlineStr"/>
       <c r="G91" t="inlineStr"/>
+      <c r="H91" s="3" t="inlineStr"/>
+      <c r="I91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -3192,9 +3716,15 @@
       <c r="F92" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>2783</t>
+      <c r="G92" t="n">
+        <v>2783</v>
+      </c>
+      <c r="H92" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>2772</t>
         </is>
       </c>
     </row>
@@ -3223,9 +3753,15 @@
       <c r="F93" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>2751</t>
+      <c r="G93" t="n">
+        <v>2751</v>
+      </c>
+      <c r="H93" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>2829</t>
         </is>
       </c>
     </row>
@@ -3254,7 +3790,13 @@
       <c r="F94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G94" t="inlineStr">
+      <c r="G94" t="n">
+        <v>0</v>
+      </c>
+      <c r="H94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3285,9 +3827,15 @@
       <c r="F95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>2399</t>
+      <c r="G95" t="n">
+        <v>2399</v>
+      </c>
+      <c r="H95" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>2592</t>
         </is>
       </c>
     </row>
@@ -3316,9 +3864,15 @@
       <c r="F96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>2078</t>
+      <c r="G96" t="n">
+        <v>2078</v>
+      </c>
+      <c r="H96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>2087</t>
         </is>
       </c>
     </row>
@@ -3347,9 +3901,15 @@
       <c r="F97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>2553</t>
+      <c r="G97" t="n">
+        <v>2553</v>
+      </c>
+      <c r="H97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>2568</t>
         </is>
       </c>
     </row>
@@ -3378,9 +3938,15 @@
       <c r="F98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>2299</t>
+      <c r="G98" t="n">
+        <v>2299</v>
+      </c>
+      <c r="H98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>2284</t>
         </is>
       </c>
     </row>
@@ -3406,12 +3972,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F99" s="5" t="n">
+      <c r="F99" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="G99" t="inlineStr">
-        <is>
-          <t>3030</t>
+      <c r="G99" t="n">
+        <v>3030</v>
+      </c>
+      <c r="H99" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>3238</t>
         </is>
       </c>
     </row>
@@ -3437,12 +4009,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F100" s="5" t="n">
+      <c r="F100" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="G100" t="inlineStr">
-        <is>
-          <t>2383</t>
+      <c r="G100" t="n">
+        <v>2383</v>
+      </c>
+      <c r="H100" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>2447</t>
         </is>
       </c>
     </row>
@@ -3471,9 +4049,15 @@
       <c r="F101" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G101" t="inlineStr">
-        <is>
-          <t>3709</t>
+      <c r="G101" t="n">
+        <v>3709</v>
+      </c>
+      <c r="H101" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>3823</t>
         </is>
       </c>
     </row>
@@ -3502,9 +4086,15 @@
       <c r="F102" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G102" t="inlineStr">
-        <is>
-          <t>3335</t>
+      <c r="G102" t="n">
+        <v>3335</v>
+      </c>
+      <c r="H102" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>3513</t>
         </is>
       </c>
     </row>
@@ -3533,9 +4123,15 @@
       <c r="F103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G103" t="inlineStr">
-        <is>
-          <t>2864</t>
+      <c r="G103" t="n">
+        <v>2864</v>
+      </c>
+      <c r="H103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>2847</t>
         </is>
       </c>
     </row>
@@ -3564,9 +4160,15 @@
       <c r="F104" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G104" t="inlineStr">
-        <is>
-          <t>3736</t>
+      <c r="G104" t="n">
+        <v>3736</v>
+      </c>
+      <c r="H104" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>3858</t>
         </is>
       </c>
     </row>
@@ -3592,12 +4194,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F105" s="5" t="n">
+      <c r="F105" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="G105" t="inlineStr">
-        <is>
-          <t>3335</t>
+      <c r="G105" t="n">
+        <v>3335</v>
+      </c>
+      <c r="H105" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>3444</t>
         </is>
       </c>
     </row>
@@ -3626,9 +4234,15 @@
       <c r="F106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G106" t="inlineStr">
-        <is>
-          <t>2447</t>
+      <c r="G106" t="n">
+        <v>2447</v>
+      </c>
+      <c r="H106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>2428</t>
         </is>
       </c>
     </row>
@@ -3657,9 +4271,15 @@
       <c r="F107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G107" t="inlineStr">
-        <is>
-          <t>2614</t>
+      <c r="G107" t="n">
+        <v>2614</v>
+      </c>
+      <c r="H107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>2642</t>
         </is>
       </c>
     </row>
@@ -3688,9 +4308,15 @@
       <c r="F108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G108" t="inlineStr">
-        <is>
-          <t>2563</t>
+      <c r="G108" t="n">
+        <v>2563</v>
+      </c>
+      <c r="H108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>2592</t>
         </is>
       </c>
     </row>
@@ -3719,9 +4345,15 @@
       <c r="F109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G109" t="inlineStr">
-        <is>
-          <t>3318</t>
+      <c r="G109" t="n">
+        <v>3318</v>
+      </c>
+      <c r="H109" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>3395</t>
         </is>
       </c>
     </row>
@@ -3750,9 +4382,15 @@
       <c r="F110" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="G110" t="inlineStr">
-        <is>
-          <t>3235</t>
+      <c r="G110" t="n">
+        <v>3235</v>
+      </c>
+      <c r="H110" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>3289</t>
         </is>
       </c>
     </row>
@@ -3781,9 +4419,15 @@
       <c r="F111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G111" t="inlineStr">
-        <is>
-          <t>2638</t>
+      <c r="G111" t="n">
+        <v>2638</v>
+      </c>
+      <c r="H111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>2693</t>
         </is>
       </c>
     </row>
@@ -3812,9 +4456,15 @@
       <c r="F112" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G112" t="inlineStr">
-        <is>
-          <t>2715</t>
+      <c r="G112" t="n">
+        <v>2715</v>
+      </c>
+      <c r="H112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>2720</t>
         </is>
       </c>
     </row>
@@ -3840,12 +4490,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F113" s="5" t="n">
+      <c r="F113" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="G113" t="inlineStr">
-        <is>
-          <t>2996</t>
+      <c r="G113" t="n">
+        <v>2996</v>
+      </c>
+      <c r="H113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>3010</t>
         </is>
       </c>
     </row>
@@ -3874,9 +4530,15 @@
       <c r="F114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G114" t="inlineStr">
-        <is>
-          <t>3020</t>
+      <c r="G114" t="n">
+        <v>3020</v>
+      </c>
+      <c r="H114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>3412</t>
         </is>
       </c>
     </row>
@@ -3905,11 +4567,11 @@
       <c r="F115" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G115" t="inlineStr">
-        <is>
-          <t>3624</t>
-        </is>
-      </c>
+      <c r="G115" t="n">
+        <v>3624</v>
+      </c>
+      <c r="H115" s="3" t="inlineStr"/>
+      <c r="I115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -3933,12 +4595,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F116" s="5" t="n">
+      <c r="F116" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="G116" t="inlineStr">
-        <is>
-          <t>2544</t>
+      <c r="G116" t="n">
+        <v>2544</v>
+      </c>
+      <c r="H116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>2527</t>
         </is>
       </c>
     </row>
@@ -3964,12 +4632,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F117" s="5" t="n">
+      <c r="F117" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="G117" t="inlineStr">
-        <is>
-          <t>2869</t>
+      <c r="G117" t="n">
+        <v>2869</v>
+      </c>
+      <c r="H117" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>2950</t>
         </is>
       </c>
     </row>
@@ -3998,9 +4672,15 @@
       <c r="F118" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G118" t="inlineStr">
-        <is>
-          <t>3166</t>
+      <c r="G118" t="n">
+        <v>3166</v>
+      </c>
+      <c r="H118" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>3170</t>
         </is>
       </c>
     </row>
@@ -4029,7 +4709,13 @@
       <c r="F119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G119" t="inlineStr">
+      <c r="G119" t="n">
+        <v>0</v>
+      </c>
+      <c r="H119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I119" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4060,9 +4746,15 @@
       <c r="F120" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G120" t="inlineStr">
-        <is>
-          <t>3322</t>
+      <c r="G120" t="n">
+        <v>3322</v>
+      </c>
+      <c r="H120" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>3415</t>
         </is>
       </c>
     </row>
@@ -4091,9 +4783,15 @@
       <c r="F121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G121" t="inlineStr">
-        <is>
-          <t>2665</t>
+      <c r="G121" t="n">
+        <v>2665</v>
+      </c>
+      <c r="H121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>2659</t>
         </is>
       </c>
     </row>
@@ -4122,9 +4820,15 @@
       <c r="F122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G122" t="inlineStr">
-        <is>
-          <t>2821</t>
+      <c r="G122" t="n">
+        <v>2821</v>
+      </c>
+      <c r="H122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>2850</t>
         </is>
       </c>
     </row>
@@ -4153,9 +4857,15 @@
       <c r="F123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G123" t="inlineStr">
-        <is>
-          <t>2472</t>
+      <c r="G123" t="n">
+        <v>2472</v>
+      </c>
+      <c r="H123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>2483</t>
         </is>
       </c>
     </row>
@@ -4181,12 +4891,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F124" s="5" t="n">
+      <c r="F124" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="G124" t="inlineStr">
-        <is>
-          <t>2954</t>
+      <c r="G124" t="n">
+        <v>2954</v>
+      </c>
+      <c r="H124" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>2972</t>
         </is>
       </c>
     </row>
@@ -4215,9 +4931,15 @@
       <c r="F125" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G125" t="inlineStr">
-        <is>
-          <t>2971</t>
+      <c r="G125" t="n">
+        <v>2971</v>
+      </c>
+      <c r="H125" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="I125" t="inlineStr">
+        <is>
+          <t>2988</t>
         </is>
       </c>
     </row>
@@ -4246,9 +4968,15 @@
       <c r="F126" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G126" t="inlineStr">
-        <is>
-          <t>3254</t>
+      <c r="G126" t="n">
+        <v>3254</v>
+      </c>
+      <c r="H126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>3223</t>
         </is>
       </c>
     </row>
@@ -4277,9 +5005,15 @@
       <c r="F127" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G127" t="inlineStr">
-        <is>
-          <t>3016</t>
+      <c r="G127" t="n">
+        <v>3016</v>
+      </c>
+      <c r="H127" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I127" t="inlineStr">
+        <is>
+          <t>3036</t>
         </is>
       </c>
     </row>
@@ -4308,7 +5042,13 @@
       <c r="F128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G128" t="inlineStr">
+      <c r="G128" t="n">
+        <v>0</v>
+      </c>
+      <c r="H128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4339,7 +5079,13 @@
       <c r="F129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G129" t="inlineStr">
+      <c r="G129" t="n">
+        <v>0</v>
+      </c>
+      <c r="H129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4370,9 +5116,15 @@
       <c r="F130" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G130" t="inlineStr">
-        <is>
-          <t>2825</t>
+      <c r="G130" t="n">
+        <v>2825</v>
+      </c>
+      <c r="H130" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I130" t="inlineStr">
+        <is>
+          <t>2863</t>
         </is>
       </c>
     </row>
@@ -4401,9 +5153,15 @@
       <c r="F131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G131" t="inlineStr">
-        <is>
-          <t>2661</t>
+      <c r="G131" t="n">
+        <v>2661</v>
+      </c>
+      <c r="H131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I131" t="inlineStr">
+        <is>
+          <t>2679</t>
         </is>
       </c>
     </row>
@@ -4432,7 +5190,13 @@
       <c r="F132" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G132" t="inlineStr">
+      <c r="G132" t="n">
+        <v>0</v>
+      </c>
+      <c r="H132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I132" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4460,12 +5224,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F133" s="5" t="n">
+      <c r="F133" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="G133" t="inlineStr">
-        <is>
-          <t>2108</t>
+      <c r="G133" t="n">
+        <v>2108</v>
+      </c>
+      <c r="H133" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="I133" t="inlineStr">
+        <is>
+          <t>2196</t>
         </is>
       </c>
     </row>
@@ -4494,9 +5264,15 @@
       <c r="F134" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G134" t="inlineStr">
-        <is>
-          <t>3072</t>
+      <c r="G134" t="n">
+        <v>3072</v>
+      </c>
+      <c r="H134" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I134" t="inlineStr">
+        <is>
+          <t>3059</t>
         </is>
       </c>
     </row>
@@ -4525,7 +5301,13 @@
       <c r="F135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G135" t="inlineStr">
+      <c r="G135" t="n">
+        <v>0</v>
+      </c>
+      <c r="H135" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I135" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4556,9 +5338,15 @@
       <c r="F136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G136" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G136" t="n">
+        <v>0</v>
+      </c>
+      <c r="H136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I136" t="inlineStr">
+        <is>
+          <t>999</t>
         </is>
       </c>
     </row>
@@ -4587,7 +5375,13 @@
       <c r="F137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G137" t="inlineStr">
+      <c r="G137" t="n">
+        <v>0</v>
+      </c>
+      <c r="H137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4618,9 +5412,15 @@
       <c r="F138" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G138" t="inlineStr">
-        <is>
-          <t>2975</t>
+      <c r="G138" t="n">
+        <v>2975</v>
+      </c>
+      <c r="H138" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="I138" t="inlineStr">
+        <is>
+          <t>3038</t>
         </is>
       </c>
     </row>
@@ -4649,7 +5449,13 @@
       <c r="F139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G139" t="inlineStr">
+      <c r="G139" t="n">
+        <v>0</v>
+      </c>
+      <c r="H139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I139" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4677,12 +5483,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F140" s="5" t="n">
+      <c r="F140" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="G140" t="inlineStr">
-        <is>
-          <t>2636</t>
+      <c r="G140" t="n">
+        <v>2636</v>
+      </c>
+      <c r="H140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I140" t="inlineStr">
+        <is>
+          <t>2605</t>
         </is>
       </c>
     </row>
@@ -4711,7 +5523,13 @@
       <c r="F141" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G141" t="inlineStr">
+      <c r="G141" t="n">
+        <v>0</v>
+      </c>
+      <c r="H141" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I141" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4742,9 +5560,15 @@
       <c r="F142" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G142" t="inlineStr">
-        <is>
-          <t>2789</t>
+      <c r="G142" t="n">
+        <v>2789</v>
+      </c>
+      <c r="H142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I142" t="inlineStr">
+        <is>
+          <t>2741</t>
         </is>
       </c>
     </row>
@@ -4768,6 +5592,8 @@
       <c r="E143" t="inlineStr"/>
       <c r="F143" s="3" t="inlineStr"/>
       <c r="G143" t="inlineStr"/>
+      <c r="H143" s="3" t="inlineStr"/>
+      <c r="I143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -4794,9 +5620,15 @@
       <c r="F144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G144" t="inlineStr">
-        <is>
-          <t>2494</t>
+      <c r="G144" t="n">
+        <v>2494</v>
+      </c>
+      <c r="H144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I144" t="inlineStr">
+        <is>
+          <t>2466</t>
         </is>
       </c>
     </row>
@@ -4825,7 +5657,13 @@
       <c r="F145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G145" t="inlineStr">
+      <c r="G145" t="n">
+        <v>0</v>
+      </c>
+      <c r="H145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I145" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4856,7 +5694,13 @@
       <c r="F146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G146" t="inlineStr">
+      <c r="G146" t="n">
+        <v>0</v>
+      </c>
+      <c r="H146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4887,7 +5731,13 @@
       <c r="F147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G147" t="inlineStr">
+      <c r="G147" t="n">
+        <v>0</v>
+      </c>
+      <c r="H147" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I147" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4918,7 +5768,13 @@
       <c r="F148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G148" t="inlineStr">
+      <c r="G148" t="n">
+        <v>0</v>
+      </c>
+      <c r="H148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4949,7 +5805,13 @@
       <c r="F149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G149" t="inlineStr">
+      <c r="G149" t="n">
+        <v>0</v>
+      </c>
+      <c r="H149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I149" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4977,12 +5839,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F150" s="5" t="n">
+      <c r="F150" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="G150" t="inlineStr">
-        <is>
-          <t>2346</t>
+      <c r="G150" t="n">
+        <v>2346</v>
+      </c>
+      <c r="H150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I150" t="inlineStr">
+        <is>
+          <t>2385</t>
         </is>
       </c>
     </row>
@@ -5011,7 +5879,13 @@
       <c r="F151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G151" t="inlineStr">
+      <c r="G151" t="n">
+        <v>0</v>
+      </c>
+      <c r="H151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I151" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5042,9 +5916,15 @@
       <c r="F152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G152" t="inlineStr">
-        <is>
-          <t>1611</t>
+      <c r="G152" t="n">
+        <v>1611</v>
+      </c>
+      <c r="H152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I152" t="inlineStr">
+        <is>
+          <t>1604</t>
         </is>
       </c>
     </row>
@@ -5070,12 +5950,18 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F153" s="5" t="n">
+      <c r="F153" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G153" t="inlineStr">
-        <is>
-          <t>1825</t>
+      <c r="G153" t="n">
+        <v>1825</v>
+      </c>
+      <c r="H153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I153" t="inlineStr">
+        <is>
+          <t>1829</t>
         </is>
       </c>
     </row>
@@ -5104,7 +5990,13 @@
       <c r="F154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G154" t="inlineStr">
+      <c r="G154" t="n">
+        <v>0</v>
+      </c>
+      <c r="H154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5132,12 +6024,18 @@
           <t>Chinese</t>
         </is>
       </c>
-      <c r="F155" s="5" t="n">
+      <c r="F155" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G155" t="inlineStr">
-        <is>
-          <t>3738</t>
+      <c r="G155" t="n">
+        <v>3738</v>
+      </c>
+      <c r="H155" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="I155" t="inlineStr">
+        <is>
+          <t>3926</t>
         </is>
       </c>
     </row>
@@ -5166,7 +6064,13 @@
       <c r="F156" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G156" t="inlineStr">
+      <c r="G156" t="n">
+        <v>0</v>
+      </c>
+      <c r="H156" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I156" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5197,7 +6101,13 @@
       <c r="F157" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G157" t="inlineStr">
+      <c r="G157" t="n">
+        <v>0</v>
+      </c>
+      <c r="H157" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I157" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5225,12 +6135,18 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F158" s="4" t="n">
+      <c r="F158" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="G158" t="inlineStr">
-        <is>
-          <t>4479</t>
+      <c r="G158" t="n">
+        <v>4479</v>
+      </c>
+      <c r="H158" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="I158" t="inlineStr">
+        <is>
+          <t>4733</t>
         </is>
       </c>
     </row>
@@ -5259,7 +6175,13 @@
       <c r="F159" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G159" t="inlineStr">
+      <c r="G159" t="n">
+        <v>0</v>
+      </c>
+      <c r="H159" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I159" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5290,9 +6212,15 @@
       <c r="F160" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G160" t="inlineStr">
-        <is>
-          <t>2791</t>
+      <c r="G160" t="n">
+        <v>2791</v>
+      </c>
+      <c r="H160" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I160" t="inlineStr">
+        <is>
+          <t>2808</t>
         </is>
       </c>
     </row>
@@ -5321,7 +6249,13 @@
       <c r="F161" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G161" t="inlineStr">
+      <c r="G161" t="n">
+        <v>0</v>
+      </c>
+      <c r="H161" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I161" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5352,9 +6286,15 @@
       <c r="F162" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G162" t="inlineStr">
-        <is>
-          <t>2759</t>
+      <c r="G162" t="n">
+        <v>2759</v>
+      </c>
+      <c r="H162" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I162" t="inlineStr">
+        <is>
+          <t>2853</t>
         </is>
       </c>
     </row>
@@ -5378,12 +6318,12 @@
       <c r="E163" t="inlineStr"/>
       <c r="F163" s="3" t="inlineStr"/>
       <c r="G163" t="inlineStr"/>
+      <c r="H163" s="3" t="inlineStr"/>
+      <c r="I163" t="inlineStr"/>
     </row>
     <row r="164">
-      <c r="A164" t="inlineStr">
-        <is>
-          <t>1304123</t>
-        </is>
+      <c r="A164" t="n">
+        <v>1304123</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
@@ -5400,17 +6340,21 @@
       <c r="F164" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G164" t="inlineStr">
-        <is>
-          <t>2424</t>
+      <c r="G164" t="n">
+        <v>2424</v>
+      </c>
+      <c r="H164" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="I164" t="inlineStr">
+        <is>
+          <t>2618</t>
         </is>
       </c>
     </row>
     <row r="165">
-      <c r="A165" t="inlineStr">
-        <is>
-          <t>58605234</t>
-        </is>
+      <c r="A165" t="n">
+        <v>58605234</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>
@@ -5427,17 +6371,21 @@
       <c r="F165" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G165" t="inlineStr">
-        <is>
-          <t>2292</t>
+      <c r="G165" t="n">
+        <v>2292</v>
+      </c>
+      <c r="H165" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="I165" t="inlineStr">
+        <is>
+          <t>2313</t>
         </is>
       </c>
     </row>
     <row r="166">
-      <c r="A166" t="inlineStr">
-        <is>
-          <t>58739336</t>
-        </is>
+      <c r="A166" t="n">
+        <v>58739336</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>
@@ -5454,17 +6402,21 @@
       <c r="F166" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G166" t="inlineStr">
-        <is>
-          <t>2255</t>
+      <c r="G166" t="n">
+        <v>2255</v>
+      </c>
+      <c r="H166" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I166" t="inlineStr">
+        <is>
+          <t>2399</t>
         </is>
       </c>
     </row>
     <row r="167">
-      <c r="A167" t="inlineStr">
-        <is>
-          <t>58739866</t>
-        </is>
+      <c r="A167" t="n">
+        <v>58739866</v>
       </c>
       <c r="B167" t="inlineStr">
         <is>
@@ -5481,9 +6433,44 @@
       <c r="F167" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G167" t="inlineStr">
-        <is>
-          <t>1485</t>
+      <c r="G167" t="n">
+        <v>1485</v>
+      </c>
+      <c r="H167" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I167" t="inlineStr">
+        <is>
+          <t>1429</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>58766144</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>EquablePrecedence38</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr"/>
+      <c r="D168" t="inlineStr"/>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F168" s="3" t="inlineStr"/>
+      <c r="G168" t="inlineStr"/>
+      <c r="H168" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I168" t="inlineStr">
+        <is>
+          <t>1535</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-02-06 11:30:33
</commit_message>
<xml_diff>
--- a/Season_Attack/83.xlsx
+++ b/Season_Attack/83.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I168"/>
+  <dimension ref="A1:K168"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,6 +436,16 @@
           <t>02-04_0</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>02-05_A</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>02-05_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -468,9 +478,15 @@
       <c r="H2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>3456</t>
+      <c r="I2" t="n">
+        <v>3456</v>
+      </c>
+      <c r="J2" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>3672</t>
         </is>
       </c>
     </row>
@@ -505,9 +521,15 @@
       <c r="H3" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>4667</t>
+      <c r="I3" t="n">
+        <v>4667</v>
+      </c>
+      <c r="J3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>5060</t>
         </is>
       </c>
     </row>
@@ -542,9 +564,15 @@
       <c r="H4" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>4553</t>
+      <c r="I4" t="n">
+        <v>4553</v>
+      </c>
+      <c r="J4" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>4773</t>
         </is>
       </c>
     </row>
@@ -567,7 +595,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F5" s="3" t="n">
@@ -579,9 +607,15 @@
       <c r="H5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>4652</t>
+      <c r="I5" t="n">
+        <v>4652</v>
+      </c>
+      <c r="J5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>4982</t>
         </is>
       </c>
     </row>
@@ -616,9 +650,15 @@
       <c r="H6" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>4624</t>
+      <c r="I6" t="n">
+        <v>4624</v>
+      </c>
+      <c r="J6" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>4893</t>
         </is>
       </c>
     </row>
@@ -653,9 +693,15 @@
       <c r="H7" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>5062</t>
+      <c r="I7" t="n">
+        <v>5062</v>
+      </c>
+      <c r="J7" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>5384</t>
         </is>
       </c>
     </row>
@@ -690,9 +736,15 @@
       <c r="H8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>4401</t>
+      <c r="I8" t="n">
+        <v>4401</v>
+      </c>
+      <c r="J8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>4548</t>
         </is>
       </c>
     </row>
@@ -726,6 +778,8 @@
       </c>
       <c r="H9" s="3" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
+      <c r="J9" s="3" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -758,9 +812,15 @@
       <c r="H10" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>4290</t>
+      <c r="I10" t="n">
+        <v>4290</v>
+      </c>
+      <c r="J10" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>4510</t>
         </is>
       </c>
     </row>
@@ -795,9 +855,15 @@
       <c r="H11" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>4447</t>
+      <c r="I11" t="n">
+        <v>4447</v>
+      </c>
+      <c r="J11" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>4702</t>
         </is>
       </c>
     </row>
@@ -832,9 +898,15 @@
       <c r="H12" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>4103</t>
+      <c r="I12" t="n">
+        <v>4103</v>
+      </c>
+      <c r="J12" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>4288</t>
         </is>
       </c>
     </row>
@@ -869,9 +941,15 @@
       <c r="H13" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>2686</t>
+      <c r="I13" t="n">
+        <v>2686</v>
+      </c>
+      <c r="J13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>2716</t>
         </is>
       </c>
     </row>
@@ -906,9 +984,15 @@
       <c r="H14" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>5299</t>
+      <c r="I14" t="n">
+        <v>5299</v>
+      </c>
+      <c r="J14" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>5621</t>
         </is>
       </c>
     </row>
@@ -943,9 +1027,15 @@
       <c r="H15" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>4457</t>
+      <c r="I15" t="n">
+        <v>4457</v>
+      </c>
+      <c r="J15" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>4779</t>
         </is>
       </c>
     </row>
@@ -980,9 +1070,15 @@
       <c r="H16" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>4635</t>
+      <c r="I16" t="n">
+        <v>4635</v>
+      </c>
+      <c r="J16" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>4759</t>
         </is>
       </c>
     </row>
@@ -1017,9 +1113,15 @@
       <c r="H17" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>3930</t>
+      <c r="I17" t="n">
+        <v>3930</v>
+      </c>
+      <c r="J17" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>4204</t>
         </is>
       </c>
     </row>
@@ -1054,9 +1156,15 @@
       <c r="H18" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>4053</t>
+      <c r="I18" t="n">
+        <v>4053</v>
+      </c>
+      <c r="J18" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>4283</t>
         </is>
       </c>
     </row>
@@ -1079,7 +1187,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F19" s="3" t="n">
@@ -1091,9 +1199,15 @@
       <c r="H19" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>4549</t>
+      <c r="I19" t="n">
+        <v>4549</v>
+      </c>
+      <c r="J19" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>4814</t>
         </is>
       </c>
     </row>
@@ -1128,9 +1242,15 @@
       <c r="H20" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>5249</t>
+      <c r="I20" t="n">
+        <v>5249</v>
+      </c>
+      <c r="J20" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>5624</t>
         </is>
       </c>
     </row>
@@ -1165,7 +1285,13 @@
       <c r="H21" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I21" t="inlineStr">
+      <c r="I21" t="n">
+        <v>3411</v>
+      </c>
+      <c r="J21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" t="inlineStr">
         <is>
           <t>3411</t>
         </is>
@@ -1202,9 +1328,15 @@
       <c r="H22" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>4580</t>
+      <c r="I22" t="n">
+        <v>4580</v>
+      </c>
+      <c r="J22" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>4771</t>
         </is>
       </c>
     </row>
@@ -1239,9 +1371,15 @@
       <c r="H23" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>3826</t>
+      <c r="I23" t="n">
+        <v>3826</v>
+      </c>
+      <c r="J23" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>4183</t>
         </is>
       </c>
     </row>
@@ -1276,9 +1414,15 @@
       <c r="H24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>4701</t>
+      <c r="I24" t="n">
+        <v>4701</v>
+      </c>
+      <c r="J24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>4815</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1457,13 @@
       <c r="H25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I25" t="inlineStr">
+      <c r="I25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1350,9 +1500,15 @@
       <c r="H26" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>4815</t>
+      <c r="I26" t="n">
+        <v>4815</v>
+      </c>
+      <c r="J26" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>5109</t>
         </is>
       </c>
     </row>
@@ -1387,9 +1543,15 @@
       <c r="H27" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>4948</t>
+      <c r="I27" t="n">
+        <v>4948</v>
+      </c>
+      <c r="J27" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>5211</t>
         </is>
       </c>
     </row>
@@ -1424,9 +1586,15 @@
       <c r="H28" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>3803</t>
+      <c r="I28" t="n">
+        <v>3803</v>
+      </c>
+      <c r="J28" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>3902</t>
         </is>
       </c>
     </row>
@@ -1461,9 +1629,15 @@
       <c r="H29" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>5198</t>
+      <c r="I29" t="n">
+        <v>5198</v>
+      </c>
+      <c r="J29" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>5486</t>
         </is>
       </c>
     </row>
@@ -1498,9 +1672,15 @@
       <c r="H30" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>4872</t>
+      <c r="I30" t="n">
+        <v>4872</v>
+      </c>
+      <c r="J30" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>4987</t>
         </is>
       </c>
     </row>
@@ -1535,9 +1715,15 @@
       <c r="H31" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>4245</t>
+      <c r="I31" t="n">
+        <v>4245</v>
+      </c>
+      <c r="J31" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>4735</t>
         </is>
       </c>
     </row>
@@ -1572,9 +1758,15 @@
       <c r="H32" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>5072</t>
+      <c r="I32" t="n">
+        <v>5072</v>
+      </c>
+      <c r="J32" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>5324</t>
         </is>
       </c>
     </row>
@@ -1609,9 +1801,15 @@
       <c r="H33" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>4908</t>
+      <c r="I33" t="n">
+        <v>4908</v>
+      </c>
+      <c r="J33" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>5180</t>
         </is>
       </c>
     </row>
@@ -1646,9 +1844,15 @@
       <c r="H34" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="I34" t="inlineStr">
-        <is>
-          <t>4727</t>
+      <c r="I34" t="n">
+        <v>4727</v>
+      </c>
+      <c r="J34" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>4905</t>
         </is>
       </c>
     </row>
@@ -1671,7 +1875,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F35" s="5" t="n">
@@ -1683,9 +1887,15 @@
       <c r="H35" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>4897</t>
+      <c r="I35" t="n">
+        <v>4897</v>
+      </c>
+      <c r="J35" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>5253</t>
         </is>
       </c>
     </row>
@@ -1720,9 +1930,15 @@
       <c r="H36" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>4635</t>
+      <c r="I36" t="n">
+        <v>4635</v>
+      </c>
+      <c r="J36" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>4763</t>
         </is>
       </c>
     </row>
@@ -1757,9 +1973,15 @@
       <c r="H37" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>4321</t>
+      <c r="I37" t="n">
+        <v>4321</v>
+      </c>
+      <c r="J37" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>4429</t>
         </is>
       </c>
     </row>
@@ -1794,9 +2016,15 @@
       <c r="H38" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>4613</t>
+      <c r="I38" t="n">
+        <v>4613</v>
+      </c>
+      <c r="J38" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>4788</t>
         </is>
       </c>
     </row>
@@ -1831,9 +2059,15 @@
       <c r="H39" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>4260</t>
+      <c r="I39" t="n">
+        <v>4260</v>
+      </c>
+      <c r="J39" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>4580</t>
         </is>
       </c>
     </row>
@@ -1868,9 +2102,15 @@
       <c r="H40" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>5223</t>
+      <c r="I40" t="n">
+        <v>5223</v>
+      </c>
+      <c r="J40" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>5450</t>
         </is>
       </c>
     </row>
@@ -1905,9 +2145,15 @@
       <c r="H41" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I41" t="inlineStr">
-        <is>
-          <t>4545</t>
+      <c r="I41" t="n">
+        <v>4545</v>
+      </c>
+      <c r="J41" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>4800</t>
         </is>
       </c>
     </row>
@@ -1942,9 +2188,15 @@
       <c r="H42" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>5071</t>
+      <c r="I42" t="n">
+        <v>5071</v>
+      </c>
+      <c r="J42" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>5448</t>
         </is>
       </c>
     </row>
@@ -1979,9 +2231,15 @@
       <c r="H43" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>4608</t>
+      <c r="I43" t="n">
+        <v>4608</v>
+      </c>
+      <c r="J43" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>4863</t>
         </is>
       </c>
     </row>
@@ -2016,9 +2274,15 @@
       <c r="H44" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>4707</t>
+      <c r="I44" t="n">
+        <v>4707</v>
+      </c>
+      <c r="J44" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>4736</t>
         </is>
       </c>
     </row>
@@ -2053,9 +2317,15 @@
       <c r="H45" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="I45" t="inlineStr">
-        <is>
-          <t>4249</t>
+      <c r="I45" t="n">
+        <v>4249</v>
+      </c>
+      <c r="J45" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>4361</t>
         </is>
       </c>
     </row>
@@ -2090,9 +2360,15 @@
       <c r="H46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I46" t="inlineStr">
-        <is>
-          <t>4142</t>
+      <c r="I46" t="n">
+        <v>4142</v>
+      </c>
+      <c r="J46" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>4372</t>
         </is>
       </c>
     </row>
@@ -2127,9 +2403,15 @@
       <c r="H47" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I47" t="inlineStr">
-        <is>
-          <t>3037</t>
+      <c r="I47" t="n">
+        <v>3037</v>
+      </c>
+      <c r="J47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>3036</t>
         </is>
       </c>
     </row>
@@ -2152,7 +2434,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F48" s="5" t="n">
@@ -2164,9 +2446,15 @@
       <c r="H48" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>4682</t>
+      <c r="I48" t="n">
+        <v>4682</v>
+      </c>
+      <c r="J48" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>4995</t>
         </is>
       </c>
     </row>
@@ -2201,9 +2489,15 @@
       <c r="H49" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="I49" t="inlineStr">
-        <is>
-          <t>3888</t>
+      <c r="I49" t="n">
+        <v>3888</v>
+      </c>
+      <c r="J49" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>4006</t>
         </is>
       </c>
     </row>
@@ -2238,9 +2532,15 @@
       <c r="H50" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="I50" t="inlineStr">
-        <is>
-          <t>4991</t>
+      <c r="I50" t="n">
+        <v>4991</v>
+      </c>
+      <c r="J50" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>5242</t>
         </is>
       </c>
     </row>
@@ -2275,9 +2575,15 @@
       <c r="H51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I51" t="inlineStr">
-        <is>
-          <t>2782</t>
+      <c r="I51" t="n">
+        <v>2782</v>
+      </c>
+      <c r="J51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>2796</t>
         </is>
       </c>
     </row>
@@ -2312,9 +2618,15 @@
       <c r="H52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>2711</t>
+      <c r="I52" t="n">
+        <v>2711</v>
+      </c>
+      <c r="J52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>2709</t>
         </is>
       </c>
     </row>
@@ -2349,9 +2661,15 @@
       <c r="H53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I53" t="inlineStr">
-        <is>
-          <t>2902</t>
+      <c r="I53" t="n">
+        <v>2902</v>
+      </c>
+      <c r="J53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>2958</t>
         </is>
       </c>
     </row>
@@ -2386,9 +2704,15 @@
       <c r="H54" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I54" t="inlineStr">
-        <is>
-          <t>4627</t>
+      <c r="I54" t="n">
+        <v>4627</v>
+      </c>
+      <c r="J54" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>4854</t>
         </is>
       </c>
     </row>
@@ -2423,9 +2747,15 @@
       <c r="H55" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="I55" t="inlineStr">
-        <is>
-          <t>3677</t>
+      <c r="I55" t="n">
+        <v>3677</v>
+      </c>
+      <c r="J55" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>3813</t>
         </is>
       </c>
     </row>
@@ -2460,9 +2790,15 @@
       <c r="H56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I56" t="inlineStr">
-        <is>
-          <t>3818</t>
+      <c r="I56" t="n">
+        <v>3818</v>
+      </c>
+      <c r="J56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>3911</t>
         </is>
       </c>
     </row>
@@ -2497,9 +2833,15 @@
       <c r="H57" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="I57" t="inlineStr">
-        <is>
-          <t>4300</t>
+      <c r="I57" t="n">
+        <v>4300</v>
+      </c>
+      <c r="J57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>4532</t>
         </is>
       </c>
     </row>
@@ -2534,9 +2876,15 @@
       <c r="H58" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="I58" t="inlineStr">
-        <is>
-          <t>3822</t>
+      <c r="I58" t="n">
+        <v>3822</v>
+      </c>
+      <c r="J58" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>3910</t>
         </is>
       </c>
     </row>
@@ -2571,9 +2919,15 @@
       <c r="H59" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I59" t="inlineStr">
-        <is>
-          <t>4296</t>
+      <c r="I59" t="n">
+        <v>4296</v>
+      </c>
+      <c r="J59" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>4412</t>
         </is>
       </c>
     </row>
@@ -2608,7 +2962,13 @@
       <c r="H60" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I60" t="inlineStr">
+      <c r="I60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J60" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K60" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2645,9 +3005,15 @@
       <c r="H61" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="I61" t="inlineStr">
-        <is>
-          <t>4474</t>
+      <c r="I61" t="n">
+        <v>4474</v>
+      </c>
+      <c r="J61" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>4627</t>
         </is>
       </c>
     </row>
@@ -2682,7 +3048,13 @@
       <c r="H62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I62" t="inlineStr">
+      <c r="I62" t="n">
+        <v>2609</v>
+      </c>
+      <c r="J62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K62" t="inlineStr">
         <is>
           <t>2609</t>
         </is>
@@ -2719,9 +3091,15 @@
       <c r="H63" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="I63" t="inlineStr">
-        <is>
-          <t>3120</t>
+      <c r="I63" t="n">
+        <v>3120</v>
+      </c>
+      <c r="J63" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>3110</t>
         </is>
       </c>
     </row>
@@ -2756,9 +3134,15 @@
       <c r="H64" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="I64" t="inlineStr">
-        <is>
-          <t>4145</t>
+      <c r="I64" t="n">
+        <v>4145</v>
+      </c>
+      <c r="J64" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>4393</t>
         </is>
       </c>
     </row>
@@ -2784,6 +3168,8 @@
       <c r="G65" t="inlineStr"/>
       <c r="H65" s="3" t="inlineStr"/>
       <c r="I65" t="inlineStr"/>
+      <c r="J65" s="3" t="inlineStr"/>
+      <c r="K65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -2816,9 +3202,15 @@
       <c r="H66" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="I66" t="inlineStr">
-        <is>
-          <t>4446</t>
+      <c r="I66" t="n">
+        <v>4446</v>
+      </c>
+      <c r="J66" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>4747</t>
         </is>
       </c>
     </row>
@@ -2853,9 +3245,15 @@
       <c r="H67" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="I67" t="inlineStr">
-        <is>
-          <t>3891</t>
+      <c r="I67" t="n">
+        <v>3891</v>
+      </c>
+      <c r="J67" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>3989</t>
         </is>
       </c>
     </row>
@@ -2890,7 +3288,13 @@
       <c r="H68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I68" t="inlineStr">
+      <c r="I68" t="n">
+        <v>2555</v>
+      </c>
+      <c r="J68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K68" t="inlineStr">
         <is>
           <t>2555</t>
         </is>
@@ -2927,9 +3331,15 @@
       <c r="H69" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="I69" t="inlineStr">
-        <is>
-          <t>3740</t>
+      <c r="I69" t="n">
+        <v>3740</v>
+      </c>
+      <c r="J69" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>3741</t>
         </is>
       </c>
     </row>
@@ -2964,9 +3374,15 @@
       <c r="H70" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="I70" t="inlineStr">
-        <is>
-          <t>3533</t>
+      <c r="I70" t="n">
+        <v>3533</v>
+      </c>
+      <c r="J70" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>3624</t>
         </is>
       </c>
     </row>
@@ -3001,9 +3417,15 @@
       <c r="H71" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I71" t="inlineStr">
-        <is>
-          <t>3688</t>
+      <c r="I71" t="n">
+        <v>3688</v>
+      </c>
+      <c r="J71" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>3866</t>
         </is>
       </c>
     </row>
@@ -3038,9 +3460,15 @@
       <c r="H72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I72" t="inlineStr">
-        <is>
-          <t>2719</t>
+      <c r="I72" t="n">
+        <v>2719</v>
+      </c>
+      <c r="J72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>2776</t>
         </is>
       </c>
     </row>
@@ -3075,9 +3503,15 @@
       <c r="H73" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="I73" t="inlineStr">
-        <is>
-          <t>3522</t>
+      <c r="I73" t="n">
+        <v>3522</v>
+      </c>
+      <c r="J73" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>3621</t>
         </is>
       </c>
     </row>
@@ -3112,9 +3546,15 @@
       <c r="H74" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I74" t="inlineStr">
-        <is>
-          <t>4177</t>
+      <c r="I74" t="n">
+        <v>4177</v>
+      </c>
+      <c r="J74" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>4375</t>
         </is>
       </c>
     </row>
@@ -3149,9 +3589,15 @@
       <c r="H75" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I75" t="inlineStr">
-        <is>
-          <t>4363</t>
+      <c r="I75" t="n">
+        <v>4363</v>
+      </c>
+      <c r="J75" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>4477</t>
         </is>
       </c>
     </row>
@@ -3177,6 +3623,8 @@
       <c r="G76" t="inlineStr"/>
       <c r="H76" s="3" t="inlineStr"/>
       <c r="I76" t="inlineStr"/>
+      <c r="J76" s="3" t="inlineStr"/>
+      <c r="K76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -3209,9 +3657,15 @@
       <c r="H77" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I77" t="inlineStr">
-        <is>
-          <t>4442</t>
+      <c r="I77" t="n">
+        <v>4442</v>
+      </c>
+      <c r="J77" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>4625</t>
         </is>
       </c>
     </row>
@@ -3246,7 +3700,13 @@
       <c r="H78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I78" t="inlineStr">
+      <c r="I78" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K78" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -3283,9 +3743,15 @@
       <c r="H79" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="I79" t="inlineStr">
-        <is>
-          <t>4011</t>
+      <c r="I79" t="n">
+        <v>4011</v>
+      </c>
+      <c r="J79" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>4121</t>
         </is>
       </c>
     </row>
@@ -3320,9 +3786,15 @@
       <c r="H80" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="I80" t="inlineStr">
-        <is>
-          <t>4180</t>
+      <c r="I80" t="n">
+        <v>4180</v>
+      </c>
+      <c r="J80" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>4306</t>
         </is>
       </c>
     </row>
@@ -3357,9 +3829,15 @@
       <c r="H81" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="I81" t="inlineStr">
-        <is>
-          <t>4122</t>
+      <c r="I81" t="n">
+        <v>4122</v>
+      </c>
+      <c r="J81" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>4227</t>
         </is>
       </c>
     </row>
@@ -3394,9 +3872,15 @@
       <c r="H82" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="I82" t="inlineStr">
-        <is>
-          <t>3815</t>
+      <c r="I82" t="n">
+        <v>3815</v>
+      </c>
+      <c r="J82" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>4018</t>
         </is>
       </c>
     </row>
@@ -3422,6 +3906,8 @@
       <c r="G83" t="inlineStr"/>
       <c r="H83" s="3" t="inlineStr"/>
       <c r="I83" t="inlineStr"/>
+      <c r="J83" s="3" t="inlineStr"/>
+      <c r="K83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -3454,9 +3940,15 @@
       <c r="H84" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="I84" t="inlineStr">
-        <is>
-          <t>3001</t>
+      <c r="I84" t="n">
+        <v>3001</v>
+      </c>
+      <c r="J84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>3096</t>
         </is>
       </c>
     </row>
@@ -3491,9 +3983,15 @@
       <c r="H85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I85" t="inlineStr">
-        <is>
-          <t>2819</t>
+      <c r="I85" t="n">
+        <v>2819</v>
+      </c>
+      <c r="J85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>2808</t>
         </is>
       </c>
     </row>
@@ -3528,9 +4026,15 @@
       <c r="H86" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="I86" t="inlineStr">
-        <is>
-          <t>3982</t>
+      <c r="I86" t="n">
+        <v>3982</v>
+      </c>
+      <c r="J86" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>4101</t>
         </is>
       </c>
     </row>
@@ -3565,9 +4069,15 @@
       <c r="H87" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I87" t="inlineStr">
-        <is>
-          <t>2867</t>
+      <c r="I87" t="n">
+        <v>2867</v>
+      </c>
+      <c r="J87" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>2957</t>
         </is>
       </c>
     </row>
@@ -3602,9 +4112,15 @@
       <c r="H88" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I88" t="inlineStr">
-        <is>
-          <t>3155</t>
+      <c r="I88" t="n">
+        <v>3155</v>
+      </c>
+      <c r="J88" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>3133</t>
         </is>
       </c>
     </row>
@@ -3630,6 +4146,8 @@
       <c r="G89" t="inlineStr"/>
       <c r="H89" s="3" t="inlineStr"/>
       <c r="I89" t="inlineStr"/>
+      <c r="J89" s="3" t="inlineStr"/>
+      <c r="K89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -3662,9 +4180,15 @@
       <c r="H90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I90" t="inlineStr">
-        <is>
-          <t>2619</t>
+      <c r="I90" t="n">
+        <v>2619</v>
+      </c>
+      <c r="J90" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>2694</t>
         </is>
       </c>
     </row>
@@ -3690,6 +4214,8 @@
       <c r="G91" t="inlineStr"/>
       <c r="H91" s="3" t="inlineStr"/>
       <c r="I91" t="inlineStr"/>
+      <c r="J91" s="3" t="inlineStr"/>
+      <c r="K91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -3722,9 +4248,15 @@
       <c r="H92" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I92" t="inlineStr">
-        <is>
-          <t>2772</t>
+      <c r="I92" t="n">
+        <v>2772</v>
+      </c>
+      <c r="J92" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>2797</t>
         </is>
       </c>
     </row>
@@ -3759,9 +4291,15 @@
       <c r="H93" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I93" t="inlineStr">
-        <is>
-          <t>2829</t>
+      <c r="I93" t="n">
+        <v>2829</v>
+      </c>
+      <c r="J93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>2797</t>
         </is>
       </c>
     </row>
@@ -3796,9 +4334,15 @@
       <c r="H94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I94" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I94" t="n">
+        <v>0</v>
+      </c>
+      <c r="J94" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>2579</t>
         </is>
       </c>
     </row>
@@ -3833,9 +4377,15 @@
       <c r="H95" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="I95" t="inlineStr">
-        <is>
-          <t>2592</t>
+      <c r="I95" t="n">
+        <v>2592</v>
+      </c>
+      <c r="J95" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>2793</t>
         </is>
       </c>
     </row>
@@ -3870,9 +4420,15 @@
       <c r="H96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I96" t="inlineStr">
-        <is>
-          <t>2087</t>
+      <c r="I96" t="n">
+        <v>2087</v>
+      </c>
+      <c r="J96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>2103</t>
         </is>
       </c>
     </row>
@@ -3907,9 +4463,15 @@
       <c r="H97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I97" t="inlineStr">
-        <is>
-          <t>2568</t>
+      <c r="I97" t="n">
+        <v>2568</v>
+      </c>
+      <c r="J97" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>2641</t>
         </is>
       </c>
     </row>
@@ -3944,9 +4506,15 @@
       <c r="H98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I98" t="inlineStr">
-        <is>
-          <t>2284</t>
+      <c r="I98" t="n">
+        <v>2284</v>
+      </c>
+      <c r="J98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>2282</t>
         </is>
       </c>
     </row>
@@ -3981,9 +4549,15 @@
       <c r="H99" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="I99" t="inlineStr">
-        <is>
-          <t>3238</t>
+      <c r="I99" t="n">
+        <v>3238</v>
+      </c>
+      <c r="J99" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>3271</t>
         </is>
       </c>
     </row>
@@ -4018,9 +4592,15 @@
       <c r="H100" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="I100" t="inlineStr">
-        <is>
-          <t>2447</t>
+      <c r="I100" t="n">
+        <v>2447</v>
+      </c>
+      <c r="J100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>2463</t>
         </is>
       </c>
     </row>
@@ -4055,9 +4635,15 @@
       <c r="H101" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I101" t="inlineStr">
-        <is>
-          <t>3823</t>
+      <c r="I101" t="n">
+        <v>3823</v>
+      </c>
+      <c r="J101" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>3891</t>
         </is>
       </c>
     </row>
@@ -4092,9 +4678,15 @@
       <c r="H102" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I102" t="inlineStr">
-        <is>
-          <t>3513</t>
+      <c r="I102" t="n">
+        <v>3513</v>
+      </c>
+      <c r="J102" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>3644</t>
         </is>
       </c>
     </row>
@@ -4129,9 +4721,15 @@
       <c r="H103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I103" t="inlineStr">
-        <is>
-          <t>2847</t>
+      <c r="I103" t="n">
+        <v>2847</v>
+      </c>
+      <c r="J103" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>3189</t>
         </is>
       </c>
     </row>
@@ -4166,9 +4764,15 @@
       <c r="H104" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I104" t="inlineStr">
-        <is>
-          <t>3858</t>
+      <c r="I104" t="n">
+        <v>3858</v>
+      </c>
+      <c r="J104" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="K104" t="inlineStr">
+        <is>
+          <t>3968</t>
         </is>
       </c>
     </row>
@@ -4203,9 +4807,15 @@
       <c r="H105" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="I105" t="inlineStr">
-        <is>
-          <t>3444</t>
+      <c r="I105" t="n">
+        <v>3444</v>
+      </c>
+      <c r="J105" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K105" t="inlineStr">
+        <is>
+          <t>3663</t>
         </is>
       </c>
     </row>
@@ -4240,9 +4850,15 @@
       <c r="H106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I106" t="inlineStr">
-        <is>
-          <t>2428</t>
+      <c r="I106" t="n">
+        <v>2428</v>
+      </c>
+      <c r="J106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>2419</t>
         </is>
       </c>
     </row>
@@ -4277,9 +4893,15 @@
       <c r="H107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I107" t="inlineStr">
-        <is>
-          <t>2642</t>
+      <c r="I107" t="n">
+        <v>2642</v>
+      </c>
+      <c r="J107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K107" t="inlineStr">
+        <is>
+          <t>2621</t>
         </is>
       </c>
     </row>
@@ -4314,9 +4936,15 @@
       <c r="H108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I108" t="inlineStr">
-        <is>
-          <t>2592</t>
+      <c r="I108" t="n">
+        <v>2592</v>
+      </c>
+      <c r="J108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K108" t="inlineStr">
+        <is>
+          <t>2621</t>
         </is>
       </c>
     </row>
@@ -4351,9 +4979,15 @@
       <c r="H109" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="I109" t="inlineStr">
-        <is>
-          <t>3395</t>
+      <c r="I109" t="n">
+        <v>3395</v>
+      </c>
+      <c r="J109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>3498</t>
         </is>
       </c>
     </row>
@@ -4388,9 +5022,15 @@
       <c r="H110" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="I110" t="inlineStr">
-        <is>
-          <t>3289</t>
+      <c r="I110" t="n">
+        <v>3289</v>
+      </c>
+      <c r="J110" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="K110" t="inlineStr">
+        <is>
+          <t>3347</t>
         </is>
       </c>
     </row>
@@ -4425,9 +5065,15 @@
       <c r="H111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I111" t="inlineStr">
-        <is>
-          <t>2693</t>
+      <c r="I111" t="n">
+        <v>2693</v>
+      </c>
+      <c r="J111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K111" t="inlineStr">
+        <is>
+          <t>2774</t>
         </is>
       </c>
     </row>
@@ -4462,9 +5108,15 @@
       <c r="H112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I112" t="inlineStr">
-        <is>
-          <t>2720</t>
+      <c r="I112" t="n">
+        <v>2720</v>
+      </c>
+      <c r="J112" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K112" t="inlineStr">
+        <is>
+          <t>3050</t>
         </is>
       </c>
     </row>
@@ -4499,9 +5151,15 @@
       <c r="H113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I113" t="inlineStr">
-        <is>
-          <t>3010</t>
+      <c r="I113" t="n">
+        <v>3010</v>
+      </c>
+      <c r="J113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>3111</t>
         </is>
       </c>
     </row>
@@ -4536,9 +5194,15 @@
       <c r="H114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I114" t="inlineStr">
-        <is>
-          <t>3412</t>
+      <c r="I114" t="n">
+        <v>3412</v>
+      </c>
+      <c r="J114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K114" t="inlineStr">
+        <is>
+          <t>3464</t>
         </is>
       </c>
     </row>
@@ -4572,6 +5236,8 @@
       </c>
       <c r="H115" s="3" t="inlineStr"/>
       <c r="I115" t="inlineStr"/>
+      <c r="J115" s="3" t="inlineStr"/>
+      <c r="K115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -4604,9 +5270,15 @@
       <c r="H116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I116" t="inlineStr">
-        <is>
-          <t>2527</t>
+      <c r="I116" t="n">
+        <v>2527</v>
+      </c>
+      <c r="J116" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>2543</t>
         </is>
       </c>
     </row>
@@ -4641,9 +5313,15 @@
       <c r="H117" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="I117" t="inlineStr">
-        <is>
-          <t>2950</t>
+      <c r="I117" t="n">
+        <v>2950</v>
+      </c>
+      <c r="J117" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>3053</t>
         </is>
       </c>
     </row>
@@ -4678,9 +5356,15 @@
       <c r="H118" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I118" t="inlineStr">
-        <is>
-          <t>3170</t>
+      <c r="I118" t="n">
+        <v>3170</v>
+      </c>
+      <c r="J118" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K118" t="inlineStr">
+        <is>
+          <t>3365</t>
         </is>
       </c>
     </row>
@@ -4715,7 +5399,13 @@
       <c r="H119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I119" t="inlineStr">
+      <c r="I119" t="n">
+        <v>0</v>
+      </c>
+      <c r="J119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K119" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4752,9 +5442,15 @@
       <c r="H120" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="I120" t="inlineStr">
-        <is>
-          <t>3415</t>
+      <c r="I120" t="n">
+        <v>3415</v>
+      </c>
+      <c r="J120" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K120" t="inlineStr">
+        <is>
+          <t>3604</t>
         </is>
       </c>
     </row>
@@ -4789,9 +5485,15 @@
       <c r="H121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I121" t="inlineStr">
-        <is>
-          <t>2659</t>
+      <c r="I121" t="n">
+        <v>2659</v>
+      </c>
+      <c r="J121" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="K121" t="inlineStr">
+        <is>
+          <t>2680</t>
         </is>
       </c>
     </row>
@@ -4826,9 +5528,15 @@
       <c r="H122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I122" t="inlineStr">
-        <is>
-          <t>2850</t>
+      <c r="I122" t="n">
+        <v>2850</v>
+      </c>
+      <c r="J122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K122" t="inlineStr">
+        <is>
+          <t>2872</t>
         </is>
       </c>
     </row>
@@ -4863,9 +5571,15 @@
       <c r="H123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I123" t="inlineStr">
-        <is>
-          <t>2483</t>
+      <c r="I123" t="n">
+        <v>2483</v>
+      </c>
+      <c r="J123" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="K123" t="inlineStr">
+        <is>
+          <t>2598</t>
         </is>
       </c>
     </row>
@@ -4900,9 +5614,15 @@
       <c r="H124" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I124" t="inlineStr">
-        <is>
-          <t>2972</t>
+      <c r="I124" t="n">
+        <v>2972</v>
+      </c>
+      <c r="J124" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K124" t="inlineStr">
+        <is>
+          <t>3100</t>
         </is>
       </c>
     </row>
@@ -4937,9 +5657,15 @@
       <c r="H125" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="I125" t="inlineStr">
-        <is>
-          <t>2988</t>
+      <c r="I125" t="n">
+        <v>2988</v>
+      </c>
+      <c r="J125" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K125" t="inlineStr">
+        <is>
+          <t>3173</t>
         </is>
       </c>
     </row>
@@ -4974,9 +5700,15 @@
       <c r="H126" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I126" t="inlineStr">
-        <is>
-          <t>3223</t>
+      <c r="I126" t="n">
+        <v>3223</v>
+      </c>
+      <c r="J126" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K126" t="inlineStr">
+        <is>
+          <t>3434</t>
         </is>
       </c>
     </row>
@@ -5011,9 +5743,15 @@
       <c r="H127" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I127" t="inlineStr">
-        <is>
-          <t>3036</t>
+      <c r="I127" t="n">
+        <v>3036</v>
+      </c>
+      <c r="J127" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K127" t="inlineStr">
+        <is>
+          <t>3074</t>
         </is>
       </c>
     </row>
@@ -5048,7 +5786,13 @@
       <c r="H128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I128" t="inlineStr">
+      <c r="I128" t="n">
+        <v>0</v>
+      </c>
+      <c r="J128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5085,7 +5829,13 @@
       <c r="H129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I129" t="inlineStr">
+      <c r="I129" t="n">
+        <v>0</v>
+      </c>
+      <c r="J129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5122,9 +5872,15 @@
       <c r="H130" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I130" t="inlineStr">
-        <is>
-          <t>2863</t>
+      <c r="I130" t="n">
+        <v>2863</v>
+      </c>
+      <c r="J130" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K130" t="inlineStr">
+        <is>
+          <t>2959</t>
         </is>
       </c>
     </row>
@@ -5159,9 +5915,15 @@
       <c r="H131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I131" t="inlineStr">
-        <is>
-          <t>2679</t>
+      <c r="I131" t="n">
+        <v>2679</v>
+      </c>
+      <c r="J131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K131" t="inlineStr">
+        <is>
+          <t>2767</t>
         </is>
       </c>
     </row>
@@ -5196,7 +5958,13 @@
       <c r="H132" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I132" t="inlineStr">
+      <c r="I132" t="n">
+        <v>0</v>
+      </c>
+      <c r="J132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K132" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5233,7 +6001,13 @@
       <c r="H133" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="I133" t="inlineStr">
+      <c r="I133" t="n">
+        <v>2196</v>
+      </c>
+      <c r="J133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K133" t="inlineStr">
         <is>
           <t>2196</t>
         </is>
@@ -5270,9 +6044,15 @@
       <c r="H134" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I134" t="inlineStr">
-        <is>
-          <t>3059</t>
+      <c r="I134" t="n">
+        <v>3059</v>
+      </c>
+      <c r="J134" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K134" t="inlineStr">
+        <is>
+          <t>3032</t>
         </is>
       </c>
     </row>
@@ -5307,9 +6087,15 @@
       <c r="H135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I135" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I135" t="n">
+        <v>0</v>
+      </c>
+      <c r="J135" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K135" t="inlineStr">
+        <is>
+          <t>2498</t>
         </is>
       </c>
     </row>
@@ -5344,9 +6130,15 @@
       <c r="H136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I136" t="inlineStr">
-        <is>
-          <t>999</t>
+      <c r="I136" t="n">
+        <v>999</v>
+      </c>
+      <c r="J136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K136" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -5381,7 +6173,13 @@
       <c r="H137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I137" t="inlineStr">
+      <c r="I137" t="n">
+        <v>0</v>
+      </c>
+      <c r="J137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5418,9 +6216,15 @@
       <c r="H138" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="I138" t="inlineStr">
-        <is>
-          <t>3038</t>
+      <c r="I138" t="n">
+        <v>3038</v>
+      </c>
+      <c r="J138" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="K138" t="inlineStr">
+        <is>
+          <t>3113</t>
         </is>
       </c>
     </row>
@@ -5455,7 +6259,13 @@
       <c r="H139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I139" t="inlineStr">
+      <c r="I139" t="n">
+        <v>0</v>
+      </c>
+      <c r="J139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K139" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5492,9 +6302,15 @@
       <c r="H140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I140" t="inlineStr">
-        <is>
-          <t>2605</t>
+      <c r="I140" t="n">
+        <v>2605</v>
+      </c>
+      <c r="J140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K140" t="inlineStr">
+        <is>
+          <t>2639</t>
         </is>
       </c>
     </row>
@@ -5529,7 +6345,13 @@
       <c r="H141" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I141" t="inlineStr">
+      <c r="I141" t="n">
+        <v>0</v>
+      </c>
+      <c r="J141" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K141" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5566,9 +6388,15 @@
       <c r="H142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I142" t="inlineStr">
-        <is>
-          <t>2741</t>
+      <c r="I142" t="n">
+        <v>2741</v>
+      </c>
+      <c r="J142" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="K142" t="inlineStr">
+        <is>
+          <t>2838</t>
         </is>
       </c>
     </row>
@@ -5594,6 +6422,8 @@
       <c r="G143" t="inlineStr"/>
       <c r="H143" s="3" t="inlineStr"/>
       <c r="I143" t="inlineStr"/>
+      <c r="J143" s="3" t="inlineStr"/>
+      <c r="K143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -5614,7 +6444,7 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F144" s="2" t="n">
@@ -5626,9 +6456,15 @@
       <c r="H144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I144" t="inlineStr">
-        <is>
-          <t>2466</t>
+      <c r="I144" t="n">
+        <v>2466</v>
+      </c>
+      <c r="J144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K144" t="inlineStr">
+        <is>
+          <t>2480</t>
         </is>
       </c>
     </row>
@@ -5663,7 +6499,13 @@
       <c r="H145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I145" t="inlineStr">
+      <c r="I145" t="n">
+        <v>0</v>
+      </c>
+      <c r="J145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K145" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5700,7 +6542,13 @@
       <c r="H146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I146" t="inlineStr">
+      <c r="I146" t="n">
+        <v>0</v>
+      </c>
+      <c r="J146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5737,7 +6585,13 @@
       <c r="H147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I147" t="inlineStr">
+      <c r="I147" t="n">
+        <v>0</v>
+      </c>
+      <c r="J147" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K147" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5774,7 +6628,13 @@
       <c r="H148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I148" t="inlineStr">
+      <c r="I148" t="n">
+        <v>0</v>
+      </c>
+      <c r="J148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5811,7 +6671,13 @@
       <c r="H149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I149" t="inlineStr">
+      <c r="I149" t="n">
+        <v>0</v>
+      </c>
+      <c r="J149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K149" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5848,9 +6714,15 @@
       <c r="H150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I150" t="inlineStr">
-        <is>
-          <t>2385</t>
+      <c r="I150" t="n">
+        <v>2385</v>
+      </c>
+      <c r="J150" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="K150" t="inlineStr">
+        <is>
+          <t>2493</t>
         </is>
       </c>
     </row>
@@ -5885,7 +6757,13 @@
       <c r="H151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I151" t="inlineStr">
+      <c r="I151" t="n">
+        <v>0</v>
+      </c>
+      <c r="J151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K151" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5922,9 +6800,15 @@
       <c r="H152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I152" t="inlineStr">
-        <is>
-          <t>1604</t>
+      <c r="I152" t="n">
+        <v>1604</v>
+      </c>
+      <c r="J152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K152" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -5959,9 +6843,15 @@
       <c r="H153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I153" t="inlineStr">
-        <is>
-          <t>1829</t>
+      <c r="I153" t="n">
+        <v>1829</v>
+      </c>
+      <c r="J153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K153" t="inlineStr">
+        <is>
+          <t>1800</t>
         </is>
       </c>
     </row>
@@ -5996,7 +6886,13 @@
       <c r="H154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I154" t="inlineStr">
+      <c r="I154" t="n">
+        <v>0</v>
+      </c>
+      <c r="J154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6033,9 +6929,15 @@
       <c r="H155" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="I155" t="inlineStr">
-        <is>
-          <t>3926</t>
+      <c r="I155" t="n">
+        <v>3926</v>
+      </c>
+      <c r="J155" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="K155" t="inlineStr">
+        <is>
+          <t>4375</t>
         </is>
       </c>
     </row>
@@ -6070,7 +6972,13 @@
       <c r="H156" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I156" t="inlineStr">
+      <c r="I156" t="n">
+        <v>0</v>
+      </c>
+      <c r="J156" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K156" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6107,9 +7015,15 @@
       <c r="H157" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I157" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I157" t="n">
+        <v>0</v>
+      </c>
+      <c r="J157" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K157" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -6144,9 +7058,15 @@
       <c r="H158" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="I158" t="inlineStr">
-        <is>
-          <t>4733</t>
+      <c r="I158" t="n">
+        <v>4733</v>
+      </c>
+      <c r="J158" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="K158" t="inlineStr">
+        <is>
+          <t>4963</t>
         </is>
       </c>
     </row>
@@ -6181,7 +7101,13 @@
       <c r="H159" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I159" t="inlineStr">
+      <c r="I159" t="n">
+        <v>0</v>
+      </c>
+      <c r="J159" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K159" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6218,9 +7144,15 @@
       <c r="H160" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I160" t="inlineStr">
-        <is>
-          <t>2808</t>
+      <c r="I160" t="n">
+        <v>2808</v>
+      </c>
+      <c r="J160" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K160" t="inlineStr">
+        <is>
+          <t>2857</t>
         </is>
       </c>
     </row>
@@ -6255,7 +7187,13 @@
       <c r="H161" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I161" t="inlineStr">
+      <c r="I161" t="n">
+        <v>0</v>
+      </c>
+      <c r="J161" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K161" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6292,9 +7230,15 @@
       <c r="H162" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I162" t="inlineStr">
-        <is>
-          <t>2853</t>
+      <c r="I162" t="n">
+        <v>2853</v>
+      </c>
+      <c r="J162" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K162" t="inlineStr">
+        <is>
+          <t>2895</t>
         </is>
       </c>
     </row>
@@ -6320,6 +7264,8 @@
       <c r="G163" t="inlineStr"/>
       <c r="H163" s="3" t="inlineStr"/>
       <c r="I163" t="inlineStr"/>
+      <c r="J163" s="3" t="inlineStr"/>
+      <c r="K163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" t="n">
@@ -6346,9 +7292,15 @@
       <c r="H164" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="I164" t="inlineStr">
-        <is>
-          <t>2618</t>
+      <c r="I164" t="n">
+        <v>2618</v>
+      </c>
+      <c r="J164" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K164" t="inlineStr">
+        <is>
+          <t>2809</t>
         </is>
       </c>
     </row>
@@ -6377,9 +7329,15 @@
       <c r="H165" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="I165" t="inlineStr">
-        <is>
-          <t>2313</t>
+      <c r="I165" t="n">
+        <v>2313</v>
+      </c>
+      <c r="J165" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="K165" t="inlineStr">
+        <is>
+          <t>2413</t>
         </is>
       </c>
     </row>
@@ -6408,9 +7366,15 @@
       <c r="H166" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I166" t="inlineStr">
-        <is>
-          <t>2399</t>
+      <c r="I166" t="n">
+        <v>2399</v>
+      </c>
+      <c r="J166" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K166" t="inlineStr">
+        <is>
+          <t>2437</t>
         </is>
       </c>
     </row>
@@ -6439,17 +7403,21 @@
       <c r="H167" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I167" t="inlineStr">
-        <is>
-          <t>1429</t>
+      <c r="I167" t="n">
+        <v>1429</v>
+      </c>
+      <c r="J167" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K167" t="inlineStr">
+        <is>
+          <t>1460</t>
         </is>
       </c>
     </row>
     <row r="168">
-      <c r="A168" t="inlineStr">
-        <is>
-          <t>58766144</t>
-        </is>
+      <c r="A168" t="n">
+        <v>58766144</v>
       </c>
       <c r="B168" t="inlineStr">
         <is>
@@ -6468,9 +7436,15 @@
       <c r="H168" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I168" t="inlineStr">
-        <is>
-          <t>1535</t>
+      <c r="I168" t="n">
+        <v>1535</v>
+      </c>
+      <c r="J168" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="K168" t="inlineStr">
+        <is>
+          <t>1615</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-02-07 11:30:31
</commit_message>
<xml_diff>
--- a/Season_Attack/83.xlsx
+++ b/Season_Attack/83.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K168"/>
+  <dimension ref="A1:M168"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,6 +446,16 @@
           <t>02-05_0</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>02-06_A</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>02-06_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -484,9 +494,15 @@
       <c r="J2" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>3672</t>
+      <c r="K2" t="n">
+        <v>3672</v>
+      </c>
+      <c r="L2" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>3808</t>
         </is>
       </c>
     </row>
@@ -527,9 +543,15 @@
       <c r="J3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>5060</t>
+      <c r="K3" t="n">
+        <v>5060</v>
+      </c>
+      <c r="L3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>5294</t>
         </is>
       </c>
     </row>
@@ -570,9 +592,15 @@
       <c r="J4" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>4773</t>
+      <c r="K4" t="n">
+        <v>4773</v>
+      </c>
+      <c r="L4" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>5035</t>
         </is>
       </c>
     </row>
@@ -613,9 +641,15 @@
       <c r="J5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>4982</t>
+      <c r="K5" t="n">
+        <v>4982</v>
+      </c>
+      <c r="L5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>5263</t>
         </is>
       </c>
     </row>
@@ -656,9 +690,15 @@
       <c r="J6" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>4893</t>
+      <c r="K6" t="n">
+        <v>4893</v>
+      </c>
+      <c r="L6" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>5149</t>
         </is>
       </c>
     </row>
@@ -699,9 +739,15 @@
       <c r="J7" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>5384</t>
+      <c r="K7" t="n">
+        <v>5384</v>
+      </c>
+      <c r="L7" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>5609</t>
         </is>
       </c>
     </row>
@@ -742,9 +788,15 @@
       <c r="J8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>4548</t>
+      <c r="K8" t="n">
+        <v>4548</v>
+      </c>
+      <c r="L8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>4727</t>
         </is>
       </c>
     </row>
@@ -780,6 +832,8 @@
       <c r="I9" t="inlineStr"/>
       <c r="J9" s="3" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
+      <c r="L9" s="3" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -818,9 +872,15 @@
       <c r="J10" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>4510</t>
+      <c r="K10" t="n">
+        <v>4510</v>
+      </c>
+      <c r="L10" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>4862</t>
         </is>
       </c>
     </row>
@@ -861,9 +921,15 @@
       <c r="J11" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>4702</t>
+      <c r="K11" t="n">
+        <v>4702</v>
+      </c>
+      <c r="L11" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>4908</t>
         </is>
       </c>
     </row>
@@ -904,9 +970,15 @@
       <c r="J12" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>4288</t>
+      <c r="K12" t="n">
+        <v>4288</v>
+      </c>
+      <c r="L12" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>4635</t>
         </is>
       </c>
     </row>
@@ -947,7 +1019,13 @@
       <c r="J13" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K13" t="inlineStr">
+      <c r="K13" t="n">
+        <v>2716</v>
+      </c>
+      <c r="L13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="inlineStr">
         <is>
           <t>2716</t>
         </is>
@@ -990,9 +1068,15 @@
       <c r="J14" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>5621</t>
+      <c r="K14" t="n">
+        <v>5621</v>
+      </c>
+      <c r="L14" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>5882</t>
         </is>
       </c>
     </row>
@@ -1033,9 +1117,15 @@
       <c r="J15" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>4779</t>
+      <c r="K15" t="n">
+        <v>4779</v>
+      </c>
+      <c r="L15" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>5075</t>
         </is>
       </c>
     </row>
@@ -1076,9 +1166,15 @@
       <c r="J16" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>4759</t>
+      <c r="K16" t="n">
+        <v>4759</v>
+      </c>
+      <c r="L16" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>5163</t>
         </is>
       </c>
     </row>
@@ -1119,9 +1215,15 @@
       <c r="J17" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>4204</t>
+      <c r="K17" t="n">
+        <v>4204</v>
+      </c>
+      <c r="L17" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>4307</t>
         </is>
       </c>
     </row>
@@ -1162,9 +1264,15 @@
       <c r="J18" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>4283</t>
+      <c r="K18" t="n">
+        <v>4283</v>
+      </c>
+      <c r="L18" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>4457</t>
         </is>
       </c>
     </row>
@@ -1205,9 +1313,15 @@
       <c r="J19" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>4814</t>
+      <c r="K19" t="n">
+        <v>4814</v>
+      </c>
+      <c r="L19" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>5069</t>
         </is>
       </c>
     </row>
@@ -1248,9 +1362,15 @@
       <c r="J20" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>5624</t>
+      <c r="K20" t="n">
+        <v>5624</v>
+      </c>
+      <c r="L20" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>5895</t>
         </is>
       </c>
     </row>
@@ -1291,9 +1411,15 @@
       <c r="J21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>3411</t>
+      <c r="K21" t="n">
+        <v>3411</v>
+      </c>
+      <c r="L21" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>3923</t>
         </is>
       </c>
     </row>
@@ -1334,9 +1460,15 @@
       <c r="J22" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>4771</t>
+      <c r="K22" t="n">
+        <v>4771</v>
+      </c>
+      <c r="L22" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>4949</t>
         </is>
       </c>
     </row>
@@ -1377,9 +1509,15 @@
       <c r="J23" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>4183</t>
+      <c r="K23" t="n">
+        <v>4183</v>
+      </c>
+      <c r="L23" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>4669</t>
         </is>
       </c>
     </row>
@@ -1420,9 +1558,15 @@
       <c r="J24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>4815</t>
+      <c r="K24" t="n">
+        <v>4815</v>
+      </c>
+      <c r="L24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>5161</t>
         </is>
       </c>
     </row>
@@ -1463,7 +1607,13 @@
       <c r="J25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K25" t="inlineStr">
+      <c r="K25" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1488,7 +1638,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F26" s="5" t="n">
@@ -1506,9 +1656,15 @@
       <c r="J26" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>5109</t>
+      <c r="K26" t="n">
+        <v>5109</v>
+      </c>
+      <c r="L26" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>5334</t>
         </is>
       </c>
     </row>
@@ -1549,9 +1705,15 @@
       <c r="J27" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="K27" t="inlineStr">
-        <is>
-          <t>5211</t>
+      <c r="K27" t="n">
+        <v>5211</v>
+      </c>
+      <c r="L27" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>5530</t>
         </is>
       </c>
     </row>
@@ -1592,9 +1754,15 @@
       <c r="J28" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>3902</t>
+      <c r="K28" t="n">
+        <v>3902</v>
+      </c>
+      <c r="L28" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>4128</t>
         </is>
       </c>
     </row>
@@ -1635,9 +1803,15 @@
       <c r="J29" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>5486</t>
+      <c r="K29" t="n">
+        <v>5486</v>
+      </c>
+      <c r="L29" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>5476</t>
         </is>
       </c>
     </row>
@@ -1660,7 +1834,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F30" s="5" t="n">
@@ -1678,9 +1852,15 @@
       <c r="J30" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="K30" t="inlineStr">
-        <is>
-          <t>4987</t>
+      <c r="K30" t="n">
+        <v>4987</v>
+      </c>
+      <c r="L30" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>5304</t>
         </is>
       </c>
     </row>
@@ -1703,7 +1883,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F31" s="5" t="n">
@@ -1721,9 +1901,15 @@
       <c r="J31" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="K31" t="inlineStr">
-        <is>
-          <t>4735</t>
+      <c r="K31" t="n">
+        <v>4735</v>
+      </c>
+      <c r="L31" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>4814</t>
         </is>
       </c>
     </row>
@@ -1764,9 +1950,15 @@
       <c r="J32" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t>5324</t>
+      <c r="K32" t="n">
+        <v>5324</v>
+      </c>
+      <c r="L32" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>5515</t>
         </is>
       </c>
     </row>
@@ -1807,9 +1999,15 @@
       <c r="J33" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="K33" t="inlineStr">
-        <is>
-          <t>5180</t>
+      <c r="K33" t="n">
+        <v>5180</v>
+      </c>
+      <c r="L33" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>5425</t>
         </is>
       </c>
     </row>
@@ -1850,9 +2048,15 @@
       <c r="J34" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>4905</t>
+      <c r="K34" t="n">
+        <v>4905</v>
+      </c>
+      <c r="L34" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>5221</t>
         </is>
       </c>
     </row>
@@ -1893,9 +2097,15 @@
       <c r="J35" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="K35" t="inlineStr">
-        <is>
-          <t>5253</t>
+      <c r="K35" t="n">
+        <v>5253</v>
+      </c>
+      <c r="L35" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>5532</t>
         </is>
       </c>
     </row>
@@ -1936,9 +2146,15 @@
       <c r="J36" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>4763</t>
+      <c r="K36" t="n">
+        <v>4763</v>
+      </c>
+      <c r="L36" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>4881</t>
         </is>
       </c>
     </row>
@@ -1979,9 +2195,15 @@
       <c r="J37" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="K37" t="inlineStr">
-        <is>
-          <t>4429</t>
+      <c r="K37" t="n">
+        <v>4429</v>
+      </c>
+      <c r="L37" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>4534</t>
         </is>
       </c>
     </row>
@@ -2022,9 +2244,15 @@
       <c r="J38" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="K38" t="inlineStr">
-        <is>
-          <t>4788</t>
+      <c r="K38" t="n">
+        <v>4788</v>
+      </c>
+      <c r="L38" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>5009</t>
         </is>
       </c>
     </row>
@@ -2065,9 +2293,15 @@
       <c r="J39" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>4580</t>
+      <c r="K39" t="n">
+        <v>4580</v>
+      </c>
+      <c r="L39" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>4785</t>
         </is>
       </c>
     </row>
@@ -2108,9 +2342,15 @@
       <c r="J40" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="K40" t="inlineStr">
-        <is>
-          <t>5450</t>
+      <c r="K40" t="n">
+        <v>5450</v>
+      </c>
+      <c r="L40" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>5706</t>
         </is>
       </c>
     </row>
@@ -2151,9 +2391,15 @@
       <c r="J41" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K41" t="inlineStr">
-        <is>
-          <t>4800</t>
+      <c r="K41" t="n">
+        <v>4800</v>
+      </c>
+      <c r="L41" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>5066</t>
         </is>
       </c>
     </row>
@@ -2194,9 +2440,15 @@
       <c r="J42" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>5448</t>
+      <c r="K42" t="n">
+        <v>5448</v>
+      </c>
+      <c r="L42" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>5770</t>
         </is>
       </c>
     </row>
@@ -2219,7 +2471,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F43" s="5" t="n">
@@ -2237,9 +2489,15 @@
       <c r="J43" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="K43" t="inlineStr">
-        <is>
-          <t>4863</t>
+      <c r="K43" t="n">
+        <v>4863</v>
+      </c>
+      <c r="L43" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>5070</t>
         </is>
       </c>
     </row>
@@ -2280,9 +2538,15 @@
       <c r="J44" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="K44" t="inlineStr">
-        <is>
-          <t>4736</t>
+      <c r="K44" t="n">
+        <v>4736</v>
+      </c>
+      <c r="L44" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>5124</t>
         </is>
       </c>
     </row>
@@ -2323,9 +2587,15 @@
       <c r="J45" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="K45" t="inlineStr">
-        <is>
-          <t>4361</t>
+      <c r="K45" t="n">
+        <v>4361</v>
+      </c>
+      <c r="L45" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>4487</t>
         </is>
       </c>
     </row>
@@ -2366,9 +2636,15 @@
       <c r="J46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>4372</t>
+      <c r="K46" t="n">
+        <v>4372</v>
+      </c>
+      <c r="L46" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>4467</t>
         </is>
       </c>
     </row>
@@ -2409,9 +2685,15 @@
       <c r="J47" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K47" t="inlineStr">
-        <is>
-          <t>3036</t>
+      <c r="K47" t="n">
+        <v>3036</v>
+      </c>
+      <c r="L47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>3035</t>
         </is>
       </c>
     </row>
@@ -2452,9 +2734,15 @@
       <c r="J48" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>4995</t>
+      <c r="K48" t="n">
+        <v>4995</v>
+      </c>
+      <c r="L48" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>5230</t>
         </is>
       </c>
     </row>
@@ -2495,9 +2783,15 @@
       <c r="J49" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>4006</t>
+      <c r="K49" t="n">
+        <v>4006</v>
+      </c>
+      <c r="L49" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>4148</t>
         </is>
       </c>
     </row>
@@ -2538,9 +2832,15 @@
       <c r="J50" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="K50" t="inlineStr">
-        <is>
-          <t>5242</t>
+      <c r="K50" t="n">
+        <v>5242</v>
+      </c>
+      <c r="L50" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>5518</t>
         </is>
       </c>
     </row>
@@ -2581,9 +2881,15 @@
       <c r="J51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K51" t="inlineStr">
-        <is>
-          <t>2796</t>
+      <c r="K51" t="n">
+        <v>2796</v>
+      </c>
+      <c r="L51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>2842</t>
         </is>
       </c>
     </row>
@@ -2624,9 +2930,15 @@
       <c r="J52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>2709</t>
+      <c r="K52" t="n">
+        <v>2709</v>
+      </c>
+      <c r="L52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>2782</t>
         </is>
       </c>
     </row>
@@ -2667,9 +2979,15 @@
       <c r="J53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K53" t="inlineStr">
-        <is>
-          <t>2958</t>
+      <c r="K53" t="n">
+        <v>2958</v>
+      </c>
+      <c r="L53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>2973</t>
         </is>
       </c>
     </row>
@@ -2710,9 +3028,15 @@
       <c r="J54" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="K54" t="inlineStr">
-        <is>
-          <t>4854</t>
+      <c r="K54" t="n">
+        <v>4854</v>
+      </c>
+      <c r="L54" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>5047</t>
         </is>
       </c>
     </row>
@@ -2753,9 +3077,15 @@
       <c r="J55" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="K55" t="inlineStr">
-        <is>
-          <t>3813</t>
+      <c r="K55" t="n">
+        <v>3813</v>
+      </c>
+      <c r="L55" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>3984</t>
         </is>
       </c>
     </row>
@@ -2796,9 +3126,15 @@
       <c r="J56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K56" t="inlineStr">
-        <is>
-          <t>3911</t>
+      <c r="K56" t="n">
+        <v>3911</v>
+      </c>
+      <c r="L56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>4059</t>
         </is>
       </c>
     </row>
@@ -2839,9 +3175,15 @@
       <c r="J57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K57" t="inlineStr">
-        <is>
-          <t>4532</t>
+      <c r="K57" t="n">
+        <v>4532</v>
+      </c>
+      <c r="L57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>4731</t>
         </is>
       </c>
     </row>
@@ -2882,9 +3224,15 @@
       <c r="J58" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="K58" t="inlineStr">
-        <is>
-          <t>3910</t>
+      <c r="K58" t="n">
+        <v>3910</v>
+      </c>
+      <c r="L58" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>4077</t>
         </is>
       </c>
     </row>
@@ -2925,9 +3273,15 @@
       <c r="J59" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K59" t="inlineStr">
-        <is>
-          <t>4412</t>
+      <c r="K59" t="n">
+        <v>4412</v>
+      </c>
+      <c r="L59" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>4611</t>
         </is>
       </c>
     </row>
@@ -2968,7 +3322,13 @@
       <c r="J60" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K60" t="inlineStr">
+      <c r="K60" t="n">
+        <v>0</v>
+      </c>
+      <c r="L60" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M60" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3011,9 +3371,15 @@
       <c r="J61" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="K61" t="inlineStr">
-        <is>
-          <t>4627</t>
+      <c r="K61" t="n">
+        <v>4627</v>
+      </c>
+      <c r="L61" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>4884</t>
         </is>
       </c>
     </row>
@@ -3054,9 +3420,15 @@
       <c r="J62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K62" t="inlineStr">
-        <is>
-          <t>2609</t>
+      <c r="K62" t="n">
+        <v>2609</v>
+      </c>
+      <c r="L62" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>3036</t>
         </is>
       </c>
     </row>
@@ -3097,9 +3469,15 @@
       <c r="J63" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="K63" t="inlineStr">
-        <is>
-          <t>3110</t>
+      <c r="K63" t="n">
+        <v>3110</v>
+      </c>
+      <c r="L63" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>3253</t>
         </is>
       </c>
     </row>
@@ -3140,9 +3518,15 @@
       <c r="J64" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="K64" t="inlineStr">
-        <is>
-          <t>4393</t>
+      <c r="K64" t="n">
+        <v>4393</v>
+      </c>
+      <c r="L64" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>4610</t>
         </is>
       </c>
     </row>
@@ -3170,6 +3554,8 @@
       <c r="I65" t="inlineStr"/>
       <c r="J65" s="3" t="inlineStr"/>
       <c r="K65" t="inlineStr"/>
+      <c r="L65" s="3" t="inlineStr"/>
+      <c r="M65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -3208,9 +3594,15 @@
       <c r="J66" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K66" t="inlineStr">
-        <is>
-          <t>4747</t>
+      <c r="K66" t="n">
+        <v>4747</v>
+      </c>
+      <c r="L66" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>5097</t>
         </is>
       </c>
     </row>
@@ -3251,9 +3643,15 @@
       <c r="J67" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="K67" t="inlineStr">
-        <is>
-          <t>3989</t>
+      <c r="K67" t="n">
+        <v>3989</v>
+      </c>
+      <c r="L67" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>4174</t>
         </is>
       </c>
     </row>
@@ -3294,7 +3692,13 @@
       <c r="J68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K68" t="inlineStr">
+      <c r="K68" t="n">
+        <v>2555</v>
+      </c>
+      <c r="L68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M68" t="inlineStr">
         <is>
           <t>2555</t>
         </is>
@@ -3337,9 +3741,15 @@
       <c r="J69" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="K69" t="inlineStr">
-        <is>
-          <t>3741</t>
+      <c r="K69" t="n">
+        <v>3741</v>
+      </c>
+      <c r="L69" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="M69" t="inlineStr">
+        <is>
+          <t>4029</t>
         </is>
       </c>
     </row>
@@ -3380,9 +3790,15 @@
       <c r="J70" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="K70" t="inlineStr">
-        <is>
-          <t>3624</t>
+      <c r="K70" t="n">
+        <v>3624</v>
+      </c>
+      <c r="L70" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="M70" t="inlineStr">
+        <is>
+          <t>3764</t>
         </is>
       </c>
     </row>
@@ -3423,9 +3839,15 @@
       <c r="J71" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K71" t="inlineStr">
-        <is>
-          <t>3866</t>
+      <c r="K71" t="n">
+        <v>3866</v>
+      </c>
+      <c r="L71" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M71" t="inlineStr">
+        <is>
+          <t>4050</t>
         </is>
       </c>
     </row>
@@ -3466,9 +3888,15 @@
       <c r="J72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K72" t="inlineStr">
-        <is>
-          <t>2776</t>
+      <c r="K72" t="n">
+        <v>2776</v>
+      </c>
+      <c r="L72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>2832</t>
         </is>
       </c>
     </row>
@@ -3509,9 +3937,15 @@
       <c r="J73" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="K73" t="inlineStr">
-        <is>
-          <t>3621</t>
+      <c r="K73" t="n">
+        <v>3621</v>
+      </c>
+      <c r="L73" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="M73" t="inlineStr">
+        <is>
+          <t>3679</t>
         </is>
       </c>
     </row>
@@ -3552,9 +3986,15 @@
       <c r="J74" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K74" t="inlineStr">
-        <is>
-          <t>4375</t>
+      <c r="K74" t="n">
+        <v>4375</v>
+      </c>
+      <c r="L74" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>4592</t>
         </is>
       </c>
     </row>
@@ -3595,9 +4035,15 @@
       <c r="J75" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K75" t="inlineStr">
-        <is>
-          <t>4477</t>
+      <c r="K75" t="n">
+        <v>4477</v>
+      </c>
+      <c r="L75" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M75" t="inlineStr">
+        <is>
+          <t>4653</t>
         </is>
       </c>
     </row>
@@ -3625,6 +4071,8 @@
       <c r="I76" t="inlineStr"/>
       <c r="J76" s="3" t="inlineStr"/>
       <c r="K76" t="inlineStr"/>
+      <c r="L76" s="3" t="inlineStr"/>
+      <c r="M76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -3663,9 +4111,15 @@
       <c r="J77" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K77" t="inlineStr">
-        <is>
-          <t>4625</t>
+      <c r="K77" t="n">
+        <v>4625</v>
+      </c>
+      <c r="L77" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>4697</t>
         </is>
       </c>
     </row>
@@ -3706,7 +4160,13 @@
       <c r="J78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K78" t="inlineStr">
+      <c r="K78" t="n">
+        <v>2500</v>
+      </c>
+      <c r="L78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M78" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -3749,9 +4209,15 @@
       <c r="J79" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K79" t="inlineStr">
-        <is>
-          <t>4121</t>
+      <c r="K79" t="n">
+        <v>4121</v>
+      </c>
+      <c r="L79" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M79" t="inlineStr">
+        <is>
+          <t>4256</t>
         </is>
       </c>
     </row>
@@ -3792,9 +4258,15 @@
       <c r="J80" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="K80" t="inlineStr">
-        <is>
-          <t>4306</t>
+      <c r="K80" t="n">
+        <v>4306</v>
+      </c>
+      <c r="L80" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="M80" t="inlineStr">
+        <is>
+          <t>4581</t>
         </is>
       </c>
     </row>
@@ -3835,9 +4307,15 @@
       <c r="J81" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K81" t="inlineStr">
-        <is>
-          <t>4227</t>
+      <c r="K81" t="n">
+        <v>4227</v>
+      </c>
+      <c r="L81" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="M81" t="inlineStr">
+        <is>
+          <t>4381</t>
         </is>
       </c>
     </row>
@@ -3878,9 +4356,15 @@
       <c r="J82" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="K82" t="inlineStr">
-        <is>
-          <t>4018</t>
+      <c r="K82" t="n">
+        <v>4018</v>
+      </c>
+      <c r="L82" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="M82" t="inlineStr">
+        <is>
+          <t>4145</t>
         </is>
       </c>
     </row>
@@ -3908,6 +4392,8 @@
       <c r="I83" t="inlineStr"/>
       <c r="J83" s="3" t="inlineStr"/>
       <c r="K83" t="inlineStr"/>
+      <c r="L83" s="3" t="inlineStr"/>
+      <c r="M83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -3946,9 +4432,15 @@
       <c r="J84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K84" t="inlineStr">
-        <is>
-          <t>3096</t>
+      <c r="K84" t="n">
+        <v>3096</v>
+      </c>
+      <c r="L84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M84" t="inlineStr">
+        <is>
+          <t>3151</t>
         </is>
       </c>
     </row>
@@ -3989,9 +4481,15 @@
       <c r="J85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K85" t="inlineStr">
-        <is>
-          <t>2808</t>
+      <c r="K85" t="n">
+        <v>2808</v>
+      </c>
+      <c r="L85" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M85" t="inlineStr">
+        <is>
+          <t>3177</t>
         </is>
       </c>
     </row>
@@ -4032,9 +4530,15 @@
       <c r="J86" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="K86" t="inlineStr">
-        <is>
-          <t>4101</t>
+      <c r="K86" t="n">
+        <v>4101</v>
+      </c>
+      <c r="L86" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="M86" t="inlineStr">
+        <is>
+          <t>4469</t>
         </is>
       </c>
     </row>
@@ -4075,9 +4579,15 @@
       <c r="J87" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K87" t="inlineStr">
-        <is>
-          <t>2957</t>
+      <c r="K87" t="n">
+        <v>2957</v>
+      </c>
+      <c r="L87" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M87" t="inlineStr">
+        <is>
+          <t>2984</t>
         </is>
       </c>
     </row>
@@ -4118,9 +4628,15 @@
       <c r="J88" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K88" t="inlineStr">
-        <is>
-          <t>3133</t>
+      <c r="K88" t="n">
+        <v>3133</v>
+      </c>
+      <c r="L88" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="M88" t="inlineStr">
+        <is>
+          <t>3244</t>
         </is>
       </c>
     </row>
@@ -4148,6 +4664,8 @@
       <c r="I89" t="inlineStr"/>
       <c r="J89" s="3" t="inlineStr"/>
       <c r="K89" t="inlineStr"/>
+      <c r="L89" s="3" t="inlineStr"/>
+      <c r="M89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -4186,9 +4704,15 @@
       <c r="J90" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K90" t="inlineStr">
-        <is>
-          <t>2694</t>
+      <c r="K90" t="n">
+        <v>2694</v>
+      </c>
+      <c r="L90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M90" t="inlineStr">
+        <is>
+          <t>2668</t>
         </is>
       </c>
     </row>
@@ -4216,6 +4740,8 @@
       <c r="I91" t="inlineStr"/>
       <c r="J91" s="3" t="inlineStr"/>
       <c r="K91" t="inlineStr"/>
+      <c r="L91" s="3" t="inlineStr"/>
+      <c r="M91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -4254,9 +4780,15 @@
       <c r="J92" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K92" t="inlineStr">
-        <is>
-          <t>2797</t>
+      <c r="K92" t="n">
+        <v>2797</v>
+      </c>
+      <c r="L92" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M92" t="inlineStr">
+        <is>
+          <t>2679</t>
         </is>
       </c>
     </row>
@@ -4297,9 +4829,15 @@
       <c r="J93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K93" t="inlineStr">
-        <is>
-          <t>2797</t>
+      <c r="K93" t="n">
+        <v>2797</v>
+      </c>
+      <c r="L93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M93" t="inlineStr">
+        <is>
+          <t>2779</t>
         </is>
       </c>
     </row>
@@ -4340,9 +4878,15 @@
       <c r="J94" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="K94" t="inlineStr">
-        <is>
-          <t>2579</t>
+      <c r="K94" t="n">
+        <v>2579</v>
+      </c>
+      <c r="L94" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M94" t="inlineStr">
+        <is>
+          <t>2890</t>
         </is>
       </c>
     </row>
@@ -4383,9 +4927,15 @@
       <c r="J95" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="K95" t="inlineStr">
-        <is>
-          <t>2793</t>
+      <c r="K95" t="n">
+        <v>2793</v>
+      </c>
+      <c r="L95" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="M95" t="inlineStr">
+        <is>
+          <t>2758</t>
         </is>
       </c>
     </row>
@@ -4426,9 +4976,15 @@
       <c r="J96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K96" t="inlineStr">
-        <is>
-          <t>2103</t>
+      <c r="K96" t="n">
+        <v>2103</v>
+      </c>
+      <c r="L96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M96" t="inlineStr">
+        <is>
+          <t>2111</t>
         </is>
       </c>
     </row>
@@ -4469,9 +5025,15 @@
       <c r="J97" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="K97" t="inlineStr">
-        <is>
-          <t>2641</t>
+      <c r="K97" t="n">
+        <v>2641</v>
+      </c>
+      <c r="L97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M97" t="inlineStr">
+        <is>
+          <t>2669</t>
         </is>
       </c>
     </row>
@@ -4512,9 +5074,15 @@
       <c r="J98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K98" t="inlineStr">
-        <is>
-          <t>2282</t>
+      <c r="K98" t="n">
+        <v>2282</v>
+      </c>
+      <c r="L98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M98" t="inlineStr">
+        <is>
+          <t>2257</t>
         </is>
       </c>
     </row>
@@ -4555,9 +5123,15 @@
       <c r="J99" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="K99" t="inlineStr">
-        <is>
-          <t>3271</t>
+      <c r="K99" t="n">
+        <v>3271</v>
+      </c>
+      <c r="L99" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="M99" t="inlineStr">
+        <is>
+          <t>3398</t>
         </is>
       </c>
     </row>
@@ -4598,9 +5172,15 @@
       <c r="J100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K100" t="inlineStr">
-        <is>
-          <t>2463</t>
+      <c r="K100" t="n">
+        <v>2463</v>
+      </c>
+      <c r="L100" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="M100" t="inlineStr">
+        <is>
+          <t>2474</t>
         </is>
       </c>
     </row>
@@ -4641,9 +5221,15 @@
       <c r="J101" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K101" t="inlineStr">
-        <is>
-          <t>3891</t>
+      <c r="K101" t="n">
+        <v>3891</v>
+      </c>
+      <c r="L101" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M101" t="inlineStr">
+        <is>
+          <t>4054</t>
         </is>
       </c>
     </row>
@@ -4684,9 +5270,15 @@
       <c r="J102" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K102" t="inlineStr">
-        <is>
-          <t>3644</t>
+      <c r="K102" t="n">
+        <v>3644</v>
+      </c>
+      <c r="L102" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M102" t="inlineStr">
+        <is>
+          <t>3753</t>
         </is>
       </c>
     </row>
@@ -4727,9 +5319,15 @@
       <c r="J103" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="K103" t="inlineStr">
-        <is>
-          <t>3189</t>
+      <c r="K103" t="n">
+        <v>3189</v>
+      </c>
+      <c r="L103" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="M103" t="inlineStr">
+        <is>
+          <t>3245</t>
         </is>
       </c>
     </row>
@@ -4770,9 +5368,15 @@
       <c r="J104" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="K104" t="inlineStr">
-        <is>
-          <t>3968</t>
+      <c r="K104" t="n">
+        <v>3968</v>
+      </c>
+      <c r="L104" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="M104" t="inlineStr">
+        <is>
+          <t>4044</t>
         </is>
       </c>
     </row>
@@ -4813,9 +5417,15 @@
       <c r="J105" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K105" t="inlineStr">
-        <is>
-          <t>3663</t>
+      <c r="K105" t="n">
+        <v>3663</v>
+      </c>
+      <c r="L105" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="M105" t="inlineStr">
+        <is>
+          <t>3895</t>
         </is>
       </c>
     </row>
@@ -4856,7 +5466,13 @@
       <c r="J106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K106" t="inlineStr">
+      <c r="K106" t="n">
+        <v>2419</v>
+      </c>
+      <c r="L106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M106" t="inlineStr">
         <is>
           <t>2419</t>
         </is>
@@ -4899,9 +5515,15 @@
       <c r="J107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K107" t="inlineStr">
-        <is>
-          <t>2621</t>
+      <c r="K107" t="n">
+        <v>2621</v>
+      </c>
+      <c r="L107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M107" t="inlineStr">
+        <is>
+          <t>2620</t>
         </is>
       </c>
     </row>
@@ -4942,9 +5564,15 @@
       <c r="J108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K108" t="inlineStr">
-        <is>
-          <t>2621</t>
+      <c r="K108" t="n">
+        <v>2621</v>
+      </c>
+      <c r="L108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M108" t="inlineStr">
+        <is>
+          <t>2682</t>
         </is>
       </c>
     </row>
@@ -4985,9 +5613,15 @@
       <c r="J109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K109" t="inlineStr">
-        <is>
-          <t>3498</t>
+      <c r="K109" t="n">
+        <v>3498</v>
+      </c>
+      <c r="L109" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="M109" t="inlineStr">
+        <is>
+          <t>3669</t>
         </is>
       </c>
     </row>
@@ -5028,9 +5662,15 @@
       <c r="J110" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="K110" t="inlineStr">
-        <is>
-          <t>3347</t>
+      <c r="K110" t="n">
+        <v>3347</v>
+      </c>
+      <c r="L110" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="M110" t="inlineStr">
+        <is>
+          <t>3419</t>
         </is>
       </c>
     </row>
@@ -5071,9 +5711,15 @@
       <c r="J111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K111" t="inlineStr">
-        <is>
-          <t>2774</t>
+      <c r="K111" t="n">
+        <v>2774</v>
+      </c>
+      <c r="L111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M111" t="inlineStr">
+        <is>
+          <t>2809</t>
         </is>
       </c>
     </row>
@@ -5114,9 +5760,15 @@
       <c r="J112" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K112" t="inlineStr">
-        <is>
-          <t>3050</t>
+      <c r="K112" t="n">
+        <v>3050</v>
+      </c>
+      <c r="L112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M112" t="inlineStr">
+        <is>
+          <t>3058</t>
         </is>
       </c>
     </row>
@@ -5157,9 +5809,15 @@
       <c r="J113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K113" t="inlineStr">
-        <is>
-          <t>3111</t>
+      <c r="K113" t="n">
+        <v>3111</v>
+      </c>
+      <c r="L113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M113" t="inlineStr">
+        <is>
+          <t>3200</t>
         </is>
       </c>
     </row>
@@ -5200,9 +5858,15 @@
       <c r="J114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K114" t="inlineStr">
-        <is>
-          <t>3464</t>
+      <c r="K114" t="n">
+        <v>3464</v>
+      </c>
+      <c r="L114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M114" t="inlineStr">
+        <is>
+          <t>3559</t>
         </is>
       </c>
     </row>
@@ -5238,6 +5902,8 @@
       <c r="I115" t="inlineStr"/>
       <c r="J115" s="3" t="inlineStr"/>
       <c r="K115" t="inlineStr"/>
+      <c r="L115" s="3" t="inlineStr"/>
+      <c r="M115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -5276,9 +5942,15 @@
       <c r="J116" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="K116" t="inlineStr">
-        <is>
-          <t>2543</t>
+      <c r="K116" t="n">
+        <v>2543</v>
+      </c>
+      <c r="L116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M116" t="inlineStr">
+        <is>
+          <t>2513</t>
         </is>
       </c>
     </row>
@@ -5319,9 +5991,15 @@
       <c r="J117" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="K117" t="inlineStr">
-        <is>
-          <t>3053</t>
+      <c r="K117" t="n">
+        <v>3053</v>
+      </c>
+      <c r="L117" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="M117" t="inlineStr">
+        <is>
+          <t>3096</t>
         </is>
       </c>
     </row>
@@ -5362,9 +6040,15 @@
       <c r="J118" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K118" t="inlineStr">
-        <is>
-          <t>3365</t>
+      <c r="K118" t="n">
+        <v>3365</v>
+      </c>
+      <c r="L118" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M118" t="inlineStr">
+        <is>
+          <t>3512</t>
         </is>
       </c>
     </row>
@@ -5405,7 +6089,13 @@
       <c r="J119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K119" t="inlineStr">
+      <c r="K119" t="n">
+        <v>0</v>
+      </c>
+      <c r="L119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M119" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5448,9 +6138,15 @@
       <c r="J120" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K120" t="inlineStr">
-        <is>
-          <t>3604</t>
+      <c r="K120" t="n">
+        <v>3604</v>
+      </c>
+      <c r="L120" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="M120" t="inlineStr">
+        <is>
+          <t>3641</t>
         </is>
       </c>
     </row>
@@ -5491,9 +6187,15 @@
       <c r="J121" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="K121" t="inlineStr">
-        <is>
-          <t>2680</t>
+      <c r="K121" t="n">
+        <v>2680</v>
+      </c>
+      <c r="L121" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="M121" t="inlineStr">
+        <is>
+          <t>2702</t>
         </is>
       </c>
     </row>
@@ -5534,9 +6236,15 @@
       <c r="J122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K122" t="inlineStr">
-        <is>
-          <t>2872</t>
+      <c r="K122" t="n">
+        <v>2872</v>
+      </c>
+      <c r="L122" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="M122" t="inlineStr">
+        <is>
+          <t>2961</t>
         </is>
       </c>
     </row>
@@ -5577,9 +6285,15 @@
       <c r="J123" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="K123" t="inlineStr">
-        <is>
-          <t>2598</t>
+      <c r="K123" t="n">
+        <v>2598</v>
+      </c>
+      <c r="L123" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="M123" t="inlineStr">
+        <is>
+          <t>2642</t>
         </is>
       </c>
     </row>
@@ -5620,9 +6334,15 @@
       <c r="J124" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K124" t="inlineStr">
-        <is>
-          <t>3100</t>
+      <c r="K124" t="n">
+        <v>3100</v>
+      </c>
+      <c r="L124" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="M124" t="inlineStr">
+        <is>
+          <t>3108</t>
         </is>
       </c>
     </row>
@@ -5663,9 +6383,15 @@
       <c r="J125" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K125" t="inlineStr">
-        <is>
-          <t>3173</t>
+      <c r="K125" t="n">
+        <v>3173</v>
+      </c>
+      <c r="L125" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="M125" t="inlineStr">
+        <is>
+          <t>3152</t>
         </is>
       </c>
     </row>
@@ -5706,9 +6432,15 @@
       <c r="J126" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K126" t="inlineStr">
-        <is>
-          <t>3434</t>
+      <c r="K126" t="n">
+        <v>3434</v>
+      </c>
+      <c r="L126" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M126" t="inlineStr">
+        <is>
+          <t>3581</t>
         </is>
       </c>
     </row>
@@ -5749,9 +6481,15 @@
       <c r="J127" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K127" t="inlineStr">
-        <is>
-          <t>3074</t>
+      <c r="K127" t="n">
+        <v>3074</v>
+      </c>
+      <c r="L127" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M127" t="inlineStr">
+        <is>
+          <t>3153</t>
         </is>
       </c>
     </row>
@@ -5792,7 +6530,13 @@
       <c r="J128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K128" t="inlineStr">
+      <c r="K128" t="n">
+        <v>0</v>
+      </c>
+      <c r="L128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5835,7 +6579,13 @@
       <c r="J129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K129" t="inlineStr">
+      <c r="K129" t="n">
+        <v>0</v>
+      </c>
+      <c r="L129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5878,9 +6628,15 @@
       <c r="J130" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K130" t="inlineStr">
-        <is>
-          <t>2959</t>
+      <c r="K130" t="n">
+        <v>2959</v>
+      </c>
+      <c r="L130" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="M130" t="inlineStr">
+        <is>
+          <t>2960</t>
         </is>
       </c>
     </row>
@@ -5921,9 +6677,15 @@
       <c r="J131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K131" t="inlineStr">
-        <is>
-          <t>2767</t>
+      <c r="K131" t="n">
+        <v>2767</v>
+      </c>
+      <c r="L131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M131" t="inlineStr">
+        <is>
+          <t>2771</t>
         </is>
       </c>
     </row>
@@ -5964,7 +6726,13 @@
       <c r="J132" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K132" t="inlineStr">
+      <c r="K132" t="n">
+        <v>0</v>
+      </c>
+      <c r="L132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M132" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6007,9 +6775,15 @@
       <c r="J133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K133" t="inlineStr">
-        <is>
-          <t>2196</t>
+      <c r="K133" t="n">
+        <v>2196</v>
+      </c>
+      <c r="L133" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="M133" t="inlineStr">
+        <is>
+          <t>2191</t>
         </is>
       </c>
     </row>
@@ -6050,9 +6824,15 @@
       <c r="J134" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K134" t="inlineStr">
-        <is>
-          <t>3032</t>
+      <c r="K134" t="n">
+        <v>3032</v>
+      </c>
+      <c r="L134" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M134" t="inlineStr">
+        <is>
+          <t>3011</t>
         </is>
       </c>
     </row>
@@ -6093,7 +6873,13 @@
       <c r="J135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K135" t="inlineStr">
+      <c r="K135" t="n">
+        <v>2498</v>
+      </c>
+      <c r="L135" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M135" t="inlineStr">
         <is>
           <t>2498</t>
         </is>
@@ -6136,7 +6922,13 @@
       <c r="J136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K136" t="inlineStr">
+      <c r="K136" t="n">
+        <v>0</v>
+      </c>
+      <c r="L136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M136" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6179,11 +6971,11 @@
       <c r="J137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K137" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="K137" t="n">
+        <v>0</v>
+      </c>
+      <c r="L137" s="3" t="inlineStr"/>
+      <c r="M137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="n">
@@ -6222,9 +7014,15 @@
       <c r="J138" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="K138" t="inlineStr">
-        <is>
-          <t>3113</t>
+      <c r="K138" t="n">
+        <v>3113</v>
+      </c>
+      <c r="L138" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="M138" t="inlineStr">
+        <is>
+          <t>3051</t>
         </is>
       </c>
     </row>
@@ -6265,7 +7063,13 @@
       <c r="J139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K139" t="inlineStr">
+      <c r="K139" t="n">
+        <v>0</v>
+      </c>
+      <c r="L139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M139" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6308,9 +7112,15 @@
       <c r="J140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K140" t="inlineStr">
-        <is>
-          <t>2639</t>
+      <c r="K140" t="n">
+        <v>2639</v>
+      </c>
+      <c r="L140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M140" t="inlineStr">
+        <is>
+          <t>2655</t>
         </is>
       </c>
     </row>
@@ -6351,11 +7161,11 @@
       <c r="J141" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K141" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="K141" t="n">
+        <v>0</v>
+      </c>
+      <c r="L141" s="3" t="inlineStr"/>
+      <c r="M141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -6394,9 +7204,15 @@
       <c r="J142" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="K142" t="inlineStr">
-        <is>
-          <t>2838</t>
+      <c r="K142" t="n">
+        <v>2838</v>
+      </c>
+      <c r="L142" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M142" t="inlineStr">
+        <is>
+          <t>2951</t>
         </is>
       </c>
     </row>
@@ -6424,6 +7240,8 @@
       <c r="I143" t="inlineStr"/>
       <c r="J143" s="3" t="inlineStr"/>
       <c r="K143" t="inlineStr"/>
+      <c r="L143" s="3" t="inlineStr"/>
+      <c r="M143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -6462,9 +7280,15 @@
       <c r="J144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K144" t="inlineStr">
-        <is>
-          <t>2480</t>
+      <c r="K144" t="n">
+        <v>2480</v>
+      </c>
+      <c r="L144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M144" t="inlineStr">
+        <is>
+          <t>2493</t>
         </is>
       </c>
     </row>
@@ -6505,7 +7329,13 @@
       <c r="J145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K145" t="inlineStr">
+      <c r="K145" t="n">
+        <v>0</v>
+      </c>
+      <c r="L145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M145" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6548,7 +7378,13 @@
       <c r="J146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K146" t="inlineStr">
+      <c r="K146" t="n">
+        <v>0</v>
+      </c>
+      <c r="L146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6591,7 +7427,13 @@
       <c r="J147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K147" t="inlineStr">
+      <c r="K147" t="n">
+        <v>0</v>
+      </c>
+      <c r="L147" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M147" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6634,11 +7476,11 @@
       <c r="J148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K148" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="K148" t="n">
+        <v>0</v>
+      </c>
+      <c r="L148" s="3" t="inlineStr"/>
+      <c r="M148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="n">
@@ -6677,11 +7519,11 @@
       <c r="J149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K149" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="K149" t="n">
+        <v>0</v>
+      </c>
+      <c r="L149" s="3" t="inlineStr"/>
+      <c r="M149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="n">
@@ -6720,9 +7562,15 @@
       <c r="J150" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="K150" t="inlineStr">
-        <is>
-          <t>2493</t>
+      <c r="K150" t="n">
+        <v>2493</v>
+      </c>
+      <c r="L150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M150" t="inlineStr">
+        <is>
+          <t>2465</t>
         </is>
       </c>
     </row>
@@ -6763,7 +7611,13 @@
       <c r="J151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K151" t="inlineStr">
+      <c r="K151" t="n">
+        <v>0</v>
+      </c>
+      <c r="L151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M151" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6806,7 +7660,13 @@
       <c r="J152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K152" t="inlineStr">
+      <c r="K152" t="n">
+        <v>0</v>
+      </c>
+      <c r="L152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6849,9 +7709,15 @@
       <c r="J153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K153" t="inlineStr">
-        <is>
-          <t>1800</t>
+      <c r="K153" t="n">
+        <v>1800</v>
+      </c>
+      <c r="L153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M153" t="inlineStr">
+        <is>
+          <t>1782</t>
         </is>
       </c>
     </row>
@@ -6892,11 +7758,11 @@
       <c r="J154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K154" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="K154" t="n">
+        <v>0</v>
+      </c>
+      <c r="L154" s="3" t="inlineStr"/>
+      <c r="M154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" t="n">
@@ -6935,9 +7801,15 @@
       <c r="J155" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="K155" t="inlineStr">
-        <is>
-          <t>4375</t>
+      <c r="K155" t="n">
+        <v>4375</v>
+      </c>
+      <c r="L155" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="M155" t="inlineStr">
+        <is>
+          <t>4920</t>
         </is>
       </c>
     </row>
@@ -6978,7 +7850,13 @@
       <c r="J156" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K156" t="inlineStr">
+      <c r="K156" t="n">
+        <v>0</v>
+      </c>
+      <c r="L156" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M156" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7021,7 +7899,13 @@
       <c r="J157" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K157" t="inlineStr">
+      <c r="K157" t="n">
+        <v>2500</v>
+      </c>
+      <c r="L157" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M157" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -7064,9 +7948,15 @@
       <c r="J158" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="K158" t="inlineStr">
-        <is>
-          <t>4963</t>
+      <c r="K158" t="n">
+        <v>4963</v>
+      </c>
+      <c r="L158" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="M158" t="inlineStr">
+        <is>
+          <t>5179</t>
         </is>
       </c>
     </row>
@@ -7107,7 +7997,13 @@
       <c r="J159" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K159" t="inlineStr">
+      <c r="K159" t="n">
+        <v>0</v>
+      </c>
+      <c r="L159" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M159" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7150,9 +8046,15 @@
       <c r="J160" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K160" t="inlineStr">
-        <is>
-          <t>2857</t>
+      <c r="K160" t="n">
+        <v>2857</v>
+      </c>
+      <c r="L160" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M160" t="inlineStr">
+        <is>
+          <t>2943</t>
         </is>
       </c>
     </row>
@@ -7193,7 +8095,13 @@
       <c r="J161" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K161" t="inlineStr">
+      <c r="K161" t="n">
+        <v>0</v>
+      </c>
+      <c r="L161" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M161" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7236,9 +8144,15 @@
       <c r="J162" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K162" t="inlineStr">
-        <is>
-          <t>2895</t>
+      <c r="K162" t="n">
+        <v>2895</v>
+      </c>
+      <c r="L162" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M162" t="inlineStr">
+        <is>
+          <t>2955</t>
         </is>
       </c>
     </row>
@@ -7266,6 +8180,8 @@
       <c r="I163" t="inlineStr"/>
       <c r="J163" s="3" t="inlineStr"/>
       <c r="K163" t="inlineStr"/>
+      <c r="L163" s="3" t="inlineStr"/>
+      <c r="M163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" t="n">
@@ -7298,9 +8214,15 @@
       <c r="J164" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K164" t="inlineStr">
-        <is>
-          <t>2809</t>
+      <c r="K164" t="n">
+        <v>2809</v>
+      </c>
+      <c r="L164" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M164" t="inlineStr">
+        <is>
+          <t>2765</t>
         </is>
       </c>
     </row>
@@ -7335,11 +8257,11 @@
       <c r="J165" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="K165" t="inlineStr">
-        <is>
-          <t>2413</t>
-        </is>
-      </c>
+      <c r="K165" t="n">
+        <v>2413</v>
+      </c>
+      <c r="L165" s="3" t="inlineStr"/>
+      <c r="M165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" t="n">
@@ -7372,9 +8294,15 @@
       <c r="J166" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K166" t="inlineStr">
-        <is>
-          <t>2437</t>
+      <c r="K166" t="n">
+        <v>2437</v>
+      </c>
+      <c r="L166" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M166" t="inlineStr">
+        <is>
+          <t>2410</t>
         </is>
       </c>
     </row>
@@ -7409,9 +8337,15 @@
       <c r="J167" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K167" t="inlineStr">
-        <is>
-          <t>1460</t>
+      <c r="K167" t="n">
+        <v>1460</v>
+      </c>
+      <c r="L167" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M167" t="inlineStr">
+        <is>
+          <t>1439</t>
         </is>
       </c>
     </row>
@@ -7442,9 +8376,15 @@
       <c r="J168" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="K168" t="inlineStr">
-        <is>
-          <t>1615</t>
+      <c r="K168" t="n">
+        <v>1615</v>
+      </c>
+      <c r="L168" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="M168" t="inlineStr">
+        <is>
+          <t>1638</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-02-08 11:30:32
</commit_message>
<xml_diff>
--- a/Season_Attack/83.xlsx
+++ b/Season_Attack/83.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M168"/>
+  <dimension ref="A1:O168"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,6 +456,16 @@
           <t>02-06_0</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>02-07_A</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>02-07_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -500,9 +510,15 @@
       <c r="L2" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>3808</t>
+      <c r="M2" t="n">
+        <v>3808</v>
+      </c>
+      <c r="N2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>3875</t>
         </is>
       </c>
     </row>
@@ -549,9 +565,15 @@
       <c r="L3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>5294</t>
+      <c r="M3" t="n">
+        <v>5294</v>
+      </c>
+      <c r="N3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>5638</t>
         </is>
       </c>
     </row>
@@ -598,9 +620,15 @@
       <c r="L4" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>5035</t>
+      <c r="M4" t="n">
+        <v>5035</v>
+      </c>
+      <c r="N4" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>5193</t>
         </is>
       </c>
     </row>
@@ -647,9 +675,15 @@
       <c r="L5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>5263</t>
+      <c r="M5" t="n">
+        <v>5263</v>
+      </c>
+      <c r="N5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>5503</t>
         </is>
       </c>
     </row>
@@ -696,9 +730,15 @@
       <c r="L6" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>5149</t>
+      <c r="M6" t="n">
+        <v>5149</v>
+      </c>
+      <c r="N6" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>5359</t>
         </is>
       </c>
     </row>
@@ -745,9 +785,15 @@
       <c r="L7" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>5609</t>
+      <c r="M7" t="n">
+        <v>5609</v>
+      </c>
+      <c r="N7" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>5956</t>
         </is>
       </c>
     </row>
@@ -770,7 +816,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F8" s="3" t="n">
@@ -794,9 +840,15 @@
       <c r="L8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>4727</t>
+      <c r="M8" t="n">
+        <v>4727</v>
+      </c>
+      <c r="N8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>4907</t>
         </is>
       </c>
     </row>
@@ -834,6 +886,8 @@
       <c r="K9" t="inlineStr"/>
       <c r="L9" s="3" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
+      <c r="N9" s="3" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -878,9 +932,15 @@
       <c r="L10" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>4862</t>
+      <c r="M10" t="n">
+        <v>4862</v>
+      </c>
+      <c r="N10" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>5145</t>
         </is>
       </c>
     </row>
@@ -927,9 +987,15 @@
       <c r="L11" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>4908</t>
+      <c r="M11" t="n">
+        <v>4908</v>
+      </c>
+      <c r="N11" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>5408</t>
         </is>
       </c>
     </row>
@@ -976,9 +1042,15 @@
       <c r="L12" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>4635</t>
+      <c r="M12" t="n">
+        <v>4635</v>
+      </c>
+      <c r="N12" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>5003</t>
         </is>
       </c>
     </row>
@@ -1025,9 +1097,15 @@
       <c r="L13" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>2716</t>
+      <c r="M13" t="n">
+        <v>2716</v>
+      </c>
+      <c r="N13" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>2777</t>
         </is>
       </c>
     </row>
@@ -1074,9 +1152,15 @@
       <c r="L14" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>5882</t>
+      <c r="M14" t="n">
+        <v>5882</v>
+      </c>
+      <c r="N14" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>6178</t>
         </is>
       </c>
     </row>
@@ -1123,9 +1207,15 @@
       <c r="L15" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>5075</t>
+      <c r="M15" t="n">
+        <v>5075</v>
+      </c>
+      <c r="N15" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>5253</t>
         </is>
       </c>
     </row>
@@ -1172,9 +1262,15 @@
       <c r="L16" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>5163</t>
+      <c r="M16" t="n">
+        <v>5163</v>
+      </c>
+      <c r="N16" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>5535</t>
         </is>
       </c>
     </row>
@@ -1221,9 +1317,15 @@
       <c r="L17" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>4307</t>
+      <c r="M17" t="n">
+        <v>4307</v>
+      </c>
+      <c r="N17" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>4515</t>
         </is>
       </c>
     </row>
@@ -1270,9 +1372,15 @@
       <c r="L18" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>4457</t>
+      <c r="M18" t="n">
+        <v>4457</v>
+      </c>
+      <c r="N18" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>4742</t>
         </is>
       </c>
     </row>
@@ -1319,9 +1427,15 @@
       <c r="L19" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>5069</t>
+      <c r="M19" t="n">
+        <v>5069</v>
+      </c>
+      <c r="N19" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>5321</t>
         </is>
       </c>
     </row>
@@ -1368,9 +1482,15 @@
       <c r="L20" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>5895</t>
+      <c r="M20" t="n">
+        <v>5895</v>
+      </c>
+      <c r="N20" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>6158</t>
         </is>
       </c>
     </row>
@@ -1417,7 +1537,13 @@
       <c r="L21" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="M21" t="inlineStr">
+      <c r="M21" t="n">
+        <v>3923</v>
+      </c>
+      <c r="N21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O21" t="inlineStr">
         <is>
           <t>3923</t>
         </is>
@@ -1466,9 +1592,15 @@
       <c r="L22" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="M22" t="inlineStr">
-        <is>
-          <t>4949</t>
+      <c r="M22" t="n">
+        <v>4949</v>
+      </c>
+      <c r="N22" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>5160</t>
         </is>
       </c>
     </row>
@@ -1515,9 +1647,15 @@
       <c r="L23" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="M23" t="inlineStr">
-        <is>
-          <t>4669</t>
+      <c r="M23" t="n">
+        <v>4669</v>
+      </c>
+      <c r="N23" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>5122</t>
         </is>
       </c>
     </row>
@@ -1564,9 +1702,15 @@
       <c r="L24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="M24" t="inlineStr">
-        <is>
-          <t>5161</t>
+      <c r="M24" t="n">
+        <v>5161</v>
+      </c>
+      <c r="N24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>5408</t>
         </is>
       </c>
     </row>
@@ -1613,7 +1757,13 @@
       <c r="L25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M25" t="inlineStr">
+      <c r="M25" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1662,9 +1812,15 @@
       <c r="L26" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="M26" t="inlineStr">
-        <is>
-          <t>5334</t>
+      <c r="M26" t="n">
+        <v>5334</v>
+      </c>
+      <c r="N26" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>5597</t>
         </is>
       </c>
     </row>
@@ -1711,9 +1867,15 @@
       <c r="L27" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="M27" t="inlineStr">
-        <is>
-          <t>5530</t>
+      <c r="M27" t="n">
+        <v>5530</v>
+      </c>
+      <c r="N27" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>5792</t>
         </is>
       </c>
     </row>
@@ -1760,9 +1922,15 @@
       <c r="L28" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="M28" t="inlineStr">
-        <is>
-          <t>4128</t>
+      <c r="M28" t="n">
+        <v>4128</v>
+      </c>
+      <c r="N28" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>4677</t>
         </is>
       </c>
     </row>
@@ -1809,9 +1977,15 @@
       <c r="L29" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="M29" t="inlineStr">
-        <is>
-          <t>5476</t>
+      <c r="M29" t="n">
+        <v>5476</v>
+      </c>
+      <c r="N29" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>6000</t>
         </is>
       </c>
     </row>
@@ -1858,9 +2032,15 @@
       <c r="L30" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="M30" t="inlineStr">
-        <is>
-          <t>5304</t>
+      <c r="M30" t="n">
+        <v>5304</v>
+      </c>
+      <c r="N30" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>5538</t>
         </is>
       </c>
     </row>
@@ -1907,9 +2087,15 @@
       <c r="L31" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="M31" t="inlineStr">
-        <is>
-          <t>4814</t>
+      <c r="M31" t="n">
+        <v>4814</v>
+      </c>
+      <c r="N31" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>4937</t>
         </is>
       </c>
     </row>
@@ -1956,9 +2142,15 @@
       <c r="L32" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="M32" t="inlineStr">
-        <is>
-          <t>5515</t>
+      <c r="M32" t="n">
+        <v>5515</v>
+      </c>
+      <c r="N32" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>5743</t>
         </is>
       </c>
     </row>
@@ -2005,9 +2197,15 @@
       <c r="L33" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="M33" t="inlineStr">
-        <is>
-          <t>5425</t>
+      <c r="M33" t="n">
+        <v>5425</v>
+      </c>
+      <c r="N33" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>5777</t>
         </is>
       </c>
     </row>
@@ -2054,9 +2252,15 @@
       <c r="L34" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="M34" t="inlineStr">
-        <is>
-          <t>5221</t>
+      <c r="M34" t="n">
+        <v>5221</v>
+      </c>
+      <c r="N34" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>5410</t>
         </is>
       </c>
     </row>
@@ -2103,9 +2307,15 @@
       <c r="L35" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="M35" t="inlineStr">
-        <is>
-          <t>5532</t>
+      <c r="M35" t="n">
+        <v>5532</v>
+      </c>
+      <c r="N35" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>5826</t>
         </is>
       </c>
     </row>
@@ -2152,9 +2362,15 @@
       <c r="L36" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="M36" t="inlineStr">
-        <is>
-          <t>4881</t>
+      <c r="M36" t="n">
+        <v>4881</v>
+      </c>
+      <c r="N36" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>5141</t>
         </is>
       </c>
     </row>
@@ -2201,9 +2417,15 @@
       <c r="L37" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="M37" t="inlineStr">
-        <is>
-          <t>4534</t>
+      <c r="M37" t="n">
+        <v>4534</v>
+      </c>
+      <c r="N37" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>4712</t>
         </is>
       </c>
     </row>
@@ -2250,9 +2472,15 @@
       <c r="L38" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M38" t="inlineStr">
-        <is>
-          <t>5009</t>
+      <c r="M38" t="n">
+        <v>5009</v>
+      </c>
+      <c r="N38" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>5211</t>
         </is>
       </c>
     </row>
@@ -2299,9 +2527,15 @@
       <c r="L39" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="M39" t="inlineStr">
-        <is>
-          <t>4785</t>
+      <c r="M39" t="n">
+        <v>4785</v>
+      </c>
+      <c r="N39" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>5005</t>
         </is>
       </c>
     </row>
@@ -2348,9 +2582,15 @@
       <c r="L40" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="M40" t="inlineStr">
-        <is>
-          <t>5706</t>
+      <c r="M40" t="n">
+        <v>5706</v>
+      </c>
+      <c r="N40" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>5819</t>
         </is>
       </c>
     </row>
@@ -2397,9 +2637,15 @@
       <c r="L41" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M41" t="inlineStr">
-        <is>
-          <t>5066</t>
+      <c r="M41" t="n">
+        <v>5066</v>
+      </c>
+      <c r="N41" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>5346</t>
         </is>
       </c>
     </row>
@@ -2446,9 +2692,15 @@
       <c r="L42" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="M42" t="inlineStr">
-        <is>
-          <t>5770</t>
+      <c r="M42" t="n">
+        <v>5770</v>
+      </c>
+      <c r="N42" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>6163</t>
         </is>
       </c>
     </row>
@@ -2495,9 +2747,15 @@
       <c r="L43" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="M43" t="inlineStr">
-        <is>
-          <t>5070</t>
+      <c r="M43" t="n">
+        <v>5070</v>
+      </c>
+      <c r="N43" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>5442</t>
         </is>
       </c>
     </row>
@@ -2544,9 +2802,15 @@
       <c r="L44" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="M44" t="inlineStr">
-        <is>
-          <t>5124</t>
+      <c r="M44" t="n">
+        <v>5124</v>
+      </c>
+      <c r="N44" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>5295</t>
         </is>
       </c>
     </row>
@@ -2593,9 +2857,15 @@
       <c r="L45" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="M45" t="inlineStr">
-        <is>
-          <t>4487</t>
+      <c r="M45" t="n">
+        <v>4487</v>
+      </c>
+      <c r="N45" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>4771</t>
         </is>
       </c>
     </row>
@@ -2642,9 +2912,15 @@
       <c r="L46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M46" t="inlineStr">
-        <is>
-          <t>4467</t>
+      <c r="M46" t="n">
+        <v>4467</v>
+      </c>
+      <c r="N46" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>4977</t>
         </is>
       </c>
     </row>
@@ -2691,7 +2967,13 @@
       <c r="L47" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M47" t="inlineStr">
+      <c r="M47" t="n">
+        <v>3035</v>
+      </c>
+      <c r="N47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O47" t="inlineStr">
         <is>
           <t>3035</t>
         </is>
@@ -2740,9 +3022,15 @@
       <c r="L48" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="M48" t="inlineStr">
-        <is>
-          <t>5230</t>
+      <c r="M48" t="n">
+        <v>5230</v>
+      </c>
+      <c r="N48" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>5529</t>
         </is>
       </c>
     </row>
@@ -2789,9 +3077,15 @@
       <c r="L49" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="M49" t="inlineStr">
-        <is>
-          <t>4148</t>
+      <c r="M49" t="n">
+        <v>4148</v>
+      </c>
+      <c r="N49" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>4351</t>
         </is>
       </c>
     </row>
@@ -2838,9 +3132,15 @@
       <c r="L50" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="M50" t="inlineStr">
-        <is>
-          <t>5518</t>
+      <c r="M50" t="n">
+        <v>5518</v>
+      </c>
+      <c r="N50" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>5727</t>
         </is>
       </c>
     </row>
@@ -2887,9 +3187,15 @@
       <c r="L51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M51" t="inlineStr">
-        <is>
-          <t>2842</t>
+      <c r="M51" t="n">
+        <v>2842</v>
+      </c>
+      <c r="N51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>2839</t>
         </is>
       </c>
     </row>
@@ -2936,9 +3242,15 @@
       <c r="L52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M52" t="inlineStr">
-        <is>
-          <t>2782</t>
+      <c r="M52" t="n">
+        <v>2782</v>
+      </c>
+      <c r="N52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>2781</t>
         </is>
       </c>
     </row>
@@ -2985,9 +3297,15 @@
       <c r="L53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M53" t="inlineStr">
-        <is>
-          <t>2973</t>
+      <c r="M53" t="n">
+        <v>2973</v>
+      </c>
+      <c r="N53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>3008</t>
         </is>
       </c>
     </row>
@@ -3034,9 +3352,15 @@
       <c r="L54" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="M54" t="inlineStr">
-        <is>
-          <t>5047</t>
+      <c r="M54" t="n">
+        <v>5047</v>
+      </c>
+      <c r="N54" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>5272</t>
         </is>
       </c>
     </row>
@@ -3083,9 +3407,15 @@
       <c r="L55" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="M55" t="inlineStr">
-        <is>
-          <t>3984</t>
+      <c r="M55" t="n">
+        <v>3984</v>
+      </c>
+      <c r="N55" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>4160</t>
         </is>
       </c>
     </row>
@@ -3132,9 +3462,15 @@
       <c r="L56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M56" t="inlineStr">
-        <is>
-          <t>4059</t>
+      <c r="M56" t="n">
+        <v>4059</v>
+      </c>
+      <c r="N56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>4228</t>
         </is>
       </c>
     </row>
@@ -3181,9 +3517,15 @@
       <c r="L57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M57" t="inlineStr">
-        <is>
-          <t>4731</t>
+      <c r="M57" t="n">
+        <v>4731</v>
+      </c>
+      <c r="N57" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>4938</t>
         </is>
       </c>
     </row>
@@ -3230,9 +3572,15 @@
       <c r="L58" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="M58" t="inlineStr">
-        <is>
-          <t>4077</t>
+      <c r="M58" t="n">
+        <v>4077</v>
+      </c>
+      <c r="N58" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>4125</t>
         </is>
       </c>
     </row>
@@ -3279,9 +3627,15 @@
       <c r="L59" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="M59" t="inlineStr">
-        <is>
-          <t>4611</t>
+      <c r="M59" t="n">
+        <v>4611</v>
+      </c>
+      <c r="N59" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O59" t="inlineStr">
+        <is>
+          <t>4768</t>
         </is>
       </c>
     </row>
@@ -3328,7 +3682,13 @@
       <c r="L60" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M60" t="inlineStr">
+      <c r="M60" t="n">
+        <v>0</v>
+      </c>
+      <c r="N60" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O60" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3377,9 +3737,15 @@
       <c r="L61" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="M61" t="inlineStr">
-        <is>
-          <t>4884</t>
+      <c r="M61" t="n">
+        <v>4884</v>
+      </c>
+      <c r="N61" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>5063</t>
         </is>
       </c>
     </row>
@@ -3426,7 +3792,13 @@
       <c r="L62" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="M62" t="inlineStr">
+      <c r="M62" t="n">
+        <v>3036</v>
+      </c>
+      <c r="N62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O62" t="inlineStr">
         <is>
           <t>3036</t>
         </is>
@@ -3475,9 +3847,15 @@
       <c r="L63" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M63" t="inlineStr">
-        <is>
-          <t>3253</t>
+      <c r="M63" t="n">
+        <v>3253</v>
+      </c>
+      <c r="N63" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>3317</t>
         </is>
       </c>
     </row>
@@ -3524,9 +3902,15 @@
       <c r="L64" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="M64" t="inlineStr">
-        <is>
-          <t>4610</t>
+      <c r="M64" t="n">
+        <v>4610</v>
+      </c>
+      <c r="N64" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="O64" t="inlineStr">
+        <is>
+          <t>4744</t>
         </is>
       </c>
     </row>
@@ -3556,6 +3940,8 @@
       <c r="K65" t="inlineStr"/>
       <c r="L65" s="3" t="inlineStr"/>
       <c r="M65" t="inlineStr"/>
+      <c r="N65" s="3" t="inlineStr"/>
+      <c r="O65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -3600,9 +3986,15 @@
       <c r="L66" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M66" t="inlineStr">
-        <is>
-          <t>5097</t>
+      <c r="M66" t="n">
+        <v>5097</v>
+      </c>
+      <c r="N66" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>5287</t>
         </is>
       </c>
     </row>
@@ -3649,9 +4041,15 @@
       <c r="L67" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="M67" t="inlineStr">
-        <is>
-          <t>4174</t>
+      <c r="M67" t="n">
+        <v>4174</v>
+      </c>
+      <c r="N67" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>4257</t>
         </is>
       </c>
     </row>
@@ -3698,9 +4096,15 @@
       <c r="L68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M68" t="inlineStr">
-        <is>
-          <t>2555</t>
+      <c r="M68" t="n">
+        <v>2555</v>
+      </c>
+      <c r="N68" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O68" t="inlineStr">
+        <is>
+          <t>3132</t>
         </is>
       </c>
     </row>
@@ -3747,9 +4151,15 @@
       <c r="L69" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="M69" t="inlineStr">
-        <is>
-          <t>4029</t>
+      <c r="M69" t="n">
+        <v>4029</v>
+      </c>
+      <c r="N69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>4142</t>
         </is>
       </c>
     </row>
@@ -3796,9 +4206,15 @@
       <c r="L70" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="M70" t="inlineStr">
-        <is>
-          <t>3764</t>
+      <c r="M70" t="n">
+        <v>3764</v>
+      </c>
+      <c r="N70" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="O70" t="inlineStr">
+        <is>
+          <t>3852</t>
         </is>
       </c>
     </row>
@@ -3845,9 +4261,15 @@
       <c r="L71" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M71" t="inlineStr">
-        <is>
-          <t>4050</t>
+      <c r="M71" t="n">
+        <v>4050</v>
+      </c>
+      <c r="N71" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>4257</t>
         </is>
       </c>
     </row>
@@ -3894,9 +4316,15 @@
       <c r="L72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M72" t="inlineStr">
-        <is>
-          <t>2832</t>
+      <c r="M72" t="n">
+        <v>2832</v>
+      </c>
+      <c r="N72" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O72" t="inlineStr">
+        <is>
+          <t>3248</t>
         </is>
       </c>
     </row>
@@ -3943,9 +4371,15 @@
       <c r="L73" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="M73" t="inlineStr">
-        <is>
-          <t>3679</t>
+      <c r="M73" t="n">
+        <v>3679</v>
+      </c>
+      <c r="N73" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>3853</t>
         </is>
       </c>
     </row>
@@ -3992,9 +4426,15 @@
       <c r="L74" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="M74" t="inlineStr">
-        <is>
-          <t>4592</t>
+      <c r="M74" t="n">
+        <v>4592</v>
+      </c>
+      <c r="N74" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>4809</t>
         </is>
       </c>
     </row>
@@ -4041,9 +4481,15 @@
       <c r="L75" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M75" t="inlineStr">
-        <is>
-          <t>4653</t>
+      <c r="M75" t="n">
+        <v>4653</v>
+      </c>
+      <c r="N75" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>4837</t>
         </is>
       </c>
     </row>
@@ -4073,6 +4519,8 @@
       <c r="K76" t="inlineStr"/>
       <c r="L76" s="3" t="inlineStr"/>
       <c r="M76" t="inlineStr"/>
+      <c r="N76" s="3" t="inlineStr"/>
+      <c r="O76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -4117,9 +4565,15 @@
       <c r="L77" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M77" t="inlineStr">
-        <is>
-          <t>4697</t>
+      <c r="M77" t="n">
+        <v>4697</v>
+      </c>
+      <c r="N77" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>4899</t>
         </is>
       </c>
     </row>
@@ -4166,7 +4620,13 @@
       <c r="L78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M78" t="inlineStr">
+      <c r="M78" t="n">
+        <v>2500</v>
+      </c>
+      <c r="N78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O78" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -4215,9 +4675,15 @@
       <c r="L79" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M79" t="inlineStr">
-        <is>
-          <t>4256</t>
+      <c r="M79" t="n">
+        <v>4256</v>
+      </c>
+      <c r="N79" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>4433</t>
         </is>
       </c>
     </row>
@@ -4264,9 +4730,15 @@
       <c r="L80" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="M80" t="inlineStr">
-        <is>
-          <t>4581</t>
+      <c r="M80" t="n">
+        <v>4581</v>
+      </c>
+      <c r="N80" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>4691</t>
         </is>
       </c>
     </row>
@@ -4313,9 +4785,15 @@
       <c r="L81" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="M81" t="inlineStr">
-        <is>
-          <t>4381</t>
+      <c r="M81" t="n">
+        <v>4381</v>
+      </c>
+      <c r="N81" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>4509</t>
         </is>
       </c>
     </row>
@@ -4362,9 +4840,15 @@
       <c r="L82" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="M82" t="inlineStr">
-        <is>
-          <t>4145</t>
+      <c r="M82" t="n">
+        <v>4145</v>
+      </c>
+      <c r="N82" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>4267</t>
         </is>
       </c>
     </row>
@@ -4394,6 +4878,8 @@
       <c r="K83" t="inlineStr"/>
       <c r="L83" s="3" t="inlineStr"/>
       <c r="M83" t="inlineStr"/>
+      <c r="N83" s="3" t="inlineStr"/>
+      <c r="O83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -4438,9 +4924,15 @@
       <c r="L84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M84" t="inlineStr">
-        <is>
-          <t>3151</t>
+      <c r="M84" t="n">
+        <v>3151</v>
+      </c>
+      <c r="N84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>3249</t>
         </is>
       </c>
     </row>
@@ -4487,9 +4979,15 @@
       <c r="L85" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M85" t="inlineStr">
-        <is>
-          <t>3177</t>
+      <c r="M85" t="n">
+        <v>3177</v>
+      </c>
+      <c r="N85" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>3482</t>
         </is>
       </c>
     </row>
@@ -4536,9 +5034,15 @@
       <c r="L86" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="M86" t="inlineStr">
-        <is>
-          <t>4469</t>
+      <c r="M86" t="n">
+        <v>4469</v>
+      </c>
+      <c r="N86" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="O86" t="inlineStr">
+        <is>
+          <t>4628</t>
         </is>
       </c>
     </row>
@@ -4585,9 +5089,15 @@
       <c r="L87" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M87" t="inlineStr">
-        <is>
-          <t>2984</t>
+      <c r="M87" t="n">
+        <v>2984</v>
+      </c>
+      <c r="N87" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O87" t="inlineStr">
+        <is>
+          <t>2976</t>
         </is>
       </c>
     </row>
@@ -4634,9 +5144,15 @@
       <c r="L88" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="M88" t="inlineStr">
-        <is>
-          <t>3244</t>
+      <c r="M88" t="n">
+        <v>3244</v>
+      </c>
+      <c r="N88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O88" t="inlineStr">
+        <is>
+          <t>3183</t>
         </is>
       </c>
     </row>
@@ -4666,6 +5182,8 @@
       <c r="K89" t="inlineStr"/>
       <c r="L89" s="3" t="inlineStr"/>
       <c r="M89" t="inlineStr"/>
+      <c r="N89" s="3" t="inlineStr"/>
+      <c r="O89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -4710,9 +5228,15 @@
       <c r="L90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M90" t="inlineStr">
-        <is>
-          <t>2668</t>
+      <c r="M90" t="n">
+        <v>2668</v>
+      </c>
+      <c r="N90" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>2782</t>
         </is>
       </c>
     </row>
@@ -4742,6 +5266,8 @@
       <c r="K91" t="inlineStr"/>
       <c r="L91" s="3" t="inlineStr"/>
       <c r="M91" t="inlineStr"/>
+      <c r="N91" s="3" t="inlineStr"/>
+      <c r="O91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -4786,9 +5312,15 @@
       <c r="L92" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M92" t="inlineStr">
-        <is>
-          <t>2679</t>
+      <c r="M92" t="n">
+        <v>2679</v>
+      </c>
+      <c r="N92" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="O92" t="inlineStr">
+        <is>
+          <t>2693</t>
         </is>
       </c>
     </row>
@@ -4835,9 +5367,15 @@
       <c r="L93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M93" t="inlineStr">
-        <is>
-          <t>2779</t>
+      <c r="M93" t="n">
+        <v>2779</v>
+      </c>
+      <c r="N93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O93" t="inlineStr">
+        <is>
+          <t>2741</t>
         </is>
       </c>
     </row>
@@ -4884,9 +5422,15 @@
       <c r="L94" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M94" t="inlineStr">
-        <is>
-          <t>2890</t>
+      <c r="M94" t="n">
+        <v>2890</v>
+      </c>
+      <c r="N94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O94" t="inlineStr">
+        <is>
+          <t>2937</t>
         </is>
       </c>
     </row>
@@ -4933,9 +5477,15 @@
       <c r="L95" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="M95" t="inlineStr">
-        <is>
-          <t>2758</t>
+      <c r="M95" t="n">
+        <v>2758</v>
+      </c>
+      <c r="N95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O95" t="inlineStr">
+        <is>
+          <t>2736</t>
         </is>
       </c>
     </row>
@@ -4982,9 +5532,15 @@
       <c r="L96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M96" t="inlineStr">
-        <is>
-          <t>2111</t>
+      <c r="M96" t="n">
+        <v>2111</v>
+      </c>
+      <c r="N96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O96" t="inlineStr">
+        <is>
+          <t>2133</t>
         </is>
       </c>
     </row>
@@ -5031,9 +5587,15 @@
       <c r="L97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M97" t="inlineStr">
-        <is>
-          <t>2669</t>
+      <c r="M97" t="n">
+        <v>2669</v>
+      </c>
+      <c r="N97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O97" t="inlineStr">
+        <is>
+          <t>2668</t>
         </is>
       </c>
     </row>
@@ -5080,9 +5642,15 @@
       <c r="L98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M98" t="inlineStr">
-        <is>
-          <t>2257</t>
+      <c r="M98" t="n">
+        <v>2257</v>
+      </c>
+      <c r="N98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O98" t="inlineStr">
+        <is>
+          <t>2249</t>
         </is>
       </c>
     </row>
@@ -5129,9 +5697,15 @@
       <c r="L99" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="M99" t="inlineStr">
-        <is>
-          <t>3398</t>
+      <c r="M99" t="n">
+        <v>3398</v>
+      </c>
+      <c r="N99" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="O99" t="inlineStr">
+        <is>
+          <t>3709</t>
         </is>
       </c>
     </row>
@@ -5178,9 +5752,15 @@
       <c r="L100" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="M100" t="inlineStr">
-        <is>
-          <t>2474</t>
+      <c r="M100" t="n">
+        <v>2474</v>
+      </c>
+      <c r="N100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O100" t="inlineStr">
+        <is>
+          <t>2490</t>
         </is>
       </c>
     </row>
@@ -5227,9 +5807,15 @@
       <c r="L101" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M101" t="inlineStr">
-        <is>
-          <t>4054</t>
+      <c r="M101" t="n">
+        <v>4054</v>
+      </c>
+      <c r="N101" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O101" t="inlineStr">
+        <is>
+          <t>4151</t>
         </is>
       </c>
     </row>
@@ -5276,9 +5862,15 @@
       <c r="L102" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M102" t="inlineStr">
-        <is>
-          <t>3753</t>
+      <c r="M102" t="n">
+        <v>3753</v>
+      </c>
+      <c r="N102" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O102" t="inlineStr">
+        <is>
+          <t>3899</t>
         </is>
       </c>
     </row>
@@ -5325,9 +5917,15 @@
       <c r="L103" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="M103" t="inlineStr">
-        <is>
-          <t>3245</t>
+      <c r="M103" t="n">
+        <v>3245</v>
+      </c>
+      <c r="N103" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="O103" t="inlineStr">
+        <is>
+          <t>3632</t>
         </is>
       </c>
     </row>
@@ -5374,9 +5972,15 @@
       <c r="L104" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="M104" t="inlineStr">
-        <is>
-          <t>4044</t>
+      <c r="M104" t="n">
+        <v>4044</v>
+      </c>
+      <c r="N104" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="O104" t="inlineStr">
+        <is>
+          <t>4185</t>
         </is>
       </c>
     </row>
@@ -5423,9 +6027,15 @@
       <c r="L105" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="M105" t="inlineStr">
-        <is>
-          <t>3895</t>
+      <c r="M105" t="n">
+        <v>3895</v>
+      </c>
+      <c r="N105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O105" t="inlineStr">
+        <is>
+          <t>3802</t>
         </is>
       </c>
     </row>
@@ -5472,9 +6082,15 @@
       <c r="L106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M106" t="inlineStr">
-        <is>
-          <t>2419</t>
+      <c r="M106" t="n">
+        <v>2419</v>
+      </c>
+      <c r="N106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O106" t="inlineStr">
+        <is>
+          <t>2388</t>
         </is>
       </c>
     </row>
@@ -5521,9 +6137,15 @@
       <c r="L107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M107" t="inlineStr">
-        <is>
-          <t>2620</t>
+      <c r="M107" t="n">
+        <v>2620</v>
+      </c>
+      <c r="N107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O107" t="inlineStr">
+        <is>
+          <t>2667</t>
         </is>
       </c>
     </row>
@@ -5570,9 +6192,15 @@
       <c r="L108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M108" t="inlineStr">
-        <is>
-          <t>2682</t>
+      <c r="M108" t="n">
+        <v>2682</v>
+      </c>
+      <c r="N108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O108" t="inlineStr">
+        <is>
+          <t>2713</t>
         </is>
       </c>
     </row>
@@ -5619,9 +6247,15 @@
       <c r="L109" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="M109" t="inlineStr">
-        <is>
-          <t>3669</t>
+      <c r="M109" t="n">
+        <v>3669</v>
+      </c>
+      <c r="N109" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O109" t="inlineStr">
+        <is>
+          <t>3841</t>
         </is>
       </c>
     </row>
@@ -5668,9 +6302,15 @@
       <c r="L110" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="M110" t="inlineStr">
-        <is>
-          <t>3419</t>
+      <c r="M110" t="n">
+        <v>3419</v>
+      </c>
+      <c r="N110" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="O110" t="inlineStr">
+        <is>
+          <t>3490</t>
         </is>
       </c>
     </row>
@@ -5717,9 +6357,15 @@
       <c r="L111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M111" t="inlineStr">
-        <is>
-          <t>2809</t>
+      <c r="M111" t="n">
+        <v>2809</v>
+      </c>
+      <c r="N111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O111" t="inlineStr">
+        <is>
+          <t>2851</t>
         </is>
       </c>
     </row>
@@ -5766,9 +6412,15 @@
       <c r="L112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M112" t="inlineStr">
-        <is>
-          <t>3058</t>
+      <c r="M112" t="n">
+        <v>3058</v>
+      </c>
+      <c r="N112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O112" t="inlineStr">
+        <is>
+          <t>3099</t>
         </is>
       </c>
     </row>
@@ -5815,9 +6467,15 @@
       <c r="L113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M113" t="inlineStr">
-        <is>
-          <t>3200</t>
+      <c r="M113" t="n">
+        <v>3200</v>
+      </c>
+      <c r="N113" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="O113" t="inlineStr">
+        <is>
+          <t>3252</t>
         </is>
       </c>
     </row>
@@ -5864,9 +6522,15 @@
       <c r="L114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M114" t="inlineStr">
-        <is>
-          <t>3559</t>
+      <c r="M114" t="n">
+        <v>3559</v>
+      </c>
+      <c r="N114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O114" t="inlineStr">
+        <is>
+          <t>3584</t>
         </is>
       </c>
     </row>
@@ -5904,6 +6568,8 @@
       <c r="K115" t="inlineStr"/>
       <c r="L115" s="3" t="inlineStr"/>
       <c r="M115" t="inlineStr"/>
+      <c r="N115" s="3" t="inlineStr"/>
+      <c r="O115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -5948,9 +6614,15 @@
       <c r="L116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M116" t="inlineStr">
-        <is>
-          <t>2513</t>
+      <c r="M116" t="n">
+        <v>2513</v>
+      </c>
+      <c r="N116" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="O116" t="inlineStr">
+        <is>
+          <t>2535</t>
         </is>
       </c>
     </row>
@@ -5997,9 +6669,15 @@
       <c r="L117" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="M117" t="inlineStr">
-        <is>
-          <t>3096</t>
+      <c r="M117" t="n">
+        <v>3096</v>
+      </c>
+      <c r="N117" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="O117" t="inlineStr">
+        <is>
+          <t>3132</t>
         </is>
       </c>
     </row>
@@ -6046,9 +6724,15 @@
       <c r="L118" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M118" t="inlineStr">
-        <is>
-          <t>3512</t>
+      <c r="M118" t="n">
+        <v>3512</v>
+      </c>
+      <c r="N118" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="O118" t="inlineStr">
+        <is>
+          <t>3474</t>
         </is>
       </c>
     </row>
@@ -6095,7 +6779,13 @@
       <c r="L119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M119" t="inlineStr">
+      <c r="M119" t="n">
+        <v>0</v>
+      </c>
+      <c r="N119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O119" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6144,9 +6834,15 @@
       <c r="L120" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="M120" t="inlineStr">
-        <is>
-          <t>3641</t>
+      <c r="M120" t="n">
+        <v>3641</v>
+      </c>
+      <c r="N120" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="O120" t="inlineStr">
+        <is>
+          <t>3756</t>
         </is>
       </c>
     </row>
@@ -6193,9 +6889,15 @@
       <c r="L121" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="M121" t="inlineStr">
-        <is>
-          <t>2702</t>
+      <c r="M121" t="n">
+        <v>2702</v>
+      </c>
+      <c r="N121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O121" t="inlineStr">
+        <is>
+          <t>2691</t>
         </is>
       </c>
     </row>
@@ -6242,9 +6944,15 @@
       <c r="L122" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="M122" t="inlineStr">
-        <is>
-          <t>2961</t>
+      <c r="M122" t="n">
+        <v>2961</v>
+      </c>
+      <c r="N122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O122" t="inlineStr">
+        <is>
+          <t>3023</t>
         </is>
       </c>
     </row>
@@ -6291,9 +6999,15 @@
       <c r="L123" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="M123" t="inlineStr">
-        <is>
-          <t>2642</t>
+      <c r="M123" t="n">
+        <v>2642</v>
+      </c>
+      <c r="N123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O123" t="inlineStr">
+        <is>
+          <t>2623</t>
         </is>
       </c>
     </row>
@@ -6340,9 +7054,15 @@
       <c r="L124" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="M124" t="inlineStr">
-        <is>
-          <t>3108</t>
+      <c r="M124" t="n">
+        <v>3108</v>
+      </c>
+      <c r="N124" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O124" t="inlineStr">
+        <is>
+          <t>3216</t>
         </is>
       </c>
     </row>
@@ -6389,9 +7109,15 @@
       <c r="L125" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="M125" t="inlineStr">
-        <is>
-          <t>3152</t>
+      <c r="M125" t="n">
+        <v>3152</v>
+      </c>
+      <c r="N125" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O125" t="inlineStr">
+        <is>
+          <t>3239</t>
         </is>
       </c>
     </row>
@@ -6438,9 +7164,15 @@
       <c r="L126" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M126" t="inlineStr">
-        <is>
-          <t>3581</t>
+      <c r="M126" t="n">
+        <v>3581</v>
+      </c>
+      <c r="N126" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O126" t="inlineStr">
+        <is>
+          <t>3699</t>
         </is>
       </c>
     </row>
@@ -6487,9 +7219,15 @@
       <c r="L127" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M127" t="inlineStr">
-        <is>
-          <t>3153</t>
+      <c r="M127" t="n">
+        <v>3153</v>
+      </c>
+      <c r="N127" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O127" t="inlineStr">
+        <is>
+          <t>3218</t>
         </is>
       </c>
     </row>
@@ -6536,7 +7274,13 @@
       <c r="L128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M128" t="inlineStr">
+      <c r="M128" t="n">
+        <v>0</v>
+      </c>
+      <c r="N128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6585,7 +7329,13 @@
       <c r="L129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M129" t="inlineStr">
+      <c r="M129" t="n">
+        <v>0</v>
+      </c>
+      <c r="N129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6634,9 +7384,15 @@
       <c r="L130" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="M130" t="inlineStr">
-        <is>
-          <t>2960</t>
+      <c r="M130" t="n">
+        <v>2960</v>
+      </c>
+      <c r="N130" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O130" t="inlineStr">
+        <is>
+          <t>2988</t>
         </is>
       </c>
     </row>
@@ -6683,9 +7439,15 @@
       <c r="L131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M131" t="inlineStr">
-        <is>
-          <t>2771</t>
+      <c r="M131" t="n">
+        <v>2771</v>
+      </c>
+      <c r="N131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O131" t="inlineStr">
+        <is>
+          <t>2791</t>
         </is>
       </c>
     </row>
@@ -6732,7 +7494,13 @@
       <c r="L132" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M132" t="inlineStr">
+      <c r="M132" t="n">
+        <v>0</v>
+      </c>
+      <c r="N132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O132" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6781,9 +7549,15 @@
       <c r="L133" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="M133" t="inlineStr">
-        <is>
-          <t>2191</t>
+      <c r="M133" t="n">
+        <v>2191</v>
+      </c>
+      <c r="N133" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="O133" t="inlineStr">
+        <is>
+          <t>2186</t>
         </is>
       </c>
     </row>
@@ -6830,9 +7604,15 @@
       <c r="L134" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M134" t="inlineStr">
-        <is>
-          <t>3011</t>
+      <c r="M134" t="n">
+        <v>3011</v>
+      </c>
+      <c r="N134" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O134" t="inlineStr">
+        <is>
+          <t>3003</t>
         </is>
       </c>
     </row>
@@ -6879,7 +7659,13 @@
       <c r="L135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M135" t="inlineStr">
+      <c r="M135" t="n">
+        <v>2498</v>
+      </c>
+      <c r="N135" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O135" t="inlineStr">
         <is>
           <t>2498</t>
         </is>
@@ -6928,7 +7714,13 @@
       <c r="L136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M136" t="inlineStr">
+      <c r="M136" t="n">
+        <v>0</v>
+      </c>
+      <c r="N136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O136" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6976,6 +7768,8 @@
       </c>
       <c r="L137" s="3" t="inlineStr"/>
       <c r="M137" t="inlineStr"/>
+      <c r="N137" s="3" t="inlineStr"/>
+      <c r="O137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="n">
@@ -7020,9 +7814,15 @@
       <c r="L138" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="M138" t="inlineStr">
-        <is>
-          <t>3051</t>
+      <c r="M138" t="n">
+        <v>3051</v>
+      </c>
+      <c r="N138" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O138" t="inlineStr">
+        <is>
+          <t>3026</t>
         </is>
       </c>
     </row>
@@ -7069,7 +7869,13 @@
       <c r="L139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M139" t="inlineStr">
+      <c r="M139" t="n">
+        <v>0</v>
+      </c>
+      <c r="N139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O139" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7118,9 +7924,15 @@
       <c r="L140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M140" t="inlineStr">
-        <is>
-          <t>2655</t>
+      <c r="M140" t="n">
+        <v>2655</v>
+      </c>
+      <c r="N140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O140" t="inlineStr">
+        <is>
+          <t>2679</t>
         </is>
       </c>
     </row>
@@ -7166,6 +7978,8 @@
       </c>
       <c r="L141" s="3" t="inlineStr"/>
       <c r="M141" t="inlineStr"/>
+      <c r="N141" s="3" t="inlineStr"/>
+      <c r="O141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -7210,9 +8024,15 @@
       <c r="L142" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M142" t="inlineStr">
-        <is>
-          <t>2951</t>
+      <c r="M142" t="n">
+        <v>2951</v>
+      </c>
+      <c r="N142" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O142" t="inlineStr">
+        <is>
+          <t>2980</t>
         </is>
       </c>
     </row>
@@ -7242,6 +8062,8 @@
       <c r="K143" t="inlineStr"/>
       <c r="L143" s="3" t="inlineStr"/>
       <c r="M143" t="inlineStr"/>
+      <c r="N143" s="3" t="inlineStr"/>
+      <c r="O143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -7286,9 +8108,15 @@
       <c r="L144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M144" t="inlineStr">
-        <is>
-          <t>2493</t>
+      <c r="M144" t="n">
+        <v>2493</v>
+      </c>
+      <c r="N144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O144" t="inlineStr">
+        <is>
+          <t>2487</t>
         </is>
       </c>
     </row>
@@ -7335,7 +8163,13 @@
       <c r="L145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M145" t="inlineStr">
+      <c r="M145" t="n">
+        <v>0</v>
+      </c>
+      <c r="N145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O145" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7384,7 +8218,13 @@
       <c r="L146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M146" t="inlineStr">
+      <c r="M146" t="n">
+        <v>0</v>
+      </c>
+      <c r="N146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7433,7 +8273,13 @@
       <c r="L147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M147" t="inlineStr">
+      <c r="M147" t="n">
+        <v>0</v>
+      </c>
+      <c r="N147" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O147" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7481,6 +8327,8 @@
       </c>
       <c r="L148" s="3" t="inlineStr"/>
       <c r="M148" t="inlineStr"/>
+      <c r="N148" s="3" t="inlineStr"/>
+      <c r="O148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="n">
@@ -7524,6 +8372,8 @@
       </c>
       <c r="L149" s="3" t="inlineStr"/>
       <c r="M149" t="inlineStr"/>
+      <c r="N149" s="3" t="inlineStr"/>
+      <c r="O149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="n">
@@ -7568,9 +8418,15 @@
       <c r="L150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M150" t="inlineStr">
-        <is>
-          <t>2465</t>
+      <c r="M150" t="n">
+        <v>2465</v>
+      </c>
+      <c r="N150" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="O150" t="inlineStr">
+        <is>
+          <t>2476</t>
         </is>
       </c>
     </row>
@@ -7617,7 +8473,13 @@
       <c r="L151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M151" t="inlineStr">
+      <c r="M151" t="n">
+        <v>0</v>
+      </c>
+      <c r="N151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O151" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7666,7 +8528,13 @@
       <c r="L152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M152" t="inlineStr">
+      <c r="M152" t="n">
+        <v>0</v>
+      </c>
+      <c r="N152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7715,9 +8583,15 @@
       <c r="L153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M153" t="inlineStr">
-        <is>
-          <t>1782</t>
+      <c r="M153" t="n">
+        <v>1782</v>
+      </c>
+      <c r="N153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O153" t="inlineStr">
+        <is>
+          <t>1796</t>
         </is>
       </c>
     </row>
@@ -7763,6 +8637,8 @@
       </c>
       <c r="L154" s="3" t="inlineStr"/>
       <c r="M154" t="inlineStr"/>
+      <c r="N154" s="3" t="inlineStr"/>
+      <c r="O154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" t="n">
@@ -7807,9 +8683,15 @@
       <c r="L155" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="M155" t="inlineStr">
-        <is>
-          <t>4920</t>
+      <c r="M155" t="n">
+        <v>4920</v>
+      </c>
+      <c r="N155" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="O155" t="inlineStr">
+        <is>
+          <t>5160</t>
         </is>
       </c>
     </row>
@@ -7856,7 +8738,13 @@
       <c r="L156" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M156" t="inlineStr">
+      <c r="M156" t="n">
+        <v>0</v>
+      </c>
+      <c r="N156" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O156" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7905,7 +8793,13 @@
       <c r="L157" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M157" t="inlineStr">
+      <c r="M157" t="n">
+        <v>2500</v>
+      </c>
+      <c r="N157" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O157" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -7954,9 +8848,15 @@
       <c r="L158" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="M158" t="inlineStr">
-        <is>
-          <t>5179</t>
+      <c r="M158" t="n">
+        <v>5179</v>
+      </c>
+      <c r="N158" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="O158" t="inlineStr">
+        <is>
+          <t>5504</t>
         </is>
       </c>
     </row>
@@ -8003,7 +8903,13 @@
       <c r="L159" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M159" t="inlineStr">
+      <c r="M159" t="n">
+        <v>0</v>
+      </c>
+      <c r="N159" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O159" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8052,9 +8958,15 @@
       <c r="L160" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M160" t="inlineStr">
-        <is>
-          <t>2943</t>
+      <c r="M160" t="n">
+        <v>2943</v>
+      </c>
+      <c r="N160" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="O160" t="inlineStr">
+        <is>
+          <t>3041</t>
         </is>
       </c>
     </row>
@@ -8101,7 +9013,13 @@
       <c r="L161" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M161" t="inlineStr">
+      <c r="M161" t="n">
+        <v>0</v>
+      </c>
+      <c r="N161" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O161" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8150,9 +9068,15 @@
       <c r="L162" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M162" t="inlineStr">
-        <is>
-          <t>2955</t>
+      <c r="M162" t="n">
+        <v>2955</v>
+      </c>
+      <c r="N162" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O162" t="inlineStr">
+        <is>
+          <t>2952</t>
         </is>
       </c>
     </row>
@@ -8182,6 +9106,8 @@
       <c r="K163" t="inlineStr"/>
       <c r="L163" s="3" t="inlineStr"/>
       <c r="M163" t="inlineStr"/>
+      <c r="N163" s="3" t="inlineStr"/>
+      <c r="O163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" t="n">
@@ -8220,9 +9146,15 @@
       <c r="L164" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M164" t="inlineStr">
-        <is>
-          <t>2765</t>
+      <c r="M164" t="n">
+        <v>2765</v>
+      </c>
+      <c r="N164" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O164" t="inlineStr">
+        <is>
+          <t>2720</t>
         </is>
       </c>
     </row>
@@ -8262,6 +9194,8 @@
       </c>
       <c r="L165" s="3" t="inlineStr"/>
       <c r="M165" t="inlineStr"/>
+      <c r="N165" s="3" t="inlineStr"/>
+      <c r="O165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" t="n">
@@ -8300,9 +9234,15 @@
       <c r="L166" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M166" t="inlineStr">
-        <is>
-          <t>2410</t>
+      <c r="M166" t="n">
+        <v>2410</v>
+      </c>
+      <c r="N166" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O166" t="inlineStr">
+        <is>
+          <t>2380</t>
         </is>
       </c>
     </row>
@@ -8343,9 +9283,15 @@
       <c r="L167" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M167" t="inlineStr">
-        <is>
-          <t>1439</t>
+      <c r="M167" t="n">
+        <v>1439</v>
+      </c>
+      <c r="N167" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O167" t="inlineStr">
+        <is>
+          <t>1420</t>
         </is>
       </c>
     </row>
@@ -8382,9 +9328,15 @@
       <c r="L168" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="M168" t="inlineStr">
-        <is>
-          <t>1638</t>
+      <c r="M168" t="n">
+        <v>1638</v>
+      </c>
+      <c r="N168" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O168" t="inlineStr">
+        <is>
+          <t>1614</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-02-09 11:30:35
</commit_message>
<xml_diff>
--- a/Season_Attack/83.xlsx
+++ b/Season_Attack/83.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O168"/>
+  <dimension ref="A1:Q169"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,6 +466,16 @@
           <t>02-07_0</t>
         </is>
       </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>02-08_A</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>02-08_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -516,9 +526,15 @@
       <c r="N2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>3875</t>
+      <c r="O2" t="n">
+        <v>3875</v>
+      </c>
+      <c r="P2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>3968</t>
         </is>
       </c>
     </row>
@@ -571,9 +587,15 @@
       <c r="N3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>5638</t>
+      <c r="O3" t="n">
+        <v>5638</v>
+      </c>
+      <c r="P3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>5999</t>
         </is>
       </c>
     </row>
@@ -626,9 +648,15 @@
       <c r="N4" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>5193</t>
+      <c r="O4" t="n">
+        <v>5193</v>
+      </c>
+      <c r="P4" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>5459</t>
         </is>
       </c>
     </row>
@@ -681,9 +709,15 @@
       <c r="N5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>5503</t>
+      <c r="O5" t="n">
+        <v>5503</v>
+      </c>
+      <c r="P5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>5764</t>
         </is>
       </c>
     </row>
@@ -736,9 +770,15 @@
       <c r="N6" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>5359</t>
+      <c r="O6" t="n">
+        <v>5359</v>
+      </c>
+      <c r="P6" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>5567</t>
         </is>
       </c>
     </row>
@@ -791,9 +831,15 @@
       <c r="N7" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>5956</t>
+      <c r="O7" t="n">
+        <v>5956</v>
+      </c>
+      <c r="P7" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>6191</t>
         </is>
       </c>
     </row>
@@ -846,9 +892,15 @@
       <c r="N8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>4907</t>
+      <c r="O8" t="n">
+        <v>4907</v>
+      </c>
+      <c r="P8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>5075</t>
         </is>
       </c>
     </row>
@@ -888,6 +940,8 @@
       <c r="M9" t="inlineStr"/>
       <c r="N9" s="3" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
+      <c r="P9" s="3" t="inlineStr"/>
+      <c r="Q9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -938,9 +992,15 @@
       <c r="N10" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>5145</t>
+      <c r="O10" t="n">
+        <v>5145</v>
+      </c>
+      <c r="P10" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>5323</t>
         </is>
       </c>
     </row>
@@ -993,9 +1053,15 @@
       <c r="N11" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>5408</t>
+      <c r="O11" t="n">
+        <v>5408</v>
+      </c>
+      <c r="P11" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>6018</t>
         </is>
       </c>
     </row>
@@ -1048,9 +1114,15 @@
       <c r="N12" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>5003</t>
+      <c r="O12" t="n">
+        <v>5003</v>
+      </c>
+      <c r="P12" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>5434</t>
         </is>
       </c>
     </row>
@@ -1103,9 +1175,15 @@
       <c r="N13" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>2777</t>
+      <c r="O13" t="n">
+        <v>2777</v>
+      </c>
+      <c r="P13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>2824</t>
         </is>
       </c>
     </row>
@@ -1158,9 +1236,15 @@
       <c r="N14" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>6178</t>
+      <c r="O14" t="n">
+        <v>6178</v>
+      </c>
+      <c r="P14" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>6502</t>
         </is>
       </c>
     </row>
@@ -1213,9 +1297,15 @@
       <c r="N15" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>5253</t>
+      <c r="O15" t="n">
+        <v>5253</v>
+      </c>
+      <c r="P15" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>5586</t>
         </is>
       </c>
     </row>
@@ -1268,9 +1358,15 @@
       <c r="N16" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>5535</t>
+      <c r="O16" t="n">
+        <v>5535</v>
+      </c>
+      <c r="P16" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>5791</t>
         </is>
       </c>
     </row>
@@ -1323,9 +1419,15 @@
       <c r="N17" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="O17" t="inlineStr">
-        <is>
-          <t>4515</t>
+      <c r="O17" t="n">
+        <v>4515</v>
+      </c>
+      <c r="P17" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>4616</t>
         </is>
       </c>
     </row>
@@ -1378,9 +1480,15 @@
       <c r="N18" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>4742</t>
+      <c r="O18" t="n">
+        <v>4742</v>
+      </c>
+      <c r="P18" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>4748</t>
         </is>
       </c>
     </row>
@@ -1433,9 +1541,15 @@
       <c r="N19" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="O19" t="inlineStr">
-        <is>
-          <t>5321</t>
+      <c r="O19" t="n">
+        <v>5321</v>
+      </c>
+      <c r="P19" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>5584</t>
         </is>
       </c>
     </row>
@@ -1488,9 +1602,15 @@
       <c r="N20" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="O20" t="inlineStr">
-        <is>
-          <t>6158</t>
+      <c r="O20" t="n">
+        <v>6158</v>
+      </c>
+      <c r="P20" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>6474</t>
         </is>
       </c>
     </row>
@@ -1543,9 +1663,15 @@
       <c r="N21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O21" t="inlineStr">
-        <is>
-          <t>3923</t>
+      <c r="O21" t="n">
+        <v>3923</v>
+      </c>
+      <c r="P21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>3952</t>
         </is>
       </c>
     </row>
@@ -1598,9 +1724,15 @@
       <c r="N22" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="O22" t="inlineStr">
-        <is>
-          <t>5160</t>
+      <c r="O22" t="n">
+        <v>5160</v>
+      </c>
+      <c r="P22" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>5359</t>
         </is>
       </c>
     </row>
@@ -1653,9 +1785,15 @@
       <c r="N23" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>5122</t>
+      <c r="O23" t="n">
+        <v>5122</v>
+      </c>
+      <c r="P23" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>5479</t>
         </is>
       </c>
     </row>
@@ -1708,9 +1846,15 @@
       <c r="N24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="O24" t="inlineStr">
-        <is>
-          <t>5408</t>
+      <c r="O24" t="n">
+        <v>5408</v>
+      </c>
+      <c r="P24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>5576</t>
         </is>
       </c>
     </row>
@@ -1763,7 +1907,13 @@
       <c r="N25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O25" t="inlineStr">
+      <c r="O25" t="n">
+        <v>0</v>
+      </c>
+      <c r="P25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1818,9 +1968,15 @@
       <c r="N26" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="O26" t="inlineStr">
-        <is>
-          <t>5597</t>
+      <c r="O26" t="n">
+        <v>5597</v>
+      </c>
+      <c r="P26" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>5785</t>
         </is>
       </c>
     </row>
@@ -1873,9 +2029,15 @@
       <c r="N27" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="O27" t="inlineStr">
-        <is>
-          <t>5792</t>
+      <c r="O27" t="n">
+        <v>5792</v>
+      </c>
+      <c r="P27" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>6054</t>
         </is>
       </c>
     </row>
@@ -1928,9 +2090,15 @@
       <c r="N28" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="O28" t="inlineStr">
-        <is>
-          <t>4677</t>
+      <c r="O28" t="n">
+        <v>4677</v>
+      </c>
+      <c r="P28" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>5132</t>
         </is>
       </c>
     </row>
@@ -1983,9 +2151,15 @@
       <c r="N29" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="O29" t="inlineStr">
-        <is>
-          <t>6000</t>
+      <c r="O29" t="n">
+        <v>6000</v>
+      </c>
+      <c r="P29" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>6413</t>
         </is>
       </c>
     </row>
@@ -2038,9 +2212,15 @@
       <c r="N30" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="O30" t="inlineStr">
-        <is>
-          <t>5538</t>
+      <c r="O30" t="n">
+        <v>5538</v>
+      </c>
+      <c r="P30" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>5813</t>
         </is>
       </c>
     </row>
@@ -2093,9 +2273,15 @@
       <c r="N31" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="O31" t="inlineStr">
-        <is>
-          <t>4937</t>
+      <c r="O31" t="n">
+        <v>4937</v>
+      </c>
+      <c r="P31" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>5001</t>
         </is>
       </c>
     </row>
@@ -2148,9 +2334,15 @@
       <c r="N32" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="O32" t="inlineStr">
-        <is>
-          <t>5743</t>
+      <c r="O32" t="n">
+        <v>5743</v>
+      </c>
+      <c r="P32" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>5966</t>
         </is>
       </c>
     </row>
@@ -2203,9 +2395,15 @@
       <c r="N33" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="O33" t="inlineStr">
-        <is>
-          <t>5777</t>
+      <c r="O33" t="n">
+        <v>5777</v>
+      </c>
+      <c r="P33" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>6076</t>
         </is>
       </c>
     </row>
@@ -2258,9 +2456,15 @@
       <c r="N34" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="O34" t="inlineStr">
-        <is>
-          <t>5410</t>
+      <c r="O34" t="n">
+        <v>5410</v>
+      </c>
+      <c r="P34" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>5665</t>
         </is>
       </c>
     </row>
@@ -2313,9 +2517,15 @@
       <c r="N35" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="O35" t="inlineStr">
-        <is>
-          <t>5826</t>
+      <c r="O35" t="n">
+        <v>5826</v>
+      </c>
+      <c r="P35" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>6079</t>
         </is>
       </c>
     </row>
@@ -2368,9 +2578,15 @@
       <c r="N36" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="O36" t="inlineStr">
-        <is>
-          <t>5141</t>
+      <c r="O36" t="n">
+        <v>5141</v>
+      </c>
+      <c r="P36" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>5434</t>
         </is>
       </c>
     </row>
@@ -2423,9 +2639,15 @@
       <c r="N37" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="O37" t="inlineStr">
-        <is>
-          <t>4712</t>
+      <c r="O37" t="n">
+        <v>4712</v>
+      </c>
+      <c r="P37" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>4872</t>
         </is>
       </c>
     </row>
@@ -2448,7 +2670,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F38" s="5" t="n">
@@ -2478,9 +2700,15 @@
       <c r="N38" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="O38" t="inlineStr">
-        <is>
-          <t>5211</t>
+      <c r="O38" t="n">
+        <v>5211</v>
+      </c>
+      <c r="P38" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>5400</t>
         </is>
       </c>
     </row>
@@ -2533,9 +2761,15 @@
       <c r="N39" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="O39" t="inlineStr">
-        <is>
-          <t>5005</t>
+      <c r="O39" t="n">
+        <v>5005</v>
+      </c>
+      <c r="P39" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>5185</t>
         </is>
       </c>
     </row>
@@ -2588,9 +2822,15 @@
       <c r="N40" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="O40" t="inlineStr">
-        <is>
-          <t>5819</t>
+      <c r="O40" t="n">
+        <v>5819</v>
+      </c>
+      <c r="P40" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>6021</t>
         </is>
       </c>
     </row>
@@ -2643,9 +2883,15 @@
       <c r="N41" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O41" t="inlineStr">
-        <is>
-          <t>5346</t>
+      <c r="O41" t="n">
+        <v>5346</v>
+      </c>
+      <c r="P41" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>5531</t>
         </is>
       </c>
     </row>
@@ -2698,9 +2944,15 @@
       <c r="N42" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="O42" t="inlineStr">
-        <is>
-          <t>6163</t>
+      <c r="O42" t="n">
+        <v>6163</v>
+      </c>
+      <c r="P42" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>6369</t>
         </is>
       </c>
     </row>
@@ -2753,9 +3005,15 @@
       <c r="N43" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="O43" t="inlineStr">
-        <is>
-          <t>5442</t>
+      <c r="O43" t="n">
+        <v>5442</v>
+      </c>
+      <c r="P43" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>5609</t>
         </is>
       </c>
     </row>
@@ -2808,9 +3066,15 @@
       <c r="N44" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="O44" t="inlineStr">
-        <is>
-          <t>5295</t>
+      <c r="O44" t="n">
+        <v>5295</v>
+      </c>
+      <c r="P44" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>5434</t>
         </is>
       </c>
     </row>
@@ -2863,9 +3127,15 @@
       <c r="N45" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="O45" t="inlineStr">
-        <is>
-          <t>4771</t>
+      <c r="O45" t="n">
+        <v>4771</v>
+      </c>
+      <c r="P45" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>5362</t>
         </is>
       </c>
     </row>
@@ -2918,9 +3188,15 @@
       <c r="N46" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="O46" t="inlineStr">
-        <is>
-          <t>4977</t>
+      <c r="O46" t="n">
+        <v>4977</v>
+      </c>
+      <c r="P46" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q46" t="inlineStr">
+        <is>
+          <t>5485</t>
         </is>
       </c>
     </row>
@@ -2973,7 +3249,13 @@
       <c r="N47" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O47" t="inlineStr">
+      <c r="O47" t="n">
+        <v>3035</v>
+      </c>
+      <c r="P47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q47" t="inlineStr">
         <is>
           <t>3035</t>
         </is>
@@ -3028,9 +3310,15 @@
       <c r="N48" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="O48" t="inlineStr">
-        <is>
-          <t>5529</t>
+      <c r="O48" t="n">
+        <v>5529</v>
+      </c>
+      <c r="P48" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>5788</t>
         </is>
       </c>
     </row>
@@ -3083,9 +3371,15 @@
       <c r="N49" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="O49" t="inlineStr">
-        <is>
-          <t>4351</t>
+      <c r="O49" t="n">
+        <v>4351</v>
+      </c>
+      <c r="P49" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="Q49" t="inlineStr">
+        <is>
+          <t>4410</t>
         </is>
       </c>
     </row>
@@ -3138,9 +3432,15 @@
       <c r="N50" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="O50" t="inlineStr">
-        <is>
-          <t>5727</t>
+      <c r="O50" t="n">
+        <v>5727</v>
+      </c>
+      <c r="P50" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>6028</t>
         </is>
       </c>
     </row>
@@ -3193,9 +3493,15 @@
       <c r="N51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O51" t="inlineStr">
-        <is>
-          <t>2839</t>
+      <c r="O51" t="n">
+        <v>2839</v>
+      </c>
+      <c r="P51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q51" t="inlineStr">
+        <is>
+          <t>2908</t>
         </is>
       </c>
     </row>
@@ -3248,9 +3554,15 @@
       <c r="N52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O52" t="inlineStr">
-        <is>
-          <t>2781</t>
+      <c r="O52" t="n">
+        <v>2781</v>
+      </c>
+      <c r="P52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q52" t="inlineStr">
+        <is>
+          <t>2841</t>
         </is>
       </c>
     </row>
@@ -3303,9 +3615,15 @@
       <c r="N53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O53" t="inlineStr">
-        <is>
-          <t>3008</t>
+      <c r="O53" t="n">
+        <v>3008</v>
+      </c>
+      <c r="P53" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="Q53" t="inlineStr">
+        <is>
+          <t>3345</t>
         </is>
       </c>
     </row>
@@ -3358,9 +3676,15 @@
       <c r="N54" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="O54" t="inlineStr">
-        <is>
-          <t>5272</t>
+      <c r="O54" t="n">
+        <v>5272</v>
+      </c>
+      <c r="P54" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="Q54" t="inlineStr">
+        <is>
+          <t>5444</t>
         </is>
       </c>
     </row>
@@ -3413,9 +3737,15 @@
       <c r="N55" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="O55" t="inlineStr">
-        <is>
-          <t>4160</t>
+      <c r="O55" t="n">
+        <v>4160</v>
+      </c>
+      <c r="P55" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q55" t="inlineStr">
+        <is>
+          <t>4293</t>
         </is>
       </c>
     </row>
@@ -3468,9 +3798,15 @@
       <c r="N56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O56" t="inlineStr">
-        <is>
-          <t>4228</t>
+      <c r="O56" t="n">
+        <v>4228</v>
+      </c>
+      <c r="P56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q56" t="inlineStr">
+        <is>
+          <t>4392</t>
         </is>
       </c>
     </row>
@@ -3523,9 +3859,15 @@
       <c r="N57" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="O57" t="inlineStr">
-        <is>
-          <t>4938</t>
+      <c r="O57" t="n">
+        <v>4938</v>
+      </c>
+      <c r="P57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q57" t="inlineStr">
+        <is>
+          <t>5071</t>
         </is>
       </c>
     </row>
@@ -3578,9 +3920,15 @@
       <c r="N58" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="O58" t="inlineStr">
-        <is>
-          <t>4125</t>
+      <c r="O58" t="n">
+        <v>4125</v>
+      </c>
+      <c r="P58" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="Q58" t="inlineStr">
+        <is>
+          <t>4253</t>
         </is>
       </c>
     </row>
@@ -3633,9 +3981,15 @@
       <c r="N59" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O59" t="inlineStr">
-        <is>
-          <t>4768</t>
+      <c r="O59" t="n">
+        <v>4768</v>
+      </c>
+      <c r="P59" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q59" t="inlineStr">
+        <is>
+          <t>4935</t>
         </is>
       </c>
     </row>
@@ -3688,7 +4042,13 @@
       <c r="N60" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O60" t="inlineStr">
+      <c r="O60" t="n">
+        <v>0</v>
+      </c>
+      <c r="P60" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q60" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3743,9 +4103,15 @@
       <c r="N61" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="O61" t="inlineStr">
-        <is>
-          <t>5063</t>
+      <c r="O61" t="n">
+        <v>5063</v>
+      </c>
+      <c r="P61" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="Q61" t="inlineStr">
+        <is>
+          <t>5202</t>
         </is>
       </c>
     </row>
@@ -3798,7 +4164,13 @@
       <c r="N62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O62" t="inlineStr">
+      <c r="O62" t="n">
+        <v>3036</v>
+      </c>
+      <c r="P62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q62" t="inlineStr">
         <is>
           <t>3036</t>
         </is>
@@ -3853,9 +4225,15 @@
       <c r="N63" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="O63" t="inlineStr">
-        <is>
-          <t>3317</t>
+      <c r="O63" t="n">
+        <v>3317</v>
+      </c>
+      <c r="P63" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q63" t="inlineStr">
+        <is>
+          <t>3289</t>
         </is>
       </c>
     </row>
@@ -3908,9 +4286,15 @@
       <c r="N64" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="O64" t="inlineStr">
-        <is>
-          <t>4744</t>
+      <c r="O64" t="n">
+        <v>4744</v>
+      </c>
+      <c r="P64" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q64" t="inlineStr">
+        <is>
+          <t>4910</t>
         </is>
       </c>
     </row>
@@ -3942,6 +4326,8 @@
       <c r="M65" t="inlineStr"/>
       <c r="N65" s="3" t="inlineStr"/>
       <c r="O65" t="inlineStr"/>
+      <c r="P65" s="3" t="inlineStr"/>
+      <c r="Q65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -3992,9 +4378,15 @@
       <c r="N66" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O66" t="inlineStr">
-        <is>
-          <t>5287</t>
+      <c r="O66" t="n">
+        <v>5287</v>
+      </c>
+      <c r="P66" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="Q66" t="inlineStr">
+        <is>
+          <t>5593</t>
         </is>
       </c>
     </row>
@@ -4047,9 +4439,15 @@
       <c r="N67" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="O67" t="inlineStr">
-        <is>
-          <t>4257</t>
+      <c r="O67" t="n">
+        <v>4257</v>
+      </c>
+      <c r="P67" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q67" t="inlineStr">
+        <is>
+          <t>4415</t>
         </is>
       </c>
     </row>
@@ -4102,9 +4500,15 @@
       <c r="N68" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O68" t="inlineStr">
-        <is>
-          <t>3132</t>
+      <c r="O68" t="n">
+        <v>3132</v>
+      </c>
+      <c r="P68" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q68" t="inlineStr">
+        <is>
+          <t>3623</t>
         </is>
       </c>
     </row>
@@ -4157,9 +4561,15 @@
       <c r="N69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O69" t="inlineStr">
-        <is>
-          <t>4142</t>
+      <c r="O69" t="n">
+        <v>4142</v>
+      </c>
+      <c r="P69" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q69" t="inlineStr">
+        <is>
+          <t>4345</t>
         </is>
       </c>
     </row>
@@ -4212,9 +4622,15 @@
       <c r="N70" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="O70" t="inlineStr">
-        <is>
-          <t>3852</t>
+      <c r="O70" t="n">
+        <v>3852</v>
+      </c>
+      <c r="P70" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q70" t="inlineStr">
+        <is>
+          <t>4050</t>
         </is>
       </c>
     </row>
@@ -4267,9 +4683,15 @@
       <c r="N71" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O71" t="inlineStr">
-        <is>
-          <t>4257</t>
+      <c r="O71" t="n">
+        <v>4257</v>
+      </c>
+      <c r="P71" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q71" t="inlineStr">
+        <is>
+          <t>4357</t>
         </is>
       </c>
     </row>
@@ -4322,9 +4744,15 @@
       <c r="N72" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O72" t="inlineStr">
-        <is>
-          <t>3248</t>
+      <c r="O72" t="n">
+        <v>3248</v>
+      </c>
+      <c r="P72" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q72" t="inlineStr">
+        <is>
+          <t>3687</t>
         </is>
       </c>
     </row>
@@ -4377,9 +4805,15 @@
       <c r="N73" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="O73" t="inlineStr">
-        <is>
-          <t>3853</t>
+      <c r="O73" t="n">
+        <v>3853</v>
+      </c>
+      <c r="P73" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="Q73" t="inlineStr">
+        <is>
+          <t>3925</t>
         </is>
       </c>
     </row>
@@ -4432,9 +4866,15 @@
       <c r="N74" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O74" t="inlineStr">
-        <is>
-          <t>4809</t>
+      <c r="O74" t="n">
+        <v>4809</v>
+      </c>
+      <c r="P74" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q74" t="inlineStr">
+        <is>
+          <t>4897</t>
         </is>
       </c>
     </row>
@@ -4487,9 +4927,15 @@
       <c r="N75" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O75" t="inlineStr">
-        <is>
-          <t>4837</t>
+      <c r="O75" t="n">
+        <v>4837</v>
+      </c>
+      <c r="P75" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="Q75" t="inlineStr">
+        <is>
+          <t>4917</t>
         </is>
       </c>
     </row>
@@ -4521,6 +4967,8 @@
       <c r="M76" t="inlineStr"/>
       <c r="N76" s="3" t="inlineStr"/>
       <c r="O76" t="inlineStr"/>
+      <c r="P76" s="3" t="inlineStr"/>
+      <c r="Q76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -4571,9 +5019,15 @@
       <c r="N77" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O77" t="inlineStr">
-        <is>
-          <t>4899</t>
+      <c r="O77" t="n">
+        <v>4899</v>
+      </c>
+      <c r="P77" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q77" t="inlineStr">
+        <is>
+          <t>4987</t>
         </is>
       </c>
     </row>
@@ -4626,7 +5080,13 @@
       <c r="N78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O78" t="inlineStr">
+      <c r="O78" t="n">
+        <v>2500</v>
+      </c>
+      <c r="P78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q78" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -4681,9 +5141,15 @@
       <c r="N79" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O79" t="inlineStr">
-        <is>
-          <t>4433</t>
+      <c r="O79" t="n">
+        <v>4433</v>
+      </c>
+      <c r="P79" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q79" t="inlineStr">
+        <is>
+          <t>4604</t>
         </is>
       </c>
     </row>
@@ -4736,9 +5202,15 @@
       <c r="N80" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="O80" t="inlineStr">
-        <is>
-          <t>4691</t>
+      <c r="O80" t="n">
+        <v>4691</v>
+      </c>
+      <c r="P80" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q80" t="inlineStr">
+        <is>
+          <t>4920</t>
         </is>
       </c>
     </row>
@@ -4791,9 +5263,15 @@
       <c r="N81" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O81" t="inlineStr">
-        <is>
-          <t>4509</t>
+      <c r="O81" t="n">
+        <v>4509</v>
+      </c>
+      <c r="P81" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="Q81" t="inlineStr">
+        <is>
+          <t>4643</t>
         </is>
       </c>
     </row>
@@ -4846,9 +5324,15 @@
       <c r="N82" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="O82" t="inlineStr">
-        <is>
-          <t>4267</t>
+      <c r="O82" t="n">
+        <v>4267</v>
+      </c>
+      <c r="P82" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q82" t="inlineStr">
+        <is>
+          <t>4348</t>
         </is>
       </c>
     </row>
@@ -4880,6 +5364,8 @@
       <c r="M83" t="inlineStr"/>
       <c r="N83" s="3" t="inlineStr"/>
       <c r="O83" t="inlineStr"/>
+      <c r="P83" s="3" t="inlineStr"/>
+      <c r="Q83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -4930,9 +5416,15 @@
       <c r="N84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O84" t="inlineStr">
-        <is>
-          <t>3249</t>
+      <c r="O84" t="n">
+        <v>3249</v>
+      </c>
+      <c r="P84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q84" t="inlineStr">
+        <is>
+          <t>3275</t>
         </is>
       </c>
     </row>
@@ -4985,9 +5477,15 @@
       <c r="N85" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O85" t="inlineStr">
-        <is>
-          <t>3482</t>
+      <c r="O85" t="n">
+        <v>3482</v>
+      </c>
+      <c r="P85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q85" t="inlineStr">
+        <is>
+          <t>3473</t>
         </is>
       </c>
     </row>
@@ -5040,9 +5538,15 @@
       <c r="N86" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="O86" t="inlineStr">
-        <is>
-          <t>4628</t>
+      <c r="O86" t="n">
+        <v>4628</v>
+      </c>
+      <c r="P86" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q86" t="inlineStr">
+        <is>
+          <t>4730</t>
         </is>
       </c>
     </row>
@@ -5095,9 +5599,15 @@
       <c r="N87" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O87" t="inlineStr">
-        <is>
-          <t>2976</t>
+      <c r="O87" t="n">
+        <v>2976</v>
+      </c>
+      <c r="P87" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q87" t="inlineStr">
+        <is>
+          <t>3028</t>
         </is>
       </c>
     </row>
@@ -5150,9 +5660,15 @@
       <c r="N88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O88" t="inlineStr">
-        <is>
-          <t>3183</t>
+      <c r="O88" t="n">
+        <v>3183</v>
+      </c>
+      <c r="P88" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q88" t="inlineStr">
+        <is>
+          <t>3330</t>
         </is>
       </c>
     </row>
@@ -5184,6 +5700,8 @@
       <c r="M89" t="inlineStr"/>
       <c r="N89" s="3" t="inlineStr"/>
       <c r="O89" t="inlineStr"/>
+      <c r="P89" s="3" t="inlineStr"/>
+      <c r="Q89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -5234,9 +5752,15 @@
       <c r="N90" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O90" t="inlineStr">
-        <is>
-          <t>2782</t>
+      <c r="O90" t="n">
+        <v>2782</v>
+      </c>
+      <c r="P90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q90" t="inlineStr">
+        <is>
+          <t>2749</t>
         </is>
       </c>
     </row>
@@ -5268,6 +5792,8 @@
       <c r="M91" t="inlineStr"/>
       <c r="N91" s="3" t="inlineStr"/>
       <c r="O91" t="inlineStr"/>
+      <c r="P91" s="3" t="inlineStr"/>
+      <c r="Q91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -5318,9 +5844,15 @@
       <c r="N92" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="O92" t="inlineStr">
-        <is>
-          <t>2693</t>
+      <c r="O92" t="n">
+        <v>2693</v>
+      </c>
+      <c r="P92" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="Q92" t="inlineStr">
+        <is>
+          <t>2808</t>
         </is>
       </c>
     </row>
@@ -5373,9 +5905,15 @@
       <c r="N93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O93" t="inlineStr">
-        <is>
-          <t>2741</t>
+      <c r="O93" t="n">
+        <v>2741</v>
+      </c>
+      <c r="P93" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q93" t="inlineStr">
+        <is>
+          <t>2702</t>
         </is>
       </c>
     </row>
@@ -5428,9 +5966,15 @@
       <c r="N94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O94" t="inlineStr">
-        <is>
-          <t>2937</t>
+      <c r="O94" t="n">
+        <v>2937</v>
+      </c>
+      <c r="P94" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q94" t="inlineStr">
+        <is>
+          <t>3040</t>
         </is>
       </c>
     </row>
@@ -5483,9 +6027,15 @@
       <c r="N95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O95" t="inlineStr">
-        <is>
-          <t>2736</t>
+      <c r="O95" t="n">
+        <v>2736</v>
+      </c>
+      <c r="P95" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q95" t="inlineStr">
+        <is>
+          <t>2799</t>
         </is>
       </c>
     </row>
@@ -5538,9 +6088,15 @@
       <c r="N96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O96" t="inlineStr">
-        <is>
-          <t>2133</t>
+      <c r="O96" t="n">
+        <v>2133</v>
+      </c>
+      <c r="P96" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="Q96" t="inlineStr">
+        <is>
+          <t>2386</t>
         </is>
       </c>
     </row>
@@ -5593,9 +6149,15 @@
       <c r="N97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O97" t="inlineStr">
-        <is>
-          <t>2668</t>
+      <c r="O97" t="n">
+        <v>2668</v>
+      </c>
+      <c r="P97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q97" t="inlineStr">
+        <is>
+          <t>2667</t>
         </is>
       </c>
     </row>
@@ -5648,9 +6210,15 @@
       <c r="N98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O98" t="inlineStr">
-        <is>
-          <t>2249</t>
+      <c r="O98" t="n">
+        <v>2249</v>
+      </c>
+      <c r="P98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q98" t="inlineStr">
+        <is>
+          <t>2243</t>
         </is>
       </c>
     </row>
@@ -5703,9 +6271,15 @@
       <c r="N99" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="O99" t="inlineStr">
-        <is>
-          <t>3709</t>
+      <c r="O99" t="n">
+        <v>3709</v>
+      </c>
+      <c r="P99" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="Q99" t="inlineStr">
+        <is>
+          <t>3829</t>
         </is>
       </c>
     </row>
@@ -5758,9 +6332,15 @@
       <c r="N100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O100" t="inlineStr">
-        <is>
-          <t>2490</t>
+      <c r="O100" t="n">
+        <v>2490</v>
+      </c>
+      <c r="P100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q100" t="inlineStr">
+        <is>
+          <t>2453</t>
         </is>
       </c>
     </row>
@@ -5813,9 +6393,15 @@
       <c r="N101" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O101" t="inlineStr">
-        <is>
-          <t>4151</t>
+      <c r="O101" t="n">
+        <v>4151</v>
+      </c>
+      <c r="P101" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q101" t="inlineStr">
+        <is>
+          <t>4299</t>
         </is>
       </c>
     </row>
@@ -5868,9 +6454,15 @@
       <c r="N102" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O102" t="inlineStr">
-        <is>
-          <t>3899</t>
+      <c r="O102" t="n">
+        <v>3899</v>
+      </c>
+      <c r="P102" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q102" t="inlineStr">
+        <is>
+          <t>4036</t>
         </is>
       </c>
     </row>
@@ -5923,9 +6515,15 @@
       <c r="N103" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="O103" t="inlineStr">
-        <is>
-          <t>3632</t>
+      <c r="O103" t="n">
+        <v>3632</v>
+      </c>
+      <c r="P103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q103" t="inlineStr">
+        <is>
+          <t>3610</t>
         </is>
       </c>
     </row>
@@ -5978,9 +6576,15 @@
       <c r="N104" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="O104" t="inlineStr">
-        <is>
-          <t>4185</t>
+      <c r="O104" t="n">
+        <v>4185</v>
+      </c>
+      <c r="P104" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="Q104" t="inlineStr">
+        <is>
+          <t>4324</t>
         </is>
       </c>
     </row>
@@ -6033,9 +6637,15 @@
       <c r="N105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O105" t="inlineStr">
-        <is>
-          <t>3802</t>
+      <c r="O105" t="n">
+        <v>3802</v>
+      </c>
+      <c r="P105" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q105" t="inlineStr">
+        <is>
+          <t>3858</t>
         </is>
       </c>
     </row>
@@ -6088,9 +6698,15 @@
       <c r="N106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O106" t="inlineStr">
-        <is>
-          <t>2388</t>
+      <c r="O106" t="n">
+        <v>2388</v>
+      </c>
+      <c r="P106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q106" t="inlineStr">
+        <is>
+          <t>2386</t>
         </is>
       </c>
     </row>
@@ -6143,9 +6759,15 @@
       <c r="N107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O107" t="inlineStr">
-        <is>
-          <t>2667</t>
+      <c r="O107" t="n">
+        <v>2667</v>
+      </c>
+      <c r="P107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q107" t="inlineStr">
+        <is>
+          <t>2671</t>
         </is>
       </c>
     </row>
@@ -6198,9 +6820,15 @@
       <c r="N108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O108" t="inlineStr">
-        <is>
-          <t>2713</t>
+      <c r="O108" t="n">
+        <v>2713</v>
+      </c>
+      <c r="P108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q108" t="inlineStr">
+        <is>
+          <t>2745</t>
         </is>
       </c>
     </row>
@@ -6253,9 +6881,15 @@
       <c r="N109" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O109" t="inlineStr">
-        <is>
-          <t>3841</t>
+      <c r="O109" t="n">
+        <v>3841</v>
+      </c>
+      <c r="P109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q109" t="inlineStr">
+        <is>
+          <t>3823</t>
         </is>
       </c>
     </row>
@@ -6308,9 +6942,15 @@
       <c r="N110" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="O110" t="inlineStr">
-        <is>
-          <t>3490</t>
+      <c r="O110" t="n">
+        <v>3490</v>
+      </c>
+      <c r="P110" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="Q110" t="inlineStr">
+        <is>
+          <t>3595</t>
         </is>
       </c>
     </row>
@@ -6363,9 +7003,15 @@
       <c r="N111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O111" t="inlineStr">
-        <is>
-          <t>2851</t>
+      <c r="O111" t="n">
+        <v>2851</v>
+      </c>
+      <c r="P111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q111" t="inlineStr">
+        <is>
+          <t>2914</t>
         </is>
       </c>
     </row>
@@ -6418,9 +7064,15 @@
       <c r="N112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O112" t="inlineStr">
-        <is>
-          <t>3099</t>
+      <c r="O112" t="n">
+        <v>3099</v>
+      </c>
+      <c r="P112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q112" t="inlineStr">
+        <is>
+          <t>3152</t>
         </is>
       </c>
     </row>
@@ -6473,9 +7125,15 @@
       <c r="N113" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="O113" t="inlineStr">
-        <is>
-          <t>3252</t>
+      <c r="O113" t="n">
+        <v>3252</v>
+      </c>
+      <c r="P113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q113" t="inlineStr">
+        <is>
+          <t>3496</t>
         </is>
       </c>
     </row>
@@ -6528,9 +7186,15 @@
       <c r="N114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O114" t="inlineStr">
-        <is>
-          <t>3584</t>
+      <c r="O114" t="n">
+        <v>3584</v>
+      </c>
+      <c r="P114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q114" t="inlineStr">
+        <is>
+          <t>3778</t>
         </is>
       </c>
     </row>
@@ -6570,6 +7234,8 @@
       <c r="M115" t="inlineStr"/>
       <c r="N115" s="3" t="inlineStr"/>
       <c r="O115" t="inlineStr"/>
+      <c r="P115" s="3" t="inlineStr"/>
+      <c r="Q115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -6620,9 +7286,15 @@
       <c r="N116" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="O116" t="inlineStr">
-        <is>
-          <t>2535</t>
+      <c r="O116" t="n">
+        <v>2535</v>
+      </c>
+      <c r="P116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q116" t="inlineStr">
+        <is>
+          <t>2515</t>
         </is>
       </c>
     </row>
@@ -6675,9 +7347,15 @@
       <c r="N117" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="O117" t="inlineStr">
-        <is>
-          <t>3132</t>
+      <c r="O117" t="n">
+        <v>3132</v>
+      </c>
+      <c r="P117" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q117" t="inlineStr">
+        <is>
+          <t>3227</t>
         </is>
       </c>
     </row>
@@ -6730,9 +7408,15 @@
       <c r="N118" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="O118" t="inlineStr">
-        <is>
-          <t>3474</t>
+      <c r="O118" t="n">
+        <v>3474</v>
+      </c>
+      <c r="P118" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q118" t="inlineStr">
+        <is>
+          <t>3670</t>
         </is>
       </c>
     </row>
@@ -6785,7 +7469,13 @@
       <c r="N119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O119" t="inlineStr">
+      <c r="O119" t="n">
+        <v>0</v>
+      </c>
+      <c r="P119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q119" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6840,9 +7530,15 @@
       <c r="N120" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="O120" t="inlineStr">
-        <is>
-          <t>3756</t>
+      <c r="O120" t="n">
+        <v>3756</v>
+      </c>
+      <c r="P120" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="Q120" t="inlineStr">
+        <is>
+          <t>3958</t>
         </is>
       </c>
     </row>
@@ -6895,9 +7591,15 @@
       <c r="N121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O121" t="inlineStr">
-        <is>
-          <t>2691</t>
+      <c r="O121" t="n">
+        <v>2691</v>
+      </c>
+      <c r="P121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q121" t="inlineStr">
+        <is>
+          <t>2683</t>
         </is>
       </c>
     </row>
@@ -6950,9 +7652,15 @@
       <c r="N122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O122" t="inlineStr">
-        <is>
-          <t>3023</t>
+      <c r="O122" t="n">
+        <v>3023</v>
+      </c>
+      <c r="P122" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q122" t="inlineStr">
+        <is>
+          <t>3107</t>
         </is>
       </c>
     </row>
@@ -7005,9 +7713,15 @@
       <c r="N123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O123" t="inlineStr">
-        <is>
-          <t>2623</t>
+      <c r="O123" t="n">
+        <v>2623</v>
+      </c>
+      <c r="P123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q123" t="inlineStr">
+        <is>
+          <t>2597</t>
         </is>
       </c>
     </row>
@@ -7060,9 +7774,15 @@
       <c r="N124" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O124" t="inlineStr">
-        <is>
-          <t>3216</t>
+      <c r="O124" t="n">
+        <v>3216</v>
+      </c>
+      <c r="P124" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q124" t="inlineStr">
+        <is>
+          <t>3319</t>
         </is>
       </c>
     </row>
@@ -7115,9 +7835,15 @@
       <c r="N125" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O125" t="inlineStr">
-        <is>
-          <t>3239</t>
+      <c r="O125" t="n">
+        <v>3239</v>
+      </c>
+      <c r="P125" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="Q125" t="inlineStr">
+        <is>
+          <t>3322</t>
         </is>
       </c>
     </row>
@@ -7170,9 +7896,15 @@
       <c r="N126" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O126" t="inlineStr">
-        <is>
-          <t>3699</t>
+      <c r="O126" t="n">
+        <v>3699</v>
+      </c>
+      <c r="P126" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q126" t="inlineStr">
+        <is>
+          <t>3761</t>
         </is>
       </c>
     </row>
@@ -7225,9 +7957,15 @@
       <c r="N127" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O127" t="inlineStr">
-        <is>
-          <t>3218</t>
+      <c r="O127" t="n">
+        <v>3218</v>
+      </c>
+      <c r="P127" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q127" t="inlineStr">
+        <is>
+          <t>3336</t>
         </is>
       </c>
     </row>
@@ -7280,7 +8018,13 @@
       <c r="N128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O128" t="inlineStr">
+      <c r="O128" t="n">
+        <v>0</v>
+      </c>
+      <c r="P128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7335,7 +8079,13 @@
       <c r="N129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O129" t="inlineStr">
+      <c r="O129" t="n">
+        <v>0</v>
+      </c>
+      <c r="P129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7390,9 +8140,15 @@
       <c r="N130" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O130" t="inlineStr">
-        <is>
-          <t>2988</t>
+      <c r="O130" t="n">
+        <v>2988</v>
+      </c>
+      <c r="P130" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="Q130" t="inlineStr">
+        <is>
+          <t>3045</t>
         </is>
       </c>
     </row>
@@ -7445,9 +8201,15 @@
       <c r="N131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O131" t="inlineStr">
-        <is>
-          <t>2791</t>
+      <c r="O131" t="n">
+        <v>2791</v>
+      </c>
+      <c r="P131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q131" t="inlineStr">
+        <is>
+          <t>2814</t>
         </is>
       </c>
     </row>
@@ -7500,7 +8262,13 @@
       <c r="N132" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O132" t="inlineStr">
+      <c r="O132" t="n">
+        <v>0</v>
+      </c>
+      <c r="P132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q132" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7555,9 +8323,15 @@
       <c r="N133" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="O133" t="inlineStr">
-        <is>
-          <t>2186</t>
+      <c r="O133" t="n">
+        <v>2186</v>
+      </c>
+      <c r="P133" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q133" t="inlineStr">
+        <is>
+          <t>2242</t>
         </is>
       </c>
     </row>
@@ -7610,9 +8384,15 @@
       <c r="N134" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O134" t="inlineStr">
-        <is>
-          <t>3003</t>
+      <c r="O134" t="n">
+        <v>3003</v>
+      </c>
+      <c r="P134" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q134" t="inlineStr">
+        <is>
+          <t>3034</t>
         </is>
       </c>
     </row>
@@ -7665,7 +8445,13 @@
       <c r="N135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O135" t="inlineStr">
+      <c r="O135" t="n">
+        <v>2498</v>
+      </c>
+      <c r="P135" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q135" t="inlineStr">
         <is>
           <t>2498</t>
         </is>
@@ -7720,9 +8506,15 @@
       <c r="N136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O136" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="O136" t="n">
+        <v>0</v>
+      </c>
+      <c r="P136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q136" t="inlineStr">
+        <is>
+          <t>998</t>
         </is>
       </c>
     </row>
@@ -7770,6 +8562,8 @@
       <c r="M137" t="inlineStr"/>
       <c r="N137" s="3" t="inlineStr"/>
       <c r="O137" t="inlineStr"/>
+      <c r="P137" s="3" t="inlineStr"/>
+      <c r="Q137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="n">
@@ -7820,9 +8614,15 @@
       <c r="N138" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O138" t="inlineStr">
-        <is>
-          <t>3026</t>
+      <c r="O138" t="n">
+        <v>3026</v>
+      </c>
+      <c r="P138" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q138" t="inlineStr">
+        <is>
+          <t>3176</t>
         </is>
       </c>
     </row>
@@ -7875,7 +8675,13 @@
       <c r="N139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O139" t="inlineStr">
+      <c r="O139" t="n">
+        <v>0</v>
+      </c>
+      <c r="P139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q139" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7930,9 +8736,15 @@
       <c r="N140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O140" t="inlineStr">
-        <is>
-          <t>2679</t>
+      <c r="O140" t="n">
+        <v>2679</v>
+      </c>
+      <c r="P140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q140" t="inlineStr">
+        <is>
+          <t>2647</t>
         </is>
       </c>
     </row>
@@ -7980,6 +8792,8 @@
       <c r="M141" t="inlineStr"/>
       <c r="N141" s="3" t="inlineStr"/>
       <c r="O141" t="inlineStr"/>
+      <c r="P141" s="3" t="inlineStr"/>
+      <c r="Q141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -8030,9 +8844,15 @@
       <c r="N142" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O142" t="inlineStr">
-        <is>
-          <t>2980</t>
+      <c r="O142" t="n">
+        <v>2980</v>
+      </c>
+      <c r="P142" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q142" t="inlineStr">
+        <is>
+          <t>3020</t>
         </is>
       </c>
     </row>
@@ -8064,6 +8884,8 @@
       <c r="M143" t="inlineStr"/>
       <c r="N143" s="3" t="inlineStr"/>
       <c r="O143" t="inlineStr"/>
+      <c r="P143" s="3" t="inlineStr"/>
+      <c r="Q143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -8114,9 +8936,15 @@
       <c r="N144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O144" t="inlineStr">
-        <is>
-          <t>2487</t>
+      <c r="O144" t="n">
+        <v>2487</v>
+      </c>
+      <c r="P144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q144" t="inlineStr">
+        <is>
+          <t>2479</t>
         </is>
       </c>
     </row>
@@ -8169,7 +8997,13 @@
       <c r="N145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O145" t="inlineStr">
+      <c r="O145" t="n">
+        <v>0</v>
+      </c>
+      <c r="P145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q145" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8224,7 +9058,13 @@
       <c r="N146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O146" t="inlineStr">
+      <c r="O146" t="n">
+        <v>0</v>
+      </c>
+      <c r="P146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8279,7 +9119,13 @@
       <c r="N147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O147" t="inlineStr">
+      <c r="O147" t="n">
+        <v>0</v>
+      </c>
+      <c r="P147" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q147" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8329,6 +9175,8 @@
       <c r="M148" t="inlineStr"/>
       <c r="N148" s="3" t="inlineStr"/>
       <c r="O148" t="inlineStr"/>
+      <c r="P148" s="3" t="inlineStr"/>
+      <c r="Q148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="n">
@@ -8374,6 +9222,8 @@
       <c r="M149" t="inlineStr"/>
       <c r="N149" s="3" t="inlineStr"/>
       <c r="O149" t="inlineStr"/>
+      <c r="P149" s="3" t="inlineStr"/>
+      <c r="Q149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="n">
@@ -8424,9 +9274,15 @@
       <c r="N150" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="O150" t="inlineStr">
-        <is>
-          <t>2476</t>
+      <c r="O150" t="n">
+        <v>2476</v>
+      </c>
+      <c r="P150" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q150" t="inlineStr">
+        <is>
+          <t>2461</t>
         </is>
       </c>
     </row>
@@ -8479,7 +9335,13 @@
       <c r="N151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O151" t="inlineStr">
+      <c r="O151" t="n">
+        <v>0</v>
+      </c>
+      <c r="P151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q151" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8534,7 +9396,13 @@
       <c r="N152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O152" t="inlineStr">
+      <c r="O152" t="n">
+        <v>0</v>
+      </c>
+      <c r="P152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8589,9 +9457,15 @@
       <c r="N153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O153" t="inlineStr">
-        <is>
-          <t>1796</t>
+      <c r="O153" t="n">
+        <v>1796</v>
+      </c>
+      <c r="P153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q153" t="inlineStr">
+        <is>
+          <t>1780</t>
         </is>
       </c>
     </row>
@@ -8639,6 +9513,8 @@
       <c r="M154" t="inlineStr"/>
       <c r="N154" s="3" t="inlineStr"/>
       <c r="O154" t="inlineStr"/>
+      <c r="P154" s="3" t="inlineStr"/>
+      <c r="Q154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" t="n">
@@ -8689,9 +9565,15 @@
       <c r="N155" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="O155" t="inlineStr">
-        <is>
-          <t>5160</t>
+      <c r="O155" t="n">
+        <v>5160</v>
+      </c>
+      <c r="P155" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q155" t="inlineStr">
+        <is>
+          <t>5362</t>
         </is>
       </c>
     </row>
@@ -8744,7 +9626,13 @@
       <c r="N156" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O156" t="inlineStr">
+      <c r="O156" t="n">
+        <v>0</v>
+      </c>
+      <c r="P156" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q156" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8799,7 +9687,13 @@
       <c r="N157" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O157" t="inlineStr">
+      <c r="O157" t="n">
+        <v>2500</v>
+      </c>
+      <c r="P157" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q157" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -8854,9 +9748,15 @@
       <c r="N158" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="O158" t="inlineStr">
-        <is>
-          <t>5504</t>
+      <c r="O158" t="n">
+        <v>5504</v>
+      </c>
+      <c r="P158" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="Q158" t="inlineStr">
+        <is>
+          <t>5677</t>
         </is>
       </c>
     </row>
@@ -8909,7 +9809,13 @@
       <c r="N159" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O159" t="inlineStr">
+      <c r="O159" t="n">
+        <v>0</v>
+      </c>
+      <c r="P159" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q159" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8964,9 +9870,15 @@
       <c r="N160" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="O160" t="inlineStr">
-        <is>
-          <t>3041</t>
+      <c r="O160" t="n">
+        <v>3041</v>
+      </c>
+      <c r="P160" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q160" t="inlineStr">
+        <is>
+          <t>3098</t>
         </is>
       </c>
     </row>
@@ -9019,7 +9931,13 @@
       <c r="N161" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O161" t="inlineStr">
+      <c r="O161" t="n">
+        <v>0</v>
+      </c>
+      <c r="P161" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q161" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9074,9 +9992,15 @@
       <c r="N162" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O162" t="inlineStr">
-        <is>
-          <t>2952</t>
+      <c r="O162" t="n">
+        <v>2952</v>
+      </c>
+      <c r="P162" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q162" t="inlineStr">
+        <is>
+          <t>3060</t>
         </is>
       </c>
     </row>
@@ -9108,6 +10032,8 @@
       <c r="M163" t="inlineStr"/>
       <c r="N163" s="3" t="inlineStr"/>
       <c r="O163" t="inlineStr"/>
+      <c r="P163" s="3" t="inlineStr"/>
+      <c r="Q163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" t="n">
@@ -9152,9 +10078,15 @@
       <c r="N164" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O164" t="inlineStr">
-        <is>
-          <t>2720</t>
+      <c r="O164" t="n">
+        <v>2720</v>
+      </c>
+      <c r="P164" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="Q164" t="inlineStr">
+        <is>
+          <t>2804</t>
         </is>
       </c>
     </row>
@@ -9196,6 +10128,8 @@
       <c r="M165" t="inlineStr"/>
       <c r="N165" s="3" t="inlineStr"/>
       <c r="O165" t="inlineStr"/>
+      <c r="P165" s="3" t="inlineStr"/>
+      <c r="Q165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" t="n">
@@ -9240,9 +10174,15 @@
       <c r="N166" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O166" t="inlineStr">
-        <is>
-          <t>2380</t>
+      <c r="O166" t="n">
+        <v>2380</v>
+      </c>
+      <c r="P166" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q166" t="inlineStr">
+        <is>
+          <t>2356</t>
         </is>
       </c>
     </row>
@@ -9289,9 +10229,15 @@
       <c r="N167" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O167" t="inlineStr">
-        <is>
-          <t>1420</t>
+      <c r="O167" t="n">
+        <v>1420</v>
+      </c>
+      <c r="P167" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q167" t="inlineStr">
+        <is>
+          <t>1408</t>
         </is>
       </c>
     </row>
@@ -9334,9 +10280,52 @@
       <c r="N168" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O168" t="inlineStr">
-        <is>
-          <t>1614</t>
+      <c r="O168" t="n">
+        <v>1614</v>
+      </c>
+      <c r="P168" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q168" t="inlineStr">
+        <is>
+          <t>1603</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>58641574</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>Player-58641574</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr"/>
+      <c r="D169" t="inlineStr"/>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F169" s="3" t="inlineStr"/>
+      <c r="G169" t="inlineStr"/>
+      <c r="H169" s="3" t="inlineStr"/>
+      <c r="I169" t="inlineStr"/>
+      <c r="J169" s="3" t="inlineStr"/>
+      <c r="K169" t="inlineStr"/>
+      <c r="L169" s="3" t="inlineStr"/>
+      <c r="M169" t="inlineStr"/>
+      <c r="N169" s="3" t="inlineStr"/>
+      <c r="O169" t="inlineStr"/>
+      <c r="P169" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q169" t="inlineStr">
+        <is>
+          <t>2615</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-02-10 11:30:35
</commit_message>
<xml_diff>
--- a/Season_Attack/83.xlsx
+++ b/Season_Attack/83.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q169"/>
+  <dimension ref="A1:S173"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,6 +476,16 @@
           <t>02-08_0</t>
         </is>
       </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>02-09_A</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>02-09_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -532,9 +542,15 @@
       <c r="P2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>3968</t>
+      <c r="Q2" t="n">
+        <v>3968</v>
+      </c>
+      <c r="R2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>4009</t>
         </is>
       </c>
     </row>
@@ -593,9 +609,15 @@
       <c r="P3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>5999</t>
+      <c r="Q3" t="n">
+        <v>5999</v>
+      </c>
+      <c r="R3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>6294</t>
         </is>
       </c>
     </row>
@@ -654,9 +676,15 @@
       <c r="P4" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>5459</t>
+      <c r="Q4" t="n">
+        <v>5459</v>
+      </c>
+      <c r="R4" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>5598</t>
         </is>
       </c>
     </row>
@@ -715,9 +743,15 @@
       <c r="P5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>5764</t>
+      <c r="Q5" t="n">
+        <v>5764</v>
+      </c>
+      <c r="R5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>6006</t>
         </is>
       </c>
     </row>
@@ -776,9 +810,15 @@
       <c r="P6" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>5567</t>
+      <c r="Q6" t="n">
+        <v>5567</v>
+      </c>
+      <c r="R6" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>5820</t>
         </is>
       </c>
     </row>
@@ -837,9 +877,15 @@
       <c r="P7" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>6191</t>
+      <c r="Q7" t="n">
+        <v>6191</v>
+      </c>
+      <c r="R7" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>6588</t>
         </is>
       </c>
     </row>
@@ -898,9 +944,15 @@
       <c r="P8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>5075</t>
+      <c r="Q8" t="n">
+        <v>5075</v>
+      </c>
+      <c r="R8" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>5222</t>
         </is>
       </c>
     </row>
@@ -942,6 +994,8 @@
       <c r="O9" t="inlineStr"/>
       <c r="P9" s="3" t="inlineStr"/>
       <c r="Q9" t="inlineStr"/>
+      <c r="R9" s="3" t="inlineStr"/>
+      <c r="S9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -998,9 +1052,15 @@
       <c r="P10" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>5323</t>
+      <c r="Q10" t="n">
+        <v>5323</v>
+      </c>
+      <c r="R10" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>5804</t>
         </is>
       </c>
     </row>
@@ -1059,9 +1119,15 @@
       <c r="P11" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="Q11" t="inlineStr">
-        <is>
-          <t>6018</t>
+      <c r="Q11" t="n">
+        <v>6018</v>
+      </c>
+      <c r="R11" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>6480</t>
         </is>
       </c>
     </row>
@@ -1120,9 +1186,15 @@
       <c r="P12" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q12" t="inlineStr">
-        <is>
-          <t>5434</t>
+      <c r="Q12" t="n">
+        <v>5434</v>
+      </c>
+      <c r="R12" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>5446</t>
         </is>
       </c>
     </row>
@@ -1181,9 +1253,15 @@
       <c r="P13" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>2824</t>
+      <c r="Q13" t="n">
+        <v>2824</v>
+      </c>
+      <c r="R13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>2840</t>
         </is>
       </c>
     </row>
@@ -1242,9 +1320,15 @@
       <c r="P14" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="Q14" t="inlineStr">
-        <is>
-          <t>6502</t>
+      <c r="Q14" t="n">
+        <v>6502</v>
+      </c>
+      <c r="R14" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>6690</t>
         </is>
       </c>
     </row>
@@ -1303,9 +1387,15 @@
       <c r="P15" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Q15" t="inlineStr">
-        <is>
-          <t>5586</t>
+      <c r="Q15" t="n">
+        <v>5586</v>
+      </c>
+      <c r="R15" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>5782</t>
         </is>
       </c>
     </row>
@@ -1364,9 +1454,15 @@
       <c r="P16" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="Q16" t="inlineStr">
-        <is>
-          <t>5791</t>
+      <c r="Q16" t="n">
+        <v>5791</v>
+      </c>
+      <c r="R16" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>6101</t>
         </is>
       </c>
     </row>
@@ -1425,9 +1521,15 @@
       <c r="P17" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="Q17" t="inlineStr">
-        <is>
-          <t>4616</t>
+      <c r="Q17" t="n">
+        <v>4616</v>
+      </c>
+      <c r="R17" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>4642</t>
         </is>
       </c>
     </row>
@@ -1486,9 +1588,15 @@
       <c r="P18" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>4748</t>
+      <c r="Q18" t="n">
+        <v>4748</v>
+      </c>
+      <c r="R18" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>4881</t>
         </is>
       </c>
     </row>
@@ -1547,9 +1655,15 @@
       <c r="P19" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>5584</t>
+      <c r="Q19" t="n">
+        <v>5584</v>
+      </c>
+      <c r="R19" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>5798</t>
         </is>
       </c>
     </row>
@@ -1608,9 +1722,15 @@
       <c r="P20" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="Q20" t="inlineStr">
-        <is>
-          <t>6474</t>
+      <c r="Q20" t="n">
+        <v>6474</v>
+      </c>
+      <c r="R20" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>6690</t>
         </is>
       </c>
     </row>
@@ -1669,9 +1789,15 @@
       <c r="P21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q21" t="inlineStr">
-        <is>
-          <t>3952</t>
+      <c r="Q21" t="n">
+        <v>3952</v>
+      </c>
+      <c r="R21" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>4530</t>
         </is>
       </c>
     </row>
@@ -1730,9 +1856,15 @@
       <c r="P22" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="Q22" t="inlineStr">
-        <is>
-          <t>5359</t>
+      <c r="Q22" t="n">
+        <v>5359</v>
+      </c>
+      <c r="R22" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>5804</t>
         </is>
       </c>
     </row>
@@ -1791,9 +1923,15 @@
       <c r="P23" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="Q23" t="inlineStr">
-        <is>
-          <t>5479</t>
+      <c r="Q23" t="n">
+        <v>5479</v>
+      </c>
+      <c r="R23" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>5550</t>
         </is>
       </c>
     </row>
@@ -1852,9 +1990,15 @@
       <c r="P24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="Q24" t="inlineStr">
-        <is>
-          <t>5576</t>
+      <c r="Q24" t="n">
+        <v>5576</v>
+      </c>
+      <c r="R24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>5909</t>
         </is>
       </c>
     </row>
@@ -1913,7 +2057,13 @@
       <c r="P25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q25" t="inlineStr">
+      <c r="Q25" t="n">
+        <v>0</v>
+      </c>
+      <c r="R25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1974,9 +2124,15 @@
       <c r="P26" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="Q26" t="inlineStr">
-        <is>
-          <t>5785</t>
+      <c r="Q26" t="n">
+        <v>5785</v>
+      </c>
+      <c r="R26" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>6015</t>
         </is>
       </c>
     </row>
@@ -2035,9 +2191,15 @@
       <c r="P27" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="Q27" t="inlineStr">
-        <is>
-          <t>6054</t>
+      <c r="Q27" t="n">
+        <v>6054</v>
+      </c>
+      <c r="R27" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>6059</t>
         </is>
       </c>
     </row>
@@ -2096,9 +2258,15 @@
       <c r="P28" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="Q28" t="inlineStr">
-        <is>
-          <t>5132</t>
+      <c r="Q28" t="n">
+        <v>5132</v>
+      </c>
+      <c r="R28" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>5578</t>
         </is>
       </c>
     </row>
@@ -2157,9 +2325,15 @@
       <c r="P29" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="Q29" t="inlineStr">
-        <is>
-          <t>6413</t>
+      <c r="Q29" t="n">
+        <v>6413</v>
+      </c>
+      <c r="R29" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="S29" t="inlineStr">
+        <is>
+          <t>6741</t>
         </is>
       </c>
     </row>
@@ -2182,7 +2356,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F30" s="5" t="n">
@@ -2218,9 +2392,15 @@
       <c r="P30" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="Q30" t="inlineStr">
-        <is>
-          <t>5813</t>
+      <c r="Q30" t="n">
+        <v>5813</v>
+      </c>
+      <c r="R30" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="S30" t="inlineStr">
+        <is>
+          <t>5958</t>
         </is>
       </c>
     </row>
@@ -2279,9 +2459,15 @@
       <c r="P31" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="Q31" t="inlineStr">
-        <is>
-          <t>5001</t>
+      <c r="Q31" t="n">
+        <v>5001</v>
+      </c>
+      <c r="R31" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="S31" t="inlineStr">
+        <is>
+          <t>5147</t>
         </is>
       </c>
     </row>
@@ -2340,9 +2526,15 @@
       <c r="P32" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="Q32" t="inlineStr">
-        <is>
-          <t>5966</t>
+      <c r="Q32" t="n">
+        <v>5966</v>
+      </c>
+      <c r="R32" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="S32" t="inlineStr">
+        <is>
+          <t>5991</t>
         </is>
       </c>
     </row>
@@ -2401,9 +2593,15 @@
       <c r="P33" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="Q33" t="inlineStr">
-        <is>
-          <t>6076</t>
+      <c r="Q33" t="n">
+        <v>6076</v>
+      </c>
+      <c r="R33" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="S33" t="inlineStr">
+        <is>
+          <t>6483</t>
         </is>
       </c>
     </row>
@@ -2462,9 +2660,15 @@
       <c r="P34" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="Q34" t="inlineStr">
-        <is>
-          <t>5665</t>
+      <c r="Q34" t="n">
+        <v>5665</v>
+      </c>
+      <c r="R34" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="S34" t="inlineStr">
+        <is>
+          <t>5899</t>
         </is>
       </c>
     </row>
@@ -2487,7 +2691,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="F35" s="5" t="n">
@@ -2523,9 +2727,15 @@
       <c r="P35" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="Q35" t="inlineStr">
-        <is>
-          <t>6079</t>
+      <c r="Q35" t="n">
+        <v>6079</v>
+      </c>
+      <c r="R35" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="S35" t="inlineStr">
+        <is>
+          <t>6389</t>
         </is>
       </c>
     </row>
@@ -2584,9 +2794,15 @@
       <c r="P36" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="Q36" t="inlineStr">
-        <is>
-          <t>5434</t>
+      <c r="Q36" t="n">
+        <v>5434</v>
+      </c>
+      <c r="R36" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="S36" t="inlineStr">
+        <is>
+          <t>5700</t>
         </is>
       </c>
     </row>
@@ -2645,9 +2861,15 @@
       <c r="P37" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="Q37" t="inlineStr">
-        <is>
-          <t>4872</t>
+      <c r="Q37" t="n">
+        <v>4872</v>
+      </c>
+      <c r="R37" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="S37" t="inlineStr">
+        <is>
+          <t>4942</t>
         </is>
       </c>
     </row>
@@ -2706,9 +2928,15 @@
       <c r="P38" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q38" t="inlineStr">
-        <is>
-          <t>5400</t>
+      <c r="Q38" t="n">
+        <v>5400</v>
+      </c>
+      <c r="R38" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="S38" t="inlineStr">
+        <is>
+          <t>5709</t>
         </is>
       </c>
     </row>
@@ -2767,9 +2995,15 @@
       <c r="P39" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="Q39" t="inlineStr">
-        <is>
-          <t>5185</t>
+      <c r="Q39" t="n">
+        <v>5185</v>
+      </c>
+      <c r="R39" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S39" t="inlineStr">
+        <is>
+          <t>5249</t>
         </is>
       </c>
     </row>
@@ -2828,9 +3062,15 @@
       <c r="P40" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="Q40" t="inlineStr">
-        <is>
-          <t>6021</t>
+      <c r="Q40" t="n">
+        <v>6021</v>
+      </c>
+      <c r="R40" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="S40" t="inlineStr">
+        <is>
+          <t>6451</t>
         </is>
       </c>
     </row>
@@ -2889,9 +3129,15 @@
       <c r="P41" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="Q41" t="inlineStr">
-        <is>
-          <t>5531</t>
+      <c r="Q41" t="n">
+        <v>5531</v>
+      </c>
+      <c r="R41" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S41" t="inlineStr">
+        <is>
+          <t>5668</t>
         </is>
       </c>
     </row>
@@ -2950,9 +3196,15 @@
       <c r="P42" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="Q42" t="inlineStr">
-        <is>
-          <t>6369</t>
+      <c r="Q42" t="n">
+        <v>6369</v>
+      </c>
+      <c r="R42" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="S42" t="inlineStr">
+        <is>
+          <t>6566</t>
         </is>
       </c>
     </row>
@@ -3011,9 +3263,15 @@
       <c r="P43" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="Q43" t="inlineStr">
-        <is>
-          <t>5609</t>
+      <c r="Q43" t="n">
+        <v>5609</v>
+      </c>
+      <c r="R43" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="S43" t="inlineStr">
+        <is>
+          <t>5782</t>
         </is>
       </c>
     </row>
@@ -3072,9 +3330,15 @@
       <c r="P44" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="Q44" t="inlineStr">
-        <is>
-          <t>5434</t>
+      <c r="Q44" t="n">
+        <v>5434</v>
+      </c>
+      <c r="R44" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="S44" t="inlineStr">
+        <is>
+          <t>5723</t>
         </is>
       </c>
     </row>
@@ -3133,9 +3397,15 @@
       <c r="P45" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="Q45" t="inlineStr">
-        <is>
-          <t>5362</t>
+      <c r="Q45" t="n">
+        <v>5362</v>
+      </c>
+      <c r="R45" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="S45" t="inlineStr">
+        <is>
+          <t>5797</t>
         </is>
       </c>
     </row>
@@ -3194,9 +3464,15 @@
       <c r="P46" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="Q46" t="inlineStr">
-        <is>
-          <t>5485</t>
+      <c r="Q46" t="n">
+        <v>5485</v>
+      </c>
+      <c r="R46" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="S46" t="inlineStr">
+        <is>
+          <t>5802</t>
         </is>
       </c>
     </row>
@@ -3255,7 +3531,13 @@
       <c r="P47" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q47" t="inlineStr">
+      <c r="Q47" t="n">
+        <v>3035</v>
+      </c>
+      <c r="R47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S47" t="inlineStr">
         <is>
           <t>3035</t>
         </is>
@@ -3316,9 +3598,15 @@
       <c r="P48" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="Q48" t="inlineStr">
-        <is>
-          <t>5788</t>
+      <c r="Q48" t="n">
+        <v>5788</v>
+      </c>
+      <c r="R48" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="S48" t="inlineStr">
+        <is>
+          <t>6067</t>
         </is>
       </c>
     </row>
@@ -3377,9 +3665,15 @@
       <c r="P49" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="Q49" t="inlineStr">
-        <is>
-          <t>4410</t>
+      <c r="Q49" t="n">
+        <v>4410</v>
+      </c>
+      <c r="R49" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="S49" t="inlineStr">
+        <is>
+          <t>4789</t>
         </is>
       </c>
     </row>
@@ -3438,9 +3732,15 @@
       <c r="P50" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="Q50" t="inlineStr">
-        <is>
-          <t>6028</t>
+      <c r="Q50" t="n">
+        <v>6028</v>
+      </c>
+      <c r="R50" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="S50" t="inlineStr">
+        <is>
+          <t>6370</t>
         </is>
       </c>
     </row>
@@ -3499,9 +3799,15 @@
       <c r="P51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q51" t="inlineStr">
-        <is>
-          <t>2908</t>
+      <c r="Q51" t="n">
+        <v>2908</v>
+      </c>
+      <c r="R51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S51" t="inlineStr">
+        <is>
+          <t>2907</t>
         </is>
       </c>
     </row>
@@ -3560,9 +3866,15 @@
       <c r="P52" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q52" t="inlineStr">
-        <is>
-          <t>2841</t>
+      <c r="Q52" t="n">
+        <v>2841</v>
+      </c>
+      <c r="R52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S52" t="inlineStr">
+        <is>
+          <t>2871</t>
         </is>
       </c>
     </row>
@@ -3621,7 +3933,13 @@
       <c r="P53" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="Q53" t="inlineStr">
+      <c r="Q53" t="n">
+        <v>3345</v>
+      </c>
+      <c r="R53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S53" t="inlineStr">
         <is>
           <t>3345</t>
         </is>
@@ -3682,9 +4000,15 @@
       <c r="P54" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="Q54" t="inlineStr">
-        <is>
-          <t>5444</t>
+      <c r="Q54" t="n">
+        <v>5444</v>
+      </c>
+      <c r="R54" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="S54" t="inlineStr">
+        <is>
+          <t>5638</t>
         </is>
       </c>
     </row>
@@ -3743,9 +4067,15 @@
       <c r="P55" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="Q55" t="inlineStr">
-        <is>
-          <t>4293</t>
+      <c r="Q55" t="n">
+        <v>4293</v>
+      </c>
+      <c r="R55" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="S55" t="inlineStr">
+        <is>
+          <t>4399</t>
         </is>
       </c>
     </row>
@@ -3804,9 +4134,15 @@
       <c r="P56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q56" t="inlineStr">
-        <is>
-          <t>4392</t>
+      <c r="Q56" t="n">
+        <v>4392</v>
+      </c>
+      <c r="R56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S56" t="inlineStr">
+        <is>
+          <t>4596</t>
         </is>
       </c>
     </row>
@@ -3865,9 +4201,15 @@
       <c r="P57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q57" t="inlineStr">
-        <is>
-          <t>5071</t>
+      <c r="Q57" t="n">
+        <v>5071</v>
+      </c>
+      <c r="R57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S57" t="inlineStr">
+        <is>
+          <t>5254</t>
         </is>
       </c>
     </row>
@@ -3926,9 +4268,15 @@
       <c r="P58" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="Q58" t="inlineStr">
-        <is>
-          <t>4253</t>
+      <c r="Q58" t="n">
+        <v>4253</v>
+      </c>
+      <c r="R58" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="S58" t="inlineStr">
+        <is>
+          <t>4404</t>
         </is>
       </c>
     </row>
@@ -3987,9 +4335,15 @@
       <c r="P59" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q59" t="inlineStr">
-        <is>
-          <t>4935</t>
+      <c r="Q59" t="n">
+        <v>4935</v>
+      </c>
+      <c r="R59" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S59" t="inlineStr">
+        <is>
+          <t>5169</t>
         </is>
       </c>
     </row>
@@ -4048,7 +4402,13 @@
       <c r="P60" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q60" t="inlineStr">
+      <c r="Q60" t="n">
+        <v>0</v>
+      </c>
+      <c r="R60" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S60" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4109,9 +4469,15 @@
       <c r="P61" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="Q61" t="inlineStr">
-        <is>
-          <t>5202</t>
+      <c r="Q61" t="n">
+        <v>5202</v>
+      </c>
+      <c r="R61" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="S61" t="inlineStr">
+        <is>
+          <t>5389</t>
         </is>
       </c>
     </row>
@@ -4170,7 +4536,13 @@
       <c r="P62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q62" t="inlineStr">
+      <c r="Q62" t="n">
+        <v>3036</v>
+      </c>
+      <c r="R62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S62" t="inlineStr">
         <is>
           <t>3036</t>
         </is>
@@ -4231,9 +4603,15 @@
       <c r="P63" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q63" t="inlineStr">
-        <is>
-          <t>3289</t>
+      <c r="Q63" t="n">
+        <v>3289</v>
+      </c>
+      <c r="R63" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S63" t="inlineStr">
+        <is>
+          <t>3523</t>
         </is>
       </c>
     </row>
@@ -4292,9 +4670,15 @@
       <c r="P64" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Q64" t="inlineStr">
-        <is>
-          <t>4910</t>
+      <c r="Q64" t="n">
+        <v>4910</v>
+      </c>
+      <c r="R64" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="S64" t="inlineStr">
+        <is>
+          <t>5088</t>
         </is>
       </c>
     </row>
@@ -4328,6 +4712,8 @@
       <c r="O65" t="inlineStr"/>
       <c r="P65" s="3" t="inlineStr"/>
       <c r="Q65" t="inlineStr"/>
+      <c r="R65" s="3" t="inlineStr"/>
+      <c r="S65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -4384,9 +4770,15 @@
       <c r="P66" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="Q66" t="inlineStr">
-        <is>
-          <t>5593</t>
+      <c r="Q66" t="n">
+        <v>5593</v>
+      </c>
+      <c r="R66" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S66" t="inlineStr">
+        <is>
+          <t>5843</t>
         </is>
       </c>
     </row>
@@ -4445,9 +4837,15 @@
       <c r="P67" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q67" t="inlineStr">
-        <is>
-          <t>4415</t>
+      <c r="Q67" t="n">
+        <v>4415</v>
+      </c>
+      <c r="R67" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S67" t="inlineStr">
+        <is>
+          <t>4549</t>
         </is>
       </c>
     </row>
@@ -4506,9 +4904,15 @@
       <c r="P68" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q68" t="inlineStr">
-        <is>
-          <t>3623</t>
+      <c r="Q68" t="n">
+        <v>3623</v>
+      </c>
+      <c r="R68" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S68" t="inlineStr">
+        <is>
+          <t>4025</t>
         </is>
       </c>
     </row>
@@ -4567,9 +4971,15 @@
       <c r="P69" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Q69" t="inlineStr">
-        <is>
-          <t>4345</t>
+      <c r="Q69" t="n">
+        <v>4345</v>
+      </c>
+      <c r="R69" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="S69" t="inlineStr">
+        <is>
+          <t>4314</t>
         </is>
       </c>
     </row>
@@ -4628,9 +5038,15 @@
       <c r="P70" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q70" t="inlineStr">
-        <is>
-          <t>4050</t>
+      <c r="Q70" t="n">
+        <v>4050</v>
+      </c>
+      <c r="R70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S70" t="inlineStr">
+        <is>
+          <t>4106</t>
         </is>
       </c>
     </row>
@@ -4689,9 +5105,15 @@
       <c r="P71" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q71" t="inlineStr">
-        <is>
-          <t>4357</t>
+      <c r="Q71" t="n">
+        <v>4357</v>
+      </c>
+      <c r="R71" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S71" t="inlineStr">
+        <is>
+          <t>4413</t>
         </is>
       </c>
     </row>
@@ -4750,9 +5172,15 @@
       <c r="P72" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q72" t="inlineStr">
-        <is>
-          <t>3687</t>
+      <c r="Q72" t="n">
+        <v>3687</v>
+      </c>
+      <c r="R72" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S72" t="inlineStr">
+        <is>
+          <t>4121</t>
         </is>
       </c>
     </row>
@@ -4811,9 +5239,15 @@
       <c r="P73" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="Q73" t="inlineStr">
-        <is>
-          <t>3925</t>
+      <c r="Q73" t="n">
+        <v>3925</v>
+      </c>
+      <c r="R73" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="S73" t="inlineStr">
+        <is>
+          <t>4123</t>
         </is>
       </c>
     </row>
@@ -4872,9 +5306,15 @@
       <c r="P74" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q74" t="inlineStr">
-        <is>
-          <t>4897</t>
+      <c r="Q74" t="n">
+        <v>4897</v>
+      </c>
+      <c r="R74" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="S74" t="inlineStr">
+        <is>
+          <t>5085</t>
         </is>
       </c>
     </row>
@@ -4933,9 +5373,15 @@
       <c r="P75" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="Q75" t="inlineStr">
-        <is>
-          <t>4917</t>
+      <c r="Q75" t="n">
+        <v>4917</v>
+      </c>
+      <c r="R75" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S75" t="inlineStr">
+        <is>
+          <t>5152</t>
         </is>
       </c>
     </row>
@@ -4969,6 +5415,8 @@
       <c r="O76" t="inlineStr"/>
       <c r="P76" s="3" t="inlineStr"/>
       <c r="Q76" t="inlineStr"/>
+      <c r="R76" s="3" t="inlineStr"/>
+      <c r="S76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -5025,9 +5473,15 @@
       <c r="P77" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q77" t="inlineStr">
-        <is>
-          <t>4987</t>
+      <c r="Q77" t="n">
+        <v>4987</v>
+      </c>
+      <c r="R77" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S77" t="inlineStr">
+        <is>
+          <t>5236</t>
         </is>
       </c>
     </row>
@@ -5086,7 +5540,13 @@
       <c r="P78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q78" t="inlineStr">
+      <c r="Q78" t="n">
+        <v>2500</v>
+      </c>
+      <c r="R78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S78" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -5147,9 +5607,15 @@
       <c r="P79" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q79" t="inlineStr">
-        <is>
-          <t>4604</t>
+      <c r="Q79" t="n">
+        <v>4604</v>
+      </c>
+      <c r="R79" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S79" t="inlineStr">
+        <is>
+          <t>4788</t>
         </is>
       </c>
     </row>
@@ -5208,9 +5674,15 @@
       <c r="P80" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q80" t="inlineStr">
-        <is>
-          <t>4920</t>
+      <c r="Q80" t="n">
+        <v>4920</v>
+      </c>
+      <c r="R80" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="S80" t="inlineStr">
+        <is>
+          <t>4984</t>
         </is>
       </c>
     </row>
@@ -5269,9 +5741,15 @@
       <c r="P81" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="Q81" t="inlineStr">
-        <is>
-          <t>4643</t>
+      <c r="Q81" t="n">
+        <v>4643</v>
+      </c>
+      <c r="R81" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="S81" t="inlineStr">
+        <is>
+          <t>4922</t>
         </is>
       </c>
     </row>
@@ -5330,9 +5808,15 @@
       <c r="P82" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Q82" t="inlineStr">
-        <is>
-          <t>4348</t>
+      <c r="Q82" t="n">
+        <v>4348</v>
+      </c>
+      <c r="R82" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="S82" t="inlineStr">
+        <is>
+          <t>4561</t>
         </is>
       </c>
     </row>
@@ -5366,6 +5850,8 @@
       <c r="O83" t="inlineStr"/>
       <c r="P83" s="3" t="inlineStr"/>
       <c r="Q83" t="inlineStr"/>
+      <c r="R83" s="3" t="inlineStr"/>
+      <c r="S83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -5422,9 +5908,15 @@
       <c r="P84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q84" t="inlineStr">
-        <is>
-          <t>3275</t>
+      <c r="Q84" t="n">
+        <v>3275</v>
+      </c>
+      <c r="R84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S84" t="inlineStr">
+        <is>
+          <t>3358</t>
         </is>
       </c>
     </row>
@@ -5483,9 +5975,15 @@
       <c r="P85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q85" t="inlineStr">
-        <is>
-          <t>3473</t>
+      <c r="Q85" t="n">
+        <v>3473</v>
+      </c>
+      <c r="R85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S85" t="inlineStr">
+        <is>
+          <t>3498</t>
         </is>
       </c>
     </row>
@@ -5544,9 +6042,15 @@
       <c r="P86" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="Q86" t="inlineStr">
-        <is>
-          <t>4730</t>
+      <c r="Q86" t="n">
+        <v>4730</v>
+      </c>
+      <c r="R86" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S86" t="inlineStr">
+        <is>
+          <t>4696</t>
         </is>
       </c>
     </row>
@@ -5605,9 +6109,15 @@
       <c r="P87" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q87" t="inlineStr">
-        <is>
-          <t>3028</t>
+      <c r="Q87" t="n">
+        <v>3028</v>
+      </c>
+      <c r="R87" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S87" t="inlineStr">
+        <is>
+          <t>3070</t>
         </is>
       </c>
     </row>
@@ -5666,9 +6176,15 @@
       <c r="P88" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Q88" t="inlineStr">
-        <is>
-          <t>3330</t>
+      <c r="Q88" t="n">
+        <v>3330</v>
+      </c>
+      <c r="R88" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="S88" t="inlineStr">
+        <is>
+          <t>3451</t>
         </is>
       </c>
     </row>
@@ -5702,6 +6218,8 @@
       <c r="O89" t="inlineStr"/>
       <c r="P89" s="3" t="inlineStr"/>
       <c r="Q89" t="inlineStr"/>
+      <c r="R89" s="3" t="inlineStr"/>
+      <c r="S89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -5758,9 +6276,15 @@
       <c r="P90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q90" t="inlineStr">
-        <is>
-          <t>2749</t>
+      <c r="Q90" t="n">
+        <v>2749</v>
+      </c>
+      <c r="R90" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S90" t="inlineStr">
+        <is>
+          <t>2876</t>
         </is>
       </c>
     </row>
@@ -5794,6 +6318,8 @@
       <c r="O91" t="inlineStr"/>
       <c r="P91" s="3" t="inlineStr"/>
       <c r="Q91" t="inlineStr"/>
+      <c r="R91" s="3" t="inlineStr"/>
+      <c r="S91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -5850,9 +6376,15 @@
       <c r="P92" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="Q92" t="inlineStr">
-        <is>
-          <t>2808</t>
+      <c r="Q92" t="n">
+        <v>2808</v>
+      </c>
+      <c r="R92" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="S92" t="inlineStr">
+        <is>
+          <t>2867</t>
         </is>
       </c>
     </row>
@@ -5911,9 +6443,15 @@
       <c r="P93" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="Q93" t="inlineStr">
-        <is>
-          <t>2702</t>
+      <c r="Q93" t="n">
+        <v>2702</v>
+      </c>
+      <c r="R93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S93" t="inlineStr">
+        <is>
+          <t>2522</t>
         </is>
       </c>
     </row>
@@ -5972,9 +6510,15 @@
       <c r="P94" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="Q94" t="inlineStr">
-        <is>
-          <t>3040</t>
+      <c r="Q94" t="n">
+        <v>3040</v>
+      </c>
+      <c r="R94" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S94" t="inlineStr">
+        <is>
+          <t>3305</t>
         </is>
       </c>
     </row>
@@ -6033,9 +6577,15 @@
       <c r="P95" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="Q95" t="inlineStr">
-        <is>
-          <t>2799</t>
+      <c r="Q95" t="n">
+        <v>2799</v>
+      </c>
+      <c r="R95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S95" t="inlineStr">
+        <is>
+          <t>2772</t>
         </is>
       </c>
     </row>
@@ -6094,9 +6644,15 @@
       <c r="P96" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="Q96" t="inlineStr">
-        <is>
-          <t>2386</t>
+      <c r="Q96" t="n">
+        <v>2386</v>
+      </c>
+      <c r="R96" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="S96" t="inlineStr">
+        <is>
+          <t>2607</t>
         </is>
       </c>
     </row>
@@ -6155,9 +6711,15 @@
       <c r="P97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q97" t="inlineStr">
-        <is>
-          <t>2667</t>
+      <c r="Q97" t="n">
+        <v>2667</v>
+      </c>
+      <c r="R97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S97" t="inlineStr">
+        <is>
+          <t>2683</t>
         </is>
       </c>
     </row>
@@ -6216,9 +6778,15 @@
       <c r="P98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q98" t="inlineStr">
-        <is>
-          <t>2243</t>
+      <c r="Q98" t="n">
+        <v>2243</v>
+      </c>
+      <c r="R98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S98" t="inlineStr">
+        <is>
+          <t>2240</t>
         </is>
       </c>
     </row>
@@ -6277,9 +6845,15 @@
       <c r="P99" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="Q99" t="inlineStr">
-        <is>
-          <t>3829</t>
+      <c r="Q99" t="n">
+        <v>3829</v>
+      </c>
+      <c r="R99" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="S99" t="inlineStr">
+        <is>
+          <t>3822</t>
         </is>
       </c>
     </row>
@@ -6338,9 +6912,15 @@
       <c r="P100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q100" t="inlineStr">
-        <is>
-          <t>2453</t>
+      <c r="Q100" t="n">
+        <v>2453</v>
+      </c>
+      <c r="R100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S100" t="inlineStr">
+        <is>
+          <t>2432</t>
         </is>
       </c>
     </row>
@@ -6399,9 +6979,15 @@
       <c r="P101" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q101" t="inlineStr">
-        <is>
-          <t>4299</t>
+      <c r="Q101" t="n">
+        <v>4299</v>
+      </c>
+      <c r="R101" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S101" t="inlineStr">
+        <is>
+          <t>4435</t>
         </is>
       </c>
     </row>
@@ -6460,9 +7046,15 @@
       <c r="P102" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q102" t="inlineStr">
-        <is>
-          <t>4036</t>
+      <c r="Q102" t="n">
+        <v>4036</v>
+      </c>
+      <c r="R102" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S102" t="inlineStr">
+        <is>
+          <t>4082</t>
         </is>
       </c>
     </row>
@@ -6521,9 +7113,15 @@
       <c r="P103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q103" t="inlineStr">
-        <is>
-          <t>3610</t>
+      <c r="Q103" t="n">
+        <v>3610</v>
+      </c>
+      <c r="R103" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="S103" t="inlineStr">
+        <is>
+          <t>3849</t>
         </is>
       </c>
     </row>
@@ -6582,9 +7180,15 @@
       <c r="P104" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="Q104" t="inlineStr">
-        <is>
-          <t>4324</t>
+      <c r="Q104" t="n">
+        <v>4324</v>
+      </c>
+      <c r="R104" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="S104" t="inlineStr">
+        <is>
+          <t>4494</t>
         </is>
       </c>
     </row>
@@ -6643,9 +7247,15 @@
       <c r="P105" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="Q105" t="inlineStr">
-        <is>
-          <t>3858</t>
+      <c r="Q105" t="n">
+        <v>3858</v>
+      </c>
+      <c r="R105" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="S105" t="inlineStr">
+        <is>
+          <t>4030</t>
         </is>
       </c>
     </row>
@@ -6704,9 +7314,15 @@
       <c r="P106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q106" t="inlineStr">
-        <is>
-          <t>2386</t>
+      <c r="Q106" t="n">
+        <v>2386</v>
+      </c>
+      <c r="R106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S106" t="inlineStr">
+        <is>
+          <t>2369</t>
         </is>
       </c>
     </row>
@@ -6765,9 +7381,15 @@
       <c r="P107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q107" t="inlineStr">
-        <is>
-          <t>2671</t>
+      <c r="Q107" t="n">
+        <v>2671</v>
+      </c>
+      <c r="R107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S107" t="inlineStr">
+        <is>
+          <t>2680</t>
         </is>
       </c>
     </row>
@@ -6826,9 +7448,15 @@
       <c r="P108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q108" t="inlineStr">
-        <is>
-          <t>2745</t>
+      <c r="Q108" t="n">
+        <v>2745</v>
+      </c>
+      <c r="R108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S108" t="inlineStr">
+        <is>
+          <t>2776</t>
         </is>
       </c>
     </row>
@@ -6887,9 +7515,15 @@
       <c r="P109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q109" t="inlineStr">
-        <is>
-          <t>3823</t>
+      <c r="Q109" t="n">
+        <v>3823</v>
+      </c>
+      <c r="R109" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="S109" t="inlineStr">
+        <is>
+          <t>3997</t>
         </is>
       </c>
     </row>
@@ -6948,9 +7582,15 @@
       <c r="P110" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="Q110" t="inlineStr">
-        <is>
-          <t>3595</t>
+      <c r="Q110" t="n">
+        <v>3595</v>
+      </c>
+      <c r="R110" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="S110" t="inlineStr">
+        <is>
+          <t>3657</t>
         </is>
       </c>
     </row>
@@ -7009,9 +7649,15 @@
       <c r="P111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q111" t="inlineStr">
-        <is>
-          <t>2914</t>
+      <c r="Q111" t="n">
+        <v>2914</v>
+      </c>
+      <c r="R111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S111" t="inlineStr">
+        <is>
+          <t>2952</t>
         </is>
       </c>
     </row>
@@ -7070,9 +7716,15 @@
       <c r="P112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q112" t="inlineStr">
-        <is>
-          <t>3152</t>
+      <c r="Q112" t="n">
+        <v>3152</v>
+      </c>
+      <c r="R112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S112" t="inlineStr">
+        <is>
+          <t>3168</t>
         </is>
       </c>
     </row>
@@ -7131,9 +7783,15 @@
       <c r="P113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q113" t="inlineStr">
-        <is>
-          <t>3496</t>
+      <c r="Q113" t="n">
+        <v>3496</v>
+      </c>
+      <c r="R113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S113" t="inlineStr">
+        <is>
+          <t>3609</t>
         </is>
       </c>
     </row>
@@ -7192,9 +7850,15 @@
       <c r="P114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q114" t="inlineStr">
-        <is>
-          <t>3778</t>
+      <c r="Q114" t="n">
+        <v>3778</v>
+      </c>
+      <c r="R114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S114" t="inlineStr">
+        <is>
+          <t>3857</t>
         </is>
       </c>
     </row>
@@ -7236,6 +7900,8 @@
       <c r="O115" t="inlineStr"/>
       <c r="P115" s="3" t="inlineStr"/>
       <c r="Q115" t="inlineStr"/>
+      <c r="R115" s="3" t="inlineStr"/>
+      <c r="S115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -7292,9 +7958,15 @@
       <c r="P116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q116" t="inlineStr">
-        <is>
-          <t>2515</t>
+      <c r="Q116" t="n">
+        <v>2515</v>
+      </c>
+      <c r="R116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S116" t="inlineStr">
+        <is>
+          <t>2508</t>
         </is>
       </c>
     </row>
@@ -7353,9 +8025,15 @@
       <c r="P117" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="Q117" t="inlineStr">
-        <is>
-          <t>3227</t>
+      <c r="Q117" t="n">
+        <v>3227</v>
+      </c>
+      <c r="R117" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="S117" t="inlineStr">
+        <is>
+          <t>3319</t>
         </is>
       </c>
     </row>
@@ -7414,9 +8092,15 @@
       <c r="P118" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q118" t="inlineStr">
-        <is>
-          <t>3670</t>
+      <c r="Q118" t="n">
+        <v>3670</v>
+      </c>
+      <c r="R118" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="S118" t="inlineStr">
+        <is>
+          <t>3860</t>
         </is>
       </c>
     </row>
@@ -7475,7 +8159,13 @@
       <c r="P119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q119" t="inlineStr">
+      <c r="Q119" t="n">
+        <v>0</v>
+      </c>
+      <c r="R119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S119" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7536,9 +8226,15 @@
       <c r="P120" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="Q120" t="inlineStr">
-        <is>
-          <t>3958</t>
+      <c r="Q120" t="n">
+        <v>3958</v>
+      </c>
+      <c r="R120" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="S120" t="inlineStr">
+        <is>
+          <t>3991</t>
         </is>
       </c>
     </row>
@@ -7597,9 +8293,15 @@
       <c r="P121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q121" t="inlineStr">
-        <is>
-          <t>2683</t>
+      <c r="Q121" t="n">
+        <v>2683</v>
+      </c>
+      <c r="R121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S121" t="inlineStr">
+        <is>
+          <t>2695</t>
         </is>
       </c>
     </row>
@@ -7658,9 +8360,15 @@
       <c r="P122" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="Q122" t="inlineStr">
-        <is>
-          <t>3107</t>
+      <c r="Q122" t="n">
+        <v>3107</v>
+      </c>
+      <c r="R122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S122" t="inlineStr">
+        <is>
+          <t>3130</t>
         </is>
       </c>
     </row>
@@ -7719,9 +8427,15 @@
       <c r="P123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q123" t="inlineStr">
-        <is>
-          <t>2597</t>
+      <c r="Q123" t="n">
+        <v>2597</v>
+      </c>
+      <c r="R123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S123" t="inlineStr">
+        <is>
+          <t>2587</t>
         </is>
       </c>
     </row>
@@ -7780,9 +8494,15 @@
       <c r="P124" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q124" t="inlineStr">
-        <is>
-          <t>3319</t>
+      <c r="Q124" t="n">
+        <v>3319</v>
+      </c>
+      <c r="R124" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S124" t="inlineStr">
+        <is>
+          <t>3408</t>
         </is>
       </c>
     </row>
@@ -7841,9 +8561,15 @@
       <c r="P125" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="Q125" t="inlineStr">
-        <is>
-          <t>3322</t>
+      <c r="Q125" t="n">
+        <v>3322</v>
+      </c>
+      <c r="R125" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="S125" t="inlineStr">
+        <is>
+          <t>3358</t>
         </is>
       </c>
     </row>
@@ -7902,9 +8628,15 @@
       <c r="P126" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q126" t="inlineStr">
-        <is>
-          <t>3761</t>
+      <c r="Q126" t="n">
+        <v>3761</v>
+      </c>
+      <c r="R126" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S126" t="inlineStr">
+        <is>
+          <t>3794</t>
         </is>
       </c>
     </row>
@@ -7963,9 +8695,15 @@
       <c r="P127" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q127" t="inlineStr">
-        <is>
-          <t>3336</t>
+      <c r="Q127" t="n">
+        <v>3336</v>
+      </c>
+      <c r="R127" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="S127" t="inlineStr">
+        <is>
+          <t>3319</t>
         </is>
       </c>
     </row>
@@ -8024,7 +8762,13 @@
       <c r="P128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q128" t="inlineStr">
+      <c r="Q128" t="n">
+        <v>0</v>
+      </c>
+      <c r="R128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S128" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8085,7 +8829,13 @@
       <c r="P129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q129" t="inlineStr">
+      <c r="Q129" t="n">
+        <v>0</v>
+      </c>
+      <c r="R129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8146,9 +8896,15 @@
       <c r="P130" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="Q130" t="inlineStr">
-        <is>
-          <t>3045</t>
+      <c r="Q130" t="n">
+        <v>3045</v>
+      </c>
+      <c r="R130" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="S130" t="inlineStr">
+        <is>
+          <t>3084</t>
         </is>
       </c>
     </row>
@@ -8207,9 +8963,15 @@
       <c r="P131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q131" t="inlineStr">
-        <is>
-          <t>2814</t>
+      <c r="Q131" t="n">
+        <v>2814</v>
+      </c>
+      <c r="R131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S131" t="inlineStr">
+        <is>
+          <t>2815</t>
         </is>
       </c>
     </row>
@@ -8268,7 +9030,13 @@
       <c r="P132" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q132" t="inlineStr">
+      <c r="Q132" t="n">
+        <v>0</v>
+      </c>
+      <c r="R132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S132" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8329,9 +9097,15 @@
       <c r="P133" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="Q133" t="inlineStr">
-        <is>
-          <t>2242</t>
+      <c r="Q133" t="n">
+        <v>2242</v>
+      </c>
+      <c r="R133" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="S133" t="inlineStr">
+        <is>
+          <t>2277</t>
         </is>
       </c>
     </row>
@@ -8390,9 +9164,15 @@
       <c r="P134" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q134" t="inlineStr">
-        <is>
-          <t>3034</t>
+      <c r="Q134" t="n">
+        <v>3034</v>
+      </c>
+      <c r="R134" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S134" t="inlineStr">
+        <is>
+          <t>3105</t>
         </is>
       </c>
     </row>
@@ -8451,9 +9231,15 @@
       <c r="P135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q135" t="inlineStr">
-        <is>
-          <t>2498</t>
+      <c r="Q135" t="n">
+        <v>2498</v>
+      </c>
+      <c r="R135" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S135" t="inlineStr">
+        <is>
+          <t>2530</t>
         </is>
       </c>
     </row>
@@ -8512,9 +9298,15 @@
       <c r="P136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q136" t="inlineStr">
-        <is>
-          <t>998</t>
+      <c r="Q136" t="n">
+        <v>998</v>
+      </c>
+      <c r="R136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S136" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -8564,6 +9356,8 @@
       <c r="O137" t="inlineStr"/>
       <c r="P137" s="3" t="inlineStr"/>
       <c r="Q137" t="inlineStr"/>
+      <c r="R137" s="3" t="inlineStr"/>
+      <c r="S137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="n">
@@ -8620,9 +9414,15 @@
       <c r="P138" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="Q138" t="inlineStr">
-        <is>
-          <t>3176</t>
+      <c r="Q138" t="n">
+        <v>3176</v>
+      </c>
+      <c r="R138" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S138" t="inlineStr">
+        <is>
+          <t>3369</t>
         </is>
       </c>
     </row>
@@ -8681,11 +9481,11 @@
       <c r="P139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q139" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="Q139" t="n">
+        <v>0</v>
+      </c>
+      <c r="R139" s="3" t="inlineStr"/>
+      <c r="S139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -8742,9 +9542,15 @@
       <c r="P140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q140" t="inlineStr">
-        <is>
-          <t>2647</t>
+      <c r="Q140" t="n">
+        <v>2647</v>
+      </c>
+      <c r="R140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S140" t="inlineStr">
+        <is>
+          <t>2641</t>
         </is>
       </c>
     </row>
@@ -8794,6 +9600,8 @@
       <c r="O141" t="inlineStr"/>
       <c r="P141" s="3" t="inlineStr"/>
       <c r="Q141" t="inlineStr"/>
+      <c r="R141" s="3" t="inlineStr"/>
+      <c r="S141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -8850,9 +9658,15 @@
       <c r="P142" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q142" t="inlineStr">
-        <is>
-          <t>3020</t>
+      <c r="Q142" t="n">
+        <v>3020</v>
+      </c>
+      <c r="R142" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S142" t="inlineStr">
+        <is>
+          <t>3138</t>
         </is>
       </c>
     </row>
@@ -8886,6 +9700,8 @@
       <c r="O143" t="inlineStr"/>
       <c r="P143" s="3" t="inlineStr"/>
       <c r="Q143" t="inlineStr"/>
+      <c r="R143" s="3" t="inlineStr"/>
+      <c r="S143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -8942,9 +9758,15 @@
       <c r="P144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q144" t="inlineStr">
-        <is>
-          <t>2479</t>
+      <c r="Q144" t="n">
+        <v>2479</v>
+      </c>
+      <c r="R144" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="S144" t="inlineStr">
+        <is>
+          <t>2482</t>
         </is>
       </c>
     </row>
@@ -9003,7 +9825,13 @@
       <c r="P145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q145" t="inlineStr">
+      <c r="Q145" t="n">
+        <v>0</v>
+      </c>
+      <c r="R145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S145" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9064,11 +9892,11 @@
       <c r="P146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q146" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="Q146" t="n">
+        <v>0</v>
+      </c>
+      <c r="R146" s="3" t="inlineStr"/>
+      <c r="S146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -9125,11 +9953,11 @@
       <c r="P147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q147" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="Q147" t="n">
+        <v>0</v>
+      </c>
+      <c r="R147" s="3" t="inlineStr"/>
+      <c r="S147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -9177,6 +10005,8 @@
       <c r="O148" t="inlineStr"/>
       <c r="P148" s="3" t="inlineStr"/>
       <c r="Q148" t="inlineStr"/>
+      <c r="R148" s="3" t="inlineStr"/>
+      <c r="S148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="n">
@@ -9224,6 +10054,8 @@
       <c r="O149" t="inlineStr"/>
       <c r="P149" s="3" t="inlineStr"/>
       <c r="Q149" t="inlineStr"/>
+      <c r="R149" s="3" t="inlineStr"/>
+      <c r="S149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="n">
@@ -9280,9 +10112,15 @@
       <c r="P150" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="Q150" t="inlineStr">
-        <is>
-          <t>2461</t>
+      <c r="Q150" t="n">
+        <v>2461</v>
+      </c>
+      <c r="R150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S150" t="inlineStr">
+        <is>
+          <t>2419</t>
         </is>
       </c>
     </row>
@@ -9341,7 +10179,13 @@
       <c r="P151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q151" t="inlineStr">
+      <c r="Q151" t="n">
+        <v>0</v>
+      </c>
+      <c r="R151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S151" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9402,9 +10246,15 @@
       <c r="P152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q152" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="Q152" t="n">
+        <v>0</v>
+      </c>
+      <c r="R152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S152" t="inlineStr">
+        <is>
+          <t>1597</t>
         </is>
       </c>
     </row>
@@ -9463,9 +10313,15 @@
       <c r="P153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q153" t="inlineStr">
-        <is>
-          <t>1780</t>
+      <c r="Q153" t="n">
+        <v>1780</v>
+      </c>
+      <c r="R153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S153" t="inlineStr">
+        <is>
+          <t>1751</t>
         </is>
       </c>
     </row>
@@ -9515,6 +10371,8 @@
       <c r="O154" t="inlineStr"/>
       <c r="P154" s="3" t="inlineStr"/>
       <c r="Q154" t="inlineStr"/>
+      <c r="R154" s="3" t="inlineStr"/>
+      <c r="S154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" t="n">
@@ -9571,9 +10429,15 @@
       <c r="P155" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="Q155" t="inlineStr">
-        <is>
-          <t>5362</t>
+      <c r="Q155" t="n">
+        <v>5362</v>
+      </c>
+      <c r="R155" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="S155" t="inlineStr">
+        <is>
+          <t>5560</t>
         </is>
       </c>
     </row>
@@ -9632,7 +10496,13 @@
       <c r="P156" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q156" t="inlineStr">
+      <c r="Q156" t="n">
+        <v>0</v>
+      </c>
+      <c r="R156" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S156" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9693,7 +10563,13 @@
       <c r="P157" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q157" t="inlineStr">
+      <c r="Q157" t="n">
+        <v>2500</v>
+      </c>
+      <c r="R157" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S157" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -9754,9 +10630,15 @@
       <c r="P158" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="Q158" t="inlineStr">
-        <is>
-          <t>5677</t>
+      <c r="Q158" t="n">
+        <v>5677</v>
+      </c>
+      <c r="R158" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="S158" t="inlineStr">
+        <is>
+          <t>6016</t>
         </is>
       </c>
     </row>
@@ -9815,7 +10697,13 @@
       <c r="P159" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q159" t="inlineStr">
+      <c r="Q159" t="n">
+        <v>0</v>
+      </c>
+      <c r="R159" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S159" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9876,9 +10764,15 @@
       <c r="P160" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q160" t="inlineStr">
-        <is>
-          <t>3098</t>
+      <c r="Q160" t="n">
+        <v>3098</v>
+      </c>
+      <c r="R160" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S160" t="inlineStr">
+        <is>
+          <t>3150</t>
         </is>
       </c>
     </row>
@@ -9937,7 +10831,13 @@
       <c r="P161" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q161" t="inlineStr">
+      <c r="Q161" t="n">
+        <v>0</v>
+      </c>
+      <c r="R161" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S161" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9998,9 +10898,15 @@
       <c r="P162" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q162" t="inlineStr">
-        <is>
-          <t>3060</t>
+      <c r="Q162" t="n">
+        <v>3060</v>
+      </c>
+      <c r="R162" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S162" t="inlineStr">
+        <is>
+          <t>3088</t>
         </is>
       </c>
     </row>
@@ -10034,6 +10940,8 @@
       <c r="O163" t="inlineStr"/>
       <c r="P163" s="3" t="inlineStr"/>
       <c r="Q163" t="inlineStr"/>
+      <c r="R163" s="3" t="inlineStr"/>
+      <c r="S163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" t="n">
@@ -10084,9 +10992,15 @@
       <c r="P164" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="Q164" t="inlineStr">
-        <is>
-          <t>2804</t>
+      <c r="Q164" t="n">
+        <v>2804</v>
+      </c>
+      <c r="R164" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="S164" t="inlineStr">
+        <is>
+          <t>2882</t>
         </is>
       </c>
     </row>
@@ -10130,6 +11044,8 @@
       <c r="O165" t="inlineStr"/>
       <c r="P165" s="3" t="inlineStr"/>
       <c r="Q165" t="inlineStr"/>
+      <c r="R165" s="3" t="inlineStr"/>
+      <c r="S165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" t="n">
@@ -10180,9 +11096,15 @@
       <c r="P166" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q166" t="inlineStr">
-        <is>
-          <t>2356</t>
+      <c r="Q166" t="n">
+        <v>2356</v>
+      </c>
+      <c r="R166" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S166" t="inlineStr">
+        <is>
+          <t>2348</t>
         </is>
       </c>
     </row>
@@ -10235,9 +11157,15 @@
       <c r="P167" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q167" t="inlineStr">
-        <is>
-          <t>1408</t>
+      <c r="Q167" t="n">
+        <v>1408</v>
+      </c>
+      <c r="R167" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S167" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -10286,17 +11214,21 @@
       <c r="P168" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="Q168" t="inlineStr">
-        <is>
-          <t>1603</t>
+      <c r="Q168" t="n">
+        <v>1603</v>
+      </c>
+      <c r="R168" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S168" t="inlineStr">
+        <is>
+          <t>1587</t>
         </is>
       </c>
     </row>
     <row r="169">
-      <c r="A169" t="inlineStr">
-        <is>
-          <t>58641574</t>
-        </is>
+      <c r="A169" t="n">
+        <v>58641574</v>
       </c>
       <c r="B169" t="inlineStr">
         <is>
@@ -10323,9 +11255,171 @@
       <c r="P169" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q169" t="inlineStr">
-        <is>
-          <t>2615</t>
+      <c r="Q169" t="n">
+        <v>2615</v>
+      </c>
+      <c r="R169" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S169" t="inlineStr">
+        <is>
+          <t>2748</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>57551884</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>|maaz|</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr"/>
+      <c r="D170" t="inlineStr"/>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F170" s="3" t="inlineStr"/>
+      <c r="G170" t="inlineStr"/>
+      <c r="H170" s="3" t="inlineStr"/>
+      <c r="I170" t="inlineStr"/>
+      <c r="J170" s="3" t="inlineStr"/>
+      <c r="K170" t="inlineStr"/>
+      <c r="L170" s="3" t="inlineStr"/>
+      <c r="M170" t="inlineStr"/>
+      <c r="N170" s="3" t="inlineStr"/>
+      <c r="O170" t="inlineStr"/>
+      <c r="P170" s="3" t="inlineStr"/>
+      <c r="Q170" t="inlineStr"/>
+      <c r="R170" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="S170" t="inlineStr">
+        <is>
+          <t>3111</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>9212603</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>KymBaoNgoc</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr"/>
+      <c r="D171" t="inlineStr"/>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F171" s="3" t="inlineStr"/>
+      <c r="G171" t="inlineStr"/>
+      <c r="H171" s="3" t="inlineStr"/>
+      <c r="I171" t="inlineStr"/>
+      <c r="J171" s="3" t="inlineStr"/>
+      <c r="K171" t="inlineStr"/>
+      <c r="L171" s="3" t="inlineStr"/>
+      <c r="M171" t="inlineStr"/>
+      <c r="N171" s="3" t="inlineStr"/>
+      <c r="O171" t="inlineStr"/>
+      <c r="P171" s="3" t="inlineStr"/>
+      <c r="Q171" t="inlineStr"/>
+      <c r="R171" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S171" t="inlineStr">
+        <is>
+          <t>4202</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>11548491</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>"Thương VNG"</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr"/>
+      <c r="D172" t="inlineStr"/>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F172" s="3" t="inlineStr"/>
+      <c r="G172" t="inlineStr"/>
+      <c r="H172" s="3" t="inlineStr"/>
+      <c r="I172" t="inlineStr"/>
+      <c r="J172" s="3" t="inlineStr"/>
+      <c r="K172" t="inlineStr"/>
+      <c r="L172" s="3" t="inlineStr"/>
+      <c r="M172" t="inlineStr"/>
+      <c r="N172" s="3" t="inlineStr"/>
+      <c r="O172" t="inlineStr"/>
+      <c r="P172" s="3" t="inlineStr"/>
+      <c r="Q172" t="inlineStr"/>
+      <c r="R172" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S172" t="inlineStr">
+        <is>
+          <t>4335</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>20766468</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>Player-6160225</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr"/>
+      <c r="D173" t="inlineStr"/>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F173" s="3" t="inlineStr"/>
+      <c r="G173" t="inlineStr"/>
+      <c r="H173" s="3" t="inlineStr"/>
+      <c r="I173" t="inlineStr"/>
+      <c r="J173" s="3" t="inlineStr"/>
+      <c r="K173" t="inlineStr"/>
+      <c r="L173" s="3" t="inlineStr"/>
+      <c r="M173" t="inlineStr"/>
+      <c r="N173" s="3" t="inlineStr"/>
+      <c r="O173" t="inlineStr"/>
+      <c r="P173" s="3" t="inlineStr"/>
+      <c r="Q173" t="inlineStr"/>
+      <c r="R173" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="S173" t="inlineStr">
+        <is>
+          <t>4559</t>
         </is>
       </c>
     </row>

</xml_diff>